<commit_message>
Updated flags and analytes3 files
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4519" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A72F8220-D17A-4970-9343-C315C95C6D98}"/>
+  <xr:revisionPtr revIDLastSave="4560" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E529106A-931D-4D50-9093-CD3CC106C62F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="809" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="809" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="799">
   <si>
     <t>CodeName</t>
   </si>
@@ -2562,6 +2562,12 @@
   </si>
   <si>
     <t>Sodium, unfiltered</t>
+  </si>
+  <si>
+    <t>Removed because have in hydro</t>
+  </si>
+  <si>
+    <t>1m</t>
   </si>
 </sst>
 </file>
@@ -2893,17 +2899,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="5"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -2922,12 +2917,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3032,7 +3040,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3053,7 +3060,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3120,26 +3126,29 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3565,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23ABD6F-8266-4030-840C-1A1DE88549A1}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3818,7 +3827,7 @@
       <c r="A18" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="67" t="s">
         <v>787</v>
       </c>
       <c r="C18" t="s">
@@ -3874,7 +3883,7 @@
       <c r="A22" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="67" t="s">
         <v>789</v>
       </c>
       <c r="C22" t="s">
@@ -3930,7 +3939,7 @@
       <c r="A26" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="67" t="s">
         <v>791</v>
       </c>
       <c r="C26" t="s">
@@ -4014,7 +4023,7 @@
       <c r="A32" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="67" t="s">
         <v>63</v>
       </c>
       <c r="C32" t="s">
@@ -4028,7 +4037,7 @@
       <c r="A33" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="67" t="s">
         <v>792</v>
       </c>
       <c r="C33" t="s">
@@ -4294,7 +4303,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4310,10 +4319,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="100" t="s">
         <v>691</v>
       </c>
-      <c r="J1" s="82"/>
+      <c r="J1" s="80"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4329,7 +4338,7 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B2" t="s">
@@ -4341,13 +4350,13 @@
       <c r="G2" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="103" t="s">
+      <c r="I2" s="100" t="s">
         <v>691</v>
       </c>
       <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4363,10 +4372,10 @@
         <v>81</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="100" t="s">
         <v>691</v>
       </c>
-      <c r="J3" s="82"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -4382,7 +4391,7 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B4" t="s">
@@ -4394,13 +4403,13 @@
       <c r="G4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="103" t="s">
+      <c r="I4" s="100" t="s">
         <v>691</v>
       </c>
       <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B5" t="s">
@@ -4412,31 +4421,31 @@
       <c r="G5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="103" t="s">
+      <c r="I5" s="100" t="s">
         <v>691</v>
       </c>
       <c r="J5" s="59"/>
     </row>
-    <row r="6" spans="1:23" s="104" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="107" t="s">
+    <row r="6" spans="1:23" s="101" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="104" t="s">
         <v>701</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="G6" s="105" t="s">
+      <c r="G6" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="103" t="s">
+      <c r="I6" s="100" t="s">
         <v>691</v>
       </c>
-      <c r="J6" s="106"/>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="107" t="s">
+      <c r="A7" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B7" t="s">
@@ -4448,13 +4457,13 @@
       <c r="G7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="103" t="s">
+      <c r="I7" s="100" t="s">
         <v>691</v>
       </c>
       <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="104" t="s">
         <v>701</v>
       </c>
       <c r="B8" t="s">
@@ -4467,18 +4476,18 @@
       <c r="G8" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="I8" s="103" t="s">
+      <c r="I8" s="100" t="s">
         <v>691</v>
       </c>
       <c r="J8" s="59"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="104" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="104" t="s">
         <v>707</v>
       </c>
     </row>
@@ -5705,7 +5714,7 @@
       <c r="G9" t="s">
         <v>561</v>
       </c>
-      <c r="M9" s="100">
+      <c r="M9" s="98">
         <v>0.50069444399999996</v>
       </c>
     </row>
@@ -5725,7 +5734,7 @@
       <c r="G10" t="s">
         <v>580</v>
       </c>
-      <c r="M10" s="100">
+      <c r="M10" s="98">
         <v>0.45416600000000001</v>
       </c>
     </row>
@@ -5745,7 +5754,7 @@
       <c r="G11" t="s">
         <v>584</v>
       </c>
-      <c r="M11" s="100">
+      <c r="M11" s="98">
         <v>0.44791666699999999</v>
       </c>
     </row>
@@ -7475,8 +7484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5D57F1-DBF9-46B4-8278-09786D5200AB}">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="B37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7552,7 +7561,7 @@
       <c r="I2" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="66" t="s">
         <v>365</v>
       </c>
       <c r="K2" s="59" t="s">
@@ -7581,7 +7590,7 @@
       <c r="I3" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>369</v>
       </c>
       <c r="K3" s="59" t="s">
@@ -7699,7 +7708,7 @@
       <c r="G8" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="76" t="s">
+      <c r="H8" s="74" t="s">
         <v>135</v>
       </c>
       <c r="I8" t="s">
@@ -7725,7 +7734,7 @@
       <c r="G9" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="74" t="s">
         <v>135</v>
       </c>
       <c r="I9" t="s">
@@ -7778,7 +7787,7 @@
       <c r="I11" t="s">
         <v>113</v>
       </c>
-      <c r="J11" s="67"/>
+      <c r="J11" s="66"/>
       <c r="K11" s="59" t="s">
         <v>385</v>
       </c>
@@ -7803,7 +7812,7 @@
       <c r="I12" t="s">
         <v>113</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="66" t="s">
         <v>384</v>
       </c>
       <c r="K12" s="59" t="s">
@@ -7830,7 +7839,7 @@
       <c r="I13" t="s">
         <v>113</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="66" t="s">
         <v>384</v>
       </c>
       <c r="K13" s="59" t="s">
@@ -7857,7 +7866,7 @@
       <c r="I14" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="66" t="s">
         <v>384</v>
       </c>
       <c r="K14" s="59" t="s">
@@ -7955,7 +7964,7 @@
       <c r="I18" t="s">
         <v>113</v>
       </c>
-      <c r="J18" s="67"/>
+      <c r="J18" s="66"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -7996,7 +8005,7 @@
       <c r="G20" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="76" t="s">
+      <c r="H20" s="74" t="s">
         <v>135</v>
       </c>
       <c r="I20" s="46" t="s">
@@ -8031,10 +8040,10 @@
       <c r="I21" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="J21" s="67" t="s">
+      <c r="J21" s="66" t="s">
         <v>401</v>
       </c>
-      <c r="K21" s="67" t="s">
+      <c r="K21" s="66" t="s">
         <v>402</v>
       </c>
     </row>
@@ -8083,10 +8092,10 @@
       <c r="I23" t="s">
         <v>113</v>
       </c>
-      <c r="J23" s="67" t="s">
+      <c r="J23" s="66" t="s">
         <v>405</v>
       </c>
-      <c r="K23" s="67" t="s">
+      <c r="K23" s="66" t="s">
         <v>406</v>
       </c>
     </row>
@@ -8184,7 +8193,7 @@
       <c r="I27" t="s">
         <v>113</v>
       </c>
-      <c r="J27" s="67" t="s">
+      <c r="J27" s="66" t="s">
         <v>412</v>
       </c>
     </row>
@@ -8299,23 +8308,23 @@
       <c r="B32" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="71"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="4">
         <v>2021</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="H32" s="72" t="s">
+      <c r="H32" s="71" t="s">
         <v>83</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="J32" s="99" t="s">
+      <c r="J32" s="97" t="s">
         <v>422</v>
       </c>
-      <c r="K32" s="73"/>
+      <c r="K32" s="72"/>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -8339,7 +8348,7 @@
       <c r="J33" s="59" t="s">
         <v>425</v>
       </c>
-      <c r="K33" s="81" t="s">
+      <c r="K33" s="79" t="s">
         <v>426</v>
       </c>
     </row>
@@ -8497,7 +8506,7 @@
       <c r="F40">
         <v>2021</v>
       </c>
-      <c r="G40" s="78" t="s">
+      <c r="G40" s="76" t="s">
         <v>439</v>
       </c>
       <c r="H40" s="46" t="s">
@@ -8523,7 +8532,7 @@
       <c r="F41">
         <v>2021</v>
       </c>
-      <c r="G41" s="78" t="s">
+      <c r="G41" s="76" t="s">
         <v>439</v>
       </c>
       <c r="H41" s="46" t="s">
@@ -9005,10 +9014,10 @@
       <c r="I63" t="s">
         <v>421</v>
       </c>
-      <c r="J63" s="67" t="s">
+      <c r="J63" s="66" t="s">
         <v>477</v>
       </c>
-      <c r="K63" s="67" t="s">
+      <c r="K63" s="66" t="s">
         <v>478</v>
       </c>
     </row>
@@ -9099,7 +9108,7 @@
       <c r="B68" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="E68" s="98"/>
+      <c r="E68" s="96"/>
       <c r="F68" s="14">
         <v>2021</v>
       </c>
@@ -9112,10 +9121,10 @@
       <c r="I68" s="14" t="s">
         <v>421</v>
       </c>
-      <c r="J68" s="84" t="s">
+      <c r="J68" s="82" t="s">
         <v>485</v>
       </c>
-      <c r="K68" s="84"/>
+      <c r="K68" s="82"/>
     </row>
     <row r="69" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -9124,7 +9133,7 @@
       <c r="B69" s="46" t="s">
         <v>486</v>
       </c>
-      <c r="E69" s="97"/>
+      <c r="E69" s="95"/>
       <c r="F69" s="46">
         <v>2021</v>
       </c>
@@ -9137,10 +9146,10 @@
       <c r="I69" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J69" s="67" t="s">
+      <c r="J69" s="66" t="s">
         <v>487</v>
       </c>
-      <c r="K69" s="67"/>
+      <c r="K69" s="66"/>
     </row>
     <row r="70" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -9149,7 +9158,7 @@
       <c r="B70" s="46" t="s">
         <v>488</v>
       </c>
-      <c r="E70" s="97"/>
+      <c r="E70" s="95"/>
       <c r="F70" s="46">
         <v>2021</v>
       </c>
@@ -9162,10 +9171,10 @@
       <c r="I70" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J70" s="67" t="s">
+      <c r="J70" s="66" t="s">
         <v>489</v>
       </c>
-      <c r="K70" s="67"/>
+      <c r="K70" s="66"/>
     </row>
     <row r="71" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -9174,7 +9183,7 @@
       <c r="B71" s="46" t="s">
         <v>490</v>
       </c>
-      <c r="E71" s="97"/>
+      <c r="E71" s="95"/>
       <c r="F71" s="46">
         <v>2021</v>
       </c>
@@ -9187,10 +9196,10 @@
       <c r="I71" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J71" s="67" t="s">
+      <c r="J71" s="66" t="s">
         <v>491</v>
       </c>
-      <c r="K71" s="67"/>
+      <c r="K71" s="66"/>
     </row>
     <row r="72" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -9199,7 +9208,7 @@
       <c r="B72" s="46" t="s">
         <v>713</v>
       </c>
-      <c r="E72" s="97"/>
+      <c r="E72" s="95"/>
       <c r="F72" s="46">
         <v>2021</v>
       </c>
@@ -9212,10 +9221,10 @@
       <c r="I72" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J72" s="67" t="s">
+      <c r="J72" s="66" t="s">
         <v>494</v>
       </c>
-      <c r="K72" s="67"/>
+      <c r="K72" s="66"/>
     </row>
     <row r="73" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
@@ -9224,7 +9233,7 @@
       <c r="B73" s="46" t="s">
         <v>495</v>
       </c>
-      <c r="E73" s="97"/>
+      <c r="E73" s="95"/>
       <c r="F73" s="46">
         <v>2021</v>
       </c>
@@ -9237,10 +9246,10 @@
       <c r="I73" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J73" s="67" t="s">
+      <c r="J73" s="66" t="s">
         <v>496</v>
       </c>
-      <c r="K73" s="67"/>
+      <c r="K73" s="66"/>
     </row>
     <row r="74" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -9249,7 +9258,7 @@
       <c r="B74" s="46" t="s">
         <v>497</v>
       </c>
-      <c r="E74" s="97"/>
+      <c r="E74" s="95"/>
       <c r="F74" s="46">
         <v>2021</v>
       </c>
@@ -9262,10 +9271,10 @@
       <c r="I74" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J74" s="67" t="s">
+      <c r="J74" s="66" t="s">
         <v>498</v>
       </c>
-      <c r="K74" s="67"/>
+      <c r="K74" s="66"/>
     </row>
     <row r="75" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -9274,7 +9283,7 @@
       <c r="B75" s="46" t="s">
         <v>714</v>
       </c>
-      <c r="E75" s="97"/>
+      <c r="E75" s="95"/>
       <c r="F75" s="46">
         <v>2021</v>
       </c>
@@ -9287,10 +9296,10 @@
       <c r="I75" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J75" s="67" t="s">
+      <c r="J75" s="66" t="s">
         <v>500</v>
       </c>
-      <c r="K75" s="67"/>
+      <c r="K75" s="66"/>
     </row>
     <row r="76" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
@@ -9299,7 +9308,7 @@
       <c r="B76" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E76" s="97"/>
+      <c r="E76" s="95"/>
       <c r="F76" s="46">
         <v>2021</v>
       </c>
@@ -9312,10 +9321,10 @@
       <c r="I76" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J76" s="67" t="s">
+      <c r="J76" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="K76" s="67"/>
+      <c r="K76" s="66"/>
     </row>
     <row r="77" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
@@ -9324,7 +9333,7 @@
       <c r="B77" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="E77" s="97"/>
+      <c r="E77" s="95"/>
       <c r="F77" s="46">
         <v>2021</v>
       </c>
@@ -9337,10 +9346,10 @@
       <c r="I77" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J77" s="67" t="s">
+      <c r="J77" s="66" t="s">
         <v>653</v>
       </c>
-      <c r="K77" s="67"/>
+      <c r="K77" s="66"/>
     </row>
     <row r="78" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -9349,7 +9358,7 @@
       <c r="B78" s="46" t="s">
         <v>504</v>
       </c>
-      <c r="E78" s="97"/>
+      <c r="E78" s="95"/>
       <c r="F78" s="46">
         <v>2021</v>
       </c>
@@ -9362,10 +9371,10 @@
       <c r="I78" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J78" s="67" t="s">
+      <c r="J78" s="66" t="s">
         <v>505</v>
       </c>
-      <c r="K78" s="67"/>
+      <c r="K78" s="66"/>
     </row>
     <row r="79" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
@@ -9374,7 +9383,7 @@
       <c r="B79" s="46" t="s">
         <v>506</v>
       </c>
-      <c r="E79" s="97"/>
+      <c r="E79" s="95"/>
       <c r="F79" s="46">
         <v>2021</v>
       </c>
@@ -9387,10 +9396,10 @@
       <c r="I79" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J79" s="67" t="s">
+      <c r="J79" s="66" t="s">
         <v>505</v>
       </c>
-      <c r="K79" s="67"/>
+      <c r="K79" s="66"/>
     </row>
     <row r="80" spans="1:11" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
@@ -9399,7 +9408,7 @@
       <c r="B80" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E80" s="97" t="s">
+      <c r="E80" s="95" t="s">
         <v>507</v>
       </c>
       <c r="F80" s="46">
@@ -9414,10 +9423,10 @@
       <c r="I80" s="41" t="s">
         <v>508</v>
       </c>
-      <c r="J80" s="67" t="s">
+      <c r="J80" s="66" t="s">
         <v>509</v>
       </c>
-      <c r="K80" s="77" t="s">
+      <c r="K80" s="75" t="s">
         <v>510</v>
       </c>
     </row>
@@ -9428,7 +9437,7 @@
       <c r="B81" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="97" t="s">
+      <c r="E81" s="95" t="s">
         <v>507</v>
       </c>
       <c r="F81" s="46">
@@ -9443,10 +9452,10 @@
       <c r="I81" s="41" t="s">
         <v>508</v>
       </c>
-      <c r="J81" s="67" t="s">
+      <c r="J81" s="66" t="s">
         <v>509</v>
       </c>
-      <c r="K81" s="67"/>
+      <c r="K81" s="66"/>
     </row>
     <row r="82" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
@@ -9455,7 +9464,7 @@
       <c r="B82" s="46" t="s">
         <v>511</v>
       </c>
-      <c r="E82" s="97"/>
+      <c r="E82" s="95"/>
       <c r="F82" s="46">
         <v>2021</v>
       </c>
@@ -9468,25 +9477,25 @@
       <c r="I82" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="J82" s="67"/>
-      <c r="K82" s="67"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
     </row>
     <row r="83" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>550</v>
       </c>
-      <c r="B83" s="95" t="s">
+      <c r="B83" s="93" t="s">
         <v>484</v>
       </c>
-      <c r="C83" s="95" t="s">
+      <c r="C83" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="D83" s="95"/>
-      <c r="E83" s="96"/>
-      <c r="F83" s="95">
+      <c r="D83" s="93"/>
+      <c r="E83" s="94"/>
+      <c r="F83" s="93">
         <v>2010</v>
       </c>
-      <c r="G83" s="95" t="s">
+      <c r="G83" s="93" t="s">
         <v>512</v>
       </c>
       <c r="H83" s="4" t="s">
@@ -9495,24 +9504,24 @@
       <c r="I83" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="J83" s="73"/>
+      <c r="J83" s="72"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>550</v>
       </c>
-      <c r="B84" s="68" t="s">
+      <c r="B84" s="67" t="s">
         <v>484</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D84" s="68"/>
-      <c r="E84" s="94"/>
-      <c r="F84" s="68">
+      <c r="D84" s="67"/>
+      <c r="E84" s="92"/>
+      <c r="F84" s="67">
         <v>2010</v>
       </c>
-      <c r="G84" s="68" t="s">
+      <c r="G84" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H84" s="4" t="s">
@@ -9527,18 +9536,18 @@
       <c r="A85" t="s">
         <v>550</v>
       </c>
-      <c r="B85" s="68" t="s">
+      <c r="B85" s="67" t="s">
         <v>486</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D85" s="68"/>
-      <c r="E85" s="94"/>
-      <c r="F85" s="68">
+      <c r="D85" s="67"/>
+      <c r="E85" s="92"/>
+      <c r="F85" s="67">
         <v>2010</v>
       </c>
-      <c r="G85" s="68" t="s">
+      <c r="G85" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H85" t="s">
@@ -9553,18 +9562,18 @@
       <c r="A86" t="s">
         <v>550</v>
       </c>
-      <c r="B86" s="68" t="s">
+      <c r="B86" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D86" s="68"/>
-      <c r="E86" s="94"/>
-      <c r="F86" s="68">
+      <c r="D86" s="67"/>
+      <c r="E86" s="92"/>
+      <c r="F86" s="67">
         <v>2010</v>
       </c>
-      <c r="G86" s="68" t="s">
+      <c r="G86" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H86" s="7" t="s">
@@ -9579,18 +9588,18 @@
       <c r="A87" t="s">
         <v>550</v>
       </c>
-      <c r="B87" s="68" t="s">
+      <c r="B87" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D87" s="68"/>
-      <c r="E87" s="94"/>
-      <c r="F87" s="68">
+      <c r="D87" s="67"/>
+      <c r="E87" s="92"/>
+      <c r="F87" s="67">
         <v>2010</v>
       </c>
-      <c r="G87" s="68" t="s">
+      <c r="G87" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H87" s="7" t="s">
@@ -9605,18 +9614,18 @@
       <c r="A88" t="s">
         <v>550</v>
       </c>
-      <c r="B88" s="68" t="s">
+      <c r="B88" s="67" t="s">
         <v>488</v>
       </c>
-      <c r="C88" s="68" t="s">
+      <c r="C88" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D88" s="68"/>
-      <c r="E88" s="94"/>
-      <c r="F88" s="68">
+      <c r="D88" s="67"/>
+      <c r="E88" s="92"/>
+      <c r="F88" s="67">
         <v>2010</v>
       </c>
-      <c r="G88" s="68" t="s">
+      <c r="G88" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H88" s="7" t="s">
@@ -9631,18 +9640,18 @@
       <c r="A89" t="s">
         <v>550</v>
       </c>
-      <c r="B89" s="68" t="s">
+      <c r="B89" s="67" t="s">
         <v>488</v>
       </c>
-      <c r="C89" s="68" t="s">
+      <c r="C89" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D89" s="68"/>
-      <c r="E89" s="94"/>
-      <c r="F89" s="68">
+      <c r="D89" s="67"/>
+      <c r="E89" s="92"/>
+      <c r="F89" s="67">
         <v>2010</v>
       </c>
-      <c r="G89" s="68" t="s">
+      <c r="G89" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H89" s="7" t="s">
@@ -9657,18 +9666,18 @@
       <c r="A90" t="s">
         <v>550</v>
       </c>
-      <c r="B90" s="68" t="s">
+      <c r="B90" s="67" t="s">
         <v>490</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C90" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D90" s="68"/>
-      <c r="E90" s="94"/>
-      <c r="F90" s="68">
+      <c r="D90" s="67"/>
+      <c r="E90" s="92"/>
+      <c r="F90" s="67">
         <v>2010</v>
       </c>
-      <c r="G90" s="68" t="s">
+      <c r="G90" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H90" s="7" t="s">
@@ -9683,18 +9692,18 @@
       <c r="A91" t="s">
         <v>550</v>
       </c>
-      <c r="B91" s="68" t="s">
+      <c r="B91" s="67" t="s">
         <v>490</v>
       </c>
-      <c r="C91" s="68" t="s">
+      <c r="C91" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D91" s="68"/>
-      <c r="E91" s="94"/>
-      <c r="F91" s="68">
+      <c r="D91" s="67"/>
+      <c r="E91" s="92"/>
+      <c r="F91" s="67">
         <v>2010</v>
       </c>
-      <c r="G91" s="68" t="s">
+      <c r="G91" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H91" s="7" t="s">
@@ -9709,18 +9718,18 @@
       <c r="A92" t="s">
         <v>550</v>
       </c>
-      <c r="B92" s="68" t="s">
+      <c r="B92" s="67" t="s">
         <v>492</v>
       </c>
-      <c r="C92" s="68" t="s">
+      <c r="C92" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D92" s="68"/>
-      <c r="E92" s="94"/>
-      <c r="F92" s="68">
+      <c r="D92" s="67"/>
+      <c r="E92" s="92"/>
+      <c r="F92" s="67">
         <v>2010</v>
       </c>
-      <c r="G92" s="68" t="s">
+      <c r="G92" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H92" t="s">
@@ -9735,18 +9744,18 @@
       <c r="A93" t="s">
         <v>550</v>
       </c>
-      <c r="B93" s="68" t="s">
+      <c r="B93" s="67" t="s">
         <v>492</v>
       </c>
-      <c r="C93" s="68" t="s">
+      <c r="C93" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D93" s="68"/>
-      <c r="E93" s="94"/>
-      <c r="F93" s="68">
+      <c r="D93" s="67"/>
+      <c r="E93" s="92"/>
+      <c r="F93" s="67">
         <v>2010</v>
       </c>
-      <c r="G93" s="68" t="s">
+      <c r="G93" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H93" t="s">
@@ -9761,18 +9770,18 @@
       <c r="A94" t="s">
         <v>550</v>
       </c>
-      <c r="B94" s="68" t="s">
+      <c r="B94" s="67" t="s">
         <v>495</v>
       </c>
-      <c r="C94" s="68" t="s">
+      <c r="C94" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D94" s="68"/>
-      <c r="E94" s="94"/>
-      <c r="F94" s="68">
+      <c r="D94" s="67"/>
+      <c r="E94" s="92"/>
+      <c r="F94" s="67">
         <v>2010</v>
       </c>
-      <c r="G94" s="68" t="s">
+      <c r="G94" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H94" t="s">
@@ -9787,18 +9796,18 @@
       <c r="A95" t="s">
         <v>550</v>
       </c>
-      <c r="B95" s="68" t="s">
+      <c r="B95" s="67" t="s">
         <v>495</v>
       </c>
-      <c r="C95" s="68" t="s">
+      <c r="C95" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D95" s="68"/>
-      <c r="E95" s="94"/>
-      <c r="F95" s="68">
+      <c r="D95" s="67"/>
+      <c r="E95" s="92"/>
+      <c r="F95" s="67">
         <v>2010</v>
       </c>
-      <c r="G95" s="68" t="s">
+      <c r="G95" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H95" t="s">
@@ -9813,18 +9822,18 @@
       <c r="A96" t="s">
         <v>550</v>
       </c>
-      <c r="B96" s="68" t="s">
+      <c r="B96" s="67" t="s">
         <v>497</v>
       </c>
-      <c r="C96" s="68" t="s">
+      <c r="C96" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D96" s="68"/>
-      <c r="E96" s="94"/>
-      <c r="F96" s="68">
+      <c r="D96" s="67"/>
+      <c r="E96" s="92"/>
+      <c r="F96" s="67">
         <v>2010</v>
       </c>
-      <c r="G96" s="68" t="s">
+      <c r="G96" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H96" t="s">
@@ -9839,18 +9848,18 @@
       <c r="A97" t="s">
         <v>550</v>
       </c>
-      <c r="B97" s="68" t="s">
+      <c r="B97" s="67" t="s">
         <v>497</v>
       </c>
-      <c r="C97" s="68" t="s">
+      <c r="C97" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D97" s="68"/>
-      <c r="E97" s="94"/>
-      <c r="F97" s="68">
+      <c r="D97" s="67"/>
+      <c r="E97" s="92"/>
+      <c r="F97" s="67">
         <v>2010</v>
       </c>
-      <c r="G97" s="68" t="s">
+      <c r="G97" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H97" t="s">
@@ -9865,18 +9874,18 @@
       <c r="A98" t="s">
         <v>550</v>
       </c>
-      <c r="B98" s="68" t="s">
+      <c r="B98" s="67" t="s">
         <v>514</v>
       </c>
-      <c r="C98" s="68" t="s">
+      <c r="C98" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="D98" s="68"/>
-      <c r="E98" s="94"/>
-      <c r="F98" s="68">
+      <c r="D98" s="67"/>
+      <c r="E98" s="92"/>
+      <c r="F98" s="67">
         <v>2010</v>
       </c>
-      <c r="G98" s="68" t="s">
+      <c r="G98" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H98" s="41" t="s">
@@ -9885,7 +9894,7 @@
       <c r="I98" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J98" s="77" t="s">
+      <c r="J98" s="75" t="s">
         <v>516</v>
       </c>
       <c r="K98" t="s">
@@ -9899,18 +9908,18 @@
       <c r="A99" t="s">
         <v>550</v>
       </c>
-      <c r="B99" s="68" t="s">
+      <c r="B99" s="67" t="s">
         <v>514</v>
       </c>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D99" s="68"/>
-      <c r="E99" s="94"/>
-      <c r="F99" s="68">
+      <c r="D99" s="67"/>
+      <c r="E99" s="92"/>
+      <c r="F99" s="67">
         <v>2010</v>
       </c>
-      <c r="G99" s="68" t="s">
+      <c r="G99" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H99" s="41" t="s">
@@ -9919,7 +9928,7 @@
       <c r="I99" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J99" s="77" t="s">
+      <c r="J99" s="75" t="s">
         <v>516</v>
       </c>
       <c r="K99" t="s">
@@ -9933,18 +9942,18 @@
       <c r="A100" t="s">
         <v>550</v>
       </c>
-      <c r="B100" s="68" t="s">
+      <c r="B100" s="67" t="s">
         <v>518</v>
       </c>
-      <c r="C100" s="68" t="s">
+      <c r="C100" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="D100" s="68"/>
-      <c r="E100" s="94"/>
-      <c r="F100" s="68">
+      <c r="D100" s="67"/>
+      <c r="E100" s="92"/>
+      <c r="F100" s="67">
         <v>2010</v>
       </c>
-      <c r="G100" s="68" t="s">
+      <c r="G100" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H100" s="41" t="s">
@@ -9953,7 +9962,7 @@
       <c r="I100" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J100" s="77" t="s">
+      <c r="J100" s="75" t="s">
         <v>519</v>
       </c>
       <c r="K100" t="s">
@@ -9967,18 +9976,18 @@
       <c r="A101" t="s">
         <v>550</v>
       </c>
-      <c r="B101" s="68" t="s">
+      <c r="B101" s="67" t="s">
         <v>518</v>
       </c>
-      <c r="C101" s="68" t="s">
+      <c r="C101" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D101" s="68"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="68">
+      <c r="D101" s="67"/>
+      <c r="E101" s="92"/>
+      <c r="F101" s="67">
         <v>2010</v>
       </c>
-      <c r="G101" s="68" t="s">
+      <c r="G101" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H101" s="41" t="s">
@@ -9987,7 +9996,7 @@
       <c r="I101" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J101" s="77" t="s">
+      <c r="J101" s="75" t="s">
         <v>519</v>
       </c>
       <c r="K101" t="s">
@@ -10001,18 +10010,18 @@
       <c r="A102" t="s">
         <v>550</v>
       </c>
-      <c r="B102" s="68" t="s">
+      <c r="B102" s="67" t="s">
         <v>520</v>
       </c>
-      <c r="C102" s="68" t="s">
+      <c r="C102" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="D102" s="68"/>
-      <c r="E102" s="94"/>
-      <c r="F102" s="68">
+      <c r="D102" s="67"/>
+      <c r="E102" s="92"/>
+      <c r="F102" s="67">
         <v>2010</v>
       </c>
-      <c r="G102" s="68" t="s">
+      <c r="G102" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H102" s="41" t="s">
@@ -10021,7 +10030,7 @@
       <c r="I102" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J102" s="77" t="s">
+      <c r="J102" s="75" t="s">
         <v>521</v>
       </c>
       <c r="K102" t="s">
@@ -10035,18 +10044,18 @@
       <c r="A103" t="s">
         <v>550</v>
       </c>
-      <c r="B103" s="68" t="s">
+      <c r="B103" s="67" t="s">
         <v>520</v>
       </c>
-      <c r="C103" s="68" t="s">
+      <c r="C103" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D103" s="68"/>
-      <c r="E103" s="94"/>
-      <c r="F103" s="68">
+      <c r="D103" s="67"/>
+      <c r="E103" s="92"/>
+      <c r="F103" s="67">
         <v>2010</v>
       </c>
-      <c r="G103" s="68" t="s">
+      <c r="G103" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H103" s="41" t="s">
@@ -10055,7 +10064,7 @@
       <c r="I103" s="41" t="s">
         <v>515</v>
       </c>
-      <c r="J103" s="77" t="s">
+      <c r="J103" s="75" t="s">
         <v>521</v>
       </c>
       <c r="K103" t="s">
@@ -10069,18 +10078,18 @@
       <c r="A104" t="s">
         <v>550</v>
       </c>
-      <c r="B104" s="68" t="s">
+      <c r="B104" s="67" t="s">
         <v>499</v>
       </c>
-      <c r="C104" s="68" t="s">
+      <c r="C104" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D104" s="68"/>
-      <c r="E104" s="94"/>
-      <c r="F104" s="68">
+      <c r="D104" s="67"/>
+      <c r="E104" s="92"/>
+      <c r="F104" s="67">
         <v>2010</v>
       </c>
-      <c r="G104" s="68" t="s">
+      <c r="G104" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H104" t="s">
@@ -10095,18 +10104,18 @@
       <c r="A105" t="s">
         <v>550</v>
       </c>
-      <c r="B105" s="68" t="s">
+      <c r="B105" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="C105" s="68" t="s">
+      <c r="C105" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D105" s="68"/>
-      <c r="E105" s="94"/>
-      <c r="F105" s="68">
+      <c r="D105" s="67"/>
+      <c r="E105" s="92"/>
+      <c r="F105" s="67">
         <v>2010</v>
       </c>
-      <c r="G105" s="68" t="s">
+      <c r="G105" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H105" s="46" t="s">
@@ -10121,18 +10130,18 @@
       <c r="A106" t="s">
         <v>550</v>
       </c>
-      <c r="B106" s="68" t="s">
+      <c r="B106" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="C106" s="68" t="s">
+      <c r="C106" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D106" s="68"/>
-      <c r="E106" s="94"/>
-      <c r="F106" s="68">
+      <c r="D106" s="67"/>
+      <c r="E106" s="92"/>
+      <c r="F106" s="67">
         <v>2010</v>
       </c>
-      <c r="G106" s="68" t="s">
+      <c r="G106" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H106" s="46" t="s">
@@ -10147,18 +10156,18 @@
       <c r="A107" t="s">
         <v>550</v>
       </c>
-      <c r="B107" s="68" t="s">
+      <c r="B107" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="C107" s="68" t="s">
+      <c r="C107" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="D107" s="68"/>
-      <c r="E107" s="94"/>
-      <c r="F107" s="68">
+      <c r="D107" s="67"/>
+      <c r="E107" s="92"/>
+      <c r="F107" s="67">
         <v>2010</v>
       </c>
-      <c r="G107" s="68" t="s">
+      <c r="G107" s="67" t="s">
         <v>522</v>
       </c>
       <c r="H107" s="46" t="s">
@@ -10173,18 +10182,18 @@
       <c r="A108" t="s">
         <v>550</v>
       </c>
-      <c r="B108" s="68" t="s">
+      <c r="B108" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="C108" s="68" t="s">
+      <c r="C108" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D108" s="68"/>
-      <c r="E108" s="94"/>
-      <c r="F108" s="68">
+      <c r="D108" s="67"/>
+      <c r="E108" s="92"/>
+      <c r="F108" s="67">
         <v>2010</v>
       </c>
-      <c r="G108" s="68" t="s">
+      <c r="G108" s="67" t="s">
         <v>522</v>
       </c>
       <c r="H108" s="46" t="s">
@@ -10199,18 +10208,18 @@
       <c r="A109" t="s">
         <v>550</v>
       </c>
-      <c r="B109" s="68" t="s">
+      <c r="B109" s="67" t="s">
         <v>502</v>
       </c>
-      <c r="C109" s="68" t="s">
+      <c r="C109" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="D109" s="68"/>
-      <c r="E109" s="94"/>
-      <c r="F109" s="68">
+      <c r="D109" s="67"/>
+      <c r="E109" s="92"/>
+      <c r="F109" s="67">
         <v>2010</v>
       </c>
-      <c r="G109" s="68" t="s">
+      <c r="G109" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H109" s="46" t="s">
@@ -10219,7 +10228,7 @@
       <c r="I109" s="46" t="s">
         <v>523</v>
       </c>
-      <c r="J109" s="67" t="s">
+      <c r="J109" s="66" t="s">
         <v>652</v>
       </c>
       <c r="K109"/>
@@ -10228,18 +10237,18 @@
       <c r="A110" t="s">
         <v>550</v>
       </c>
-      <c r="B110" s="68" t="s">
+      <c r="B110" s="67" t="s">
         <v>504</v>
       </c>
-      <c r="C110" s="68" t="s">
+      <c r="C110" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D110" s="68"/>
-      <c r="E110" s="94"/>
-      <c r="F110" s="68">
+      <c r="D110" s="67"/>
+      <c r="E110" s="92"/>
+      <c r="F110" s="67">
         <v>2010</v>
       </c>
-      <c r="G110" s="68" t="s">
+      <c r="G110" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H110" s="46" t="s">
@@ -10254,18 +10263,18 @@
       <c r="A111" t="s">
         <v>550</v>
       </c>
-      <c r="B111" s="68" t="s">
+      <c r="B111" s="67" t="s">
         <v>506</v>
       </c>
-      <c r="C111" s="68" t="s">
+      <c r="C111" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D111" s="68"/>
-      <c r="E111" s="94"/>
-      <c r="F111" s="68">
+      <c r="D111" s="67"/>
+      <c r="E111" s="92"/>
+      <c r="F111" s="67">
         <v>2010</v>
       </c>
-      <c r="G111" s="68" t="s">
+      <c r="G111" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H111" s="46" t="s">
@@ -10280,18 +10289,18 @@
       <c r="A112" t="s">
         <v>550</v>
       </c>
-      <c r="B112" s="68" t="s">
+      <c r="B112" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C112" s="68" t="s">
+      <c r="C112" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D112" s="68"/>
-      <c r="E112" s="94"/>
-      <c r="F112" s="68">
+      <c r="D112" s="67"/>
+      <c r="E112" s="92"/>
+      <c r="F112" s="67">
         <v>2010</v>
       </c>
-      <c r="G112" s="68" t="s">
+      <c r="G112" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H112" s="46" t="s">
@@ -10309,18 +10318,18 @@
       <c r="A113" t="s">
         <v>550</v>
       </c>
-      <c r="B113" s="68" t="s">
+      <c r="B113" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C113" s="68" t="s">
+      <c r="C113" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D113" s="68"/>
-      <c r="E113" s="94"/>
-      <c r="F113" s="68">
+      <c r="D113" s="67"/>
+      <c r="E113" s="92"/>
+      <c r="F113" s="67">
         <v>2010</v>
       </c>
-      <c r="G113" s="68" t="s">
+      <c r="G113" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H113" s="46" t="s">
@@ -10335,18 +10344,18 @@
       <c r="A114" t="s">
         <v>550</v>
       </c>
-      <c r="B114" s="68" t="s">
+      <c r="B114" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C114" s="68" t="s">
+      <c r="C114" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D114" s="68"/>
-      <c r="E114" s="94"/>
-      <c r="F114" s="68">
+      <c r="D114" s="67"/>
+      <c r="E114" s="92"/>
+      <c r="F114" s="67">
         <v>2010</v>
       </c>
-      <c r="G114" s="68" t="s">
+      <c r="G114" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H114" s="46" t="s">
@@ -10361,18 +10370,18 @@
       <c r="A115" t="s">
         <v>550</v>
       </c>
-      <c r="B115" s="68" t="s">
+      <c r="B115" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C115" s="68" t="s">
+      <c r="C115" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D115" s="68"/>
-      <c r="E115" s="94"/>
-      <c r="F115" s="68">
+      <c r="D115" s="67"/>
+      <c r="E115" s="92"/>
+      <c r="F115" s="67">
         <v>2010</v>
       </c>
-      <c r="G115" s="68" t="s">
+      <c r="G115" s="67" t="s">
         <v>512</v>
       </c>
       <c r="H115" s="46" t="s">
@@ -10387,18 +10396,18 @@
       <c r="A116" t="s">
         <v>550</v>
       </c>
-      <c r="B116" s="68" t="s">
+      <c r="B116" s="67" t="s">
         <v>511</v>
       </c>
-      <c r="C116" s="68" t="s">
+      <c r="C116" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D116" s="68"/>
-      <c r="E116" s="94"/>
-      <c r="F116" s="68">
+      <c r="D116" s="67"/>
+      <c r="E116" s="92"/>
+      <c r="F116" s="67">
         <v>2010</v>
       </c>
-      <c r="G116" s="68" t="s">
+      <c r="G116" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H116" s="46" t="s">
@@ -10413,18 +10422,18 @@
       <c r="A117" t="s">
         <v>550</v>
       </c>
-      <c r="B117" s="68" t="s">
+      <c r="B117" s="67" t="s">
         <v>511</v>
       </c>
-      <c r="C117" s="68" t="s">
+      <c r="C117" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D117" s="68"/>
-      <c r="E117" s="94"/>
-      <c r="F117" s="68">
+      <c r="D117" s="67"/>
+      <c r="E117" s="92"/>
+      <c r="F117" s="67">
         <v>2010</v>
       </c>
-      <c r="G117" s="68" t="s">
+      <c r="G117" s="67" t="s">
         <v>513</v>
       </c>
       <c r="H117" s="46" t="s">
@@ -10455,13 +10464,20 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -10611,8 +10627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10661,10 +10677,10 @@
       <c r="J1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="93" t="s">
+      <c r="K1" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="90" t="s">
+      <c r="L1" s="88" t="s">
         <v>105</v>
       </c>
       <c r="M1" s="18" t="s">
@@ -10703,8 +10719,8 @@
       <c r="J2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K2" s="135"/>
-      <c r="L2" s="125"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="124"/>
       <c r="M2" s="19" t="s">
         <v>113</v>
       </c>
@@ -10741,8 +10757,8 @@
       <c r="J3" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K3" s="133"/>
-      <c r="L3" s="116"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="115"/>
       <c r="M3" s="20" t="s">
         <v>113</v>
       </c>
@@ -10776,8 +10792,8 @@
       <c r="J4" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="133"/>
-      <c r="L4" s="116"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="115"/>
       <c r="M4" s="20" t="s">
         <v>113</v>
       </c>
@@ -10808,8 +10824,8 @@
       <c r="J5" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K5" s="133"/>
-      <c r="L5" s="116"/>
+      <c r="K5" s="132"/>
+      <c r="L5" s="115"/>
       <c r="M5" s="20" t="s">
         <v>113</v>
       </c>
@@ -10843,10 +10859,10 @@
       <c r="J6" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K6" s="133" t="s">
+      <c r="K6" s="132" t="s">
         <v>122</v>
       </c>
-      <c r="L6" s="131"/>
+      <c r="L6" s="130"/>
       <c r="M6" s="20" t="s">
         <v>113</v>
       </c>
@@ -10880,8 +10896,8 @@
       <c r="J7" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K7" s="133"/>
-      <c r="L7" s="131"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="130"/>
       <c r="M7" s="20" t="s">
         <v>113</v>
       </c>
@@ -10912,8 +10928,8 @@
       <c r="J8" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K8" s="134"/>
-      <c r="L8" s="132"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="131"/>
       <c r="M8" s="20" t="s">
         <v>113</v>
       </c>
@@ -10950,10 +10966,10 @@
       <c r="J9" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K9" s="141" t="s">
+      <c r="K9" s="140" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="116" t="s">
+      <c r="L9" s="115" t="s">
         <v>131</v>
       </c>
       <c r="M9" s="19" t="s">
@@ -10989,8 +11005,8 @@
       <c r="J10" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K10" s="141"/>
-      <c r="L10" s="116"/>
+      <c r="K10" s="140"/>
+      <c r="L10" s="115"/>
       <c r="M10" s="20" t="s">
         <v>113</v>
       </c>
@@ -11024,8 +11040,8 @@
       <c r="J11" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K11" s="141"/>
-      <c r="L11" s="116"/>
+      <c r="K11" s="140"/>
+      <c r="L11" s="115"/>
       <c r="M11" s="21" t="s">
         <v>113</v>
       </c>
@@ -11056,10 +11072,10 @@
       <c r="J12" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="93" t="s">
+      <c r="K12" s="91" t="s">
         <v>137</v>
       </c>
-      <c r="L12" s="85" t="s">
+      <c r="L12" s="83" t="s">
         <v>138</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -11133,10 +11149,10 @@
       <c r="J14" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K14" s="89" t="s">
+      <c r="K14" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="L14" s="85" t="s">
+      <c r="L14" s="83" t="s">
         <v>145</v>
       </c>
       <c r="M14" s="19" t="s">
@@ -11172,8 +11188,8 @@
       <c r="J15" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K15" s="89"/>
-      <c r="L15" s="85"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="83"/>
       <c r="M15" s="19" t="s">
         <v>113</v>
       </c>
@@ -11210,7 +11226,7 @@
       <c r="K16" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="L16" s="87" t="s">
+      <c r="L16" s="85" t="s">
         <v>153</v>
       </c>
       <c r="M16" s="19" t="s">
@@ -11249,7 +11265,7 @@
       <c r="J17" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K17" s="89" t="s">
+      <c r="K17" s="87" t="s">
         <v>155</v>
       </c>
       <c r="L17" s="43" t="s">
@@ -11288,8 +11304,8 @@
       <c r="J18" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K18" s="127"/>
-      <c r="L18" s="85"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="83"/>
       <c r="M18" s="10" t="s">
         <v>113</v>
       </c>
@@ -11323,8 +11339,8 @@
       <c r="J19" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="K19" s="139"/>
-      <c r="L19" s="88"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="86"/>
       <c r="M19" s="31" t="s">
         <v>113</v>
       </c>
@@ -11361,10 +11377,10 @@
       <c r="J20" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K20" s="127" t="s">
+      <c r="K20" s="126" t="s">
         <v>161</v>
       </c>
-      <c r="L20" s="116" t="s">
+      <c r="L20" s="115" t="s">
         <v>162</v>
       </c>
       <c r="M20" s="10" t="s">
@@ -11400,8 +11416,8 @@
       <c r="J21" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K21" s="127"/>
-      <c r="L21" s="116"/>
+      <c r="K21" s="126"/>
+      <c r="L21" s="115"/>
       <c r="M21" s="10" t="s">
         <v>113</v>
       </c>
@@ -11432,8 +11448,8 @@
       <c r="J22" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K22" s="127"/>
-      <c r="L22" s="116"/>
+      <c r="K22" s="126"/>
+      <c r="L22" s="115"/>
       <c r="M22" s="10" t="s">
         <v>113</v>
       </c>
@@ -11467,8 +11483,8 @@
       <c r="J23" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K23" s="127"/>
-      <c r="L23" s="116"/>
+      <c r="K23" s="126"/>
+      <c r="L23" s="115"/>
       <c r="M23" s="10" t="s">
         <v>113</v>
       </c>
@@ -11502,8 +11518,8 @@
       <c r="J24" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K24" s="127"/>
-      <c r="L24" s="116"/>
+      <c r="K24" s="126"/>
+      <c r="L24" s="115"/>
       <c r="M24" s="10" t="s">
         <v>113</v>
       </c>
@@ -11537,10 +11553,10 @@
       <c r="J25" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K25" s="140" t="s">
+      <c r="K25" s="139" t="s">
         <v>167</v>
       </c>
-      <c r="L25" s="125" t="s">
+      <c r="L25" s="124" t="s">
         <v>168</v>
       </c>
       <c r="M25" s="15" t="s">
@@ -11579,8 +11595,8 @@
       <c r="J26" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K26" s="127"/>
-      <c r="L26" s="116"/>
+      <c r="K26" s="126"/>
+      <c r="L26" s="115"/>
       <c r="M26" s="10" t="s">
         <v>113</v>
       </c>
@@ -11614,8 +11630,8 @@
       <c r="J27" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K27" s="127"/>
-      <c r="L27" s="116"/>
+      <c r="K27" s="126"/>
+      <c r="L27" s="115"/>
       <c r="M27" s="10" t="s">
         <v>113</v>
       </c>
@@ -11646,8 +11662,8 @@
       <c r="J28" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K28" s="139"/>
-      <c r="L28" s="126"/>
+      <c r="K28" s="138"/>
+      <c r="L28" s="125"/>
       <c r="M28" s="11" t="s">
         <v>113</v>
       </c>
@@ -11684,10 +11700,10 @@
       <c r="J29" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K29" s="127" t="s">
+      <c r="K29" s="126" t="s">
         <v>175</v>
       </c>
-      <c r="L29" s="85"/>
+      <c r="L29" s="83"/>
       <c r="M29" s="10" t="s">
         <v>113</v>
       </c>
@@ -11721,8 +11737,8 @@
       <c r="J30" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K30" s="127"/>
-      <c r="L30" s="85"/>
+      <c r="K30" s="126"/>
+      <c r="L30" s="83"/>
       <c r="M30" s="10" t="s">
         <v>113</v>
       </c>
@@ -11756,8 +11772,8 @@
       <c r="J31" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K31" s="127"/>
-      <c r="L31" s="85"/>
+      <c r="K31" s="126"/>
+      <c r="L31" s="83"/>
       <c r="M31" s="10" t="s">
         <v>113</v>
       </c>
@@ -11788,8 +11804,8 @@
       <c r="J32" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K32" s="127"/>
-      <c r="L32" s="85"/>
+      <c r="K32" s="126"/>
+      <c r="L32" s="83"/>
       <c r="M32" s="10" t="s">
         <v>113</v>
       </c>
@@ -11823,10 +11839,10 @@
       <c r="J33" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K33" s="140" t="s">
+      <c r="K33" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="L33" s="87" t="s">
+      <c r="L33" s="85" t="s">
         <v>145</v>
       </c>
       <c r="M33" s="15" t="s">
@@ -11865,8 +11881,8 @@
       <c r="J34" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K34" s="139"/>
-      <c r="L34" s="88"/>
+      <c r="K34" s="138"/>
+      <c r="L34" s="86"/>
       <c r="M34" s="11" t="s">
         <v>113</v>
       </c>
@@ -11903,10 +11919,10 @@
       <c r="J35" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K35" s="127" t="s">
+      <c r="K35" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="L35" s="85" t="s">
+      <c r="L35" s="83" t="s">
         <v>145</v>
       </c>
       <c r="M35" s="10" t="s">
@@ -11942,8 +11958,8 @@
       <c r="J36" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K36" s="127"/>
-      <c r="L36" s="85"/>
+      <c r="K36" s="126"/>
+      <c r="L36" s="83"/>
       <c r="M36" s="10" t="s">
         <v>113</v>
       </c>
@@ -12015,8 +12031,8 @@
       <c r="J38" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K38" s="89"/>
-      <c r="L38" s="85"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="83"/>
       <c r="M38" s="10" t="s">
         <v>113</v>
       </c>
@@ -12050,10 +12066,10 @@
       <c r="J39" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K39" s="92" t="s">
+      <c r="K39" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="L39" s="125"/>
+      <c r="L39" s="124"/>
       <c r="M39" s="19" t="s">
         <v>113</v>
       </c>
@@ -12091,7 +12107,7 @@
         <v>113</v>
       </c>
       <c r="K40" s="32"/>
-      <c r="L40" s="116"/>
+      <c r="L40" s="115"/>
       <c r="M40" s="20" t="s">
         <v>113</v>
       </c>
@@ -12125,10 +12141,10 @@
       <c r="J41" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="K41" s="89" t="s">
+      <c r="K41" s="87" t="s">
         <v>190</v>
       </c>
-      <c r="L41" s="88" t="s">
+      <c r="L41" s="86" t="s">
         <v>191</v>
       </c>
       <c r="M41" s="22" t="s">
@@ -12167,10 +12183,10 @@
       <c r="J42" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K42" s="127" t="s">
+      <c r="K42" s="126" t="s">
         <v>193</v>
       </c>
-      <c r="L42" s="116" t="s">
+      <c r="L42" s="115" t="s">
         <v>194</v>
       </c>
       <c r="M42" s="19" t="s">
@@ -12206,8 +12222,8 @@
       <c r="J43" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K43" s="127"/>
-      <c r="L43" s="116"/>
+      <c r="K43" s="126"/>
+      <c r="L43" s="115"/>
       <c r="M43" s="20" t="s">
         <v>113</v>
       </c>
@@ -12241,8 +12257,8 @@
       <c r="J44" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K44" s="127"/>
-      <c r="L44" s="116"/>
+      <c r="K44" s="126"/>
+      <c r="L44" s="115"/>
       <c r="M44" s="20" t="s">
         <v>113</v>
       </c>
@@ -12273,8 +12289,8 @@
       <c r="J45" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K45" s="127"/>
-      <c r="L45" s="116"/>
+      <c r="K45" s="126"/>
+      <c r="L45" s="115"/>
       <c r="M45" s="20" t="s">
         <v>113</v>
       </c>
@@ -12308,8 +12324,8 @@
       <c r="J46" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K46" s="127"/>
-      <c r="L46" s="116"/>
+      <c r="K46" s="126"/>
+      <c r="L46" s="115"/>
       <c r="M46" s="20" t="s">
         <v>113</v>
       </c>
@@ -12343,8 +12359,8 @@
       <c r="J47" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K47" s="127"/>
-      <c r="L47" s="116"/>
+      <c r="K47" s="126"/>
+      <c r="L47" s="115"/>
       <c r="M47" s="20" t="s">
         <v>113</v>
       </c>
@@ -12420,8 +12436,8 @@
       <c r="J49" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K49" s="89"/>
-      <c r="L49" s="85"/>
+      <c r="K49" s="87"/>
+      <c r="L49" s="83"/>
       <c r="M49" s="19" t="s">
         <v>113</v>
       </c>
@@ -12455,10 +12471,10 @@
       <c r="J50" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K50" s="123" t="s">
+      <c r="K50" s="122" t="s">
         <v>206</v>
       </c>
-      <c r="L50" s="87"/>
+      <c r="L50" s="85"/>
       <c r="M50" s="23" t="s">
         <v>113</v>
       </c>
@@ -12495,8 +12511,8 @@
       <c r="J51" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K51" s="141"/>
-      <c r="L51" s="85"/>
+      <c r="K51" s="140"/>
+      <c r="L51" s="83"/>
       <c r="M51" s="23" t="s">
         <v>113</v>
       </c>
@@ -12530,8 +12546,8 @@
       <c r="J52" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K52" s="141"/>
-      <c r="L52" s="85"/>
+      <c r="K52" s="140"/>
+      <c r="L52" s="83"/>
       <c r="M52" s="23" t="s">
         <v>113</v>
       </c>
@@ -12565,8 +12581,8 @@
       <c r="J53" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K53" s="141"/>
-      <c r="L53" s="85"/>
+      <c r="K53" s="140"/>
+      <c r="L53" s="83"/>
       <c r="M53" s="23" t="s">
         <v>113</v>
       </c>
@@ -12597,8 +12613,8 @@
       <c r="J54" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K54" s="124"/>
-      <c r="L54" s="88"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="86"/>
       <c r="M54" s="23" t="s">
         <v>113</v>
       </c>
@@ -12632,11 +12648,11 @@
         <v>129</v>
       </c>
       <c r="I55"/>
-      <c r="J55" s="70"/>
-      <c r="K55" s="93" t="s">
+      <c r="J55" s="69"/>
+      <c r="K55" s="91" t="s">
         <v>216</v>
       </c>
-      <c r="L55" s="69" t="s">
+      <c r="L55" s="68" t="s">
         <v>217</v>
       </c>
       <c r="M55" s="37"/>
@@ -12709,10 +12725,10 @@
       <c r="J57" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K57" s="127" t="s">
+      <c r="K57" s="126" t="s">
         <v>223</v>
       </c>
-      <c r="L57" s="85"/>
+      <c r="L57" s="83"/>
       <c r="M57" s="23" t="s">
         <v>113</v>
       </c>
@@ -12746,8 +12762,8 @@
       <c r="J58" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K58" s="127"/>
-      <c r="L58" s="85"/>
+      <c r="K58" s="126"/>
+      <c r="L58" s="83"/>
       <c r="M58" s="21" t="s">
         <v>113</v>
       </c>
@@ -12778,8 +12794,8 @@
       <c r="J59" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K59" s="127"/>
-      <c r="L59" s="85"/>
+      <c r="K59" s="126"/>
+      <c r="L59" s="83"/>
       <c r="M59" s="21" t="s">
         <v>113</v>
       </c>
@@ -12813,10 +12829,10 @@
       <c r="J60" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="K60" s="125" t="s">
+      <c r="K60" s="124" t="s">
         <v>228</v>
       </c>
-      <c r="L60" s="87"/>
+      <c r="L60" s="85"/>
       <c r="M60" s="19" t="s">
         <v>113</v>
       </c>
@@ -12853,8 +12869,8 @@
       <c r="J61" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="K61" s="116"/>
-      <c r="L61" s="85" t="s">
+      <c r="K61" s="115"/>
+      <c r="L61" s="83" t="s">
         <v>230</v>
       </c>
       <c r="M61" s="20" t="s">
@@ -12890,8 +12906,8 @@
       <c r="J62" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K62" s="116"/>
-      <c r="L62" s="85" t="s">
+      <c r="K62" s="115"/>
+      <c r="L62" s="83" t="s">
         <v>232</v>
       </c>
       <c r="M62" s="20" t="s">
@@ -12927,8 +12943,8 @@
       <c r="J63" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="K63" s="127"/>
-      <c r="L63" s="85"/>
+      <c r="K63" s="126"/>
+      <c r="L63" s="83"/>
       <c r="M63" s="20" t="s">
         <v>113</v>
       </c>
@@ -12962,8 +12978,8 @@
       <c r="J64" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="K64" s="127"/>
-      <c r="L64" s="85"/>
+      <c r="K64" s="126"/>
+      <c r="L64" s="83"/>
       <c r="M64" s="20" t="s">
         <v>113</v>
       </c>
@@ -12997,8 +13013,8 @@
       <c r="J65" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="K65" s="127"/>
-      <c r="L65" s="85" t="s">
+      <c r="K65" s="126"/>
+      <c r="L65" s="83" t="s">
         <v>232</v>
       </c>
       <c r="M65" s="20" t="s">
@@ -13032,7 +13048,7 @@
       <c r="J66" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="K66" s="127"/>
+      <c r="K66" s="126"/>
       <c r="L66" s="44"/>
       <c r="M66" s="45" t="s">
         <v>113</v>
@@ -13071,7 +13087,7 @@
         <v>113</v>
       </c>
       <c r="K67" s="39"/>
-      <c r="L67" s="91"/>
+      <c r="L67" s="89"/>
       <c r="M67" s="20" t="s">
         <v>113</v>
       </c>
@@ -13106,7 +13122,7 @@
         <v>113</v>
       </c>
       <c r="K68" s="26"/>
-      <c r="L68" s="88"/>
+      <c r="L68" s="86"/>
       <c r="M68" s="23" t="s">
         <v>113</v>
       </c>
@@ -13143,10 +13159,10 @@
       <c r="J69" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K69" s="127" t="s">
+      <c r="K69" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="L69" s="85" t="s">
+      <c r="L69" s="83" t="s">
         <v>145</v>
       </c>
       <c r="M69" s="23" t="s">
@@ -13182,8 +13198,8 @@
       <c r="J70" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K70" s="127"/>
-      <c r="L70" s="85"/>
+      <c r="K70" s="126"/>
+      <c r="L70" s="83"/>
       <c r="M70" s="21" t="s">
         <v>113</v>
       </c>
@@ -13214,10 +13230,10 @@
       <c r="J71" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K71" s="92" t="s">
+      <c r="K71" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="L71" s="87" t="s">
+      <c r="L71" s="85" t="s">
         <v>242</v>
       </c>
       <c r="M71" s="19" t="s">
@@ -13256,8 +13272,8 @@
       <c r="J72" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K72" s="127"/>
-      <c r="L72" s="85"/>
+      <c r="K72" s="126"/>
+      <c r="L72" s="83"/>
       <c r="M72" s="21" t="s">
         <v>113</v>
       </c>
@@ -13288,8 +13304,8 @@
       <c r="J73" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K73" s="127"/>
-      <c r="L73" s="85"/>
+      <c r="K73" s="126"/>
+      <c r="L73" s="83"/>
       <c r="M73" s="21" t="s">
         <v>113</v>
       </c>
@@ -13320,8 +13336,8 @@
       <c r="J74" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K74" s="127"/>
-      <c r="L74" s="85"/>
+      <c r="K74" s="126"/>
+      <c r="L74" s="83"/>
       <c r="M74" s="21" t="s">
         <v>113</v>
       </c>
@@ -13349,8 +13365,8 @@
       <c r="J75" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K75" s="139"/>
-      <c r="L75" s="88"/>
+      <c r="K75" s="138"/>
+      <c r="L75" s="86"/>
       <c r="M75" s="21" t="s">
         <v>113</v>
       </c>
@@ -13387,8 +13403,8 @@
       <c r="J76" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K76" s="89"/>
-      <c r="L76" s="85"/>
+      <c r="K76" s="87"/>
+      <c r="L76" s="83"/>
       <c r="M76" s="23" t="s">
         <v>113</v>
       </c>
@@ -13418,16 +13434,16 @@
       <c r="H77" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I77" s="101" t="s">
+      <c r="I77" s="99" t="s">
         <v>649</v>
       </c>
       <c r="J77" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K77" s="123" t="s">
+      <c r="K77" s="122" t="s">
         <v>250</v>
       </c>
-      <c r="L77" s="128" t="s">
+      <c r="L77" s="127" t="s">
         <v>251</v>
       </c>
       <c r="M77" s="19" t="s">
@@ -13462,14 +13478,14 @@
       <c r="H78" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I78" s="101" t="s">
+      <c r="I78" s="99" t="s">
         <v>649</v>
       </c>
       <c r="J78" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K78" s="124"/>
-      <c r="L78" s="129"/>
+      <c r="K78" s="123"/>
+      <c r="L78" s="128"/>
       <c r="M78" s="45" t="s">
         <v>113</v>
       </c>
@@ -13506,10 +13522,10 @@
       <c r="J79" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K79" s="85" t="s">
+      <c r="K79" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="L79" s="129"/>
+      <c r="L79" s="128"/>
       <c r="M79" s="45" t="s">
         <v>113</v>
       </c>
@@ -13537,16 +13553,16 @@
       <c r="H80" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I80" s="101" t="s">
+      <c r="I80" s="99" t="s">
         <v>649</v>
       </c>
       <c r="J80" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K80" s="85" t="s">
+      <c r="K80" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="L80" s="130"/>
+      <c r="L80" s="129"/>
       <c r="M80" s="20" t="s">
         <v>113</v>
       </c>
@@ -13583,10 +13599,10 @@
       <c r="J81" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K81" s="127" t="s">
+      <c r="K81" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="L81" s="85" t="s">
+      <c r="L81" s="83" t="s">
         <v>145</v>
       </c>
       <c r="M81" s="23" t="s">
@@ -13622,8 +13638,8 @@
       <c r="J82" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K82" s="127"/>
-      <c r="L82" s="85"/>
+      <c r="K82" s="126"/>
+      <c r="L82" s="83"/>
       <c r="M82" s="21" t="s">
         <v>113</v>
       </c>
@@ -13647,7 +13663,7 @@
       <c r="F83" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G83" s="79" t="s">
+      <c r="G83" s="77" t="s">
         <v>86</v>
       </c>
       <c r="H83" s="5" t="s">
@@ -13657,7 +13673,7 @@
       <c r="J83" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="K83" s="80" t="s">
+      <c r="K83" s="78" t="s">
         <v>258</v>
       </c>
       <c r="L83" s="27"/>
@@ -13696,10 +13712,10 @@
       <c r="J84" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="K84" s="89" t="s">
+      <c r="K84" s="87" t="s">
         <v>262</v>
       </c>
-      <c r="L84" s="85" t="s">
+      <c r="L84" s="83" t="s">
         <v>263</v>
       </c>
       <c r="M84" s="19" t="s">
@@ -13734,7 +13750,7 @@
       <c r="J85" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K85" s="127" t="s">
+      <c r="K85" s="126" t="s">
         <v>264</v>
       </c>
       <c r="L85" s="28"/>
@@ -13770,7 +13786,7 @@
       <c r="J86" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K86" s="127"/>
+      <c r="K86" s="126"/>
       <c r="L86" s="28"/>
       <c r="M86" s="21" t="s">
         <v>113</v>
@@ -13804,7 +13820,7 @@
       <c r="J87" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K87" s="127"/>
+      <c r="K87" s="126"/>
       <c r="L87" s="28"/>
       <c r="M87" s="21" t="s">
         <v>113</v>
@@ -13835,7 +13851,7 @@
       <c r="J88" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K88" s="127"/>
+      <c r="K88" s="126"/>
       <c r="L88" s="28"/>
       <c r="M88" s="21" t="s">
         <v>113</v>
@@ -13869,7 +13885,7 @@
       <c r="J89" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K89" s="127"/>
+      <c r="K89" s="126"/>
       <c r="L89" s="28"/>
       <c r="M89" s="21" t="s">
         <v>113</v>
@@ -13903,7 +13919,7 @@
       <c r="J90" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="K90" s="127"/>
+      <c r="K90" s="126"/>
       <c r="L90" s="28"/>
       <c r="M90" s="21" t="s">
         <v>113</v>
@@ -13938,10 +13954,10 @@
       <c r="J91" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K91" s="117" t="s">
+      <c r="K91" s="116" t="s">
         <v>270</v>
       </c>
-      <c r="L91" s="136" t="s">
+      <c r="L91" s="135" t="s">
         <v>271</v>
       </c>
       <c r="M91" s="23" t="s">
@@ -13980,8 +13996,8 @@
       <c r="J92" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K92" s="118"/>
-      <c r="L92" s="137"/>
+      <c r="K92" s="117"/>
+      <c r="L92" s="136"/>
       <c r="M92" s="21" t="s">
         <v>113</v>
       </c>
@@ -14015,8 +14031,8 @@
       <c r="J93" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="K93" s="118"/>
-      <c r="L93" s="137"/>
+      <c r="K93" s="117"/>
+      <c r="L93" s="136"/>
       <c r="M93" s="21" t="s">
         <v>113</v>
       </c>
@@ -14047,8 +14063,8 @@
       <c r="J94" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="K94" s="119"/>
-      <c r="L94" s="138"/>
+      <c r="K94" s="118"/>
+      <c r="L94" s="137"/>
       <c r="M94" s="21" t="s">
         <v>113</v>
       </c>
@@ -14084,7 +14100,7 @@
       <c r="J95" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K95" s="120"/>
+      <c r="K95" s="119"/>
       <c r="L95" s="28"/>
       <c r="M95" s="23" t="s">
         <v>113</v>
@@ -14118,7 +14134,7 @@
       <c r="J96" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K96" s="121"/>
+      <c r="K96" s="120"/>
       <c r="L96" s="28"/>
       <c r="M96" s="23" t="s">
         <v>113</v>
@@ -14152,7 +14168,7 @@
       <c r="J97" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K97" s="121"/>
+      <c r="K97" s="120"/>
       <c r="L97" s="28"/>
       <c r="M97" s="23" t="s">
         <v>113</v>
@@ -14186,7 +14202,7 @@
       <c r="J98" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="K98" s="121"/>
+      <c r="K98" s="120"/>
       <c r="L98" s="28"/>
       <c r="M98" s="23" t="s">
         <v>113</v>
@@ -14219,8 +14235,8 @@
       <c r="J99" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="K99" s="122"/>
-      <c r="L99" s="86"/>
+      <c r="K99" s="121"/>
+      <c r="L99" s="84"/>
       <c r="M99" s="30" t="s">
         <v>113</v>
       </c>
@@ -15074,10 +15090,10 @@
       <c r="H25">
         <v>2010</v>
       </c>
-      <c r="I25" s="114" t="s">
+      <c r="I25" s="108" t="s">
         <v>763</v>
       </c>
-      <c r="J25" s="115" t="s">
+      <c r="J25" s="109" t="s">
         <v>764</v>
       </c>
     </row>
@@ -15933,21 +15949,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149AB136-B663-43F8-8265-AB28C3254826}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="9" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="7" max="7" width="11" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11" style="112" customWidth="1"/>
     <col min="9" max="9" width="55.6640625" style="59" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.33203125" style="59" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -15959,7 +15975,7 @@
     <col min="18" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="65" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="62" t="s">
         <v>586</v>
       </c>
@@ -15978,13 +15994,13 @@
       <c r="F1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="111" t="s">
         <v>703</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="64" t="s">
         <v>704</v>
       </c>
       <c r="J1" s="49" t="s">
@@ -16013,14 +16029,13 @@
       <c r="F2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="83" t="s">
+      <c r="I2" s="81" t="s">
         <v>332</v>
       </c>
-      <c r="J2" s="82"/>
+      <c r="J2" s="80"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -16048,10 +16063,10 @@
       <c r="F3" t="s">
         <v>340</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="66" t="s">
         <v>341</v>
       </c>
     </row>
@@ -16068,13 +16083,13 @@
       <c r="F4" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="66" t="s">
         <v>346</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>659</v>
       </c>
     </row>
@@ -16085,10 +16100,10 @@
       <c r="B5" t="s">
         <v>654</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="82" t="s">
+      <c r="I5" s="80" t="s">
         <v>702</v>
       </c>
     </row>
@@ -16107,12 +16122,11 @@
       <c r="F6" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -16140,11 +16154,11 @@
       <c r="F7" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="67" t="s">
+      <c r="H7" s="38"/>
+      <c r="I7" s="66" t="s">
         <v>342</v>
       </c>
       <c r="J7" s="59" t="s">
@@ -16164,12 +16178,11 @@
         <v>279</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -16184,46 +16197,48 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:23" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I9" s="67" t="s">
+      <c r="H9" s="112"/>
+      <c r="I9" s="81" t="s">
         <v>337</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="80" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>647</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="73"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="80"/>
       <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
@@ -16241,11 +16256,10 @@
       <c r="F11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="81" t="s">
         <v>347</v>
       </c>
       <c r="J11" s="59" t="s">
@@ -16265,33 +16279,34 @@
       <c r="F12" t="s">
         <v>331</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="81" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:23" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="67" t="s">
+      <c r="H13" s="113"/>
+      <c r="I13" s="82" t="s">
         <v>346</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="82" t="s">
         <v>659</v>
       </c>
     </row>
@@ -16302,10 +16317,10 @@
       <c r="B14" t="s">
         <v>654</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="82" t="s">
+      <c r="I14" s="80" t="s">
         <v>702</v>
       </c>
     </row>
@@ -16322,7 +16337,7 @@
       <c r="F15" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="2" t="s">
         <v>135</v>
       </c>
       <c r="I15" s="59" t="s">
@@ -16342,7 +16357,7 @@
       <c r="F16" s="46" t="s">
         <v>329</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="2" t="s">
         <v>54</v>
       </c>
       <c r="J16" s="59" t="s">
@@ -16362,10 +16377,10 @@
       <c r="F17" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I17" s="67" t="s">
+      <c r="I17" s="66" t="s">
         <v>332</v>
       </c>
       <c r="J17" s="59" t="s">
@@ -16385,10 +16400,10 @@
       <c r="F18" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I18" s="67" t="s">
+      <c r="I18" s="66" t="s">
         <v>332</v>
       </c>
       <c r="J18" s="59" t="s">
@@ -16408,7 +16423,7 @@
       <c r="F19" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J19" s="59" t="s">
@@ -16428,10 +16443,10 @@
       <c r="F20" t="s">
         <v>358</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I20" s="67" t="s">
+      <c r="I20" s="66" t="s">
         <v>337</v>
       </c>
       <c r="J20" s="59" t="s">
@@ -16451,7 +16466,7 @@
       <c r="F21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="2" t="s">
         <v>83</v>
       </c>
       <c r="J21" s="59" t="s">
@@ -16473,14 +16488,13 @@
       <c r="F22" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="82" t="s">
+      <c r="I22" s="80" t="s">
         <v>350</v>
       </c>
-      <c r="J22" s="82" t="s">
+      <c r="J22" s="80" t="s">
         <v>351</v>
       </c>
       <c r="K22" s="2"/>
@@ -16497,55 +16511,55 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
+    <row r="23" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>655</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I23" s="82"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="H23" s="114"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
+    </row>
+    <row r="24" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
         <v>701</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="83" t="s">
+      <c r="H24" s="113"/>
+      <c r="I24" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="J24" s="82" t="s">
+      <c r="J24" s="72" t="s">
         <v>282</v>
       </c>
-      <c r="K24" s="2"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73"/>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="73"/>
+      <c r="U24" s="73"/>
+      <c r="V24" s="73"/>
+      <c r="W24" s="73"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
@@ -16563,7 +16577,7 @@
       <c r="F25" t="s">
         <v>285</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O25" s="52"/>
@@ -16592,10 +16606,10 @@
       <c r="F26" t="s">
         <v>287</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I26" s="67" t="s">
+      <c r="I26" s="66" t="s">
         <v>288</v>
       </c>
       <c r="J26" s="59" t="s">
@@ -16627,7 +16641,7 @@
       <c r="F27" t="s">
         <v>291</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="7" t="s">
         <v>81</v>
       </c>
       <c r="O27" s="52"/>
@@ -16640,69 +16654,73 @@
       <c r="V27" s="52"/>
       <c r="W27" s="54"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O28" s="52"/>
-      <c r="P28" s="52"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="V28" s="52"/>
-      <c r="W28" s="54"/>
-    </row>
-    <row r="29" spans="1:23" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H28" s="112"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="105"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="105"/>
+      <c r="S28" s="105"/>
+      <c r="T28" s="105"/>
+      <c r="U28" s="105"/>
+      <c r="V28" s="105"/>
+      <c r="W28" s="107"/>
+    </row>
+    <row r="29" spans="1:23" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I29" s="84" t="s">
+      <c r="H29" s="112"/>
+      <c r="I29" s="81" t="s">
         <v>296</v>
       </c>
-      <c r="J29" s="73" t="s">
+      <c r="J29" s="80" t="s">
         <v>297</v>
       </c>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
-      <c r="S29" s="74"/>
-      <c r="T29" s="74"/>
-      <c r="U29" s="74"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="105"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="105"/>
+      <c r="S29" s="105"/>
+      <c r="T29" s="105"/>
+      <c r="U29" s="105"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="105"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
@@ -16721,25 +16739,24 @@
       <c r="F30" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="108"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="108"/>
-      <c r="T30" s="108"/>
-      <c r="U30" s="108"/>
-      <c r="V30" s="108"/>
-      <c r="W30" s="113"/>
+      <c r="O30" s="105"/>
+      <c r="P30" s="105"/>
+      <c r="Q30" s="105"/>
+      <c r="R30" s="105"/>
+      <c r="S30" s="105"/>
+      <c r="T30" s="105"/>
+      <c r="U30" s="105"/>
+      <c r="V30" s="105"/>
+      <c r="W30" s="107"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
@@ -16757,7 +16774,7 @@
       <c r="F31" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="O31" s="52"/>
@@ -16770,46 +16787,41 @@
       <c r="V31" s="52"/>
       <c r="W31" s="52"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="83" t="s">
+      <c r="H32" s="113"/>
+      <c r="I32" s="82" t="s">
         <v>281</v>
       </c>
-      <c r="J32" s="59" t="s">
+      <c r="J32" s="72" t="s">
         <v>282</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="108"/>
-      <c r="P32" s="108"/>
-      <c r="Q32" s="108"/>
-      <c r="R32" s="108"/>
-      <c r="S32" s="108"/>
-      <c r="T32" s="108"/>
-      <c r="U32" s="108"/>
-      <c r="V32" s="108"/>
-      <c r="W32" s="108"/>
+      <c r="O32" s="73"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="73"/>
+      <c r="V32" s="73"/>
+      <c r="W32" s="73"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -16824,10 +16836,10 @@
       <c r="F33" t="s">
         <v>305</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="83" t="s">
+      <c r="I33" s="81" t="s">
         <v>281</v>
       </c>
       <c r="J33" s="59" t="s">
@@ -16859,7 +16871,7 @@
       <c r="F34" t="s">
         <v>307</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O34" s="52"/>
@@ -16885,7 +16897,7 @@
       <c r="F35" t="s">
         <v>307</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O35" s="52"/>
@@ -16911,13 +16923,13 @@
       <c r="F36" t="s">
         <v>309</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I36" s="67" t="s">
+      <c r="I36" s="66" t="s">
         <v>281</v>
       </c>
-      <c r="J36" s="67" t="s">
+      <c r="J36" s="66" t="s">
         <v>282</v>
       </c>
       <c r="O36" s="52"/>
@@ -16930,66 +16942,71 @@
       <c r="V36" s="52"/>
       <c r="W36" s="54"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I37" s="59" t="s">
+      <c r="H37" s="112"/>
+      <c r="I37" s="80" t="s">
         <v>648</v>
       </c>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="52"/>
-      <c r="T37" s="52"/>
-      <c r="U37" s="52"/>
-      <c r="V37" s="52"/>
-      <c r="W37" s="52"/>
-    </row>
-    <row r="38" spans="1:23" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J37" s="80" t="s">
+        <v>797</v>
+      </c>
+      <c r="O37" s="105"/>
+      <c r="P37" s="105"/>
+      <c r="Q37" s="105"/>
+      <c r="R37" s="105"/>
+      <c r="S37" s="105"/>
+      <c r="T37" s="105"/>
+      <c r="U37" s="105"/>
+      <c r="V37" s="105"/>
+      <c r="W37" s="105"/>
+    </row>
+    <row r="38" spans="1:23" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>705</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="I38" s="84" t="s">
+      <c r="H38" s="112"/>
+      <c r="I38" s="81" t="s">
         <v>288</v>
       </c>
-      <c r="J38" s="73" t="s">
+      <c r="J38" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
-      <c r="T38" s="74"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="74"/>
-      <c r="W38" s="74"/>
+      <c r="O38" s="105"/>
+      <c r="P38" s="105"/>
+      <c r="Q38" s="105"/>
+      <c r="R38" s="105"/>
+      <c r="S38" s="105"/>
+      <c r="T38" s="105"/>
+      <c r="U38" s="105"/>
+      <c r="V38" s="105"/>
+      <c r="W38" s="105"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -17008,29 +17025,28 @@
       <c r="F39" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="83" t="s">
+      <c r="I39" s="81" t="s">
         <v>658</v>
       </c>
-      <c r="J39" s="82" t="s">
+      <c r="J39" s="80" t="s">
         <v>282</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="108"/>
-      <c r="P39" s="108"/>
-      <c r="Q39" s="108"/>
-      <c r="R39" s="108"/>
-      <c r="S39" s="108"/>
-      <c r="T39" s="108"/>
-      <c r="U39" s="108"/>
-      <c r="V39" s="108"/>
-      <c r="W39" s="108"/>
+      <c r="O39" s="105"/>
+      <c r="P39" s="105"/>
+      <c r="Q39" s="105"/>
+      <c r="R39" s="105"/>
+      <c r="S39" s="105"/>
+      <c r="T39" s="105"/>
+      <c r="U39" s="105"/>
+      <c r="V39" s="105"/>
+      <c r="W39" s="105"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -17045,10 +17061,10 @@
       <c r="F40" t="s">
         <v>305</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I40" s="67" t="s">
+      <c r="I40" s="66" t="s">
         <v>658</v>
       </c>
       <c r="J40" s="59" t="s">
@@ -17077,10 +17093,10 @@
       <c r="F41" t="s">
         <v>305</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I41" s="67" t="s">
+      <c r="I41" s="66" t="s">
         <v>658</v>
       </c>
       <c r="J41" s="59" t="s">
@@ -17112,7 +17128,7 @@
       <c r="F42" t="s">
         <v>309</v>
       </c>
-      <c r="G42" s="10" t="s">
+      <c r="G42" s="7" t="s">
         <v>46</v>
       </c>
       <c r="O42" s="52"/>
@@ -17138,7 +17154,7 @@
       <c r="F43" t="s">
         <v>309</v>
       </c>
-      <c r="G43" s="10" t="s">
+      <c r="G43" s="7" t="s">
         <v>46</v>
       </c>
       <c r="O43" s="52"/>
@@ -17164,11 +17180,14 @@
       <c r="F44" t="s">
         <v>317</v>
       </c>
-      <c r="G44" s="10" t="s">
+      <c r="G44" s="7" t="s">
         <v>135</v>
       </c>
       <c r="I44" s="59" t="s">
         <v>648</v>
+      </c>
+      <c r="J44" s="80" t="s">
+        <v>797</v>
       </c>
       <c r="O44" s="52"/>
       <c r="P44" s="52"/>
@@ -17196,7 +17215,7 @@
       <c r="F45" t="s">
         <v>319</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="7" t="s">
         <v>65</v>
       </c>
       <c r="O45" s="52"/>
@@ -17209,66 +17228,70 @@
       <c r="V45" s="52"/>
       <c r="W45" s="52"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="52"/>
-      <c r="S46" s="52"/>
-      <c r="T46" s="52"/>
-      <c r="U46" s="52"/>
-      <c r="V46" s="52"/>
-      <c r="W46" s="52"/>
-    </row>
-    <row r="47" spans="1:23" s="102" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H46" s="112"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="80"/>
+      <c r="O46" s="105"/>
+      <c r="P46" s="105"/>
+      <c r="Q46" s="105"/>
+      <c r="R46" s="105"/>
+      <c r="S46" s="105"/>
+      <c r="T46" s="105"/>
+      <c r="U46" s="105"/>
+      <c r="V46" s="105"/>
+      <c r="W46" s="105"/>
+    </row>
+    <row r="47" spans="1:23" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>705</v>
       </c>
-      <c r="C47" s="102" t="s">
+      <c r="C47" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D47" s="102" t="s">
+      <c r="D47" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E47" s="102" t="s">
+      <c r="E47" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F47" s="102" t="s">
+      <c r="F47" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="G47" s="110" t="s">
+      <c r="G47" s="7" t="s">
         <v>651</v>
       </c>
-      <c r="I47" s="111" t="s">
+      <c r="H47" s="112"/>
+      <c r="I47" s="81" t="s">
         <v>322</v>
       </c>
-      <c r="J47" s="111" t="s">
+      <c r="J47" s="81" t="s">
         <v>656</v>
       </c>
-      <c r="O47" s="112"/>
-      <c r="P47" s="112"/>
-      <c r="Q47" s="112"/>
-      <c r="R47" s="112"/>
-      <c r="S47" s="112"/>
-      <c r="T47" s="112"/>
-      <c r="U47" s="112"/>
-      <c r="V47" s="112"/>
-      <c r="W47" s="112"/>
+      <c r="O47" s="105"/>
+      <c r="P47" s="105"/>
+      <c r="Q47" s="105"/>
+      <c r="R47" s="105"/>
+      <c r="S47" s="105"/>
+      <c r="T47" s="105"/>
+      <c r="U47" s="105"/>
+      <c r="V47" s="105"/>
+      <c r="W47" s="105"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -17285,25 +17308,24 @@
       <c r="F48" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="103"/>
-      <c r="J48" s="82"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="80"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="108"/>
-      <c r="P48" s="108"/>
-      <c r="Q48" s="108"/>
-      <c r="R48" s="108"/>
-      <c r="S48" s="108"/>
-      <c r="T48" s="108"/>
-      <c r="U48" s="108"/>
-      <c r="V48" s="108"/>
-      <c r="W48" s="108"/>
+      <c r="O48" s="105"/>
+      <c r="P48" s="105"/>
+      <c r="Q48" s="105"/>
+      <c r="R48" s="105"/>
+      <c r="S48" s="105"/>
+      <c r="T48" s="105"/>
+      <c r="U48" s="105"/>
+      <c r="V48" s="105"/>
+      <c r="W48" s="105"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -17321,10 +17343,10 @@
       <c r="F49" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G49" s="10" t="s">
+      <c r="G49" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I49" s="103"/>
+      <c r="I49" s="80"/>
       <c r="O49" s="52"/>
       <c r="P49" s="52"/>
       <c r="Q49" s="52"/>
@@ -17348,14 +17370,14 @@
       <c r="F50" t="s">
         <v>309</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H50" s="46"/>
-      <c r="I50" s="111" t="s">
+      <c r="H50" s="38"/>
+      <c r="I50" s="81" t="s">
         <v>327</v>
       </c>
-      <c r="J50" s="67" t="s">
+      <c r="J50" s="66" t="s">
         <v>657</v>
       </c>
       <c r="O50" s="52"/>
@@ -17378,10 +17400,10 @@
       <c r="D51" t="s">
         <v>313</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I51" s="103" t="s">
+      <c r="I51" s="80" t="s">
         <v>702</v>
       </c>
     </row>
@@ -17396,14 +17418,13 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="103" t="s">
+      <c r="I52" s="80" t="s">
         <v>702</v>
       </c>
-      <c r="J52" s="82"/>
+      <c r="J52" s="80"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
@@ -17446,10 +17467,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FB7270-85D5-483E-AE4E-A5BD24F9C240}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17555,7 +17576,7 @@
       <c r="D7" t="s">
         <v>532</v>
       </c>
-      <c r="E7" s="109" t="s">
+      <c r="E7" s="106" t="s">
         <v>699</v>
       </c>
     </row>
@@ -17575,7 +17596,7 @@
         <v>683</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -17583,10 +17604,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>512</v>
+        <v>683</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -17594,10 +17615,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -17605,65 +17626,65 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>513</v>
+        <v>685</v>
       </c>
       <c r="C12">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>687</v>
+        <v>512</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>513</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>686</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>687</v>
       </c>
       <c r="C14">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B15" t="s">
-        <v>512</v>
+      <c r="B15" s="7" t="s">
+        <v>686</v>
       </c>
       <c r="C15">
         <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>688</v>
+      <c r="A16" s="7" t="s">
+        <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>512</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>688</v>
       </c>
       <c r="B17" t="s">
-        <v>689</v>
+        <v>274</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -17674,10 +17695,10 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -17685,7 +17706,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C19">
         <v>1000</v>
@@ -17693,21 +17714,70 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>513</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C20">
         <v>1000</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>513</v>
+      </c>
+      <c r="B21" t="s">
+        <v>698</v>
+      </c>
+      <c r="C21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>798</v>
+      </c>
+      <c r="B22" t="s">
+        <v>798</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>513</v>
+      </c>
+      <c r="B23" t="s">
+        <v>681</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>513</v>
+      </c>
+      <c r="B24" t="s">
+        <v>685</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C37">
-    <sortCondition ref="A2:A37"/>
-    <sortCondition ref="B2:B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
+    <sortCondition ref="A2:A38"/>
+    <sortCondition ref="B2:B38"/>
   </sortState>
-  <conditionalFormatting sqref="A15 A8:B14">
+  <conditionalFormatting sqref="A16 A8:B15">
     <cfRule type="expression" priority="3">
       <formula>EXACT($N8, n)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added NCCA 2020 analyte names
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4670" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA05FB8-E276-4769-AF57-488643848963}"/>
+  <xr:revisionPtr revIDLastSave="4710" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C18B00A-B4D7-46E9-824B-1253E1994E00}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-9450" windowWidth="29040" windowHeight="15720" tabRatio="809" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="809" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3581" uniqueCount="798">
   <si>
     <t>CodeName</t>
   </si>
@@ -2548,6 +2548,15 @@
   </si>
   <si>
     <t>Ammonia/ammonium, dissolved</t>
+  </si>
+  <si>
+    <t>Note this is dealt with by manually selecting columns by number in the code</t>
+  </si>
+  <si>
+    <t>NCCA_WChem_2020</t>
+  </si>
+  <si>
+    <t>2020-2020</t>
   </si>
 </sst>
 </file>
@@ -2915,7 +2924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3033,7 +3042,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3090,9 +3098,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3542,8 +3547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23ABD6F-8266-4030-840C-1A1DE88549A1}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A72" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4334,7 +4339,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4350,10 +4355,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="93" t="s">
         <v>680</v>
       </c>
-      <c r="J1" s="75"/>
+      <c r="J1" s="74"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -4369,7 +4374,7 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B2" t="s">
@@ -4381,13 +4386,13 @@
       <c r="G2" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="I2" s="93" t="s">
         <v>680</v>
       </c>
       <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4403,10 +4408,10 @@
         <v>75</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="95" t="s">
+      <c r="I3" s="93" t="s">
         <v>680</v>
       </c>
-      <c r="J3" s="75"/>
+      <c r="J3" s="74"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -4422,7 +4427,7 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B4" t="s">
@@ -4434,13 +4439,13 @@
       <c r="G4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="95" t="s">
+      <c r="I4" s="93" t="s">
         <v>680</v>
       </c>
       <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B5" t="s">
@@ -4452,31 +4457,31 @@
       <c r="G5" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="93" t="s">
         <v>680</v>
       </c>
       <c r="J5" s="58"/>
     </row>
-    <row r="6" spans="1:23" s="96" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="99" t="s">
+    <row r="6" spans="1:23" s="94" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="97" t="s">
         <v>690</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="94" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="94" t="s">
         <v>291</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="95" t="s">
+      <c r="I6" s="93" t="s">
         <v>680</v>
       </c>
-      <c r="J6" s="98"/>
+      <c r="J6" s="96"/>
     </row>
     <row r="7" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B7" t="s">
@@ -4488,13 +4493,13 @@
       <c r="G7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="95" t="s">
+      <c r="I7" s="93" t="s">
         <v>680</v>
       </c>
       <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="97" t="s">
         <v>690</v>
       </c>
       <c r="B8" t="s">
@@ -4507,18 +4512,18 @@
       <c r="G8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="I8" s="93" t="s">
         <v>680</v>
       </c>
       <c r="J8" s="58"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="97" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="97" t="s">
         <v>696</v>
       </c>
     </row>
@@ -5745,7 +5750,7 @@
       <c r="G9" t="s">
         <v>550</v>
       </c>
-      <c r="M9" s="93">
+      <c r="M9" s="91">
         <v>0.50069444399999996</v>
       </c>
     </row>
@@ -5765,7 +5770,7 @@
       <c r="G10" t="s">
         <v>569</v>
       </c>
-      <c r="M10" s="93">
+      <c r="M10" s="91">
         <v>0.45416600000000001</v>
       </c>
     </row>
@@ -5785,7 +5790,7 @@
       <c r="G11" t="s">
         <v>573</v>
       </c>
-      <c r="M11" s="93">
+      <c r="M11" s="91">
         <v>0.44791666699999999</v>
       </c>
     </row>
@@ -7515,8 +7520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5D57F1-DBF9-46B4-8278-09786D5200AB}">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7739,7 +7744,7 @@
       <c r="G8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="72" t="s">
+      <c r="H8" s="71" t="s">
         <v>127</v>
       </c>
       <c r="I8" t="s">
@@ -7765,7 +7770,7 @@
       <c r="G9" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="72" t="s">
+      <c r="H9" s="71" t="s">
         <v>127</v>
       </c>
       <c r="I9" t="s">
@@ -8036,7 +8041,7 @@
       <c r="G20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="72" t="s">
+      <c r="H20" s="71" t="s">
         <v>127</v>
       </c>
       <c r="I20" s="45" t="s">
@@ -8332,7 +8337,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>705</v>
       </c>
@@ -8346,16 +8351,18 @@
       <c r="G32" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="H32" s="69" t="s">
+      <c r="H32" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="J32" s="92" t="s">
+      <c r="J32" s="76" t="s">
         <v>413</v>
       </c>
-      <c r="K32" s="70"/>
+      <c r="K32" s="69" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -8379,7 +8386,7 @@
       <c r="J33" s="58" t="s">
         <v>416</v>
       </c>
-      <c r="K33" s="74" t="s">
+      <c r="K33" s="73" t="s">
         <v>417</v>
       </c>
     </row>
@@ -8537,7 +8544,7 @@
       <c r="F40">
         <v>2021</v>
       </c>
-      <c r="G40" s="73" t="s">
+      <c r="G40" s="72" t="s">
         <v>430</v>
       </c>
       <c r="H40" s="45" t="s">
@@ -8563,7 +8570,7 @@
       <c r="F41">
         <v>2021</v>
       </c>
-      <c r="G41" s="73" t="s">
+      <c r="G41" s="72" t="s">
         <v>430</v>
       </c>
       <c r="H41" s="45" t="s">
@@ -8759,7 +8766,7 @@
     </row>
     <row r="50" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B50" t="s">
         <v>446</v>
@@ -8782,7 +8789,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B51" t="s">
         <v>449</v>
@@ -8802,7 +8809,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B52" t="s">
         <v>451</v>
@@ -8822,7 +8829,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B53" t="s">
         <v>452</v>
@@ -8842,7 +8849,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B54" t="s">
         <v>453</v>
@@ -8862,7 +8869,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B55" t="s">
         <v>454</v>
@@ -8882,7 +8889,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B56" t="s">
         <v>456</v>
@@ -8902,7 +8909,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B57" t="s">
         <v>457</v>
@@ -8922,7 +8929,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B58" t="s">
         <v>458</v>
@@ -8942,7 +8949,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B59" t="s">
         <v>459</v>
@@ -8962,7 +8969,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B60" t="s">
         <v>461</v>
@@ -8985,7 +8992,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B61" t="s">
         <v>77</v>
@@ -8996,7 +9003,7 @@
       <c r="G61" t="s">
         <v>460</v>
       </c>
-      <c r="H61" s="40" t="s">
+      <c r="H61" s="45" t="s">
         <v>127</v>
       </c>
       <c r="I61" t="s">
@@ -9008,7 +9015,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B62" t="s">
         <v>464</v>
@@ -9028,7 +9035,7 @@
     </row>
     <row r="63" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B63" t="s">
         <v>466</v>
@@ -9054,7 +9061,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B64" t="s">
         <v>470</v>
@@ -9074,7 +9081,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B65" t="s">
         <v>472</v>
@@ -9094,7 +9101,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B66" t="s">
         <v>473</v>
@@ -9114,7 +9121,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B67" t="s">
         <v>474</v>
@@ -9139,7 +9146,7 @@
       <c r="B68" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="E68" s="91"/>
+      <c r="E68" s="90"/>
       <c r="F68" s="14">
         <v>2021</v>
       </c>
@@ -9152,10 +9159,10 @@
       <c r="I68" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="J68" s="77" t="s">
+      <c r="J68" s="76" t="s">
         <v>476</v>
       </c>
-      <c r="K68" s="77"/>
+      <c r="K68" s="76"/>
     </row>
     <row r="69" spans="1:11" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -9164,7 +9171,7 @@
       <c r="B69" s="45" t="s">
         <v>477</v>
       </c>
-      <c r="E69" s="90"/>
+      <c r="E69" s="89"/>
       <c r="F69" s="45">
         <v>2021</v>
       </c>
@@ -9189,7 +9196,7 @@
       <c r="B70" s="45" t="s">
         <v>479</v>
       </c>
-      <c r="E70" s="90"/>
+      <c r="E70" s="89"/>
       <c r="F70" s="45">
         <v>2021</v>
       </c>
@@ -9214,7 +9221,7 @@
       <c r="B71" s="45" t="s">
         <v>481</v>
       </c>
-      <c r="E71" s="90"/>
+      <c r="E71" s="89"/>
       <c r="F71" s="45">
         <v>2021</v>
       </c>
@@ -9239,7 +9246,7 @@
       <c r="B72" s="45" t="s">
         <v>702</v>
       </c>
-      <c r="E72" s="90"/>
+      <c r="E72" s="89"/>
       <c r="F72" s="45">
         <v>2021</v>
       </c>
@@ -9264,7 +9271,7 @@
       <c r="B73" s="45" t="s">
         <v>486</v>
       </c>
-      <c r="E73" s="90"/>
+      <c r="E73" s="89"/>
       <c r="F73" s="45">
         <v>2021</v>
       </c>
@@ -9289,7 +9296,7 @@
       <c r="B74" s="45" t="s">
         <v>488</v>
       </c>
-      <c r="E74" s="90"/>
+      <c r="E74" s="89"/>
       <c r="F74" s="45">
         <v>2021</v>
       </c>
@@ -9314,7 +9321,7 @@
       <c r="B75" s="45" t="s">
         <v>703</v>
       </c>
-      <c r="E75" s="90"/>
+      <c r="E75" s="89"/>
       <c r="F75" s="45">
         <v>2021</v>
       </c>
@@ -9339,7 +9346,7 @@
       <c r="B76" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="90"/>
+      <c r="E76" s="89"/>
       <c r="F76" s="45">
         <v>2021</v>
       </c>
@@ -9364,7 +9371,7 @@
       <c r="B77" s="45" t="s">
         <v>493</v>
       </c>
-      <c r="E77" s="90"/>
+      <c r="E77" s="89"/>
       <c r="F77" s="45">
         <v>2021</v>
       </c>
@@ -9389,7 +9396,7 @@
       <c r="B78" s="45" t="s">
         <v>495</v>
       </c>
-      <c r="E78" s="90"/>
+      <c r="E78" s="89"/>
       <c r="F78" s="45">
         <v>2021</v>
       </c>
@@ -9414,7 +9421,7 @@
       <c r="B79" s="45" t="s">
         <v>497</v>
       </c>
-      <c r="E79" s="90"/>
+      <c r="E79" s="89"/>
       <c r="F79" s="45">
         <v>2021</v>
       </c>
@@ -9439,7 +9446,7 @@
       <c r="B80" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="E80" s="90" t="s">
+      <c r="E80" s="89" t="s">
         <v>498</v>
       </c>
       <c r="F80" s="45">
@@ -9468,7 +9475,7 @@
       <c r="B81" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E81" s="90" t="s">
+      <c r="E81" s="89" t="s">
         <v>498</v>
       </c>
       <c r="F81" s="45">
@@ -9497,7 +9504,7 @@
       <c r="B82" s="45" t="s">
         <v>500</v>
       </c>
-      <c r="E82" s="90"/>
+      <c r="E82" s="89"/>
       <c r="F82" s="45">
         <v>2021</v>
       </c>
@@ -9517,18 +9524,18 @@
       <c r="A83" t="s">
         <v>539</v>
       </c>
-      <c r="B83" s="88" t="s">
+      <c r="B83" s="87" t="s">
         <v>475</v>
       </c>
-      <c r="C83" s="88" t="s">
+      <c r="C83" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="D83" s="88"/>
-      <c r="E83" s="89"/>
-      <c r="F83" s="88">
+      <c r="D83" s="87"/>
+      <c r="E83" s="88"/>
+      <c r="F83" s="87">
         <v>2010</v>
       </c>
-      <c r="G83" s="88" t="s">
+      <c r="G83" s="87" t="s">
         <v>501</v>
       </c>
       <c r="H83" s="4" t="s">
@@ -9537,7 +9544,7 @@
       <c r="I83" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="J83" s="70"/>
+      <c r="J83" s="69"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
@@ -9550,7 +9557,7 @@
         <v>53</v>
       </c>
       <c r="D84" s="66"/>
-      <c r="E84" s="87"/>
+      <c r="E84" s="86"/>
       <c r="F84" s="66">
         <v>2010</v>
       </c>
@@ -9576,7 +9583,7 @@
         <v>119</v>
       </c>
       <c r="D85" s="66"/>
-      <c r="E85" s="87"/>
+      <c r="E85" s="86"/>
       <c r="F85" s="66">
         <v>2010</v>
       </c>
@@ -9602,7 +9609,7 @@
         <v>119</v>
       </c>
       <c r="D86" s="66"/>
-      <c r="E86" s="87"/>
+      <c r="E86" s="86"/>
       <c r="F86" s="66">
         <v>2010</v>
       </c>
@@ -9628,7 +9635,7 @@
         <v>53</v>
       </c>
       <c r="D87" s="66"/>
-      <c r="E87" s="87"/>
+      <c r="E87" s="86"/>
       <c r="F87" s="66">
         <v>2010</v>
       </c>
@@ -9654,7 +9661,7 @@
         <v>119</v>
       </c>
       <c r="D88" s="66"/>
-      <c r="E88" s="87"/>
+      <c r="E88" s="86"/>
       <c r="F88" s="66">
         <v>2010</v>
       </c>
@@ -9680,7 +9687,7 @@
         <v>53</v>
       </c>
       <c r="D89" s="66"/>
-      <c r="E89" s="87"/>
+      <c r="E89" s="86"/>
       <c r="F89" s="66">
         <v>2010</v>
       </c>
@@ -9706,7 +9713,7 @@
         <v>119</v>
       </c>
       <c r="D90" s="66"/>
-      <c r="E90" s="87"/>
+      <c r="E90" s="86"/>
       <c r="F90" s="66">
         <v>2010</v>
       </c>
@@ -9732,7 +9739,7 @@
         <v>53</v>
       </c>
       <c r="D91" s="66"/>
-      <c r="E91" s="87"/>
+      <c r="E91" s="86"/>
       <c r="F91" s="66">
         <v>2010</v>
       </c>
@@ -9758,7 +9765,7 @@
         <v>119</v>
       </c>
       <c r="D92" s="66"/>
-      <c r="E92" s="87"/>
+      <c r="E92" s="86"/>
       <c r="F92" s="66">
         <v>2010</v>
       </c>
@@ -9784,7 +9791,7 @@
         <v>53</v>
       </c>
       <c r="D93" s="66"/>
-      <c r="E93" s="87"/>
+      <c r="E93" s="86"/>
       <c r="F93" s="66">
         <v>2010</v>
       </c>
@@ -9810,7 +9817,7 @@
         <v>119</v>
       </c>
       <c r="D94" s="66"/>
-      <c r="E94" s="87"/>
+      <c r="E94" s="86"/>
       <c r="F94" s="66">
         <v>2010</v>
       </c>
@@ -9836,7 +9843,7 @@
         <v>53</v>
       </c>
       <c r="D95" s="66"/>
-      <c r="E95" s="87"/>
+      <c r="E95" s="86"/>
       <c r="F95" s="66">
         <v>2010</v>
       </c>
@@ -9862,7 +9869,7 @@
         <v>119</v>
       </c>
       <c r="D96" s="66"/>
-      <c r="E96" s="87"/>
+      <c r="E96" s="86"/>
       <c r="F96" s="66">
         <v>2010</v>
       </c>
@@ -9888,7 +9895,7 @@
         <v>53</v>
       </c>
       <c r="D97" s="66"/>
-      <c r="E97" s="87"/>
+      <c r="E97" s="86"/>
       <c r="F97" s="66">
         <v>2010</v>
       </c>
@@ -9914,7 +9921,7 @@
         <v>149</v>
       </c>
       <c r="D98" s="66"/>
-      <c r="E98" s="87"/>
+      <c r="E98" s="86"/>
       <c r="F98" s="66">
         <v>2010</v>
       </c>
@@ -9948,7 +9955,7 @@
         <v>53</v>
       </c>
       <c r="D99" s="66"/>
-      <c r="E99" s="87"/>
+      <c r="E99" s="86"/>
       <c r="F99" s="66">
         <v>2010</v>
       </c>
@@ -9982,7 +9989,7 @@
         <v>149</v>
       </c>
       <c r="D100" s="66"/>
-      <c r="E100" s="87"/>
+      <c r="E100" s="86"/>
       <c r="F100" s="66">
         <v>2010</v>
       </c>
@@ -10016,7 +10023,7 @@
         <v>53</v>
       </c>
       <c r="D101" s="66"/>
-      <c r="E101" s="87"/>
+      <c r="E101" s="86"/>
       <c r="F101" s="66">
         <v>2010</v>
       </c>
@@ -10050,7 +10057,7 @@
         <v>149</v>
       </c>
       <c r="D102" s="66"/>
-      <c r="E102" s="87"/>
+      <c r="E102" s="86"/>
       <c r="F102" s="66">
         <v>2010</v>
       </c>
@@ -10084,7 +10091,7 @@
         <v>53</v>
       </c>
       <c r="D103" s="66"/>
-      <c r="E103" s="87"/>
+      <c r="E103" s="86"/>
       <c r="F103" s="66">
         <v>2010</v>
       </c>
@@ -10118,7 +10125,7 @@
         <v>119</v>
       </c>
       <c r="D104" s="66"/>
-      <c r="E104" s="87"/>
+      <c r="E104" s="86"/>
       <c r="F104" s="66">
         <v>2010</v>
       </c>
@@ -10144,7 +10151,7 @@
         <v>119</v>
       </c>
       <c r="D105" s="66"/>
-      <c r="E105" s="87"/>
+      <c r="E105" s="86"/>
       <c r="F105" s="66">
         <v>2010</v>
       </c>
@@ -10170,7 +10177,7 @@
         <v>53</v>
       </c>
       <c r="D106" s="66"/>
-      <c r="E106" s="87"/>
+      <c r="E106" s="86"/>
       <c r="F106" s="66">
         <v>2010</v>
       </c>
@@ -10196,7 +10203,7 @@
         <v>149</v>
       </c>
       <c r="D107" s="66"/>
-      <c r="E107" s="87"/>
+      <c r="E107" s="86"/>
       <c r="F107" s="66">
         <v>2010</v>
       </c>
@@ -10222,7 +10229,7 @@
         <v>53</v>
       </c>
       <c r="D108" s="66"/>
-      <c r="E108" s="87"/>
+      <c r="E108" s="86"/>
       <c r="F108" s="66">
         <v>2010</v>
       </c>
@@ -10248,7 +10255,7 @@
         <v>119</v>
       </c>
       <c r="D109" s="66"/>
-      <c r="E109" s="87"/>
+      <c r="E109" s="86"/>
       <c r="F109" s="66">
         <v>2010</v>
       </c>
@@ -10277,7 +10284,7 @@
         <v>106</v>
       </c>
       <c r="D110" s="66"/>
-      <c r="E110" s="87"/>
+      <c r="E110" s="86"/>
       <c r="F110" s="66">
         <v>2010</v>
       </c>
@@ -10303,7 +10310,7 @@
         <v>106</v>
       </c>
       <c r="D111" s="66"/>
-      <c r="E111" s="87"/>
+      <c r="E111" s="86"/>
       <c r="F111" s="66">
         <v>2010</v>
       </c>
@@ -10329,7 +10336,7 @@
         <v>106</v>
       </c>
       <c r="D112" s="66"/>
-      <c r="E112" s="87"/>
+      <c r="E112" s="86"/>
       <c r="F112" s="66">
         <v>2010</v>
       </c>
@@ -10360,7 +10367,7 @@
         <v>53</v>
       </c>
       <c r="D113" s="66"/>
-      <c r="E113" s="87"/>
+      <c r="E113" s="86"/>
       <c r="F113" s="66">
         <v>2010</v>
       </c>
@@ -10388,7 +10395,7 @@
         <v>106</v>
       </c>
       <c r="D114" s="66"/>
-      <c r="E114" s="87"/>
+      <c r="E114" s="86"/>
       <c r="F114" s="66">
         <v>2010</v>
       </c>
@@ -10416,7 +10423,7 @@
         <v>53</v>
       </c>
       <c r="D115" s="66"/>
-      <c r="E115" s="87"/>
+      <c r="E115" s="86"/>
       <c r="F115" s="66">
         <v>2010</v>
       </c>
@@ -10444,7 +10451,7 @@
         <v>106</v>
       </c>
       <c r="D116" s="66"/>
-      <c r="E116" s="87"/>
+      <c r="E116" s="86"/>
       <c r="F116" s="66">
         <v>2010</v>
       </c>
@@ -10470,7 +10477,7 @@
         <v>53</v>
       </c>
       <c r="D117" s="66"/>
-      <c r="E117" s="87"/>
+      <c r="E117" s="86"/>
       <c r="F117" s="66">
         <v>2010</v>
       </c>
@@ -10668,8 +10675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10718,10 +10725,10 @@
       <c r="J1" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="82" t="s">
         <v>97</v>
       </c>
       <c r="M1" s="18" t="s">
@@ -10760,8 +10767,8 @@
       <c r="J2" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="129"/>
-      <c r="L2" s="119"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="117"/>
       <c r="M2" s="19" t="s">
         <v>105</v>
       </c>
@@ -10798,8 +10805,8 @@
       <c r="J3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="127"/>
-      <c r="L3" s="110"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="108"/>
       <c r="M3" s="20" t="s">
         <v>105</v>
       </c>
@@ -10833,8 +10840,8 @@
       <c r="J4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="127"/>
-      <c r="L4" s="110"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="108"/>
       <c r="M4" s="20" t="s">
         <v>105</v>
       </c>
@@ -10865,8 +10872,8 @@
       <c r="J5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="127"/>
-      <c r="L5" s="110"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="108"/>
       <c r="M5" s="20" t="s">
         <v>105</v>
       </c>
@@ -10900,10 +10907,10 @@
       <c r="J6" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="127" t="s">
+      <c r="K6" s="125" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="125"/>
+      <c r="L6" s="123"/>
       <c r="M6" s="20" t="s">
         <v>105</v>
       </c>
@@ -10937,8 +10944,8 @@
       <c r="J7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="127"/>
-      <c r="L7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="123"/>
       <c r="M7" s="20" t="s">
         <v>105</v>
       </c>
@@ -10969,8 +10976,8 @@
       <c r="J8" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="128"/>
-      <c r="L8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="124"/>
       <c r="M8" s="20" t="s">
         <v>105</v>
       </c>
@@ -11007,10 +11014,10 @@
       <c r="J9" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="135" t="s">
+      <c r="K9" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="110" t="s">
+      <c r="L9" s="108" t="s">
         <v>123</v>
       </c>
       <c r="M9" s="19" t="s">
@@ -11046,8 +11053,8 @@
       <c r="J10" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="135"/>
-      <c r="L10" s="110"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="108"/>
       <c r="M10" s="20" t="s">
         <v>105</v>
       </c>
@@ -11081,8 +11088,8 @@
       <c r="J11" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K11" s="135"/>
-      <c r="L11" s="110"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="108"/>
       <c r="M11" s="21" t="s">
         <v>105</v>
       </c>
@@ -11113,10 +11120,10 @@
       <c r="J12" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K12" s="86" t="s">
+      <c r="K12" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="L12" s="78" t="s">
+      <c r="L12" s="77" t="s">
         <v>130</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -11190,10 +11197,10 @@
       <c r="J14" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K14" s="82" t="s">
+      <c r="K14" s="81" t="s">
         <v>136</v>
       </c>
-      <c r="L14" s="78" t="s">
+      <c r="L14" s="77" t="s">
         <v>137</v>
       </c>
       <c r="M14" s="19" t="s">
@@ -11229,8 +11236,8 @@
       <c r="J15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K15" s="82"/>
-      <c r="L15" s="78"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="77"/>
       <c r="M15" s="19" t="s">
         <v>105</v>
       </c>
@@ -11267,7 +11274,7 @@
       <c r="K16" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="L16" s="80" t="s">
+      <c r="L16" s="79" t="s">
         <v>145</v>
       </c>
       <c r="M16" s="19" t="s">
@@ -11306,7 +11313,7 @@
       <c r="J17" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="81" t="s">
         <v>147</v>
       </c>
       <c r="L17" s="42" t="s">
@@ -11345,8 +11352,8 @@
       <c r="J18" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="121"/>
-      <c r="L18" s="78"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="77"/>
       <c r="M18" s="10" t="s">
         <v>105</v>
       </c>
@@ -11380,8 +11387,8 @@
       <c r="J19" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="133"/>
-      <c r="L19" s="81"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="80"/>
       <c r="M19" s="31" t="s">
         <v>105</v>
       </c>
@@ -11418,10 +11425,10 @@
       <c r="J20" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="121" t="s">
+      <c r="K20" s="119" t="s">
         <v>153</v>
       </c>
-      <c r="L20" s="110" t="s">
+      <c r="L20" s="108" t="s">
         <v>154</v>
       </c>
       <c r="M20" s="10" t="s">
@@ -11457,8 +11464,8 @@
       <c r="J21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K21" s="121"/>
-      <c r="L21" s="110"/>
+      <c r="K21" s="119"/>
+      <c r="L21" s="108"/>
       <c r="M21" s="10" t="s">
         <v>105</v>
       </c>
@@ -11489,8 +11496,8 @@
       <c r="J22" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="121"/>
-      <c r="L22" s="110"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="108"/>
       <c r="M22" s="10" t="s">
         <v>105</v>
       </c>
@@ -11524,8 +11531,8 @@
       <c r="J23" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="121"/>
-      <c r="L23" s="110"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="108"/>
       <c r="M23" s="10" t="s">
         <v>105</v>
       </c>
@@ -11559,8 +11566,8 @@
       <c r="J24" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K24" s="121"/>
-      <c r="L24" s="110"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="108"/>
       <c r="M24" s="10" t="s">
         <v>105</v>
       </c>
@@ -11594,10 +11601,10 @@
       <c r="J25" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K25" s="134" t="s">
+      <c r="K25" s="132" t="s">
         <v>159</v>
       </c>
-      <c r="L25" s="119" t="s">
+      <c r="L25" s="117" t="s">
         <v>160</v>
       </c>
       <c r="M25" s="15" t="s">
@@ -11636,8 +11643,8 @@
       <c r="J26" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K26" s="121"/>
-      <c r="L26" s="110"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="108"/>
       <c r="M26" s="10" t="s">
         <v>105</v>
       </c>
@@ -11671,8 +11678,8 @@
       <c r="J27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K27" s="121"/>
-      <c r="L27" s="110"/>
+      <c r="K27" s="119"/>
+      <c r="L27" s="108"/>
       <c r="M27" s="10" t="s">
         <v>105</v>
       </c>
@@ -11703,8 +11710,8 @@
       <c r="J28" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K28" s="133"/>
-      <c r="L28" s="120"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="118"/>
       <c r="M28" s="11" t="s">
         <v>105</v>
       </c>
@@ -11741,10 +11748,10 @@
       <c r="J29" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K29" s="121" t="s">
+      <c r="K29" s="119" t="s">
         <v>167</v>
       </c>
-      <c r="L29" s="78"/>
+      <c r="L29" s="77"/>
       <c r="M29" s="10" t="s">
         <v>105</v>
       </c>
@@ -11778,8 +11785,8 @@
       <c r="J30" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K30" s="121"/>
-      <c r="L30" s="78"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="77"/>
       <c r="M30" s="10" t="s">
         <v>105</v>
       </c>
@@ -11813,8 +11820,8 @@
       <c r="J31" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K31" s="121"/>
-      <c r="L31" s="78"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="77"/>
       <c r="M31" s="10" t="s">
         <v>105</v>
       </c>
@@ -11845,8 +11852,8 @@
       <c r="J32" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K32" s="121"/>
-      <c r="L32" s="78"/>
+      <c r="K32" s="119"/>
+      <c r="L32" s="77"/>
       <c r="M32" s="10" t="s">
         <v>105</v>
       </c>
@@ -11880,10 +11887,10 @@
       <c r="J33" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="134" t="s">
+      <c r="K33" s="132" t="s">
         <v>136</v>
       </c>
-      <c r="L33" s="80" t="s">
+      <c r="L33" s="79" t="s">
         <v>137</v>
       </c>
       <c r="M33" s="15" t="s">
@@ -11922,8 +11929,8 @@
       <c r="J34" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K34" s="133"/>
-      <c r="L34" s="81"/>
+      <c r="K34" s="131"/>
+      <c r="L34" s="80"/>
       <c r="M34" s="11" t="s">
         <v>105</v>
       </c>
@@ -11960,10 +11967,10 @@
       <c r="J35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K35" s="121" t="s">
+      <c r="K35" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="L35" s="78" t="s">
+      <c r="L35" s="77" t="s">
         <v>137</v>
       </c>
       <c r="M35" s="10" t="s">
@@ -11999,8 +12006,8 @@
       <c r="J36" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K36" s="121"/>
-      <c r="L36" s="78"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="77"/>
       <c r="M36" s="10" t="s">
         <v>105</v>
       </c>
@@ -12072,8 +12079,8 @@
       <c r="J38" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K38" s="82"/>
-      <c r="L38" s="78"/>
+      <c r="K38" s="81"/>
+      <c r="L38" s="77"/>
       <c r="M38" s="10" t="s">
         <v>105</v>
       </c>
@@ -12107,10 +12114,10 @@
       <c r="J39" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K39" s="85" t="s">
+      <c r="K39" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="L39" s="119"/>
+      <c r="L39" s="117"/>
       <c r="M39" s="19" t="s">
         <v>105</v>
       </c>
@@ -12148,7 +12155,7 @@
         <v>105</v>
       </c>
       <c r="K40" s="32"/>
-      <c r="L40" s="110"/>
+      <c r="L40" s="108"/>
       <c r="M40" s="20" t="s">
         <v>105</v>
       </c>
@@ -12182,10 +12189,10 @@
       <c r="J41" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="K41" s="82" t="s">
+      <c r="K41" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="L41" s="81" t="s">
+      <c r="L41" s="80" t="s">
         <v>183</v>
       </c>
       <c r="M41" s="22" t="s">
@@ -12224,10 +12231,10 @@
       <c r="J42" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K42" s="121" t="s">
+      <c r="K42" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="L42" s="110" t="s">
+      <c r="L42" s="108" t="s">
         <v>186</v>
       </c>
       <c r="M42" s="19" t="s">
@@ -12263,8 +12270,8 @@
       <c r="J43" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="121"/>
-      <c r="L43" s="110"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="108"/>
       <c r="M43" s="20" t="s">
         <v>105</v>
       </c>
@@ -12298,8 +12305,8 @@
       <c r="J44" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K44" s="121"/>
-      <c r="L44" s="110"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="108"/>
       <c r="M44" s="20" t="s">
         <v>105</v>
       </c>
@@ -12330,8 +12337,8 @@
       <c r="J45" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K45" s="121"/>
-      <c r="L45" s="110"/>
+      <c r="K45" s="119"/>
+      <c r="L45" s="108"/>
       <c r="M45" s="20" t="s">
         <v>105</v>
       </c>
@@ -12365,8 +12372,8 @@
       <c r="J46" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K46" s="121"/>
-      <c r="L46" s="110"/>
+      <c r="K46" s="119"/>
+      <c r="L46" s="108"/>
       <c r="M46" s="20" t="s">
         <v>105</v>
       </c>
@@ -12400,8 +12407,8 @@
       <c r="J47" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K47" s="121"/>
-      <c r="L47" s="110"/>
+      <c r="K47" s="119"/>
+      <c r="L47" s="108"/>
       <c r="M47" s="20" t="s">
         <v>105</v>
       </c>
@@ -12477,8 +12484,8 @@
       <c r="J49" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K49" s="82"/>
-      <c r="L49" s="78"/>
+      <c r="K49" s="81"/>
+      <c r="L49" s="77"/>
       <c r="M49" s="19" t="s">
         <v>105</v>
       </c>
@@ -12512,10 +12519,10 @@
       <c r="J50" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K50" s="117" t="s">
+      <c r="K50" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="L50" s="80"/>
+      <c r="L50" s="79"/>
       <c r="M50" s="23" t="s">
         <v>105</v>
       </c>
@@ -12552,8 +12559,8 @@
       <c r="J51" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K51" s="135"/>
-      <c r="L51" s="78"/>
+      <c r="K51" s="133"/>
+      <c r="L51" s="77"/>
       <c r="M51" s="23" t="s">
         <v>105</v>
       </c>
@@ -12587,8 +12594,8 @@
       <c r="J52" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K52" s="135"/>
-      <c r="L52" s="78"/>
+      <c r="K52" s="133"/>
+      <c r="L52" s="77"/>
       <c r="M52" s="23" t="s">
         <v>105</v>
       </c>
@@ -12622,8 +12629,8 @@
       <c r="J53" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K53" s="135"/>
-      <c r="L53" s="78"/>
+      <c r="K53" s="133"/>
+      <c r="L53" s="77"/>
       <c r="M53" s="23" t="s">
         <v>105</v>
       </c>
@@ -12654,8 +12661,8 @@
       <c r="J54" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K54" s="118"/>
-      <c r="L54" s="81"/>
+      <c r="K54" s="116"/>
+      <c r="L54" s="80"/>
       <c r="M54" s="23" t="s">
         <v>105</v>
       </c>
@@ -12692,7 +12699,7 @@
       <c r="J55" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K55" s="86" t="s">
+      <c r="K55" s="85" t="s">
         <v>208</v>
       </c>
       <c r="L55" s="67" t="s">
@@ -12770,10 +12777,10 @@
       <c r="J57" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K57" s="121" t="s">
+      <c r="K57" s="119" t="s">
         <v>214</v>
       </c>
-      <c r="L57" s="78"/>
+      <c r="L57" s="77"/>
       <c r="M57" s="23" t="s">
         <v>105</v>
       </c>
@@ -12807,8 +12814,8 @@
       <c r="J58" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K58" s="121"/>
-      <c r="L58" s="78"/>
+      <c r="K58" s="119"/>
+      <c r="L58" s="77"/>
       <c r="M58" s="21" t="s">
         <v>105</v>
       </c>
@@ -12839,8 +12846,8 @@
       <c r="J59" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K59" s="121"/>
-      <c r="L59" s="78"/>
+      <c r="K59" s="119"/>
+      <c r="L59" s="77"/>
       <c r="M59" s="21" t="s">
         <v>105</v>
       </c>
@@ -12874,10 +12881,10 @@
       <c r="J60" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K60" s="119" t="s">
+      <c r="K60" s="117" t="s">
         <v>219</v>
       </c>
-      <c r="L60" s="80"/>
+      <c r="L60" s="79"/>
       <c r="M60" s="19" t="s">
         <v>105</v>
       </c>
@@ -12914,8 +12921,8 @@
       <c r="J61" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K61" s="110"/>
-      <c r="L61" s="78" t="s">
+      <c r="K61" s="108"/>
+      <c r="L61" s="77" t="s">
         <v>221</v>
       </c>
       <c r="M61" s="20" t="s">
@@ -12951,8 +12958,8 @@
       <c r="J62" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K62" s="110"/>
-      <c r="L62" s="78" t="s">
+      <c r="K62" s="108"/>
+      <c r="L62" s="77" t="s">
         <v>223</v>
       </c>
       <c r="M62" s="20" t="s">
@@ -12988,8 +12995,8 @@
       <c r="J63" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K63" s="121"/>
-      <c r="L63" s="78"/>
+      <c r="K63" s="119"/>
+      <c r="L63" s="77"/>
       <c r="M63" s="20" t="s">
         <v>105</v>
       </c>
@@ -13023,8 +13030,8 @@
       <c r="J64" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K64" s="121"/>
-      <c r="L64" s="78"/>
+      <c r="K64" s="119"/>
+      <c r="L64" s="77"/>
       <c r="M64" s="20" t="s">
         <v>105</v>
       </c>
@@ -13058,8 +13065,8 @@
       <c r="J65" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K65" s="121"/>
-      <c r="L65" s="78" t="s">
+      <c r="K65" s="119"/>
+      <c r="L65" s="77" t="s">
         <v>223</v>
       </c>
       <c r="M65" s="20" t="s">
@@ -13093,7 +13100,7 @@
       <c r="J66" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K66" s="121"/>
+      <c r="K66" s="119"/>
       <c r="L66" s="43"/>
       <c r="M66" s="44" t="s">
         <v>105</v>
@@ -13132,7 +13139,7 @@
         <v>105</v>
       </c>
       <c r="K67" s="38"/>
-      <c r="L67" s="84"/>
+      <c r="L67" s="83"/>
       <c r="M67" s="20" t="s">
         <v>105</v>
       </c>
@@ -13167,7 +13174,7 @@
         <v>105</v>
       </c>
       <c r="K68" s="26"/>
-      <c r="L68" s="81"/>
+      <c r="L68" s="80"/>
       <c r="M68" s="23" t="s">
         <v>105</v>
       </c>
@@ -13204,10 +13211,10 @@
       <c r="J69" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K69" s="121" t="s">
+      <c r="K69" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="L69" s="78" t="s">
+      <c r="L69" s="77" t="s">
         <v>137</v>
       </c>
       <c r="M69" s="23" t="s">
@@ -13243,8 +13250,8 @@
       <c r="J70" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K70" s="121"/>
-      <c r="L70" s="78"/>
+      <c r="K70" s="119"/>
+      <c r="L70" s="77"/>
       <c r="M70" s="21" t="s">
         <v>105</v>
       </c>
@@ -13275,10 +13282,10 @@
       <c r="J71" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K71" s="85" t="s">
+      <c r="K71" s="84" t="s">
         <v>232</v>
       </c>
-      <c r="L71" s="80" t="s">
+      <c r="L71" s="79" t="s">
         <v>233</v>
       </c>
       <c r="M71" s="19" t="s">
@@ -13317,8 +13324,8 @@
       <c r="J72" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K72" s="121"/>
-      <c r="L72" s="78"/>
+      <c r="K72" s="119"/>
+      <c r="L72" s="77"/>
       <c r="M72" s="21" t="s">
         <v>105</v>
       </c>
@@ -13349,8 +13356,8 @@
       <c r="J73" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K73" s="121"/>
-      <c r="L73" s="78"/>
+      <c r="K73" s="119"/>
+      <c r="L73" s="77"/>
       <c r="M73" s="21" t="s">
         <v>105</v>
       </c>
@@ -13381,8 +13388,8 @@
       <c r="J74" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K74" s="121"/>
-      <c r="L74" s="78"/>
+      <c r="K74" s="119"/>
+      <c r="L74" s="77"/>
       <c r="M74" s="21" t="s">
         <v>105</v>
       </c>
@@ -13410,8 +13417,8 @@
       <c r="J75" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K75" s="133"/>
-      <c r="L75" s="81"/>
+      <c r="K75" s="131"/>
+      <c r="L75" s="80"/>
       <c r="M75" s="21" t="s">
         <v>105</v>
       </c>
@@ -13448,8 +13455,8 @@
       <c r="J76" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K76" s="82"/>
-      <c r="L76" s="78"/>
+      <c r="K76" s="81"/>
+      <c r="L76" s="77"/>
       <c r="M76" s="23" t="s">
         <v>105</v>
       </c>
@@ -13479,16 +13486,16 @@
       <c r="H77" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I77" s="94" t="s">
+      <c r="I77" s="92" t="s">
         <v>638</v>
       </c>
       <c r="J77" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K77" s="117" t="s">
+      <c r="K77" s="115" t="s">
         <v>241</v>
       </c>
-      <c r="L77" s="122" t="s">
+      <c r="L77" s="120" t="s">
         <v>242</v>
       </c>
       <c r="M77" s="19" t="s">
@@ -13523,14 +13530,14 @@
       <c r="H78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I78" s="94" t="s">
+      <c r="I78" s="92" t="s">
         <v>638</v>
       </c>
       <c r="J78" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K78" s="118"/>
-      <c r="L78" s="123"/>
+      <c r="K78" s="116"/>
+      <c r="L78" s="121"/>
       <c r="M78" s="44" t="s">
         <v>105</v>
       </c>
@@ -13567,10 +13574,10 @@
       <c r="J79" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K79" s="78" t="s">
+      <c r="K79" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L79" s="123"/>
+      <c r="L79" s="121"/>
       <c r="M79" s="44" t="s">
         <v>105</v>
       </c>
@@ -13598,16 +13605,16 @@
       <c r="H80" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I80" s="94" t="s">
+      <c r="I80" s="92" t="s">
         <v>638</v>
       </c>
       <c r="J80" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K80" s="78" t="s">
+      <c r="K80" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L80" s="124"/>
+      <c r="L80" s="122"/>
       <c r="M80" s="20" t="s">
         <v>105</v>
       </c>
@@ -13644,10 +13651,10 @@
       <c r="J81" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K81" s="121" t="s">
+      <c r="K81" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="L81" s="78" t="s">
+      <c r="L81" s="77" t="s">
         <v>137</v>
       </c>
       <c r="M81" s="23" t="s">
@@ -13683,8 +13690,8 @@
       <c r="J82" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K82" s="121"/>
-      <c r="L82" s="78"/>
+      <c r="K82" s="119"/>
+      <c r="L82" s="77"/>
       <c r="M82" s="21" t="s">
         <v>105</v>
       </c>
@@ -13759,10 +13766,10 @@
       <c r="J84" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K84" s="82" t="s">
+      <c r="K84" s="81" t="s">
         <v>253</v>
       </c>
-      <c r="L84" s="78" t="s">
+      <c r="L84" s="77" t="s">
         <v>254</v>
       </c>
       <c r="M84" s="19" t="s">
@@ -13797,7 +13804,7 @@
       <c r="J85" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K85" s="121" t="s">
+      <c r="K85" s="119" t="s">
         <v>255</v>
       </c>
       <c r="L85" s="28"/>
@@ -13833,7 +13840,7 @@
       <c r="J86" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K86" s="121"/>
+      <c r="K86" s="119"/>
       <c r="L86" s="28"/>
       <c r="M86" s="21" t="s">
         <v>105</v>
@@ -13867,7 +13874,7 @@
       <c r="J87" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K87" s="121"/>
+      <c r="K87" s="119"/>
       <c r="L87" s="28"/>
       <c r="M87" s="21" t="s">
         <v>105</v>
@@ -13898,7 +13905,7 @@
       <c r="J88" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K88" s="121"/>
+      <c r="K88" s="119"/>
       <c r="L88" s="28"/>
       <c r="M88" s="21" t="s">
         <v>105</v>
@@ -13932,7 +13939,7 @@
       <c r="J89" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K89" s="121"/>
+      <c r="K89" s="119"/>
       <c r="L89" s="28"/>
       <c r="M89" s="21" t="s">
         <v>105</v>
@@ -13966,7 +13973,7 @@
       <c r="J90" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K90" s="121"/>
+      <c r="K90" s="119"/>
       <c r="L90" s="28"/>
       <c r="M90" s="21" t="s">
         <v>105</v>
@@ -14001,10 +14008,10 @@
       <c r="J91" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K91" s="111" t="s">
+      <c r="K91" s="109" t="s">
         <v>261</v>
       </c>
-      <c r="L91" s="130" t="s">
+      <c r="L91" s="128" t="s">
         <v>262</v>
       </c>
       <c r="M91" s="23" t="s">
@@ -14043,8 +14050,8 @@
       <c r="J92" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K92" s="112"/>
-      <c r="L92" s="131"/>
+      <c r="K92" s="110"/>
+      <c r="L92" s="129"/>
       <c r="M92" s="21" t="s">
         <v>105</v>
       </c>
@@ -14078,8 +14085,8 @@
       <c r="J93" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K93" s="112"/>
-      <c r="L93" s="131"/>
+      <c r="K93" s="110"/>
+      <c r="L93" s="129"/>
       <c r="M93" s="21" t="s">
         <v>105</v>
       </c>
@@ -14110,8 +14117,8 @@
       <c r="J94" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K94" s="113"/>
-      <c r="L94" s="132"/>
+      <c r="K94" s="111"/>
+      <c r="L94" s="130"/>
       <c r="M94" s="21" t="s">
         <v>105</v>
       </c>
@@ -14147,7 +14154,7 @@
       <c r="J95" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K95" s="114"/>
+      <c r="K95" s="112"/>
       <c r="L95" s="28"/>
       <c r="M95" s="23" t="s">
         <v>105</v>
@@ -14181,7 +14188,7 @@
       <c r="J96" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K96" s="115"/>
+      <c r="K96" s="113"/>
       <c r="L96" s="28"/>
       <c r="M96" s="23" t="s">
         <v>105</v>
@@ -14215,7 +14222,7 @@
       <c r="J97" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K97" s="115"/>
+      <c r="K97" s="113"/>
       <c r="L97" s="28"/>
       <c r="M97" s="23" t="s">
         <v>105</v>
@@ -14249,7 +14256,7 @@
       <c r="J98" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K98" s="115"/>
+      <c r="K98" s="113"/>
       <c r="L98" s="28"/>
       <c r="M98" s="23" t="s">
         <v>105</v>
@@ -14282,8 +14289,8 @@
       <c r="J99" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K99" s="116"/>
-      <c r="L99" s="79"/>
+      <c r="K99" s="114"/>
+      <c r="L99" s="78"/>
       <c r="M99" s="30" t="s">
         <v>105</v>
       </c>
@@ -15137,10 +15144,10 @@
       <c r="H25">
         <v>2010</v>
       </c>
-      <c r="I25" s="103" t="s">
+      <c r="I25" s="101" t="s">
         <v>752</v>
       </c>
-      <c r="J25" s="104" t="s">
+      <c r="J25" s="102" t="s">
         <v>753</v>
       </c>
     </row>
@@ -15994,11 +16001,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149AB136-B663-43F8-8265-AB28C3254826}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16010,7 +16017,7 @@
     <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11" style="107" customWidth="1"/>
+    <col min="8" max="8" width="11" style="105" customWidth="1"/>
     <col min="9" max="9" width="55.6640625" style="58" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.33203125" style="58" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -16044,7 +16051,7 @@
       <c r="G1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="104" t="s">
         <v>692</v>
       </c>
       <c r="I1" s="63" t="s">
@@ -16079,10 +16086,10 @@
       <c r="G2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="I2" s="75" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="75"/>
+      <c r="J2" s="74"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -16150,7 +16157,7 @@
       <c r="G5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="75" t="s">
+      <c r="I5" s="74" t="s">
         <v>691</v>
       </c>
     </row>
@@ -16172,8 +16179,8 @@
       <c r="G6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -16228,8 +16235,8 @@
       <c r="G8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -16260,11 +16267,11 @@
       <c r="G9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="107"/>
-      <c r="I9" s="76" t="s">
+      <c r="H9" s="105"/>
+      <c r="I9" s="75" t="s">
         <v>328</v>
       </c>
-      <c r="J9" s="75" t="s">
+      <c r="J9" s="74" t="s">
         <v>329</v>
       </c>
     </row>
@@ -16284,8 +16291,8 @@
       <c r="G10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="107"/>
-      <c r="I10" s="75"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
@@ -16306,7 +16313,7 @@
       <c r="G11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I11" s="76" t="s">
+      <c r="I11" s="75" t="s">
         <v>338</v>
       </c>
       <c r="J11" s="58" t="s">
@@ -16329,7 +16336,7 @@
       <c r="G12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="76" t="s">
+      <c r="I12" s="75" t="s">
         <v>323</v>
       </c>
     </row>
@@ -16349,11 +16356,11 @@
       <c r="G13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="108"/>
-      <c r="I13" s="77" t="s">
+      <c r="H13" s="106"/>
+      <c r="I13" s="76" t="s">
         <v>337</v>
       </c>
-      <c r="J13" s="77" t="s">
+      <c r="J13" s="76" t="s">
         <v>648</v>
       </c>
     </row>
@@ -16367,7 +16374,7 @@
       <c r="G14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="75" t="s">
+      <c r="I14" s="74" t="s">
         <v>691</v>
       </c>
     </row>
@@ -16538,10 +16545,10 @@
       <c r="G22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="I22" s="75" t="s">
+      <c r="I22" s="74" t="s">
         <v>341</v>
       </c>
-      <c r="J22" s="75" t="s">
+      <c r="J22" s="74" t="s">
         <v>342</v>
       </c>
       <c r="K22" s="2"/>
@@ -16568,9 +16575,9 @@
       <c r="G23" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="109"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="103"/>
     </row>
     <row r="24" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
@@ -16591,22 +16598,22 @@
       <c r="G24" t="s">
         <v>793</v>
       </c>
-      <c r="H24" s="108"/>
-      <c r="I24" s="77" t="s">
+      <c r="H24" s="106"/>
+      <c r="I24" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="J24" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="O24" s="71"/>
-      <c r="P24" s="71"/>
-      <c r="Q24" s="71"/>
-      <c r="R24" s="71"/>
-      <c r="S24" s="71"/>
-      <c r="T24" s="71"/>
-      <c r="U24" s="71"/>
-      <c r="V24" s="71"/>
-      <c r="W24" s="71"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="70"/>
+      <c r="R24" s="70"/>
+      <c r="S24" s="70"/>
+      <c r="T24" s="70"/>
+      <c r="U24" s="70"/>
+      <c r="V24" s="70"/>
+      <c r="W24" s="70"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
@@ -16720,18 +16727,18 @@
       <c r="G28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="107"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="O28" s="100"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="100"/>
-      <c r="R28" s="100"/>
-      <c r="S28" s="100"/>
-      <c r="T28" s="100"/>
-      <c r="U28" s="100"/>
-      <c r="V28" s="100"/>
-      <c r="W28" s="102"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="O28" s="98"/>
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="98"/>
+      <c r="V28" s="98"/>
+      <c r="W28" s="100"/>
     </row>
     <row r="29" spans="1:23" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
@@ -16752,22 +16759,22 @@
       <c r="G29" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H29" s="107"/>
-      <c r="I29" s="76" t="s">
+      <c r="H29" s="105"/>
+      <c r="I29" s="75" t="s">
         <v>287</v>
       </c>
-      <c r="J29" s="75" t="s">
+      <c r="J29" s="74" t="s">
         <v>288</v>
       </c>
-      <c r="O29" s="100"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
-      <c r="S29" s="100"/>
-      <c r="T29" s="100"/>
-      <c r="U29" s="100"/>
-      <c r="V29" s="100"/>
-      <c r="W29" s="100"/>
+      <c r="O29" s="98"/>
+      <c r="P29" s="98"/>
+      <c r="Q29" s="98"/>
+      <c r="R29" s="98"/>
+      <c r="S29" s="98"/>
+      <c r="T29" s="98"/>
+      <c r="U29" s="98"/>
+      <c r="V29" s="98"/>
+      <c r="W29" s="98"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
@@ -16789,21 +16796,21 @@
       <c r="G30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="100"/>
-      <c r="P30" s="100"/>
-      <c r="Q30" s="100"/>
-      <c r="R30" s="100"/>
-      <c r="S30" s="100"/>
-      <c r="T30" s="100"/>
-      <c r="U30" s="100"/>
-      <c r="V30" s="100"/>
-      <c r="W30" s="102"/>
+      <c r="O30" s="98"/>
+      <c r="P30" s="98"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="98"/>
+      <c r="S30" s="98"/>
+      <c r="T30" s="98"/>
+      <c r="U30" s="98"/>
+      <c r="V30" s="98"/>
+      <c r="W30" s="100"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
@@ -16853,22 +16860,22 @@
       <c r="G32" t="s">
         <v>793</v>
       </c>
-      <c r="H32" s="108"/>
-      <c r="I32" s="77" t="s">
+      <c r="H32" s="106"/>
+      <c r="I32" s="76" t="s">
         <v>272</v>
       </c>
-      <c r="J32" s="70" t="s">
+      <c r="J32" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="O32" s="71"/>
-      <c r="P32" s="71"/>
-      <c r="Q32" s="71"/>
-      <c r="R32" s="71"/>
-      <c r="S32" s="71"/>
-      <c r="T32" s="71"/>
-      <c r="U32" s="71"/>
-      <c r="V32" s="71"/>
-      <c r="W32" s="71"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="70"/>
+      <c r="Q32" s="70"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="70"/>
+      <c r="T32" s="70"/>
+      <c r="U32" s="70"/>
+      <c r="V32" s="70"/>
+      <c r="W32" s="70"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -16886,7 +16893,7 @@
       <c r="G33" t="s">
         <v>793</v>
       </c>
-      <c r="I33" s="76" t="s">
+      <c r="I33" s="75" t="s">
         <v>272</v>
       </c>
       <c r="J33" s="58" t="s">
@@ -17005,22 +17012,22 @@
       <c r="G37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H37" s="107"/>
-      <c r="I37" s="75" t="s">
+      <c r="H37" s="105"/>
+      <c r="I37" s="74" t="s">
         <v>637</v>
       </c>
-      <c r="J37" s="75" t="s">
+      <c r="J37" s="74" t="s">
         <v>786</v>
       </c>
-      <c r="O37" s="100"/>
-      <c r="P37" s="100"/>
-      <c r="Q37" s="100"/>
-      <c r="R37" s="100"/>
-      <c r="S37" s="100"/>
-      <c r="T37" s="100"/>
-      <c r="U37" s="100"/>
-      <c r="V37" s="100"/>
-      <c r="W37" s="100"/>
+      <c r="O37" s="98"/>
+      <c r="P37" s="98"/>
+      <c r="Q37" s="98"/>
+      <c r="R37" s="98"/>
+      <c r="S37" s="98"/>
+      <c r="T37" s="98"/>
+      <c r="U37" s="98"/>
+      <c r="V37" s="98"/>
+      <c r="W37" s="98"/>
     </row>
     <row r="38" spans="1:23" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -17038,22 +17045,22 @@
       <c r="G38" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H38" s="107"/>
-      <c r="I38" s="76" t="s">
+      <c r="H38" s="105"/>
+      <c r="I38" s="75" t="s">
         <v>279</v>
       </c>
-      <c r="J38" s="75" t="s">
+      <c r="J38" s="74" t="s">
         <v>280</v>
       </c>
-      <c r="O38" s="100"/>
-      <c r="P38" s="100"/>
-      <c r="Q38" s="100"/>
-      <c r="R38" s="100"/>
-      <c r="S38" s="100"/>
-      <c r="T38" s="100"/>
-      <c r="U38" s="100"/>
-      <c r="V38" s="100"/>
-      <c r="W38" s="100"/>
+      <c r="O38" s="98"/>
+      <c r="P38" s="98"/>
+      <c r="Q38" s="98"/>
+      <c r="R38" s="98"/>
+      <c r="S38" s="98"/>
+      <c r="T38" s="98"/>
+      <c r="U38" s="98"/>
+      <c r="V38" s="98"/>
+      <c r="W38" s="98"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -17075,25 +17082,25 @@
       <c r="G39" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="76" t="s">
+      <c r="I39" s="75" t="s">
         <v>647</v>
       </c>
-      <c r="J39" s="75" t="s">
+      <c r="J39" s="74" t="s">
         <v>273</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="100"/>
-      <c r="Q39" s="100"/>
-      <c r="R39" s="100"/>
-      <c r="S39" s="100"/>
-      <c r="T39" s="100"/>
-      <c r="U39" s="100"/>
-      <c r="V39" s="100"/>
-      <c r="W39" s="100"/>
+      <c r="O39" s="98"/>
+      <c r="P39" s="98"/>
+      <c r="Q39" s="98"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="98"/>
+      <c r="T39" s="98"/>
+      <c r="U39" s="98"/>
+      <c r="V39" s="98"/>
+      <c r="W39" s="98"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
@@ -17233,7 +17240,7 @@
       <c r="I44" s="58" t="s">
         <v>637</v>
       </c>
-      <c r="J44" s="75" t="s">
+      <c r="J44" s="74" t="s">
         <v>786</v>
       </c>
       <c r="O44" s="51"/>
@@ -17291,18 +17298,18 @@
       <c r="G46" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="H46" s="107"/>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
-      <c r="O46" s="100"/>
-      <c r="P46" s="100"/>
-      <c r="Q46" s="100"/>
-      <c r="R46" s="100"/>
-      <c r="S46" s="100"/>
-      <c r="T46" s="100"/>
-      <c r="U46" s="100"/>
-      <c r="V46" s="100"/>
-      <c r="W46" s="100"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="98"/>
+      <c r="Q46" s="98"/>
+      <c r="R46" s="98"/>
+      <c r="S46" s="98"/>
+      <c r="T46" s="98"/>
+      <c r="U46" s="98"/>
+      <c r="V46" s="98"/>
+      <c r="W46" s="98"/>
     </row>
     <row r="47" spans="1:23" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -17323,22 +17330,22 @@
       <c r="G47" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="H47" s="107"/>
-      <c r="I47" s="76" t="s">
+      <c r="H47" s="105"/>
+      <c r="I47" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="J47" s="76" t="s">
+      <c r="J47" s="75" t="s">
         <v>645</v>
       </c>
-      <c r="O47" s="100"/>
-      <c r="P47" s="100"/>
-      <c r="Q47" s="100"/>
-      <c r="R47" s="100"/>
-      <c r="S47" s="100"/>
-      <c r="T47" s="100"/>
-      <c r="U47" s="100"/>
-      <c r="V47" s="100"/>
-      <c r="W47" s="100"/>
+      <c r="O47" s="98"/>
+      <c r="P47" s="98"/>
+      <c r="Q47" s="98"/>
+      <c r="R47" s="98"/>
+      <c r="S47" s="98"/>
+      <c r="T47" s="98"/>
+      <c r="U47" s="98"/>
+      <c r="V47" s="98"/>
+      <c r="W47" s="98"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
@@ -17358,21 +17365,21 @@
       <c r="G48" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I48" s="75"/>
-      <c r="J48" s="75"/>
+      <c r="I48" s="74"/>
+      <c r="J48" s="74"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="100"/>
-      <c r="P48" s="100"/>
-      <c r="Q48" s="100"/>
-      <c r="R48" s="100"/>
-      <c r="S48" s="100"/>
-      <c r="T48" s="100"/>
-      <c r="U48" s="100"/>
-      <c r="V48" s="100"/>
-      <c r="W48" s="100"/>
+      <c r="O48" s="98"/>
+      <c r="P48" s="98"/>
+      <c r="Q48" s="98"/>
+      <c r="R48" s="98"/>
+      <c r="S48" s="98"/>
+      <c r="T48" s="98"/>
+      <c r="U48" s="98"/>
+      <c r="V48" s="98"/>
+      <c r="W48" s="98"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -17393,7 +17400,7 @@
       <c r="G49" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I49" s="75"/>
+      <c r="I49" s="74"/>
       <c r="O49" s="51"/>
       <c r="P49" s="51"/>
       <c r="Q49" s="51"/>
@@ -17421,7 +17428,7 @@
         <v>73</v>
       </c>
       <c r="H50" s="37"/>
-      <c r="I50" s="76" t="s">
+      <c r="I50" s="75" t="s">
         <v>318</v>
       </c>
       <c r="J50" s="65" t="s">
@@ -17447,10 +17454,13 @@
       <c r="D51" t="s">
         <v>304</v>
       </c>
+      <c r="E51" t="s">
+        <v>295</v>
+      </c>
       <c r="G51" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I51" s="75" t="s">
+      <c r="I51" s="74" t="s">
         <v>691</v>
       </c>
     </row>
@@ -17463,15 +17473,17 @@
         <v>48</v>
       </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
+      <c r="E52" t="s">
+        <v>295</v>
+      </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I52" s="75" t="s">
+      <c r="I52" s="74" t="s">
         <v>691</v>
       </c>
-      <c r="J52" s="75"/>
+      <c r="J52" s="74"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
@@ -17485,6 +17497,205 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
       <c r="W52" s="2"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>796</v>
+      </c>
+      <c r="C53" t="s">
+        <v>292</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>796</v>
+      </c>
+      <c r="C54" t="s">
+        <v>290</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>796</v>
+      </c>
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>796</v>
+      </c>
+      <c r="C56" t="s">
+        <v>301</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>796</v>
+      </c>
+      <c r="C57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>796</v>
+      </c>
+      <c r="C58" t="s">
+        <v>286</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>796</v>
+      </c>
+      <c r="C59" t="s">
+        <v>293</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G59" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>796</v>
+      </c>
+      <c r="C60" t="s">
+        <v>299</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>796</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>796</v>
+      </c>
+      <c r="C62" t="s">
+        <v>317</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>796</v>
+      </c>
+      <c r="C63" t="s">
+        <v>307</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>796</v>
+      </c>
+      <c r="C64" t="s">
+        <v>275</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>796</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>796</v>
+      </c>
+      <c r="C66" t="s">
+        <v>311</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E1048576" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:W52">
@@ -17516,8 +17727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50FB7270-85D5-483E-AE4E-A5BD24F9C240}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17623,7 +17834,7 @@
       <c r="D7" t="s">
         <v>521</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="99" t="s">
         <v>688</v>
       </c>
     </row>
@@ -17815,12 +18026,6 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>665</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
       <c r="C25">
         <v>1</v>
       </c>
@@ -17843,14 +18048,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c71394a73500791d9f4b659570ff6f6">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0993cb8e7f28d1e7915cb051b812a71" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdc1734568a56db4c93babc30e64c3dd">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2332e6491ccd53482df8a38b341b6af1" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
     <xsd:import namespace="4da7f078-0f32-436f-b12a-21525bae5a0e"/>
     <xsd:element name="properties">
@@ -17865,6 +18064,12 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -17893,6 +18098,35 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="13" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -17924,6 +18158,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{83de6cd9-5cfd-49e4-9ce5-249e9e22fd83}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="4da7f078-0f32-436f-b12a-21525bae5a0e">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -18025,7 +18270,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -18034,17 +18279,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013AD9E7-5ED9-4240-9E80-4B7BF5375D95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a318c9bd-5828-4914-8ac9-a57d8c01df7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4da7f078-0f32-436f-b12a-21525bae5a0e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{358B428F-6B5B-4315-8B12-5337C9BB4513}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5894F413-BEBD-4D32-9133-427F18632D1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -18062,10 +18309,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F7EAA9-3149-4D1D-AC50-D48674558E43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013AD9E7-5ED9-4240-9E80-4B7BF5375D95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
+    <ds:schemaRef ds:uri="4da7f078-0f32-436f-b12a-21525bae5a0e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added periods to CPAR and specific conductance for 2021
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4667" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59565A28-1FCB-4529-8844-8AF1D87BEE36}"/>
+  <xr:revisionPtr revIDLastSave="4669" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BA07F7-DD1D-4436-A366-268F0945B917}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="809" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="809" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="2" r:id="rId1"/>
@@ -2282,12 +2282,6 @@
     <t>CSMI_2021_CTD</t>
   </si>
   <si>
-    <t>SpecificConductance</t>
-  </si>
-  <si>
-    <t>CPARCorrectedIrradiance</t>
-  </si>
-  <si>
     <t>LongName</t>
   </si>
   <si>
@@ -2557,6 +2551,12 @@
   </si>
   <si>
     <t>2020-2020</t>
+  </si>
+  <si>
+    <t>Specific.Conductance</t>
+  </si>
+  <si>
+    <t>CPAR.Corrected.Irradiance</t>
   </si>
 </sst>
 </file>
@@ -3125,7 +3125,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3146,19 +3191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3169,39 +3202,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C1" s="39" t="s">
         <v>1</v>
@@ -3573,7 +3573,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -3595,10 +3595,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B3" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -3615,7 +3615,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -3649,7 +3649,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3768,7 +3768,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -3802,7 +3802,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3819,7 +3819,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C16" t="s">
         <v>665</v>
@@ -3836,7 +3836,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3887,7 +3887,7 @@
         <v>40</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -3904,7 +3904,7 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3955,7 +3955,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -4009,13 +4009,13 @@
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -4057,7 +4057,7 @@
         <v>58</v>
       </c>
       <c r="B30" s="66" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -4074,7 +4074,7 @@
         <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
@@ -4125,7 +4125,7 @@
         <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -4159,7 +4159,7 @@
         <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -4210,7 +4210,7 @@
         <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -7520,8 +7520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5D57F1-DBF9-46B4-8278-09786D5200AB}">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView topLeftCell="E42" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7995,7 +7995,7 @@
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I18" t="s">
         <v>105</v>
@@ -8361,7 +8361,7 @@
         <v>413</v>
       </c>
       <c r="K32" s="69" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
@@ -8441,7 +8441,7 @@
         <v>705</v>
       </c>
       <c r="B36" t="s">
-        <v>706</v>
+        <v>796</v>
       </c>
       <c r="F36">
         <v>2021</v>
@@ -8591,7 +8591,7 @@
         <v>705</v>
       </c>
       <c r="B42" t="s">
-        <v>707</v>
+        <v>797</v>
       </c>
       <c r="F42">
         <v>2021</v>
@@ -9254,7 +9254,7 @@
         <v>484</v>
       </c>
       <c r="H72" s="45" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I72" s="45" t="s">
         <v>412</v>
@@ -9465,7 +9465,7 @@
         <v>499</v>
       </c>
       <c r="K80" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="45" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9494,7 +9494,7 @@
         <v>499</v>
       </c>
       <c r="K81" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="45" customFormat="1" x14ac:dyDescent="0.3">
@@ -9773,7 +9773,7 @@
         <v>502</v>
       </c>
       <c r="H92" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I92" t="s">
         <v>412</v>
@@ -9799,7 +9799,7 @@
         <v>502</v>
       </c>
       <c r="H93" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I93" t="s">
         <v>412</v>
@@ -9938,7 +9938,7 @@
         <v>505</v>
       </c>
       <c r="K98" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="L98" t="s">
         <v>250</v>
@@ -10353,7 +10353,7 @@
         <v>514</v>
       </c>
       <c r="K112" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -10381,7 +10381,7 @@
         <v>513</v>
       </c>
       <c r="K113" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -10409,7 +10409,7 @@
         <v>513</v>
       </c>
       <c r="K114" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -10437,7 +10437,7 @@
         <v>513</v>
       </c>
       <c r="K115" s="65" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
@@ -10559,10 +10559,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D2" t="s">
         <v>79</v>
@@ -10573,10 +10573,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>707</v>
+      </c>
+      <c r="B3" t="s">
         <v>709</v>
-      </c>
-      <c r="B3" t="s">
-        <v>711</v>
       </c>
       <c r="D3" t="s">
         <v>67</v>
@@ -10587,10 +10587,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D4" t="s">
         <v>121</v>
@@ -10601,10 +10601,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B5" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D5" t="s">
         <v>121</v>
@@ -10615,10 +10615,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D6" t="s">
         <v>121</v>
@@ -10629,7 +10629,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B7" t="s">
         <v>672</v>
@@ -10641,15 +10641,15 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B8" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D8" t="s">
         <v>104</v>
@@ -10658,7 +10658,7 @@
         <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -10767,8 +10767,8 @@
       <c r="J2" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="127"/>
-      <c r="L2" s="117"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="110"/>
       <c r="M2" s="19" t="s">
         <v>105</v>
       </c>
@@ -10805,8 +10805,8 @@
       <c r="J3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="125"/>
-      <c r="L3" s="108"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="111"/>
       <c r="M3" s="20" t="s">
         <v>105</v>
       </c>
@@ -10840,8 +10840,8 @@
       <c r="J4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="125"/>
-      <c r="L4" s="108"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="111"/>
       <c r="M4" s="20" t="s">
         <v>105</v>
       </c>
@@ -10872,8 +10872,8 @@
       <c r="J5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="125"/>
-      <c r="L5" s="108"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="111"/>
       <c r="M5" s="20" t="s">
         <v>105</v>
       </c>
@@ -10907,10 +10907,10 @@
       <c r="J6" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="125" t="s">
+      <c r="K6" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="123"/>
+      <c r="L6" s="108"/>
       <c r="M6" s="20" t="s">
         <v>105</v>
       </c>
@@ -10944,8 +10944,8 @@
       <c r="J7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="125"/>
-      <c r="L7" s="123"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="108"/>
       <c r="M7" s="20" t="s">
         <v>105</v>
       </c>
@@ -10976,8 +10976,8 @@
       <c r="J8" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="126"/>
-      <c r="L8" s="124"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="109"/>
       <c r="M8" s="20" t="s">
         <v>105</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>120</v>
       </c>
       <c r="G9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>121</v>
@@ -11014,10 +11014,10 @@
       <c r="J9" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="133" t="s">
+      <c r="K9" s="121" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="108" t="s">
+      <c r="L9" s="111" t="s">
         <v>123</v>
       </c>
       <c r="M9" s="19" t="s">
@@ -11044,7 +11044,7 @@
         <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>104</v>
@@ -11053,8 +11053,8 @@
       <c r="J10" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="133"/>
-      <c r="L10" s="108"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="111"/>
       <c r="M10" s="20" t="s">
         <v>105</v>
       </c>
@@ -11088,8 +11088,8 @@
       <c r="J11" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K11" s="133"/>
-      <c r="L11" s="108"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="111"/>
       <c r="M11" s="21" t="s">
         <v>105</v>
       </c>
@@ -11111,7 +11111,7 @@
         <v>111</v>
       </c>
       <c r="G12" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>104</v>
@@ -11352,7 +11352,7 @@
       <c r="J18" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="119"/>
+      <c r="K18" s="118"/>
       <c r="L18" s="77"/>
       <c r="M18" s="10" t="s">
         <v>105</v>
@@ -11387,7 +11387,7 @@
       <c r="J19" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="131"/>
+      <c r="K19" s="119"/>
       <c r="L19" s="80"/>
       <c r="M19" s="31" t="s">
         <v>105</v>
@@ -11425,10 +11425,10 @@
       <c r="J20" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="119" t="s">
+      <c r="K20" s="118" t="s">
         <v>153</v>
       </c>
-      <c r="L20" s="108" t="s">
+      <c r="L20" s="111" t="s">
         <v>154</v>
       </c>
       <c r="M20" s="10" t="s">
@@ -11464,8 +11464,8 @@
       <c r="J21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K21" s="119"/>
-      <c r="L21" s="108"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="111"/>
       <c r="M21" s="10" t="s">
         <v>105</v>
       </c>
@@ -11496,8 +11496,8 @@
       <c r="J22" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="119"/>
-      <c r="L22" s="108"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="111"/>
       <c r="M22" s="10" t="s">
         <v>105</v>
       </c>
@@ -11531,8 +11531,8 @@
       <c r="J23" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="119"/>
-      <c r="L23" s="108"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="111"/>
       <c r="M23" s="10" t="s">
         <v>105</v>
       </c>
@@ -11566,8 +11566,8 @@
       <c r="J24" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K24" s="119"/>
-      <c r="L24" s="108"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="111"/>
       <c r="M24" s="10" t="s">
         <v>105</v>
       </c>
@@ -11601,10 +11601,10 @@
       <c r="J25" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K25" s="132" t="s">
+      <c r="K25" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="L25" s="117" t="s">
+      <c r="L25" s="110" t="s">
         <v>160</v>
       </c>
       <c r="M25" s="15" t="s">
@@ -11643,8 +11643,8 @@
       <c r="J26" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K26" s="119"/>
-      <c r="L26" s="108"/>
+      <c r="K26" s="118"/>
+      <c r="L26" s="111"/>
       <c r="M26" s="10" t="s">
         <v>105</v>
       </c>
@@ -11678,8 +11678,8 @@
       <c r="J27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K27" s="119"/>
-      <c r="L27" s="108"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="111"/>
       <c r="M27" s="10" t="s">
         <v>105</v>
       </c>
@@ -11710,8 +11710,8 @@
       <c r="J28" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K28" s="131"/>
-      <c r="L28" s="118"/>
+      <c r="K28" s="119"/>
+      <c r="L28" s="130"/>
       <c r="M28" s="11" t="s">
         <v>105</v>
       </c>
@@ -11748,7 +11748,7 @@
       <c r="J29" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K29" s="119" t="s">
+      <c r="K29" s="118" t="s">
         <v>167</v>
       </c>
       <c r="L29" s="77"/>
@@ -11785,7 +11785,7 @@
       <c r="J30" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K30" s="119"/>
+      <c r="K30" s="118"/>
       <c r="L30" s="77"/>
       <c r="M30" s="10" t="s">
         <v>105</v>
@@ -11820,7 +11820,7 @@
       <c r="J31" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K31" s="119"/>
+      <c r="K31" s="118"/>
       <c r="L31" s="77"/>
       <c r="M31" s="10" t="s">
         <v>105</v>
@@ -11852,7 +11852,7 @@
       <c r="J32" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K32" s="119"/>
+      <c r="K32" s="118"/>
       <c r="L32" s="77"/>
       <c r="M32" s="10" t="s">
         <v>105</v>
@@ -11887,7 +11887,7 @@
       <c r="J33" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="132" t="s">
+      <c r="K33" s="120" t="s">
         <v>136</v>
       </c>
       <c r="L33" s="79" t="s">
@@ -11929,7 +11929,7 @@
       <c r="J34" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K34" s="131"/>
+      <c r="K34" s="119"/>
       <c r="L34" s="80"/>
       <c r="M34" s="11" t="s">
         <v>105</v>
@@ -11967,7 +11967,7 @@
       <c r="J35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K35" s="119" t="s">
+      <c r="K35" s="118" t="s">
         <v>136</v>
       </c>
       <c r="L35" s="77" t="s">
@@ -12006,7 +12006,7 @@
       <c r="J36" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K36" s="119"/>
+      <c r="K36" s="118"/>
       <c r="L36" s="77"/>
       <c r="M36" s="10" t="s">
         <v>105</v>
@@ -12117,7 +12117,7 @@
       <c r="K39" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="L39" s="117"/>
+      <c r="L39" s="110"/>
       <c r="M39" s="19" t="s">
         <v>105</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>105</v>
       </c>
       <c r="K40" s="32"/>
-      <c r="L40" s="108"/>
+      <c r="L40" s="111"/>
       <c r="M40" s="20" t="s">
         <v>105</v>
       </c>
@@ -12231,10 +12231,10 @@
       <c r="J42" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K42" s="119" t="s">
+      <c r="K42" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="L42" s="108" t="s">
+      <c r="L42" s="111" t="s">
         <v>186</v>
       </c>
       <c r="M42" s="19" t="s">
@@ -12270,8 +12270,8 @@
       <c r="J43" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="119"/>
-      <c r="L43" s="108"/>
+      <c r="K43" s="118"/>
+      <c r="L43" s="111"/>
       <c r="M43" s="20" t="s">
         <v>105</v>
       </c>
@@ -12305,8 +12305,8 @@
       <c r="J44" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K44" s="119"/>
-      <c r="L44" s="108"/>
+      <c r="K44" s="118"/>
+      <c r="L44" s="111"/>
       <c r="M44" s="20" t="s">
         <v>105</v>
       </c>
@@ -12337,8 +12337,8 @@
       <c r="J45" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K45" s="119"/>
-      <c r="L45" s="108"/>
+      <c r="K45" s="118"/>
+      <c r="L45" s="111"/>
       <c r="M45" s="20" t="s">
         <v>105</v>
       </c>
@@ -12372,8 +12372,8 @@
       <c r="J46" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K46" s="119"/>
-      <c r="L46" s="108"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="111"/>
       <c r="M46" s="20" t="s">
         <v>105</v>
       </c>
@@ -12407,8 +12407,8 @@
       <c r="J47" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K47" s="119"/>
-      <c r="L47" s="108"/>
+      <c r="K47" s="118"/>
+      <c r="L47" s="111"/>
       <c r="M47" s="20" t="s">
         <v>105</v>
       </c>
@@ -12519,7 +12519,7 @@
       <c r="J50" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K50" s="115" t="s">
+      <c r="K50" s="122" t="s">
         <v>198</v>
       </c>
       <c r="L50" s="79"/>
@@ -12559,7 +12559,7 @@
       <c r="J51" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K51" s="133"/>
+      <c r="K51" s="121"/>
       <c r="L51" s="77"/>
       <c r="M51" s="23" t="s">
         <v>105</v>
@@ -12594,7 +12594,7 @@
       <c r="J52" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K52" s="133"/>
+      <c r="K52" s="121"/>
       <c r="L52" s="77"/>
       <c r="M52" s="23" t="s">
         <v>105</v>
@@ -12629,7 +12629,7 @@
       <c r="J53" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K53" s="133"/>
+      <c r="K53" s="121"/>
       <c r="L53" s="77"/>
       <c r="M53" s="23" t="s">
         <v>105</v>
@@ -12661,7 +12661,7 @@
       <c r="J54" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K54" s="116"/>
+      <c r="K54" s="123"/>
       <c r="L54" s="80"/>
       <c r="M54" s="23" t="s">
         <v>105</v>
@@ -12703,7 +12703,7 @@
         <v>208</v>
       </c>
       <c r="L55" s="67" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="M55" s="19" t="s">
         <v>105</v>
@@ -12777,7 +12777,7 @@
       <c r="J57" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K57" s="119" t="s">
+      <c r="K57" s="118" t="s">
         <v>214</v>
       </c>
       <c r="L57" s="77"/>
@@ -12814,7 +12814,7 @@
       <c r="J58" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K58" s="119"/>
+      <c r="K58" s="118"/>
       <c r="L58" s="77"/>
       <c r="M58" s="21" t="s">
         <v>105</v>
@@ -12846,7 +12846,7 @@
       <c r="J59" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K59" s="119"/>
+      <c r="K59" s="118"/>
       <c r="L59" s="77"/>
       <c r="M59" s="21" t="s">
         <v>105</v>
@@ -12881,7 +12881,7 @@
       <c r="J60" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K60" s="117" t="s">
+      <c r="K60" s="110" t="s">
         <v>219</v>
       </c>
       <c r="L60" s="79"/>
@@ -12921,7 +12921,7 @@
       <c r="J61" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K61" s="108"/>
+      <c r="K61" s="111"/>
       <c r="L61" s="77" t="s">
         <v>221</v>
       </c>
@@ -12958,7 +12958,7 @@
       <c r="J62" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K62" s="108"/>
+      <c r="K62" s="111"/>
       <c r="L62" s="77" t="s">
         <v>223</v>
       </c>
@@ -12995,7 +12995,7 @@
       <c r="J63" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K63" s="119"/>
+      <c r="K63" s="118"/>
       <c r="L63" s="77"/>
       <c r="M63" s="20" t="s">
         <v>105</v>
@@ -13030,7 +13030,7 @@
       <c r="J64" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K64" s="119"/>
+      <c r="K64" s="118"/>
       <c r="L64" s="77"/>
       <c r="M64" s="20" t="s">
         <v>105</v>
@@ -13065,7 +13065,7 @@
       <c r="J65" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K65" s="119"/>
+      <c r="K65" s="118"/>
       <c r="L65" s="77" t="s">
         <v>223</v>
       </c>
@@ -13100,7 +13100,7 @@
       <c r="J66" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K66" s="119"/>
+      <c r="K66" s="118"/>
       <c r="L66" s="43"/>
       <c r="M66" s="44" t="s">
         <v>105</v>
@@ -13211,7 +13211,7 @@
       <c r="J69" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K69" s="119" t="s">
+      <c r="K69" s="118" t="s">
         <v>136</v>
       </c>
       <c r="L69" s="77" t="s">
@@ -13250,7 +13250,7 @@
       <c r="J70" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K70" s="119"/>
+      <c r="K70" s="118"/>
       <c r="L70" s="77"/>
       <c r="M70" s="21" t="s">
         <v>105</v>
@@ -13324,7 +13324,7 @@
       <c r="J72" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K72" s="119"/>
+      <c r="K72" s="118"/>
       <c r="L72" s="77"/>
       <c r="M72" s="21" t="s">
         <v>105</v>
@@ -13356,7 +13356,7 @@
       <c r="J73" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K73" s="119"/>
+      <c r="K73" s="118"/>
       <c r="L73" s="77"/>
       <c r="M73" s="21" t="s">
         <v>105</v>
@@ -13388,7 +13388,7 @@
       <c r="J74" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K74" s="119"/>
+      <c r="K74" s="118"/>
       <c r="L74" s="77"/>
       <c r="M74" s="21" t="s">
         <v>105</v>
@@ -13417,7 +13417,7 @@
       <c r="J75" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K75" s="131"/>
+      <c r="K75" s="119"/>
       <c r="L75" s="80"/>
       <c r="M75" s="21" t="s">
         <v>105</v>
@@ -13492,10 +13492,10 @@
       <c r="J77" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K77" s="115" t="s">
+      <c r="K77" s="122" t="s">
         <v>241</v>
       </c>
-      <c r="L77" s="120" t="s">
+      <c r="L77" s="131" t="s">
         <v>242</v>
       </c>
       <c r="M77" s="19" t="s">
@@ -13536,8 +13536,8 @@
       <c r="J78" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K78" s="116"/>
-      <c r="L78" s="121"/>
+      <c r="K78" s="123"/>
+      <c r="L78" s="132"/>
       <c r="M78" s="44" t="s">
         <v>105</v>
       </c>
@@ -13577,7 +13577,7 @@
       <c r="K79" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L79" s="121"/>
+      <c r="L79" s="132"/>
       <c r="M79" s="44" t="s">
         <v>105</v>
       </c>
@@ -13614,7 +13614,7 @@
       <c r="K80" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L80" s="122"/>
+      <c r="L80" s="133"/>
       <c r="M80" s="20" t="s">
         <v>105</v>
       </c>
@@ -13651,7 +13651,7 @@
       <c r="J81" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K81" s="119" t="s">
+      <c r="K81" s="118" t="s">
         <v>136</v>
       </c>
       <c r="L81" s="77" t="s">
@@ -13690,7 +13690,7 @@
       <c r="J82" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K82" s="119"/>
+      <c r="K82" s="118"/>
       <c r="L82" s="77"/>
       <c r="M82" s="21" t="s">
         <v>105</v>
@@ -13729,7 +13729,7 @@
         <v>249</v>
       </c>
       <c r="L83" s="27" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="M83" s="19" t="s">
         <v>105</v>
@@ -13804,7 +13804,7 @@
       <c r="J85" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K85" s="119" t="s">
+      <c r="K85" s="118" t="s">
         <v>255</v>
       </c>
       <c r="L85" s="28"/>
@@ -13840,7 +13840,7 @@
       <c r="J86" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K86" s="119"/>
+      <c r="K86" s="118"/>
       <c r="L86" s="28"/>
       <c r="M86" s="21" t="s">
         <v>105</v>
@@ -13874,7 +13874,7 @@
       <c r="J87" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K87" s="119"/>
+      <c r="K87" s="118"/>
       <c r="L87" s="28"/>
       <c r="M87" s="21" t="s">
         <v>105</v>
@@ -13905,7 +13905,7 @@
       <c r="J88" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K88" s="119"/>
+      <c r="K88" s="118"/>
       <c r="L88" s="28"/>
       <c r="M88" s="21" t="s">
         <v>105</v>
@@ -13939,7 +13939,7 @@
       <c r="J89" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K89" s="119"/>
+      <c r="K89" s="118"/>
       <c r="L89" s="28"/>
       <c r="M89" s="21" t="s">
         <v>105</v>
@@ -13973,7 +13973,7 @@
       <c r="J90" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K90" s="119"/>
+      <c r="K90" s="118"/>
       <c r="L90" s="28"/>
       <c r="M90" s="21" t="s">
         <v>105</v>
@@ -14008,10 +14008,10 @@
       <c r="J91" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K91" s="109" t="s">
+      <c r="K91" s="124" t="s">
         <v>261</v>
       </c>
-      <c r="L91" s="128" t="s">
+      <c r="L91" s="115" t="s">
         <v>262</v>
       </c>
       <c r="M91" s="23" t="s">
@@ -14050,8 +14050,8 @@
       <c r="J92" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K92" s="110"/>
-      <c r="L92" s="129"/>
+      <c r="K92" s="125"/>
+      <c r="L92" s="116"/>
       <c r="M92" s="21" t="s">
         <v>105</v>
       </c>
@@ -14085,8 +14085,8 @@
       <c r="J93" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K93" s="110"/>
-      <c r="L93" s="129"/>
+      <c r="K93" s="125"/>
+      <c r="L93" s="116"/>
       <c r="M93" s="21" t="s">
         <v>105</v>
       </c>
@@ -14117,8 +14117,8 @@
       <c r="J94" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K94" s="111"/>
-      <c r="L94" s="130"/>
+      <c r="K94" s="126"/>
+      <c r="L94" s="117"/>
       <c r="M94" s="21" t="s">
         <v>105</v>
       </c>
@@ -14154,7 +14154,7 @@
       <c r="J95" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K95" s="112"/>
+      <c r="K95" s="127"/>
       <c r="L95" s="28"/>
       <c r="M95" s="23" t="s">
         <v>105</v>
@@ -14188,7 +14188,7 @@
       <c r="J96" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K96" s="113"/>
+      <c r="K96" s="128"/>
       <c r="L96" s="28"/>
       <c r="M96" s="23" t="s">
         <v>105</v>
@@ -14222,7 +14222,7 @@
       <c r="J97" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K97" s="113"/>
+      <c r="K97" s="128"/>
       <c r="L97" s="28"/>
       <c r="M97" s="23" t="s">
         <v>105</v>
@@ -14256,7 +14256,7 @@
       <c r="J98" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K98" s="113"/>
+      <c r="K98" s="128"/>
       <c r="L98" s="28"/>
       <c r="M98" s="23" t="s">
         <v>105</v>
@@ -14289,7 +14289,7 @@
       <c r="J99" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K99" s="114"/>
+      <c r="K99" s="129"/>
       <c r="L99" s="78"/>
       <c r="M99" s="30" t="s">
         <v>105</v>
@@ -14310,6 +14310,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K91:K94"/>
+    <mergeCell ref="K95:K99"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K81:K82"/>
+    <mergeCell ref="K85:K90"/>
+    <mergeCell ref="L77:L80"/>
     <mergeCell ref="L6:L8"/>
     <mergeCell ref="L2:L5"/>
     <mergeCell ref="K6:K8"/>
@@ -14326,20 +14340,6 @@
     <mergeCell ref="K42:K47"/>
     <mergeCell ref="K50:K54"/>
     <mergeCell ref="K57:K59"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K91:K94"/>
-    <mergeCell ref="K95:K99"/>
-    <mergeCell ref="K77:K78"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="K85:K90"/>
-    <mergeCell ref="L77:L80"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="M7:M8 M3:M5 L40 L91 M86:M94 M78:M80 J55:K55 J77:M77 M55 J78:K80 I1:M2 B1:H8 I6:M6 I3:J5 I9:M37 I39:L39 I40:J40 I95:M99 I91:K94 I7:J8 I41:M54 I81:M90 I56:M76 B39:H99 B11:H11 B9:F10 H9:H10 B13:H37 B12:F12 H12">
@@ -14392,28 +14392,28 @@
         <v>266</v>
       </c>
       <c r="C1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1" t="s">
+        <v>716</v>
+      </c>
+      <c r="E1" t="s">
         <v>717</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G1" t="s">
         <v>718</v>
-      </c>
-      <c r="E1" t="s">
-        <v>719</v>
-      </c>
-      <c r="F1" t="s">
-        <v>715</v>
-      </c>
-      <c r="G1" t="s">
-        <v>720</v>
       </c>
       <c r="H1" t="s">
         <v>557</v>
       </c>
       <c r="I1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="J1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -14424,28 +14424,28 @@
         <v>53</v>
       </c>
       <c r="C2" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2" t="s">
         <v>723</v>
-      </c>
-      <c r="D2" t="s">
-        <v>724</v>
-      </c>
-      <c r="E2" t="s">
-        <v>725</v>
       </c>
       <c r="F2">
         <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H2">
         <v>2010</v>
       </c>
       <c r="I2" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="J2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -14456,10 +14456,10 @@
         <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E3" t="s">
         <v>53</v>
@@ -14468,13 +14468,13 @@
         <v>370</v>
       </c>
       <c r="G3" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H3">
         <v>2010</v>
       </c>
       <c r="I3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -14485,10 +14485,10 @@
         <v>289</v>
       </c>
       <c r="C4" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D4" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
@@ -14497,13 +14497,13 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H4">
         <v>2010</v>
       </c>
       <c r="I4" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -14514,10 +14514,10 @@
         <v>268</v>
       </c>
       <c r="C5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E5" t="s">
         <v>53</v>
@@ -14526,16 +14526,16 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H5">
         <v>2010</v>
       </c>
       <c r="I5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -14546,10 +14546,10 @@
         <v>268</v>
       </c>
       <c r="C6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D6" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E6" t="s">
         <v>53</v>
@@ -14558,16 +14558,16 @@
         <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H6">
         <v>2010</v>
       </c>
       <c r="I6" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="J6" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -14578,10 +14578,10 @@
         <v>281</v>
       </c>
       <c r="C7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
@@ -14590,16 +14590,16 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H7">
         <v>2010</v>
       </c>
       <c r="I7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="J7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -14610,10 +14610,10 @@
         <v>291</v>
       </c>
       <c r="C8" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D8" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E8" t="s">
         <v>53</v>
@@ -14622,16 +14622,16 @@
         <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H8">
         <v>2010</v>
       </c>
       <c r="I8" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="J8" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -14645,7 +14645,7 @@
         <v>250</v>
       </c>
       <c r="D9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E9" t="s">
         <v>53</v>
@@ -14654,16 +14654,16 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H9">
         <v>2010</v>
       </c>
       <c r="I9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J9" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -14677,7 +14677,7 @@
         <v>250</v>
       </c>
       <c r="D10" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
@@ -14686,16 +14686,16 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H10">
         <v>2010</v>
       </c>
       <c r="I10" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J10" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -14709,7 +14709,7 @@
         <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E11" t="s">
         <v>53</v>
@@ -14718,16 +14718,16 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H11">
         <v>2010</v>
       </c>
       <c r="I11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -14741,7 +14741,7 @@
         <v>250</v>
       </c>
       <c r="D12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E12" t="s">
         <v>53</v>
@@ -14750,16 +14750,16 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H12">
         <v>2010</v>
       </c>
       <c r="I12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -14773,7 +14773,7 @@
         <v>250</v>
       </c>
       <c r="D13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E13" t="s">
         <v>53</v>
@@ -14782,16 +14782,16 @@
         <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H13">
         <v>2010</v>
       </c>
       <c r="I13" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J13" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -14805,7 +14805,7 @@
         <v>250</v>
       </c>
       <c r="D14" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
@@ -14814,16 +14814,16 @@
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H14">
         <v>2010</v>
       </c>
       <c r="I14" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J14" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -14837,7 +14837,7 @@
         <v>250</v>
       </c>
       <c r="D15" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
@@ -14846,16 +14846,16 @@
         <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H15">
         <v>2010</v>
       </c>
       <c r="I15" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J15" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -14878,13 +14878,13 @@
         <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H16">
         <v>2010</v>
       </c>
       <c r="I16" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -14895,10 +14895,10 @@
         <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D17" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E17" t="s">
         <v>53</v>
@@ -14907,7 +14907,7 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H17">
         <v>2010</v>
@@ -14918,16 +14918,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D18" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E18" t="s">
         <v>53</v>
@@ -14936,7 +14936,7 @@
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H18">
         <v>2010</v>
@@ -14953,10 +14953,10 @@
         <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D19" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E19" t="s">
         <v>53</v>
@@ -14965,7 +14965,7 @@
         <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H19">
         <v>2010</v>
@@ -14982,10 +14982,10 @@
         <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D20" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -14994,7 +14994,7 @@
         <v>15</v>
       </c>
       <c r="G20" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H20">
         <v>2010</v>
@@ -15011,10 +15011,10 @@
         <v>283</v>
       </c>
       <c r="C21" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D21" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E21" t="s">
         <v>53</v>
@@ -15023,13 +15023,13 @@
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H21">
         <v>2010</v>
       </c>
       <c r="I21" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -15040,10 +15040,10 @@
         <v>291</v>
       </c>
       <c r="C22" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D22" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E22" t="s">
         <v>53</v>
@@ -15052,13 +15052,13 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H22">
         <v>2010</v>
       </c>
       <c r="I22" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -15069,19 +15069,19 @@
         <v>53</v>
       </c>
       <c r="C23" t="s">
+        <v>744</v>
+      </c>
+      <c r="D23" t="s">
+        <v>745</v>
+      </c>
+      <c r="E23" t="s">
         <v>746</v>
-      </c>
-      <c r="D23" t="s">
-        <v>747</v>
-      </c>
-      <c r="E23" t="s">
-        <v>748</v>
       </c>
       <c r="F23">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H23">
         <v>2010</v>
@@ -15098,19 +15098,19 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
+        <v>744</v>
+      </c>
+      <c r="D24" t="s">
+        <v>745</v>
+      </c>
+      <c r="E24" t="s">
         <v>746</v>
-      </c>
-      <c r="D24" t="s">
-        <v>747</v>
-      </c>
-      <c r="E24" t="s">
-        <v>748</v>
       </c>
       <c r="F24">
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H24">
         <v>2010</v>
@@ -15127,28 +15127,28 @@
         <v>53</v>
       </c>
       <c r="C25" t="s">
+        <v>747</v>
+      </c>
+      <c r="D25" t="s">
+        <v>748</v>
+      </c>
+      <c r="E25" t="s">
         <v>749</v>
-      </c>
-      <c r="D25" t="s">
-        <v>750</v>
-      </c>
-      <c r="E25" t="s">
-        <v>751</v>
       </c>
       <c r="F25">
         <v>262</v>
       </c>
       <c r="G25" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H25">
         <v>2010</v>
       </c>
       <c r="I25" s="101" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J25" s="102" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -15159,10 +15159,10 @@
         <v>277</v>
       </c>
       <c r="C26" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D26" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
@@ -15171,13 +15171,13 @@
         <v>402</v>
       </c>
       <c r="G26" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H26">
         <v>2010</v>
       </c>
       <c r="I26" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -15188,10 +15188,10 @@
         <v>289</v>
       </c>
       <c r="C27" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D27" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="E27" t="s">
         <v>53</v>
@@ -15200,13 +15200,13 @@
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H27">
         <v>2010</v>
       </c>
       <c r="I27" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -15217,19 +15217,19 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
+        <v>754</v>
+      </c>
+      <c r="D28" t="s">
+        <v>755</v>
+      </c>
+      <c r="E28" t="s">
         <v>756</v>
-      </c>
-      <c r="D28" t="s">
-        <v>757</v>
-      </c>
-      <c r="E28" t="s">
-        <v>758</v>
       </c>
       <c r="F28">
         <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H28">
         <v>2010</v>
@@ -15240,25 +15240,25 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
       </c>
       <c r="C29" t="s">
+        <v>754</v>
+      </c>
+      <c r="D29" t="s">
+        <v>755</v>
+      </c>
+      <c r="E29" t="s">
         <v>756</v>
-      </c>
-      <c r="D29" t="s">
-        <v>757</v>
-      </c>
-      <c r="E29" t="s">
-        <v>758</v>
       </c>
       <c r="F29">
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H29">
         <v>2010</v>
@@ -15275,19 +15275,19 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
+        <v>754</v>
+      </c>
+      <c r="D30" t="s">
+        <v>755</v>
+      </c>
+      <c r="E30" t="s">
         <v>756</v>
-      </c>
-      <c r="D30" t="s">
-        <v>757</v>
-      </c>
-      <c r="E30" t="s">
-        <v>758</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H30">
         <v>2010</v>
@@ -15304,19 +15304,19 @@
         <v>53</v>
       </c>
       <c r="C31" t="s">
+        <v>754</v>
+      </c>
+      <c r="D31" t="s">
+        <v>755</v>
+      </c>
+      <c r="E31" t="s">
         <v>756</v>
-      </c>
-      <c r="D31" t="s">
-        <v>757</v>
-      </c>
-      <c r="E31" t="s">
-        <v>758</v>
       </c>
       <c r="F31">
         <v>16</v>
       </c>
       <c r="G31" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H31">
         <v>2010</v>
@@ -15333,10 +15333,10 @@
         <v>290</v>
       </c>
       <c r="C32" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D32" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E32" t="s">
         <v>53</v>
@@ -15345,13 +15345,13 @@
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H32">
         <v>2015</v>
       </c>
       <c r="I32" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -15362,10 +15362,10 @@
         <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D33" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E33" t="s">
         <v>53</v>
@@ -15374,13 +15374,13 @@
         <v>23</v>
       </c>
       <c r="G33" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H33">
         <v>2015</v>
       </c>
       <c r="I33" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -15391,10 +15391,10 @@
         <v>299</v>
       </c>
       <c r="C34" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D34" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E34" t="s">
         <v>53</v>
@@ -15403,13 +15403,13 @@
         <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H34">
         <v>2015</v>
       </c>
       <c r="I34" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -15420,10 +15420,10 @@
         <v>293</v>
       </c>
       <c r="C35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D35" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
@@ -15432,13 +15432,13 @@
         <v>5</v>
       </c>
       <c r="G35" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H35">
         <v>2015</v>
       </c>
       <c r="I35" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -15449,10 +15449,10 @@
         <v>317</v>
       </c>
       <c r="C36" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D36" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E36" t="s">
         <v>53</v>
@@ -15461,13 +15461,13 @@
         <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H36">
         <v>2015</v>
       </c>
       <c r="I36" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -15478,10 +15478,10 @@
         <v>486</v>
       </c>
       <c r="C37" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D37" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E37" t="s">
         <v>53</v>
@@ -15490,13 +15490,13 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H37">
         <v>2015</v>
       </c>
       <c r="I37" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -15507,10 +15507,10 @@
         <v>292</v>
       </c>
       <c r="C38" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D38" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E38" t="s">
         <v>53</v>
@@ -15519,16 +15519,16 @@
         <v>15</v>
       </c>
       <c r="G38" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H38">
         <v>2015</v>
       </c>
       <c r="I38" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="J38" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -15539,7 +15539,7 @@
         <v>293</v>
       </c>
       <c r="C39" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D39" t="s">
         <v>53</v>
@@ -15551,16 +15551,16 @@
         <v>72</v>
       </c>
       <c r="G39" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H39">
         <v>2015</v>
       </c>
       <c r="I39" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J39" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -15571,7 +15571,7 @@
         <v>486</v>
       </c>
       <c r="C40" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D40" t="s">
         <v>53</v>
@@ -15583,16 +15583,16 @@
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H40">
         <v>2015</v>
       </c>
       <c r="I40" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J40" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -15603,7 +15603,7 @@
         <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D41" t="s">
         <v>53</v>
@@ -15615,16 +15615,16 @@
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H41">
         <v>2015</v>
       </c>
       <c r="I41" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J41" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -15635,7 +15635,7 @@
         <v>292</v>
       </c>
       <c r="C42" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -15647,16 +15647,16 @@
         <v>4</v>
       </c>
       <c r="G42" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H42">
         <v>2015</v>
       </c>
       <c r="I42" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J42" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -15667,7 +15667,7 @@
         <v>293</v>
       </c>
       <c r="C43" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
@@ -15679,16 +15679,16 @@
         <v>2</v>
       </c>
       <c r="G43" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H43">
         <v>2015</v>
       </c>
       <c r="I43" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J43" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -15699,7 +15699,7 @@
         <v>486</v>
       </c>
       <c r="C44" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D44" t="s">
         <v>53</v>
@@ -15711,16 +15711,16 @@
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H44">
         <v>2015</v>
       </c>
       <c r="I44" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J44" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -15731,7 +15731,7 @@
         <v>292</v>
       </c>
       <c r="C45" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D45" t="s">
         <v>53</v>
@@ -15743,16 +15743,16 @@
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H45">
         <v>2015</v>
       </c>
       <c r="I45" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="J45" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -15763,19 +15763,19 @@
         <v>275</v>
       </c>
       <c r="C46" t="s">
+        <v>765</v>
+      </c>
+      <c r="D46" t="s">
+        <v>766</v>
+      </c>
+      <c r="E46" t="s">
         <v>767</v>
-      </c>
-      <c r="D46" t="s">
-        <v>768</v>
-      </c>
-      <c r="E46" t="s">
-        <v>769</v>
       </c>
       <c r="F46">
         <v>23</v>
       </c>
       <c r="G46" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H46">
         <v>2015</v>
@@ -15784,7 +15784,7 @@
         <v>127</v>
       </c>
       <c r="J46" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -15795,28 +15795,28 @@
         <v>290</v>
       </c>
       <c r="C47" t="s">
+        <v>765</v>
+      </c>
+      <c r="D47" t="s">
+        <v>766</v>
+      </c>
+      <c r="E47" t="s">
         <v>767</v>
-      </c>
-      <c r="D47" t="s">
-        <v>768</v>
-      </c>
-      <c r="E47" t="s">
-        <v>769</v>
       </c>
       <c r="F47">
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H47">
         <v>2015</v>
       </c>
       <c r="I47" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="J47" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -15827,28 +15827,28 @@
         <v>292</v>
       </c>
       <c r="C48" t="s">
+        <v>765</v>
+      </c>
+      <c r="D48" t="s">
+        <v>766</v>
+      </c>
+      <c r="E48" t="s">
         <v>767</v>
-      </c>
-      <c r="D48" t="s">
-        <v>768</v>
-      </c>
-      <c r="E48" t="s">
-        <v>769</v>
       </c>
       <c r="F48">
         <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H48">
         <v>2015</v>
       </c>
       <c r="I48" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="J48" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -16003,9 +16003,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149AB136-B663-43F8-8265-AB28C3254826}">
   <dimension ref="A1:W66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16596,7 +16596,7 @@
         <v>271</v>
       </c>
       <c r="G24" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H24" s="106"/>
       <c r="I24" s="76" t="s">
@@ -16858,7 +16858,7 @@
         <v>296</v>
       </c>
       <c r="G32" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H32" s="106"/>
       <c r="I32" s="76" t="s">
@@ -16891,7 +16891,7 @@
         <v>296</v>
       </c>
       <c r="G33" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I33" s="75" t="s">
         <v>272</v>
@@ -17017,7 +17017,7 @@
         <v>637</v>
       </c>
       <c r="J37" s="74" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="O37" s="98"/>
       <c r="P37" s="98"/>
@@ -17241,7 +17241,7 @@
         <v>637</v>
       </c>
       <c r="J44" s="74" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="O44" s="51"/>
       <c r="P44" s="51"/>
@@ -17495,13 +17495,13 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C53" t="s">
         <v>292</v>
       </c>
       <c r="E53" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G53" t="s">
         <v>59</v>
@@ -17509,13 +17509,13 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C54" t="s">
         <v>290</v>
       </c>
       <c r="E54" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G54" t="s">
         <v>42</v>
@@ -17523,13 +17523,13 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C55" t="s">
         <v>75</v>
       </c>
       <c r="E55" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G55" t="s">
         <v>75</v>
@@ -17537,13 +17537,13 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C56" t="s">
         <v>301</v>
       </c>
       <c r="E56" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G56" t="s">
         <v>22</v>
@@ -17551,13 +17551,13 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C57" t="s">
         <v>48</v>
       </c>
       <c r="E57" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G57" t="s">
         <v>48</v>
@@ -17565,13 +17565,13 @@
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C58" t="s">
         <v>286</v>
       </c>
       <c r="E58" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G58" t="s">
         <v>127</v>
@@ -17579,27 +17579,27 @@
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C59" t="s">
         <v>293</v>
       </c>
       <c r="E59" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G59" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C60" t="s">
         <v>299</v>
       </c>
       <c r="E60" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G60" t="s">
         <v>18</v>
@@ -17607,13 +17607,13 @@
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C61" t="s">
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G61" t="s">
         <v>127</v>
@@ -17621,13 +17621,13 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C62" t="s">
         <v>317</v>
       </c>
       <c r="E62" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G62" t="s">
         <v>73</v>
@@ -17635,13 +17635,13 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C63" t="s">
         <v>307</v>
       </c>
       <c r="E63" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G63" t="s">
         <v>52</v>
@@ -17649,13 +17649,13 @@
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C64" t="s">
         <v>275</v>
       </c>
       <c r="E64" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G64" t="s">
         <v>20</v>
@@ -17663,13 +17663,13 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
       </c>
       <c r="E65" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G65" t="s">
         <v>127</v>
@@ -17677,13 +17677,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C66" t="s">
         <v>311</v>
       </c>
       <c r="E66" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G66" t="s">
         <v>640</v>
@@ -17986,10 +17986,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B22" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -18263,15 +18263,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a318c9bd-5828-4914-8ac9-a57d8c01df7a">
@@ -18280,6 +18271,15 @@
     <TaxCatchAll xmlns="4da7f078-0f32-436f-b12a-21525bae5a0e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18302,14 +18302,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F7EAA9-3149-4D1D-AC50-D48674558E43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013AD9E7-5ED9-4240-9E80-4B7BF5375D95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -18318,4 +18310,12 @@
     <ds:schemaRef ds:uri="4da7f078-0f32-436f-b12a-21525bae5a0e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F7EAA9-3149-4D1D-AC50-D48674558E43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Additional period at end of CPAR to make the join happy
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4669" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52BA07F7-DD1D-4436-A366-268F0945B917}"/>
+  <xr:revisionPtr revIDLastSave="4670" documentId="8_{D82D06AB-5E11-4340-B04B-6FA55AFBCF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A41A4F1-F030-44F6-9841-305BBAE067AB}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="809" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2556,7 +2556,7 @@
     <t>Specific.Conductance</t>
   </si>
   <si>
-    <t>CPAR.Corrected.Irradiance</t>
+    <t>CPAR.Corrected.Irradiance.</t>
   </si>
 </sst>
 </file>
@@ -3125,16 +3125,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3155,9 +3194,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3166,42 +3202,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7521,7 +7521,7 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10767,8 +10767,8 @@
       <c r="J2" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="114"/>
-      <c r="L2" s="110"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="117"/>
       <c r="M2" s="19" t="s">
         <v>105</v>
       </c>
@@ -10805,8 +10805,8 @@
       <c r="J3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="112"/>
-      <c r="L3" s="111"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="108"/>
       <c r="M3" s="20" t="s">
         <v>105</v>
       </c>
@@ -10840,8 +10840,8 @@
       <c r="J4" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="112"/>
-      <c r="L4" s="111"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="108"/>
       <c r="M4" s="20" t="s">
         <v>105</v>
       </c>
@@ -10872,8 +10872,8 @@
       <c r="J5" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="111"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="108"/>
       <c r="M5" s="20" t="s">
         <v>105</v>
       </c>
@@ -10907,10 +10907,10 @@
       <c r="J6" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="112" t="s">
+      <c r="K6" s="125" t="s">
         <v>114</v>
       </c>
-      <c r="L6" s="108"/>
+      <c r="L6" s="123"/>
       <c r="M6" s="20" t="s">
         <v>105</v>
       </c>
@@ -10944,8 +10944,8 @@
       <c r="J7" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="112"/>
-      <c r="L7" s="108"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="123"/>
       <c r="M7" s="20" t="s">
         <v>105</v>
       </c>
@@ -10976,8 +10976,8 @@
       <c r="J8" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="113"/>
-      <c r="L8" s="109"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="124"/>
       <c r="M8" s="20" t="s">
         <v>105</v>
       </c>
@@ -11014,10 +11014,10 @@
       <c r="J9" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K9" s="121" t="s">
+      <c r="K9" s="133" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="111" t="s">
+      <c r="L9" s="108" t="s">
         <v>123</v>
       </c>
       <c r="M9" s="19" t="s">
@@ -11053,8 +11053,8 @@
       <c r="J10" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="121"/>
-      <c r="L10" s="111"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="108"/>
       <c r="M10" s="20" t="s">
         <v>105</v>
       </c>
@@ -11088,8 +11088,8 @@
       <c r="J11" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K11" s="121"/>
-      <c r="L11" s="111"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="108"/>
       <c r="M11" s="21" t="s">
         <v>105</v>
       </c>
@@ -11352,7 +11352,7 @@
       <c r="J18" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="118"/>
+      <c r="K18" s="119"/>
       <c r="L18" s="77"/>
       <c r="M18" s="10" t="s">
         <v>105</v>
@@ -11387,7 +11387,7 @@
       <c r="J19" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="119"/>
+      <c r="K19" s="131"/>
       <c r="L19" s="80"/>
       <c r="M19" s="31" t="s">
         <v>105</v>
@@ -11425,10 +11425,10 @@
       <c r="J20" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K20" s="118" t="s">
+      <c r="K20" s="119" t="s">
         <v>153</v>
       </c>
-      <c r="L20" s="111" t="s">
+      <c r="L20" s="108" t="s">
         <v>154</v>
       </c>
       <c r="M20" s="10" t="s">
@@ -11464,8 +11464,8 @@
       <c r="J21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K21" s="118"/>
-      <c r="L21" s="111"/>
+      <c r="K21" s="119"/>
+      <c r="L21" s="108"/>
       <c r="M21" s="10" t="s">
         <v>105</v>
       </c>
@@ -11496,8 +11496,8 @@
       <c r="J22" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K22" s="118"/>
-      <c r="L22" s="111"/>
+      <c r="K22" s="119"/>
+      <c r="L22" s="108"/>
       <c r="M22" s="10" t="s">
         <v>105</v>
       </c>
@@ -11531,8 +11531,8 @@
       <c r="J23" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K23" s="118"/>
-      <c r="L23" s="111"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="108"/>
       <c r="M23" s="10" t="s">
         <v>105</v>
       </c>
@@ -11566,8 +11566,8 @@
       <c r="J24" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K24" s="118"/>
-      <c r="L24" s="111"/>
+      <c r="K24" s="119"/>
+      <c r="L24" s="108"/>
       <c r="M24" s="10" t="s">
         <v>105</v>
       </c>
@@ -11601,10 +11601,10 @@
       <c r="J25" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K25" s="120" t="s">
+      <c r="K25" s="132" t="s">
         <v>159</v>
       </c>
-      <c r="L25" s="110" t="s">
+      <c r="L25" s="117" t="s">
         <v>160</v>
       </c>
       <c r="M25" s="15" t="s">
@@ -11643,8 +11643,8 @@
       <c r="J26" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K26" s="118"/>
-      <c r="L26" s="111"/>
+      <c r="K26" s="119"/>
+      <c r="L26" s="108"/>
       <c r="M26" s="10" t="s">
         <v>105</v>
       </c>
@@ -11678,8 +11678,8 @@
       <c r="J27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K27" s="118"/>
-      <c r="L27" s="111"/>
+      <c r="K27" s="119"/>
+      <c r="L27" s="108"/>
       <c r="M27" s="10" t="s">
         <v>105</v>
       </c>
@@ -11710,8 +11710,8 @@
       <c r="J28" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K28" s="119"/>
-      <c r="L28" s="130"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="118"/>
       <c r="M28" s="11" t="s">
         <v>105</v>
       </c>
@@ -11748,7 +11748,7 @@
       <c r="J29" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K29" s="118" t="s">
+      <c r="K29" s="119" t="s">
         <v>167</v>
       </c>
       <c r="L29" s="77"/>
@@ -11785,7 +11785,7 @@
       <c r="J30" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K30" s="118"/>
+      <c r="K30" s="119"/>
       <c r="L30" s="77"/>
       <c r="M30" s="10" t="s">
         <v>105</v>
@@ -11820,7 +11820,7 @@
       <c r="J31" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K31" s="118"/>
+      <c r="K31" s="119"/>
       <c r="L31" s="77"/>
       <c r="M31" s="10" t="s">
         <v>105</v>
@@ -11852,7 +11852,7 @@
       <c r="J32" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K32" s="118"/>
+      <c r="K32" s="119"/>
       <c r="L32" s="77"/>
       <c r="M32" s="10" t="s">
         <v>105</v>
@@ -11887,7 +11887,7 @@
       <c r="J33" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="120" t="s">
+      <c r="K33" s="132" t="s">
         <v>136</v>
       </c>
       <c r="L33" s="79" t="s">
@@ -11929,7 +11929,7 @@
       <c r="J34" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K34" s="119"/>
+      <c r="K34" s="131"/>
       <c r="L34" s="80"/>
       <c r="M34" s="11" t="s">
         <v>105</v>
@@ -11967,7 +11967,7 @@
       <c r="J35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K35" s="118" t="s">
+      <c r="K35" s="119" t="s">
         <v>136</v>
       </c>
       <c r="L35" s="77" t="s">
@@ -12006,7 +12006,7 @@
       <c r="J36" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K36" s="118"/>
+      <c r="K36" s="119"/>
       <c r="L36" s="77"/>
       <c r="M36" s="10" t="s">
         <v>105</v>
@@ -12117,7 +12117,7 @@
       <c r="K39" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="L39" s="110"/>
+      <c r="L39" s="117"/>
       <c r="M39" s="19" t="s">
         <v>105</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>105</v>
       </c>
       <c r="K40" s="32"/>
-      <c r="L40" s="111"/>
+      <c r="L40" s="108"/>
       <c r="M40" s="20" t="s">
         <v>105</v>
       </c>
@@ -12231,10 +12231,10 @@
       <c r="J42" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K42" s="118" t="s">
+      <c r="K42" s="119" t="s">
         <v>185</v>
       </c>
-      <c r="L42" s="111" t="s">
+      <c r="L42" s="108" t="s">
         <v>186</v>
       </c>
       <c r="M42" s="19" t="s">
@@ -12270,8 +12270,8 @@
       <c r="J43" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="118"/>
-      <c r="L43" s="111"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="108"/>
       <c r="M43" s="20" t="s">
         <v>105</v>
       </c>
@@ -12305,8 +12305,8 @@
       <c r="J44" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K44" s="118"/>
-      <c r="L44" s="111"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="108"/>
       <c r="M44" s="20" t="s">
         <v>105</v>
       </c>
@@ -12337,8 +12337,8 @@
       <c r="J45" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K45" s="118"/>
-      <c r="L45" s="111"/>
+      <c r="K45" s="119"/>
+      <c r="L45" s="108"/>
       <c r="M45" s="20" t="s">
         <v>105</v>
       </c>
@@ -12372,8 +12372,8 @@
       <c r="J46" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K46" s="118"/>
-      <c r="L46" s="111"/>
+      <c r="K46" s="119"/>
+      <c r="L46" s="108"/>
       <c r="M46" s="20" t="s">
         <v>105</v>
       </c>
@@ -12407,8 +12407,8 @@
       <c r="J47" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K47" s="118"/>
-      <c r="L47" s="111"/>
+      <c r="K47" s="119"/>
+      <c r="L47" s="108"/>
       <c r="M47" s="20" t="s">
         <v>105</v>
       </c>
@@ -12519,7 +12519,7 @@
       <c r="J50" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K50" s="122" t="s">
+      <c r="K50" s="115" t="s">
         <v>198</v>
       </c>
       <c r="L50" s="79"/>
@@ -12559,7 +12559,7 @@
       <c r="J51" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K51" s="121"/>
+      <c r="K51" s="133"/>
       <c r="L51" s="77"/>
       <c r="M51" s="23" t="s">
         <v>105</v>
@@ -12594,7 +12594,7 @@
       <c r="J52" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K52" s="121"/>
+      <c r="K52" s="133"/>
       <c r="L52" s="77"/>
       <c r="M52" s="23" t="s">
         <v>105</v>
@@ -12629,7 +12629,7 @@
       <c r="J53" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K53" s="121"/>
+      <c r="K53" s="133"/>
       <c r="L53" s="77"/>
       <c r="M53" s="23" t="s">
         <v>105</v>
@@ -12661,7 +12661,7 @@
       <c r="J54" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K54" s="123"/>
+      <c r="K54" s="116"/>
       <c r="L54" s="80"/>
       <c r="M54" s="23" t="s">
         <v>105</v>
@@ -12777,7 +12777,7 @@
       <c r="J57" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K57" s="118" t="s">
+      <c r="K57" s="119" t="s">
         <v>214</v>
       </c>
       <c r="L57" s="77"/>
@@ -12814,7 +12814,7 @@
       <c r="J58" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K58" s="118"/>
+      <c r="K58" s="119"/>
       <c r="L58" s="77"/>
       <c r="M58" s="21" t="s">
         <v>105</v>
@@ -12846,7 +12846,7 @@
       <c r="J59" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K59" s="118"/>
+      <c r="K59" s="119"/>
       <c r="L59" s="77"/>
       <c r="M59" s="21" t="s">
         <v>105</v>
@@ -12881,7 +12881,7 @@
       <c r="J60" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="K60" s="110" t="s">
+      <c r="K60" s="117" t="s">
         <v>219</v>
       </c>
       <c r="L60" s="79"/>
@@ -12921,7 +12921,7 @@
       <c r="J61" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K61" s="111"/>
+      <c r="K61" s="108"/>
       <c r="L61" s="77" t="s">
         <v>221</v>
       </c>
@@ -12958,7 +12958,7 @@
       <c r="J62" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K62" s="111"/>
+      <c r="K62" s="108"/>
       <c r="L62" s="77" t="s">
         <v>223</v>
       </c>
@@ -12995,7 +12995,7 @@
       <c r="J63" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K63" s="118"/>
+      <c r="K63" s="119"/>
       <c r="L63" s="77"/>
       <c r="M63" s="20" t="s">
         <v>105</v>
@@ -13030,7 +13030,7 @@
       <c r="J64" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K64" s="118"/>
+      <c r="K64" s="119"/>
       <c r="L64" s="77"/>
       <c r="M64" s="20" t="s">
         <v>105</v>
@@ -13065,7 +13065,7 @@
       <c r="J65" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K65" s="118"/>
+      <c r="K65" s="119"/>
       <c r="L65" s="77" t="s">
         <v>223</v>
       </c>
@@ -13100,7 +13100,7 @@
       <c r="J66" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="K66" s="118"/>
+      <c r="K66" s="119"/>
       <c r="L66" s="43"/>
       <c r="M66" s="44" t="s">
         <v>105</v>
@@ -13211,7 +13211,7 @@
       <c r="J69" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K69" s="118" t="s">
+      <c r="K69" s="119" t="s">
         <v>136</v>
       </c>
       <c r="L69" s="77" t="s">
@@ -13250,7 +13250,7 @@
       <c r="J70" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K70" s="118"/>
+      <c r="K70" s="119"/>
       <c r="L70" s="77"/>
       <c r="M70" s="21" t="s">
         <v>105</v>
@@ -13324,7 +13324,7 @@
       <c r="J72" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K72" s="118"/>
+      <c r="K72" s="119"/>
       <c r="L72" s="77"/>
       <c r="M72" s="21" t="s">
         <v>105</v>
@@ -13356,7 +13356,7 @@
       <c r="J73" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K73" s="118"/>
+      <c r="K73" s="119"/>
       <c r="L73" s="77"/>
       <c r="M73" s="21" t="s">
         <v>105</v>
@@ -13388,7 +13388,7 @@
       <c r="J74" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K74" s="118"/>
+      <c r="K74" s="119"/>
       <c r="L74" s="77"/>
       <c r="M74" s="21" t="s">
         <v>105</v>
@@ -13417,7 +13417,7 @@
       <c r="J75" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K75" s="119"/>
+      <c r="K75" s="131"/>
       <c r="L75" s="80"/>
       <c r="M75" s="21" t="s">
         <v>105</v>
@@ -13492,10 +13492,10 @@
       <c r="J77" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K77" s="122" t="s">
+      <c r="K77" s="115" t="s">
         <v>241</v>
       </c>
-      <c r="L77" s="131" t="s">
+      <c r="L77" s="120" t="s">
         <v>242</v>
       </c>
       <c r="M77" s="19" t="s">
@@ -13536,8 +13536,8 @@
       <c r="J78" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K78" s="123"/>
-      <c r="L78" s="132"/>
+      <c r="K78" s="116"/>
+      <c r="L78" s="121"/>
       <c r="M78" s="44" t="s">
         <v>105</v>
       </c>
@@ -13577,7 +13577,7 @@
       <c r="K79" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L79" s="132"/>
+      <c r="L79" s="121"/>
       <c r="M79" s="44" t="s">
         <v>105</v>
       </c>
@@ -13614,7 +13614,7 @@
       <c r="K80" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="L80" s="133"/>
+      <c r="L80" s="122"/>
       <c r="M80" s="20" t="s">
         <v>105</v>
       </c>
@@ -13651,7 +13651,7 @@
       <c r="J81" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K81" s="118" t="s">
+      <c r="K81" s="119" t="s">
         <v>136</v>
       </c>
       <c r="L81" s="77" t="s">
@@ -13690,7 +13690,7 @@
       <c r="J82" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="K82" s="118"/>
+      <c r="K82" s="119"/>
       <c r="L82" s="77"/>
       <c r="M82" s="21" t="s">
         <v>105</v>
@@ -13804,7 +13804,7 @@
       <c r="J85" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K85" s="118" t="s">
+      <c r="K85" s="119" t="s">
         <v>255</v>
       </c>
       <c r="L85" s="28"/>
@@ -13840,7 +13840,7 @@
       <c r="J86" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K86" s="118"/>
+      <c r="K86" s="119"/>
       <c r="L86" s="28"/>
       <c r="M86" s="21" t="s">
         <v>105</v>
@@ -13874,7 +13874,7 @@
       <c r="J87" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K87" s="118"/>
+      <c r="K87" s="119"/>
       <c r="L87" s="28"/>
       <c r="M87" s="21" t="s">
         <v>105</v>
@@ -13905,7 +13905,7 @@
       <c r="J88" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K88" s="118"/>
+      <c r="K88" s="119"/>
       <c r="L88" s="28"/>
       <c r="M88" s="21" t="s">
         <v>105</v>
@@ -13939,7 +13939,7 @@
       <c r="J89" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K89" s="118"/>
+      <c r="K89" s="119"/>
       <c r="L89" s="28"/>
       <c r="M89" s="21" t="s">
         <v>105</v>
@@ -13973,7 +13973,7 @@
       <c r="J90" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K90" s="118"/>
+      <c r="K90" s="119"/>
       <c r="L90" s="28"/>
       <c r="M90" s="21" t="s">
         <v>105</v>
@@ -14008,10 +14008,10 @@
       <c r="J91" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K91" s="124" t="s">
+      <c r="K91" s="109" t="s">
         <v>261</v>
       </c>
-      <c r="L91" s="115" t="s">
+      <c r="L91" s="128" t="s">
         <v>262</v>
       </c>
       <c r="M91" s="23" t="s">
@@ -14050,8 +14050,8 @@
       <c r="J92" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K92" s="125"/>
-      <c r="L92" s="116"/>
+      <c r="K92" s="110"/>
+      <c r="L92" s="129"/>
       <c r="M92" s="21" t="s">
         <v>105</v>
       </c>
@@ -14085,8 +14085,8 @@
       <c r="J93" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K93" s="125"/>
-      <c r="L93" s="116"/>
+      <c r="K93" s="110"/>
+      <c r="L93" s="129"/>
       <c r="M93" s="21" t="s">
         <v>105</v>
       </c>
@@ -14117,8 +14117,8 @@
       <c r="J94" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K94" s="126"/>
-      <c r="L94" s="117"/>
+      <c r="K94" s="111"/>
+      <c r="L94" s="130"/>
       <c r="M94" s="21" t="s">
         <v>105</v>
       </c>
@@ -14154,7 +14154,7 @@
       <c r="J95" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K95" s="127"/>
+      <c r="K95" s="112"/>
       <c r="L95" s="28"/>
       <c r="M95" s="23" t="s">
         <v>105</v>
@@ -14188,7 +14188,7 @@
       <c r="J96" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K96" s="128"/>
+      <c r="K96" s="113"/>
       <c r="L96" s="28"/>
       <c r="M96" s="23" t="s">
         <v>105</v>
@@ -14222,7 +14222,7 @@
       <c r="J97" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K97" s="128"/>
+      <c r="K97" s="113"/>
       <c r="L97" s="28"/>
       <c r="M97" s="23" t="s">
         <v>105</v>
@@ -14256,7 +14256,7 @@
       <c r="J98" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K98" s="128"/>
+      <c r="K98" s="113"/>
       <c r="L98" s="28"/>
       <c r="M98" s="23" t="s">
         <v>105</v>
@@ -14289,7 +14289,7 @@
       <c r="J99" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K99" s="129"/>
+      <c r="K99" s="114"/>
       <c r="L99" s="78"/>
       <c r="M99" s="30" t="s">
         <v>105</v>
@@ -14310,20 +14310,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K91:K94"/>
-    <mergeCell ref="K95:K99"/>
-    <mergeCell ref="K77:K78"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="K85:K90"/>
-    <mergeCell ref="L77:L80"/>
     <mergeCell ref="L6:L8"/>
     <mergeCell ref="L2:L5"/>
     <mergeCell ref="K6:K8"/>
@@ -14340,6 +14326,20 @@
     <mergeCell ref="K42:K47"/>
     <mergeCell ref="K50:K54"/>
     <mergeCell ref="K57:K59"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K91:K94"/>
+    <mergeCell ref="K95:K99"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K81:K82"/>
+    <mergeCell ref="K85:K90"/>
+    <mergeCell ref="L77:L80"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="M7:M8 M3:M5 L40 L91 M86:M94 M78:M80 J55:K55 J77:M77 M55 J78:K80 I1:M2 B1:H8 I6:M6 I3:J5 I9:M37 I39:L39 I40:J40 I95:M99 I91:K94 I7:J8 I41:M54 I81:M90 I56:M76 B39:H99 B11:H11 B9:F10 H9:H10 B13:H37 B12:F12 H12">
@@ -18040,6 +18040,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a318c9bd-5828-4914-8ac9-a57d8c01df7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4da7f078-0f32-436f-b12a-21525bae5a0e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdc1734568a56db4c93babc30e64c3dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2332e6491ccd53482df8a38b341b6af1" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
@@ -18262,27 +18282,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a318c9bd-5828-4914-8ac9-a57d8c01df7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4da7f078-0f32-436f-b12a-21525bae5a0e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F7EAA9-3149-4D1D-AC50-D48674558E43}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013AD9E7-5ED9-4240-9E80-4B7BF5375D95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
+    <ds:schemaRef ds:uri="4da7f078-0f32-436f-b12a-21525bae5a0e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5894F413-BEBD-4D32-9133-427F18632D1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18299,23 +18318,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{013AD9E7-5ED9-4240-9E80-4B7BF5375D95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
-    <ds:schemaRef ds:uri="4da7f078-0f32-436f-b12a-21525bae5a0e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A4F7EAA9-3149-4D1D-AC50-D48674558E43}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added mappings for NOAA CTD analytes
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41C7C777-B700-4213-AF96-E0D69987F272}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D38B74-D02D-4FBA-AA47-AED37ABDE78C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="800">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2451,6 +2451,18 @@
   </si>
   <si>
     <t>Turbidity, Nephelometric Turbidity Units</t>
+  </si>
+  <si>
+    <t>NOAActd</t>
+  </si>
+  <si>
+    <t>mll</t>
+  </si>
+  <si>
+    <t>Guessing this was mislabeled for noaa ctd DO</t>
+  </si>
+  <si>
+    <t>oce remves this need to figure outu why…</t>
   </si>
 </sst>
 </file>
@@ -3066,11 +3078,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3078,10 +3114,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3095,30 +3131,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3427,7 +3439,9 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11609,9 +11623,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11791,6 +11807,59 @@
         <v>620</v>
       </c>
       <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11894,8 +11963,8 @@
       <c r="J2" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K2" s="93"/>
-      <c r="L2" s="95"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="103"/>
       <c r="M2" s="53" t="s">
         <v>435</v>
       </c>
@@ -11932,8 +12001,8 @@
       <c r="J3" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="96"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="104"/>
       <c r="M3" s="7" t="s">
         <v>435</v>
       </c>
@@ -11970,8 +12039,8 @@
       <c r="J4" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="96"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="7" t="s">
         <v>435</v>
       </c>
@@ -12006,8 +12075,8 @@
       <c r="J5" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="96"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="104"/>
       <c r="M5" s="7" t="s">
         <v>435</v>
       </c>
@@ -12044,10 +12113,10 @@
       <c r="J6" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="102" t="s">
         <v>445</v>
       </c>
-      <c r="L6" s="99"/>
+      <c r="L6" s="107"/>
       <c r="M6" s="7" t="s">
         <v>435</v>
       </c>
@@ -12084,8 +12153,8 @@
       <c r="J7" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="108"/>
       <c r="M7" s="7" t="s">
         <v>435</v>
       </c>
@@ -12120,8 +12189,8 @@
       <c r="J8" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K8" s="98"/>
-      <c r="L8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="109"/>
       <c r="M8" s="7" t="s">
         <v>435</v>
       </c>
@@ -12158,10 +12227,10 @@
       <c r="J9" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K9" s="102" t="s">
+      <c r="K9" s="110" t="s">
         <v>453</v>
       </c>
-      <c r="L9" s="104" t="s">
+      <c r="L9" s="105" t="s">
         <v>454</v>
       </c>
       <c r="M9" s="53" t="s">
@@ -12200,8 +12269,8 @@
       <c r="J10" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K10" s="103"/>
-      <c r="L10" s="96"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="104"/>
       <c r="M10" s="7" t="s">
         <v>435</v>
       </c>
@@ -12238,8 +12307,8 @@
       <c r="J11" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K11" s="103"/>
-      <c r="L11" s="96"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="104"/>
       <c r="M11" s="7" t="s">
         <v>435</v>
       </c>
@@ -12518,7 +12587,7 @@
       <c r="J18" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K18" s="97"/>
+      <c r="K18" s="102"/>
       <c r="L18" s="56"/>
       <c r="M18" s="7" t="s">
         <v>435</v>
@@ -12556,7 +12625,7 @@
       <c r="J19" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K19" s="98"/>
+      <c r="K19" s="101"/>
       <c r="L19" s="66"/>
       <c r="M19" s="58" t="s">
         <v>435</v>
@@ -12594,10 +12663,10 @@
       <c r="J20" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K20" s="97" t="s">
+      <c r="K20" s="102" t="s">
         <v>488</v>
       </c>
-      <c r="L20" s="104" t="s">
+      <c r="L20" s="105" t="s">
         <v>489</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -12636,8 +12705,8 @@
       <c r="J21" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K21" s="94"/>
-      <c r="L21" s="96"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="104"/>
       <c r="M21" s="7" t="s">
         <v>435</v>
       </c>
@@ -12672,8 +12741,8 @@
       <c r="J22" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="96"/>
+      <c r="K22" s="100"/>
+      <c r="L22" s="104"/>
       <c r="M22" s="7" t="s">
         <v>435</v>
       </c>
@@ -12710,8 +12779,8 @@
       <c r="J23" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K23" s="94"/>
-      <c r="L23" s="96"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="104"/>
       <c r="M23" s="7" t="s">
         <v>435</v>
       </c>
@@ -12748,8 +12817,8 @@
       <c r="J24" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K24" s="94"/>
-      <c r="L24" s="96"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="104"/>
       <c r="M24" s="7" t="s">
         <v>435</v>
       </c>
@@ -12786,10 +12855,10 @@
       <c r="J25" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K25" s="93" t="s">
+      <c r="K25" s="99" t="s">
         <v>495</v>
       </c>
-      <c r="L25" s="95" t="s">
+      <c r="L25" s="103" t="s">
         <v>496</v>
       </c>
       <c r="M25" s="53" t="s">
@@ -12828,8 +12897,8 @@
       <c r="J26" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K26" s="94"/>
-      <c r="L26" s="96"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="104"/>
       <c r="M26" s="7" t="s">
         <v>435</v>
       </c>
@@ -12866,8 +12935,8 @@
       <c r="J27" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K27" s="94"/>
-      <c r="L27" s="96"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="104"/>
       <c r="M27" s="7" t="s">
         <v>435</v>
       </c>
@@ -12902,8 +12971,8 @@
       <c r="J28" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K28" s="98"/>
-      <c r="L28" s="105"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="106"/>
       <c r="M28" s="58" t="s">
         <v>435</v>
       </c>
@@ -12940,7 +13009,7 @@
       <c r="J29" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K29" s="97" t="s">
+      <c r="K29" s="102" t="s">
         <v>501</v>
       </c>
       <c r="L29" s="56"/>
@@ -12980,7 +13049,7 @@
       <c r="J30" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K30" s="94"/>
+      <c r="K30" s="100"/>
       <c r="L30" s="56"/>
       <c r="M30" s="7" t="s">
         <v>435</v>
@@ -13018,7 +13087,7 @@
       <c r="J31" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K31" s="94"/>
+      <c r="K31" s="100"/>
       <c r="L31" s="56"/>
       <c r="M31" s="7" t="s">
         <v>435</v>
@@ -13054,7 +13123,7 @@
       <c r="J32" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K32" s="94"/>
+      <c r="K32" s="100"/>
       <c r="L32" s="56"/>
       <c r="M32" s="7" t="s">
         <v>435</v>
@@ -13092,7 +13161,7 @@
       <c r="J33" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K33" s="93" t="s">
+      <c r="K33" s="99" t="s">
         <v>468</v>
       </c>
       <c r="L33" s="65" t="s">
@@ -13134,7 +13203,7 @@
       <c r="J34" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K34" s="98"/>
+      <c r="K34" s="101"/>
       <c r="L34" s="66"/>
       <c r="M34" s="58" t="s">
         <v>435</v>
@@ -13172,7 +13241,7 @@
       <c r="J35" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K35" s="97" t="s">
+      <c r="K35" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L35" s="56" t="s">
@@ -13214,7 +13283,7 @@
       <c r="J36" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K36" s="94"/>
+      <c r="K36" s="100"/>
       <c r="L36" s="56"/>
       <c r="M36" s="7" t="s">
         <v>435</v>
@@ -13331,7 +13400,7 @@
       <c r="K39" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="L39" s="95"/>
+      <c r="L39" s="103"/>
       <c r="M39" s="53" t="s">
         <v>435</v>
       </c>
@@ -13369,7 +13438,7 @@
         <v>435</v>
       </c>
       <c r="K40" s="55"/>
-      <c r="L40" s="96"/>
+      <c r="L40" s="104"/>
       <c r="M40" s="7" t="s">
         <v>435</v>
       </c>
@@ -13448,10 +13517,10 @@
       <c r="J42" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K42" s="97" t="s">
+      <c r="K42" s="102" t="s">
         <v>525</v>
       </c>
-      <c r="L42" s="104" t="s">
+      <c r="L42" s="105" t="s">
         <v>526</v>
       </c>
       <c r="M42" s="53" t="s">
@@ -13490,8 +13559,8 @@
       <c r="J43" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K43" s="94"/>
-      <c r="L43" s="96"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="104"/>
       <c r="M43" s="7" t="s">
         <v>435</v>
       </c>
@@ -13528,8 +13597,8 @@
       <c r="J44" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K44" s="94"/>
-      <c r="L44" s="96"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="104"/>
       <c r="M44" s="7" t="s">
         <v>435</v>
       </c>
@@ -13564,8 +13633,8 @@
       <c r="J45" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K45" s="94"/>
-      <c r="L45" s="96"/>
+      <c r="K45" s="100"/>
+      <c r="L45" s="104"/>
       <c r="M45" s="7" t="s">
         <v>435</v>
       </c>
@@ -13602,8 +13671,8 @@
       <c r="J46" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K46" s="94"/>
-      <c r="L46" s="96"/>
+      <c r="K46" s="100"/>
+      <c r="L46" s="104"/>
       <c r="M46" s="7" t="s">
         <v>435</v>
       </c>
@@ -13640,8 +13709,8 @@
       <c r="J47" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K47" s="94"/>
-      <c r="L47" s="96"/>
+      <c r="K47" s="100"/>
+      <c r="L47" s="104"/>
       <c r="M47" s="7" t="s">
         <v>435</v>
       </c>
@@ -13758,7 +13827,7 @@
       <c r="J50" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K50" s="106" t="s">
+      <c r="K50" s="93" t="s">
         <v>539</v>
       </c>
       <c r="L50" s="65"/>
@@ -13798,7 +13867,7 @@
       <c r="J51" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K51" s="103"/>
+      <c r="K51" s="94"/>
       <c r="L51" s="56"/>
       <c r="M51" s="53" t="s">
         <v>435</v>
@@ -13836,7 +13905,7 @@
       <c r="J52" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K52" s="103"/>
+      <c r="K52" s="94"/>
       <c r="L52" s="56"/>
       <c r="M52" s="53" t="s">
         <v>435</v>
@@ -13874,7 +13943,7 @@
       <c r="J53" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K53" s="103"/>
+      <c r="K53" s="94"/>
       <c r="L53" s="56"/>
       <c r="M53" s="53" t="s">
         <v>435</v>
@@ -13910,7 +13979,7 @@
       <c r="J54" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K54" s="107"/>
+      <c r="K54" s="95"/>
       <c r="L54" s="66"/>
       <c r="M54" s="53" t="s">
         <v>435</v>
@@ -14030,7 +14099,7 @@
       <c r="J57" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K57" s="97" t="s">
+      <c r="K57" s="102" t="s">
         <v>556</v>
       </c>
       <c r="L57" s="56"/>
@@ -14070,7 +14139,7 @@
       <c r="J58" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K58" s="94"/>
+      <c r="K58" s="100"/>
       <c r="L58" s="56"/>
       <c r="M58" s="7" t="s">
         <v>435</v>
@@ -14106,7 +14175,7 @@
       <c r="J59" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K59" s="94"/>
+      <c r="K59" s="100"/>
       <c r="L59" s="56"/>
       <c r="M59" s="7" t="s">
         <v>435</v>
@@ -14144,7 +14213,7 @@
       <c r="J60" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="K60" s="95" t="s">
+      <c r="K60" s="103" t="s">
         <v>561</v>
       </c>
       <c r="L60" s="65"/>
@@ -14184,7 +14253,7 @@
       <c r="J61" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K61" s="96"/>
+      <c r="K61" s="104"/>
       <c r="L61" s="56" t="s">
         <v>563</v>
       </c>
@@ -14224,7 +14293,7 @@
       <c r="J62" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K62" s="96"/>
+      <c r="K62" s="104"/>
       <c r="L62" s="56" t="s">
         <v>565</v>
       </c>
@@ -14264,7 +14333,7 @@
       <c r="J63" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K63" s="97"/>
+      <c r="K63" s="102"/>
       <c r="L63" s="56"/>
       <c r="M63" s="7" t="s">
         <v>435</v>
@@ -14302,7 +14371,7 @@
       <c r="J64" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K64" s="94"/>
+      <c r="K64" s="100"/>
       <c r="L64" s="56"/>
       <c r="M64" s="7" t="s">
         <v>435</v>
@@ -14340,7 +14409,7 @@
       <c r="J65" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K65" s="94"/>
+      <c r="K65" s="100"/>
       <c r="L65" s="56" t="s">
         <v>565</v>
       </c>
@@ -14378,7 +14447,7 @@
       <c r="J66" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K66" s="94"/>
+      <c r="K66" s="100"/>
       <c r="L66" s="12"/>
       <c r="M66" s="54" t="s">
         <v>435</v>
@@ -14492,7 +14561,7 @@
       <c r="J69" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K69" s="97" t="s">
+      <c r="K69" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L69" s="56" t="s">
@@ -14534,7 +14603,7 @@
       <c r="J70" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K70" s="94"/>
+      <c r="K70" s="100"/>
       <c r="L70" s="56"/>
       <c r="M70" s="7" t="s">
         <v>435</v>
@@ -14612,7 +14681,7 @@
       <c r="J72" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K72" s="97"/>
+      <c r="K72" s="102"/>
       <c r="L72" s="56"/>
       <c r="M72" s="7" t="s">
         <v>435</v>
@@ -14648,7 +14717,7 @@
       <c r="J73" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K73" s="94"/>
+      <c r="K73" s="100"/>
       <c r="L73" s="56"/>
       <c r="M73" s="7" t="s">
         <v>435</v>
@@ -14684,7 +14753,7 @@
       <c r="J74" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K74" s="94"/>
+      <c r="K74" s="100"/>
       <c r="L74" s="56"/>
       <c r="M74" s="7" t="s">
         <v>435</v>
@@ -14718,7 +14787,7 @@
       <c r="J75" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K75" s="98"/>
+      <c r="K75" s="101"/>
       <c r="L75" s="66"/>
       <c r="M75" s="7" t="s">
         <v>435</v>
@@ -14796,10 +14865,10 @@
       <c r="J77" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K77" s="106" t="s">
+      <c r="K77" s="93" t="s">
         <v>588</v>
       </c>
-      <c r="L77" s="93" t="s">
+      <c r="L77" s="99" t="s">
         <v>589</v>
       </c>
       <c r="M77" s="53" t="s">
@@ -14840,8 +14909,8 @@
       <c r="J78" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K78" s="107"/>
-      <c r="L78" s="109"/>
+      <c r="K78" s="95"/>
+      <c r="L78" s="97"/>
       <c r="M78" s="54" t="s">
         <v>435</v>
       </c>
@@ -14881,7 +14950,7 @@
       <c r="K79" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L79" s="109"/>
+      <c r="L79" s="97"/>
       <c r="M79" s="54" t="s">
         <v>435</v>
       </c>
@@ -14921,7 +14990,7 @@
       <c r="K80" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L80" s="98"/>
+      <c r="L80" s="101"/>
       <c r="M80" s="7" t="s">
         <v>435</v>
       </c>
@@ -14958,7 +15027,7 @@
       <c r="J81" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K81" s="97" t="s">
+      <c r="K81" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L81" s="56" t="s">
@@ -15000,7 +15069,7 @@
       <c r="J82" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K82" s="94"/>
+      <c r="K82" s="100"/>
       <c r="L82" s="56"/>
       <c r="M82" s="7" t="s">
         <v>435</v>
@@ -15122,7 +15191,7 @@
       <c r="J85" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K85" s="97" t="s">
+      <c r="K85" s="102" t="s">
         <v>602</v>
       </c>
       <c r="L85" s="56"/>
@@ -15162,7 +15231,7 @@
       <c r="J86" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K86" s="94"/>
+      <c r="K86" s="100"/>
       <c r="L86" s="56"/>
       <c r="M86" s="7" t="s">
         <v>435</v>
@@ -15200,7 +15269,7 @@
       <c r="J87" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K87" s="94"/>
+      <c r="K87" s="100"/>
       <c r="L87" s="56"/>
       <c r="M87" s="7" t="s">
         <v>435</v>
@@ -15236,7 +15305,7 @@
       <c r="J88" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K88" s="94"/>
+      <c r="K88" s="100"/>
       <c r="L88" s="56"/>
       <c r="M88" s="7" t="s">
         <v>435</v>
@@ -15274,7 +15343,7 @@
       <c r="J89" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K89" s="94"/>
+      <c r="K89" s="100"/>
       <c r="L89" s="56"/>
       <c r="M89" s="7" t="s">
         <v>435</v>
@@ -15312,7 +15381,7 @@
       <c r="J90" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K90" s="94"/>
+      <c r="K90" s="100"/>
       <c r="L90" s="56"/>
       <c r="M90" s="7" t="s">
         <v>435</v>
@@ -15350,10 +15419,10 @@
       <c r="J91" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K91" s="106" t="s">
+      <c r="K91" s="93" t="s">
         <v>608</v>
       </c>
-      <c r="L91" s="108" t="s">
+      <c r="L91" s="96" t="s">
         <v>609</v>
       </c>
       <c r="M91" s="53" t="s">
@@ -15392,8 +15461,8 @@
       <c r="J92" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K92" s="103"/>
-      <c r="L92" s="109"/>
+      <c r="K92" s="94"/>
+      <c r="L92" s="97"/>
       <c r="M92" s="7" t="s">
         <v>435</v>
       </c>
@@ -15430,8 +15499,8 @@
       <c r="J93" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K93" s="103"/>
-      <c r="L93" s="109"/>
+      <c r="K93" s="94"/>
+      <c r="L93" s="97"/>
       <c r="M93" s="7" t="s">
         <v>435</v>
       </c>
@@ -15466,8 +15535,8 @@
       <c r="J94" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K94" s="107"/>
-      <c r="L94" s="110"/>
+      <c r="K94" s="95"/>
+      <c r="L94" s="98"/>
       <c r="M94" s="7" t="s">
         <v>435</v>
       </c>
@@ -15504,7 +15573,7 @@
       <c r="J95" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K95" s="93"/>
+      <c r="K95" s="99"/>
       <c r="L95" s="56"/>
       <c r="M95" s="53" t="s">
         <v>435</v>
@@ -15542,7 +15611,7 @@
       <c r="J96" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K96" s="94"/>
+      <c r="K96" s="100"/>
       <c r="L96" s="56"/>
       <c r="M96" s="53" t="s">
         <v>435</v>
@@ -15580,7 +15649,7 @@
       <c r="J97" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K97" s="94"/>
+      <c r="K97" s="100"/>
       <c r="L97" s="56"/>
       <c r="M97" s="53" t="s">
         <v>435</v>
@@ -15618,7 +15687,7 @@
       <c r="J98" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K98" s="94"/>
+      <c r="K98" s="100"/>
       <c r="L98" s="56"/>
       <c r="M98" s="53" t="s">
         <v>435</v>
@@ -15654,7 +15723,7 @@
       <c r="J99" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K99" s="98"/>
+      <c r="K99" s="101"/>
       <c r="L99" s="60"/>
       <c r="M99" s="61" t="s">
         <v>435</v>
@@ -15683,6 +15752,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15691,28 +15782,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17389,7 +17458,7 @@
   </sheetPr>
   <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -20072,7 +20141,9 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20410,12 +20481,18 @@
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>797</v>
+      </c>
       <c r="C25" s="31">
         <v>1</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>798</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusting conversions to accomaadate noaa ctd
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D38B74-D02D-4FBA-AA47-AED37ABDE78C}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4473F49-FC0D-4010-B9AC-37141FCC559C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -3078,35 +3078,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3114,10 +3090,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3131,6 +3107,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11625,7 +11625,7 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -11963,8 +11963,8 @@
       <c r="J2" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K2" s="99"/>
-      <c r="L2" s="103"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="95"/>
       <c r="M2" s="53" t="s">
         <v>435</v>
       </c>
@@ -12001,8 +12001,8 @@
       <c r="J3" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K3" s="100"/>
-      <c r="L3" s="104"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="96"/>
       <c r="M3" s="7" t="s">
         <v>435</v>
       </c>
@@ -12039,8 +12039,8 @@
       <c r="J4" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K4" s="100"/>
-      <c r="L4" s="104"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="96"/>
       <c r="M4" s="7" t="s">
         <v>435</v>
       </c>
@@ -12075,8 +12075,8 @@
       <c r="J5" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K5" s="100"/>
-      <c r="L5" s="104"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="96"/>
       <c r="M5" s="7" t="s">
         <v>435</v>
       </c>
@@ -12113,10 +12113,10 @@
       <c r="J6" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K6" s="102" t="s">
+      <c r="K6" s="97" t="s">
         <v>445</v>
       </c>
-      <c r="L6" s="107"/>
+      <c r="L6" s="99"/>
       <c r="M6" s="7" t="s">
         <v>435</v>
       </c>
@@ -12153,8 +12153,8 @@
       <c r="J7" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K7" s="100"/>
-      <c r="L7" s="108"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="100"/>
       <c r="M7" s="7" t="s">
         <v>435</v>
       </c>
@@ -12189,8 +12189,8 @@
       <c r="J8" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K8" s="101"/>
-      <c r="L8" s="109"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="101"/>
       <c r="M8" s="7" t="s">
         <v>435</v>
       </c>
@@ -12227,10 +12227,10 @@
       <c r="J9" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K9" s="110" t="s">
+      <c r="K9" s="102" t="s">
         <v>453</v>
       </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="104" t="s">
         <v>454</v>
       </c>
       <c r="M9" s="53" t="s">
@@ -12269,8 +12269,8 @@
       <c r="J10" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K10" s="94"/>
-      <c r="L10" s="104"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="96"/>
       <c r="M10" s="7" t="s">
         <v>435</v>
       </c>
@@ -12307,8 +12307,8 @@
       <c r="J11" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="104"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="96"/>
       <c r="M11" s="7" t="s">
         <v>435</v>
       </c>
@@ -12587,7 +12587,7 @@
       <c r="J18" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K18" s="102"/>
+      <c r="K18" s="97"/>
       <c r="L18" s="56"/>
       <c r="M18" s="7" t="s">
         <v>435</v>
@@ -12625,7 +12625,7 @@
       <c r="J19" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K19" s="101"/>
+      <c r="K19" s="98"/>
       <c r="L19" s="66"/>
       <c r="M19" s="58" t="s">
         <v>435</v>
@@ -12663,10 +12663,10 @@
       <c r="J20" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K20" s="102" t="s">
+      <c r="K20" s="97" t="s">
         <v>488</v>
       </c>
-      <c r="L20" s="105" t="s">
+      <c r="L20" s="104" t="s">
         <v>489</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -12705,8 +12705,8 @@
       <c r="J21" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K21" s="100"/>
-      <c r="L21" s="104"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="96"/>
       <c r="M21" s="7" t="s">
         <v>435</v>
       </c>
@@ -12741,8 +12741,8 @@
       <c r="J22" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K22" s="100"/>
-      <c r="L22" s="104"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="96"/>
       <c r="M22" s="7" t="s">
         <v>435</v>
       </c>
@@ -12779,8 +12779,8 @@
       <c r="J23" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K23" s="100"/>
-      <c r="L23" s="104"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="96"/>
       <c r="M23" s="7" t="s">
         <v>435</v>
       </c>
@@ -12817,8 +12817,8 @@
       <c r="J24" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K24" s="100"/>
-      <c r="L24" s="104"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="96"/>
       <c r="M24" s="7" t="s">
         <v>435</v>
       </c>
@@ -12855,10 +12855,10 @@
       <c r="J25" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K25" s="99" t="s">
+      <c r="K25" s="93" t="s">
         <v>495</v>
       </c>
-      <c r="L25" s="103" t="s">
+      <c r="L25" s="95" t="s">
         <v>496</v>
       </c>
       <c r="M25" s="53" t="s">
@@ -12897,8 +12897,8 @@
       <c r="J26" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K26" s="100"/>
-      <c r="L26" s="104"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="96"/>
       <c r="M26" s="7" t="s">
         <v>435</v>
       </c>
@@ -12935,8 +12935,8 @@
       <c r="J27" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K27" s="100"/>
-      <c r="L27" s="104"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="96"/>
       <c r="M27" s="7" t="s">
         <v>435</v>
       </c>
@@ -12971,8 +12971,8 @@
       <c r="J28" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K28" s="101"/>
-      <c r="L28" s="106"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="105"/>
       <c r="M28" s="58" t="s">
         <v>435</v>
       </c>
@@ -13009,7 +13009,7 @@
       <c r="J29" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K29" s="102" t="s">
+      <c r="K29" s="97" t="s">
         <v>501</v>
       </c>
       <c r="L29" s="56"/>
@@ -13049,7 +13049,7 @@
       <c r="J30" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K30" s="100"/>
+      <c r="K30" s="94"/>
       <c r="L30" s="56"/>
       <c r="M30" s="7" t="s">
         <v>435</v>
@@ -13087,7 +13087,7 @@
       <c r="J31" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K31" s="100"/>
+      <c r="K31" s="94"/>
       <c r="L31" s="56"/>
       <c r="M31" s="7" t="s">
         <v>435</v>
@@ -13123,7 +13123,7 @@
       <c r="J32" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K32" s="100"/>
+      <c r="K32" s="94"/>
       <c r="L32" s="56"/>
       <c r="M32" s="7" t="s">
         <v>435</v>
@@ -13161,7 +13161,7 @@
       <c r="J33" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K33" s="99" t="s">
+      <c r="K33" s="93" t="s">
         <v>468</v>
       </c>
       <c r="L33" s="65" t="s">
@@ -13203,7 +13203,7 @@
       <c r="J34" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K34" s="101"/>
+      <c r="K34" s="98"/>
       <c r="L34" s="66"/>
       <c r="M34" s="58" t="s">
         <v>435</v>
@@ -13241,7 +13241,7 @@
       <c r="J35" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K35" s="102" t="s">
+      <c r="K35" s="97" t="s">
         <v>468</v>
       </c>
       <c r="L35" s="56" t="s">
@@ -13283,7 +13283,7 @@
       <c r="J36" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K36" s="100"/>
+      <c r="K36" s="94"/>
       <c r="L36" s="56"/>
       <c r="M36" s="7" t="s">
         <v>435</v>
@@ -13400,7 +13400,7 @@
       <c r="K39" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="L39" s="103"/>
+      <c r="L39" s="95"/>
       <c r="M39" s="53" t="s">
         <v>435</v>
       </c>
@@ -13438,7 +13438,7 @@
         <v>435</v>
       </c>
       <c r="K40" s="55"/>
-      <c r="L40" s="104"/>
+      <c r="L40" s="96"/>
       <c r="M40" s="7" t="s">
         <v>435</v>
       </c>
@@ -13517,10 +13517,10 @@
       <c r="J42" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K42" s="102" t="s">
+      <c r="K42" s="97" t="s">
         <v>525</v>
       </c>
-      <c r="L42" s="105" t="s">
+      <c r="L42" s="104" t="s">
         <v>526</v>
       </c>
       <c r="M42" s="53" t="s">
@@ -13559,8 +13559,8 @@
       <c r="J43" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K43" s="100"/>
-      <c r="L43" s="104"/>
+      <c r="K43" s="94"/>
+      <c r="L43" s="96"/>
       <c r="M43" s="7" t="s">
         <v>435</v>
       </c>
@@ -13597,8 +13597,8 @@
       <c r="J44" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K44" s="100"/>
-      <c r="L44" s="104"/>
+      <c r="K44" s="94"/>
+      <c r="L44" s="96"/>
       <c r="M44" s="7" t="s">
         <v>435</v>
       </c>
@@ -13633,8 +13633,8 @@
       <c r="J45" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K45" s="100"/>
-      <c r="L45" s="104"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="96"/>
       <c r="M45" s="7" t="s">
         <v>435</v>
       </c>
@@ -13671,8 +13671,8 @@
       <c r="J46" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K46" s="100"/>
-      <c r="L46" s="104"/>
+      <c r="K46" s="94"/>
+      <c r="L46" s="96"/>
       <c r="M46" s="7" t="s">
         <v>435</v>
       </c>
@@ -13709,8 +13709,8 @@
       <c r="J47" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K47" s="100"/>
-      <c r="L47" s="104"/>
+      <c r="K47" s="94"/>
+      <c r="L47" s="96"/>
       <c r="M47" s="7" t="s">
         <v>435</v>
       </c>
@@ -13827,7 +13827,7 @@
       <c r="J50" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K50" s="93" t="s">
+      <c r="K50" s="106" t="s">
         <v>539</v>
       </c>
       <c r="L50" s="65"/>
@@ -13867,7 +13867,7 @@
       <c r="J51" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K51" s="94"/>
+      <c r="K51" s="103"/>
       <c r="L51" s="56"/>
       <c r="M51" s="53" t="s">
         <v>435</v>
@@ -13905,7 +13905,7 @@
       <c r="J52" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K52" s="94"/>
+      <c r="K52" s="103"/>
       <c r="L52" s="56"/>
       <c r="M52" s="53" t="s">
         <v>435</v>
@@ -13943,7 +13943,7 @@
       <c r="J53" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K53" s="94"/>
+      <c r="K53" s="103"/>
       <c r="L53" s="56"/>
       <c r="M53" s="53" t="s">
         <v>435</v>
@@ -13979,7 +13979,7 @@
       <c r="J54" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K54" s="95"/>
+      <c r="K54" s="107"/>
       <c r="L54" s="66"/>
       <c r="M54" s="53" t="s">
         <v>435</v>
@@ -14099,7 +14099,7 @@
       <c r="J57" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K57" s="102" t="s">
+      <c r="K57" s="97" t="s">
         <v>556</v>
       </c>
       <c r="L57" s="56"/>
@@ -14139,7 +14139,7 @@
       <c r="J58" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K58" s="100"/>
+      <c r="K58" s="94"/>
       <c r="L58" s="56"/>
       <c r="M58" s="7" t="s">
         <v>435</v>
@@ -14175,7 +14175,7 @@
       <c r="J59" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K59" s="100"/>
+      <c r="K59" s="94"/>
       <c r="L59" s="56"/>
       <c r="M59" s="7" t="s">
         <v>435</v>
@@ -14213,7 +14213,7 @@
       <c r="J60" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="K60" s="103" t="s">
+      <c r="K60" s="95" t="s">
         <v>561</v>
       </c>
       <c r="L60" s="65"/>
@@ -14253,7 +14253,7 @@
       <c r="J61" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K61" s="104"/>
+      <c r="K61" s="96"/>
       <c r="L61" s="56" t="s">
         <v>563</v>
       </c>
@@ -14293,7 +14293,7 @@
       <c r="J62" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K62" s="104"/>
+      <c r="K62" s="96"/>
       <c r="L62" s="56" t="s">
         <v>565</v>
       </c>
@@ -14333,7 +14333,7 @@
       <c r="J63" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K63" s="102"/>
+      <c r="K63" s="97"/>
       <c r="L63" s="56"/>
       <c r="M63" s="7" t="s">
         <v>435</v>
@@ -14371,7 +14371,7 @@
       <c r="J64" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K64" s="100"/>
+      <c r="K64" s="94"/>
       <c r="L64" s="56"/>
       <c r="M64" s="7" t="s">
         <v>435</v>
@@ -14409,7 +14409,7 @@
       <c r="J65" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K65" s="100"/>
+      <c r="K65" s="94"/>
       <c r="L65" s="56" t="s">
         <v>565</v>
       </c>
@@ -14447,7 +14447,7 @@
       <c r="J66" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K66" s="100"/>
+      <c r="K66" s="94"/>
       <c r="L66" s="12"/>
       <c r="M66" s="54" t="s">
         <v>435</v>
@@ -14561,7 +14561,7 @@
       <c r="J69" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K69" s="102" t="s">
+      <c r="K69" s="97" t="s">
         <v>468</v>
       </c>
       <c r="L69" s="56" t="s">
@@ -14603,7 +14603,7 @@
       <c r="J70" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K70" s="100"/>
+      <c r="K70" s="94"/>
       <c r="L70" s="56"/>
       <c r="M70" s="7" t="s">
         <v>435</v>
@@ -14681,7 +14681,7 @@
       <c r="J72" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K72" s="102"/>
+      <c r="K72" s="97"/>
       <c r="L72" s="56"/>
       <c r="M72" s="7" t="s">
         <v>435</v>
@@ -14717,7 +14717,7 @@
       <c r="J73" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K73" s="100"/>
+      <c r="K73" s="94"/>
       <c r="L73" s="56"/>
       <c r="M73" s="7" t="s">
         <v>435</v>
@@ -14753,7 +14753,7 @@
       <c r="J74" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K74" s="100"/>
+      <c r="K74" s="94"/>
       <c r="L74" s="56"/>
       <c r="M74" s="7" t="s">
         <v>435</v>
@@ -14787,7 +14787,7 @@
       <c r="J75" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K75" s="101"/>
+      <c r="K75" s="98"/>
       <c r="L75" s="66"/>
       <c r="M75" s="7" t="s">
         <v>435</v>
@@ -14865,10 +14865,10 @@
       <c r="J77" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K77" s="93" t="s">
+      <c r="K77" s="106" t="s">
         <v>588</v>
       </c>
-      <c r="L77" s="99" t="s">
+      <c r="L77" s="93" t="s">
         <v>589</v>
       </c>
       <c r="M77" s="53" t="s">
@@ -14909,8 +14909,8 @@
       <c r="J78" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K78" s="95"/>
-      <c r="L78" s="97"/>
+      <c r="K78" s="107"/>
+      <c r="L78" s="109"/>
       <c r="M78" s="54" t="s">
         <v>435</v>
       </c>
@@ -14950,7 +14950,7 @@
       <c r="K79" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L79" s="97"/>
+      <c r="L79" s="109"/>
       <c r="M79" s="54" t="s">
         <v>435</v>
       </c>
@@ -14990,7 +14990,7 @@
       <c r="K80" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L80" s="101"/>
+      <c r="L80" s="98"/>
       <c r="M80" s="7" t="s">
         <v>435</v>
       </c>
@@ -15027,7 +15027,7 @@
       <c r="J81" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K81" s="102" t="s">
+      <c r="K81" s="97" t="s">
         <v>468</v>
       </c>
       <c r="L81" s="56" t="s">
@@ -15069,7 +15069,7 @@
       <c r="J82" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K82" s="100"/>
+      <c r="K82" s="94"/>
       <c r="L82" s="56"/>
       <c r="M82" s="7" t="s">
         <v>435</v>
@@ -15191,7 +15191,7 @@
       <c r="J85" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K85" s="102" t="s">
+      <c r="K85" s="97" t="s">
         <v>602</v>
       </c>
       <c r="L85" s="56"/>
@@ -15231,7 +15231,7 @@
       <c r="J86" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K86" s="100"/>
+      <c r="K86" s="94"/>
       <c r="L86" s="56"/>
       <c r="M86" s="7" t="s">
         <v>435</v>
@@ -15269,7 +15269,7 @@
       <c r="J87" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K87" s="100"/>
+      <c r="K87" s="94"/>
       <c r="L87" s="56"/>
       <c r="M87" s="7" t="s">
         <v>435</v>
@@ -15305,7 +15305,7 @@
       <c r="J88" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K88" s="100"/>
+      <c r="K88" s="94"/>
       <c r="L88" s="56"/>
       <c r="M88" s="7" t="s">
         <v>435</v>
@@ -15343,7 +15343,7 @@
       <c r="J89" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K89" s="100"/>
+      <c r="K89" s="94"/>
       <c r="L89" s="56"/>
       <c r="M89" s="7" t="s">
         <v>435</v>
@@ -15381,7 +15381,7 @@
       <c r="J90" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K90" s="100"/>
+      <c r="K90" s="94"/>
       <c r="L90" s="56"/>
       <c r="M90" s="7" t="s">
         <v>435</v>
@@ -15419,10 +15419,10 @@
       <c r="J91" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K91" s="93" t="s">
+      <c r="K91" s="106" t="s">
         <v>608</v>
       </c>
-      <c r="L91" s="96" t="s">
+      <c r="L91" s="108" t="s">
         <v>609</v>
       </c>
       <c r="M91" s="53" t="s">
@@ -15461,8 +15461,8 @@
       <c r="J92" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K92" s="94"/>
-      <c r="L92" s="97"/>
+      <c r="K92" s="103"/>
+      <c r="L92" s="109"/>
       <c r="M92" s="7" t="s">
         <v>435</v>
       </c>
@@ -15499,8 +15499,8 @@
       <c r="J93" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K93" s="94"/>
-      <c r="L93" s="97"/>
+      <c r="K93" s="103"/>
+      <c r="L93" s="109"/>
       <c r="M93" s="7" t="s">
         <v>435</v>
       </c>
@@ -15535,8 +15535,8 @@
       <c r="J94" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K94" s="95"/>
-      <c r="L94" s="98"/>
+      <c r="K94" s="107"/>
+      <c r="L94" s="110"/>
       <c r="M94" s="7" t="s">
         <v>435</v>
       </c>
@@ -15573,7 +15573,7 @@
       <c r="J95" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K95" s="99"/>
+      <c r="K95" s="93"/>
       <c r="L95" s="56"/>
       <c r="M95" s="53" t="s">
         <v>435</v>
@@ -15611,7 +15611,7 @@
       <c r="J96" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K96" s="100"/>
+      <c r="K96" s="94"/>
       <c r="L96" s="56"/>
       <c r="M96" s="53" t="s">
         <v>435</v>
@@ -15649,7 +15649,7 @@
       <c r="J97" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K97" s="100"/>
+      <c r="K97" s="94"/>
       <c r="L97" s="56"/>
       <c r="M97" s="53" t="s">
         <v>435</v>
@@ -15687,7 +15687,7 @@
       <c r="J98" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K98" s="100"/>
+      <c r="K98" s="94"/>
       <c r="L98" s="56"/>
       <c r="M98" s="53" t="s">
         <v>435</v>
@@ -15723,7 +15723,7 @@
       <c r="J99" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K99" s="101"/>
+      <c r="K99" s="98"/>
       <c r="L99" s="60"/>
       <c r="M99" s="61" t="s">
         <v>435</v>
@@ -15752,28 +15752,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15782,6 +15760,28 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20141,8 +20141,8 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added specific conductivity to noaa ctd mapping file
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4473F49-FC0D-4010-B9AC-37141FCC559C}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_44682621B0D26BC066C8CAD00103F6CB7E289151" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A0CE1A8-8B38-4A10-8E97-372367BACC28}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="799">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2460,9 +2460,6 @@
   </si>
   <si>
     <t>Guessing this was mislabeled for noaa ctd DO</t>
-  </si>
-  <si>
-    <t>oce remves this need to figure outu why…</t>
   </si>
 </sst>
 </file>
@@ -3078,11 +3075,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3090,10 +3111,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3107,30 +3128,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3439,8 +3436,8 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11625,8 +11622,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11827,10 +11824,13 @@
         <v>796</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>363</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>799</v>
+        <v>364</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -11841,7 +11841,7 @@
         <v>364</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>198</v>
+        <v>797</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>223</v>
@@ -11852,13 +11852,10 @@
         <v>796</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>797</v>
+        <v>365</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>223</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -11873,7 +11870,9 @@
   </sheetPr>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11963,8 +11962,8 @@
       <c r="J2" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K2" s="93"/>
-      <c r="L2" s="95"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="103"/>
       <c r="M2" s="53" t="s">
         <v>435</v>
       </c>
@@ -12001,8 +12000,8 @@
       <c r="J3" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K3" s="94"/>
-      <c r="L3" s="96"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="104"/>
       <c r="M3" s="7" t="s">
         <v>435</v>
       </c>
@@ -12039,8 +12038,8 @@
       <c r="J4" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="96"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="7" t="s">
         <v>435</v>
       </c>
@@ -12075,8 +12074,8 @@
       <c r="J5" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="96"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="104"/>
       <c r="M5" s="7" t="s">
         <v>435</v>
       </c>
@@ -12113,10 +12112,10 @@
       <c r="J6" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="102" t="s">
         <v>445</v>
       </c>
-      <c r="L6" s="99"/>
+      <c r="L6" s="107"/>
       <c r="M6" s="7" t="s">
         <v>435</v>
       </c>
@@ -12153,8 +12152,8 @@
       <c r="J7" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="108"/>
       <c r="M7" s="7" t="s">
         <v>435</v>
       </c>
@@ -12189,8 +12188,8 @@
       <c r="J8" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K8" s="98"/>
-      <c r="L8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="109"/>
       <c r="M8" s="7" t="s">
         <v>435</v>
       </c>
@@ -12227,10 +12226,10 @@
       <c r="J9" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K9" s="102" t="s">
+      <c r="K9" s="110" t="s">
         <v>453</v>
       </c>
-      <c r="L9" s="104" t="s">
+      <c r="L9" s="105" t="s">
         <v>454</v>
       </c>
       <c r="M9" s="53" t="s">
@@ -12269,8 +12268,8 @@
       <c r="J10" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K10" s="103"/>
-      <c r="L10" s="96"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="104"/>
       <c r="M10" s="7" t="s">
         <v>435</v>
       </c>
@@ -12307,8 +12306,8 @@
       <c r="J11" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K11" s="103"/>
-      <c r="L11" s="96"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="104"/>
       <c r="M11" s="7" t="s">
         <v>435</v>
       </c>
@@ -12587,7 +12586,7 @@
       <c r="J18" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K18" s="97"/>
+      <c r="K18" s="102"/>
       <c r="L18" s="56"/>
       <c r="M18" s="7" t="s">
         <v>435</v>
@@ -12625,7 +12624,7 @@
       <c r="J19" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K19" s="98"/>
+      <c r="K19" s="101"/>
       <c r="L19" s="66"/>
       <c r="M19" s="58" t="s">
         <v>435</v>
@@ -12663,10 +12662,10 @@
       <c r="J20" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K20" s="97" t="s">
+      <c r="K20" s="102" t="s">
         <v>488</v>
       </c>
-      <c r="L20" s="104" t="s">
+      <c r="L20" s="105" t="s">
         <v>489</v>
       </c>
       <c r="M20" s="7" t="s">
@@ -12705,8 +12704,8 @@
       <c r="J21" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K21" s="94"/>
-      <c r="L21" s="96"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="104"/>
       <c r="M21" s="7" t="s">
         <v>435</v>
       </c>
@@ -12741,8 +12740,8 @@
       <c r="J22" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K22" s="94"/>
-      <c r="L22" s="96"/>
+      <c r="K22" s="100"/>
+      <c r="L22" s="104"/>
       <c r="M22" s="7" t="s">
         <v>435</v>
       </c>
@@ -12779,8 +12778,8 @@
       <c r="J23" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K23" s="94"/>
-      <c r="L23" s="96"/>
+      <c r="K23" s="100"/>
+      <c r="L23" s="104"/>
       <c r="M23" s="7" t="s">
         <v>435</v>
       </c>
@@ -12817,8 +12816,8 @@
       <c r="J24" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K24" s="94"/>
-      <c r="L24" s="96"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="104"/>
       <c r="M24" s="7" t="s">
         <v>435</v>
       </c>
@@ -12855,10 +12854,10 @@
       <c r="J25" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K25" s="93" t="s">
+      <c r="K25" s="99" t="s">
         <v>495</v>
       </c>
-      <c r="L25" s="95" t="s">
+      <c r="L25" s="103" t="s">
         <v>496</v>
       </c>
       <c r="M25" s="53" t="s">
@@ -12897,8 +12896,8 @@
       <c r="J26" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K26" s="94"/>
-      <c r="L26" s="96"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="104"/>
       <c r="M26" s="7" t="s">
         <v>435</v>
       </c>
@@ -12935,8 +12934,8 @@
       <c r="J27" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K27" s="94"/>
-      <c r="L27" s="96"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="104"/>
       <c r="M27" s="7" t="s">
         <v>435</v>
       </c>
@@ -12971,8 +12970,8 @@
       <c r="J28" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K28" s="98"/>
-      <c r="L28" s="105"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="106"/>
       <c r="M28" s="58" t="s">
         <v>435</v>
       </c>
@@ -13009,7 +13008,7 @@
       <c r="J29" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K29" s="97" t="s">
+      <c r="K29" s="102" t="s">
         <v>501</v>
       </c>
       <c r="L29" s="56"/>
@@ -13049,7 +13048,7 @@
       <c r="J30" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K30" s="94"/>
+      <c r="K30" s="100"/>
       <c r="L30" s="56"/>
       <c r="M30" s="7" t="s">
         <v>435</v>
@@ -13087,7 +13086,7 @@
       <c r="J31" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K31" s="94"/>
+      <c r="K31" s="100"/>
       <c r="L31" s="56"/>
       <c r="M31" s="7" t="s">
         <v>435</v>
@@ -13123,7 +13122,7 @@
       <c r="J32" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K32" s="94"/>
+      <c r="K32" s="100"/>
       <c r="L32" s="56"/>
       <c r="M32" s="7" t="s">
         <v>435</v>
@@ -13161,7 +13160,7 @@
       <c r="J33" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K33" s="93" t="s">
+      <c r="K33" s="99" t="s">
         <v>468</v>
       </c>
       <c r="L33" s="65" t="s">
@@ -13203,7 +13202,7 @@
       <c r="J34" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K34" s="98"/>
+      <c r="K34" s="101"/>
       <c r="L34" s="66"/>
       <c r="M34" s="58" t="s">
         <v>435</v>
@@ -13241,7 +13240,7 @@
       <c r="J35" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K35" s="97" t="s">
+      <c r="K35" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L35" s="56" t="s">
@@ -13283,7 +13282,7 @@
       <c r="J36" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K36" s="94"/>
+      <c r="K36" s="100"/>
       <c r="L36" s="56"/>
       <c r="M36" s="7" t="s">
         <v>435</v>
@@ -13400,7 +13399,7 @@
       <c r="K39" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="L39" s="95"/>
+      <c r="L39" s="103"/>
       <c r="M39" s="53" t="s">
         <v>435</v>
       </c>
@@ -13438,7 +13437,7 @@
         <v>435</v>
       </c>
       <c r="K40" s="55"/>
-      <c r="L40" s="96"/>
+      <c r="L40" s="104"/>
       <c r="M40" s="7" t="s">
         <v>435</v>
       </c>
@@ -13517,10 +13516,10 @@
       <c r="J42" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K42" s="97" t="s">
+      <c r="K42" s="102" t="s">
         <v>525</v>
       </c>
-      <c r="L42" s="104" t="s">
+      <c r="L42" s="105" t="s">
         <v>526</v>
       </c>
       <c r="M42" s="53" t="s">
@@ -13559,8 +13558,8 @@
       <c r="J43" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K43" s="94"/>
-      <c r="L43" s="96"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="104"/>
       <c r="M43" s="7" t="s">
         <v>435</v>
       </c>
@@ -13597,8 +13596,8 @@
       <c r="J44" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K44" s="94"/>
-      <c r="L44" s="96"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="104"/>
       <c r="M44" s="7" t="s">
         <v>435</v>
       </c>
@@ -13633,8 +13632,8 @@
       <c r="J45" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K45" s="94"/>
-      <c r="L45" s="96"/>
+      <c r="K45" s="100"/>
+      <c r="L45" s="104"/>
       <c r="M45" s="7" t="s">
         <v>435</v>
       </c>
@@ -13671,8 +13670,8 @@
       <c r="J46" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K46" s="94"/>
-      <c r="L46" s="96"/>
+      <c r="K46" s="100"/>
+      <c r="L46" s="104"/>
       <c r="M46" s="7" t="s">
         <v>435</v>
       </c>
@@ -13709,8 +13708,8 @@
       <c r="J47" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K47" s="94"/>
-      <c r="L47" s="96"/>
+      <c r="K47" s="100"/>
+      <c r="L47" s="104"/>
       <c r="M47" s="7" t="s">
         <v>435</v>
       </c>
@@ -13827,7 +13826,7 @@
       <c r="J50" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K50" s="106" t="s">
+      <c r="K50" s="93" t="s">
         <v>539</v>
       </c>
       <c r="L50" s="65"/>
@@ -13867,7 +13866,7 @@
       <c r="J51" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K51" s="103"/>
+      <c r="K51" s="94"/>
       <c r="L51" s="56"/>
       <c r="M51" s="53" t="s">
         <v>435</v>
@@ -13905,7 +13904,7 @@
       <c r="J52" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K52" s="103"/>
+      <c r="K52" s="94"/>
       <c r="L52" s="56"/>
       <c r="M52" s="53" t="s">
         <v>435</v>
@@ -13943,7 +13942,7 @@
       <c r="J53" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K53" s="103"/>
+      <c r="K53" s="94"/>
       <c r="L53" s="56"/>
       <c r="M53" s="53" t="s">
         <v>435</v>
@@ -13979,7 +13978,7 @@
       <c r="J54" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K54" s="107"/>
+      <c r="K54" s="95"/>
       <c r="L54" s="66"/>
       <c r="M54" s="53" t="s">
         <v>435</v>
@@ -14099,7 +14098,7 @@
       <c r="J57" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K57" s="97" t="s">
+      <c r="K57" s="102" t="s">
         <v>556</v>
       </c>
       <c r="L57" s="56"/>
@@ -14139,7 +14138,7 @@
       <c r="J58" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K58" s="94"/>
+      <c r="K58" s="100"/>
       <c r="L58" s="56"/>
       <c r="M58" s="7" t="s">
         <v>435</v>
@@ -14175,7 +14174,7 @@
       <c r="J59" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K59" s="94"/>
+      <c r="K59" s="100"/>
       <c r="L59" s="56"/>
       <c r="M59" s="7" t="s">
         <v>435</v>
@@ -14213,7 +14212,7 @@
       <c r="J60" s="53" t="s">
         <v>435</v>
       </c>
-      <c r="K60" s="95" t="s">
+      <c r="K60" s="103" t="s">
         <v>561</v>
       </c>
       <c r="L60" s="65"/>
@@ -14253,7 +14252,7 @@
       <c r="J61" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K61" s="96"/>
+      <c r="K61" s="104"/>
       <c r="L61" s="56" t="s">
         <v>563</v>
       </c>
@@ -14293,7 +14292,7 @@
       <c r="J62" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K62" s="96"/>
+      <c r="K62" s="104"/>
       <c r="L62" s="56" t="s">
         <v>565</v>
       </c>
@@ -14333,7 +14332,7 @@
       <c r="J63" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K63" s="97"/>
+      <c r="K63" s="102"/>
       <c r="L63" s="56"/>
       <c r="M63" s="7" t="s">
         <v>435</v>
@@ -14371,7 +14370,7 @@
       <c r="J64" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K64" s="94"/>
+      <c r="K64" s="100"/>
       <c r="L64" s="56"/>
       <c r="M64" s="7" t="s">
         <v>435</v>
@@ -14409,7 +14408,7 @@
       <c r="J65" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K65" s="94"/>
+      <c r="K65" s="100"/>
       <c r="L65" s="56" t="s">
         <v>565</v>
       </c>
@@ -14447,7 +14446,7 @@
       <c r="J66" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="K66" s="94"/>
+      <c r="K66" s="100"/>
       <c r="L66" s="12"/>
       <c r="M66" s="54" t="s">
         <v>435</v>
@@ -14561,7 +14560,7 @@
       <c r="J69" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K69" s="97" t="s">
+      <c r="K69" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L69" s="56" t="s">
@@ -14603,7 +14602,7 @@
       <c r="J70" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K70" s="94"/>
+      <c r="K70" s="100"/>
       <c r="L70" s="56"/>
       <c r="M70" s="7" t="s">
         <v>435</v>
@@ -14681,7 +14680,7 @@
       <c r="J72" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K72" s="97"/>
+      <c r="K72" s="102"/>
       <c r="L72" s="56"/>
       <c r="M72" s="7" t="s">
         <v>435</v>
@@ -14717,7 +14716,7 @@
       <c r="J73" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K73" s="94"/>
+      <c r="K73" s="100"/>
       <c r="L73" s="56"/>
       <c r="M73" s="7" t="s">
         <v>435</v>
@@ -14753,7 +14752,7 @@
       <c r="J74" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K74" s="94"/>
+      <c r="K74" s="100"/>
       <c r="L74" s="56"/>
       <c r="M74" s="7" t="s">
         <v>435</v>
@@ -14787,7 +14786,7 @@
       <c r="J75" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K75" s="98"/>
+      <c r="K75" s="101"/>
       <c r="L75" s="66"/>
       <c r="M75" s="7" t="s">
         <v>435</v>
@@ -14865,10 +14864,10 @@
       <c r="J77" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="K77" s="106" t="s">
+      <c r="K77" s="93" t="s">
         <v>588</v>
       </c>
-      <c r="L77" s="93" t="s">
+      <c r="L77" s="99" t="s">
         <v>589</v>
       </c>
       <c r="M77" s="53" t="s">
@@ -14909,8 +14908,8 @@
       <c r="J78" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K78" s="107"/>
-      <c r="L78" s="109"/>
+      <c r="K78" s="95"/>
+      <c r="L78" s="97"/>
       <c r="M78" s="54" t="s">
         <v>435</v>
       </c>
@@ -14950,7 +14949,7 @@
       <c r="K79" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L79" s="109"/>
+      <c r="L79" s="97"/>
       <c r="M79" s="54" t="s">
         <v>435</v>
       </c>
@@ -14990,7 +14989,7 @@
       <c r="K80" s="56" t="s">
         <v>590</v>
       </c>
-      <c r="L80" s="98"/>
+      <c r="L80" s="101"/>
       <c r="M80" s="7" t="s">
         <v>435</v>
       </c>
@@ -15027,7 +15026,7 @@
       <c r="J81" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K81" s="97" t="s">
+      <c r="K81" s="102" t="s">
         <v>468</v>
       </c>
       <c r="L81" s="56" t="s">
@@ -15069,7 +15068,7 @@
       <c r="J82" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K82" s="94"/>
+      <c r="K82" s="100"/>
       <c r="L82" s="56"/>
       <c r="M82" s="7" t="s">
         <v>435</v>
@@ -15191,7 +15190,7 @@
       <c r="J85" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K85" s="97" t="s">
+      <c r="K85" s="102" t="s">
         <v>602</v>
       </c>
       <c r="L85" s="56"/>
@@ -15231,7 +15230,7 @@
       <c r="J86" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K86" s="94"/>
+      <c r="K86" s="100"/>
       <c r="L86" s="56"/>
       <c r="M86" s="7" t="s">
         <v>435</v>
@@ -15269,7 +15268,7 @@
       <c r="J87" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K87" s="94"/>
+      <c r="K87" s="100"/>
       <c r="L87" s="56"/>
       <c r="M87" s="7" t="s">
         <v>435</v>
@@ -15305,7 +15304,7 @@
       <c r="J88" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K88" s="94"/>
+      <c r="K88" s="100"/>
       <c r="L88" s="56"/>
       <c r="M88" s="7" t="s">
         <v>435</v>
@@ -15343,7 +15342,7 @@
       <c r="J89" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K89" s="94"/>
+      <c r="K89" s="100"/>
       <c r="L89" s="56"/>
       <c r="M89" s="7" t="s">
         <v>435</v>
@@ -15381,7 +15380,7 @@
       <c r="J90" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K90" s="94"/>
+      <c r="K90" s="100"/>
       <c r="L90" s="56"/>
       <c r="M90" s="7" t="s">
         <v>435</v>
@@ -15419,10 +15418,10 @@
       <c r="J91" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K91" s="106" t="s">
+      <c r="K91" s="93" t="s">
         <v>608</v>
       </c>
-      <c r="L91" s="108" t="s">
+      <c r="L91" s="96" t="s">
         <v>609</v>
       </c>
       <c r="M91" s="53" t="s">
@@ -15461,8 +15460,8 @@
       <c r="J92" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K92" s="103"/>
-      <c r="L92" s="109"/>
+      <c r="K92" s="94"/>
+      <c r="L92" s="97"/>
       <c r="M92" s="7" t="s">
         <v>435</v>
       </c>
@@ -15499,8 +15498,8 @@
       <c r="J93" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="K93" s="103"/>
-      <c r="L93" s="109"/>
+      <c r="K93" s="94"/>
+      <c r="L93" s="97"/>
       <c r="M93" s="7" t="s">
         <v>435</v>
       </c>
@@ -15535,8 +15534,8 @@
       <c r="J94" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K94" s="107"/>
-      <c r="L94" s="110"/>
+      <c r="K94" s="95"/>
+      <c r="L94" s="98"/>
       <c r="M94" s="7" t="s">
         <v>435</v>
       </c>
@@ -15573,7 +15572,7 @@
       <c r="J95" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K95" s="93"/>
+      <c r="K95" s="99"/>
       <c r="L95" s="56"/>
       <c r="M95" s="53" t="s">
         <v>435</v>
@@ -15611,7 +15610,7 @@
       <c r="J96" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K96" s="94"/>
+      <c r="K96" s="100"/>
       <c r="L96" s="56"/>
       <c r="M96" s="53" t="s">
         <v>435</v>
@@ -15649,7 +15648,7 @@
       <c r="J97" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K97" s="94"/>
+      <c r="K97" s="100"/>
       <c r="L97" s="56"/>
       <c r="M97" s="53" t="s">
         <v>435</v>
@@ -15687,7 +15686,7 @@
       <c r="J98" s="54" t="s">
         <v>435</v>
       </c>
-      <c r="K98" s="94"/>
+      <c r="K98" s="100"/>
       <c r="L98" s="56"/>
       <c r="M98" s="53" t="s">
         <v>435</v>
@@ -15723,7 +15722,7 @@
       <c r="J99" s="59" t="s">
         <v>435</v>
       </c>
-      <c r="K99" s="98"/>
+      <c r="K99" s="101"/>
       <c r="L99" s="60"/>
       <c r="M99" s="61" t="s">
         <v>435</v>
@@ -15752,6 +15751,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15760,28 +15781,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20141,7 +20140,7 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added more analytes to fill out csmi USGS 2021 wq data
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54058E67-7D77-42C7-AE50-5900CFE1C909}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FFC9DD3-F616-49AE-BD3E-BCF744600BD1}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Annie_Comments" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$75</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">GLENDA_Map!$B$1:$M$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Key!$A$1:$A$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">NCCA_Map!$A$1:$A$57</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3676" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3707" uniqueCount="805">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2472,6 +2472,12 @@
   </si>
   <si>
     <t>Oxy</t>
+  </si>
+  <si>
+    <t>CDOM</t>
+  </si>
+  <si>
+    <t>PAR</t>
   </si>
 </sst>
 </file>
@@ -3021,11 +3027,35 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3033,10 +3063,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3050,30 +3080,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3382,7 +3388,9 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8169,10 +8177,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
-      <selection activeCell="J101" sqref="J101"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9431,33 +9439,31 @@
       </c>
       <c r="L42" s="13"/>
     </row>
-    <row r="43" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="13"/>
+      <c r="E43" s="13" t="s">
+        <v>643</v>
+      </c>
       <c r="F43" s="23">
-        <v>2021</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>699</v>
-      </c>
-      <c r="H43" s="7" t="s">
+        <v>2015</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="20" t="s">
         <v>268</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>700</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="J43" s="13"/>
       <c r="K43" s="13" t="s">
-        <v>701</v>
+        <v>644</v>
       </c>
       <c r="L43" s="13"/>
     </row>
@@ -9466,7 +9472,7 @@
         <v>684</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>245</v>
+        <v>803</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -9477,7 +9483,7 @@
       <c r="G44" s="8" t="s">
         <v>699</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H44" s="20" t="s">
         <v>268</v>
       </c>
       <c r="I44" s="8" t="s">
@@ -9491,12 +9497,12 @@
       </c>
       <c r="L44" s="13"/>
     </row>
-    <row r="45" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>702</v>
+        <v>804</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -9505,24 +9511,28 @@
         <v>2021</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>232</v>
+        <v>699</v>
+      </c>
+      <c r="H45" s="20" t="s">
+        <v>268</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
+      <c r="J45" s="13" t="s">
+        <v>700</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>701</v>
+      </c>
       <c r="L45" s="13"/>
     </row>
-    <row r="46" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>703</v>
+        <v>244</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -9531,7 +9541,7 @@
         <v>2021</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>268</v>
@@ -9540,17 +9550,19 @@
         <v>280</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>705</v>
-      </c>
-      <c r="K46" s="13"/>
+        <v>700</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>701</v>
+      </c>
       <c r="L46" s="13"/>
     </row>
-    <row r="47" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>706</v>
+        <v>245</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -9559,7 +9571,7 @@
         <v>2021</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>268</v>
@@ -9568,9 +9580,11 @@
         <v>280</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>705</v>
-      </c>
-      <c r="K47" s="13"/>
+        <v>700</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>701</v>
+      </c>
       <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9578,7 +9592,7 @@
         <v>684</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>708</v>
+        <v>369</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -9587,17 +9601,15 @@
         <v>2021</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>709</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>268</v>
+        <v>231</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J48" s="13" t="s">
-        <v>705</v>
-      </c>
+      <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
     </row>
@@ -9606,7 +9618,7 @@
         <v>684</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -9615,17 +9627,15 @@
         <v>2021</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>13</v>
+        <v>231</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J49" s="13" t="s">
-        <v>705</v>
-      </c>
+      <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
     </row>
@@ -9634,7 +9644,7 @@
         <v>684</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -9643,7 +9653,7 @@
         <v>2021</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>268</v>
@@ -9662,7 +9672,7 @@
         <v>684</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -9671,7 +9681,7 @@
         <v>2021</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>268</v>
@@ -9690,7 +9700,7 @@
         <v>684</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>83</v>
+        <v>708</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -9699,24 +9709,26 @@
         <v>2021</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>13</v>
+        <v>709</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>83</v>
+        <v>268</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J52" s="13"/>
+      <c r="J52" s="13" t="s">
+        <v>705</v>
+      </c>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
     </row>
-    <row r="53" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -9725,7 +9737,7 @@
         <v>2021</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>715</v>
+        <v>13</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>268</v>
@@ -9733,10 +9745,10 @@
       <c r="I53" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J53" s="13"/>
-      <c r="K53" s="13" t="s">
-        <v>716</v>
-      </c>
+      <c r="J53" s="13" t="s">
+        <v>705</v>
+      </c>
+      <c r="K53" s="13"/>
       <c r="L53" s="13"/>
     </row>
     <row r="54" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9744,7 +9756,7 @@
         <v>684</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>247</v>
+        <v>711</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -9753,7 +9765,7 @@
         <v>2021</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>268</v>
@@ -9761,7 +9773,9 @@
       <c r="I54" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J54" s="13"/>
+      <c r="J54" s="13" t="s">
+        <v>705</v>
+      </c>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
     </row>
@@ -9770,7 +9784,7 @@
         <v>684</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>249</v>
+        <v>328</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -9779,15 +9793,17 @@
         <v>2021</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>717</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>268</v>
+        <v>277</v>
+      </c>
+      <c r="H55" s="20" t="s">
+        <v>609</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J55" s="13"/>
+      <c r="J55" s="13" t="s">
+        <v>705</v>
+      </c>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
     </row>
@@ -9796,7 +9812,7 @@
         <v>684</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>250</v>
+        <v>712</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -9805,7 +9821,7 @@
         <v>2021</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>268</v>
@@ -9813,7 +9829,9 @@
       <c r="I56" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J56" s="13"/>
+      <c r="J56" s="13" t="s">
+        <v>705</v>
+      </c>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
     </row>
@@ -9822,7 +9840,7 @@
         <v>684</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>251</v>
+        <v>83</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -9831,10 +9849,10 @@
         <v>2021</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>717</v>
+        <v>13</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>280</v>
@@ -9843,12 +9861,12 @@
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
     </row>
-    <row r="58" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>252</v>
+        <v>714</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -9857,7 +9875,7 @@
         <v>2021</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>253</v>
+        <v>715</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>268</v>
@@ -9866,7 +9884,9 @@
         <v>280</v>
       </c>
       <c r="J58" s="13"/>
-      <c r="K58" s="13"/>
+      <c r="K58" s="13" t="s">
+        <v>716</v>
+      </c>
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9874,7 +9894,7 @@
         <v>684</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -9900,7 +9920,7 @@
         <v>684</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -9909,7 +9929,7 @@
         <v>2021</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>231</v>
+        <v>717</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>268</v>
@@ -9926,7 +9946,7 @@
         <v>684</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>718</v>
+        <v>250</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -9935,7 +9955,7 @@
         <v>2021</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>318</v>
+        <v>717</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>268</v>
@@ -9952,7 +9972,7 @@
         <v>684</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>719</v>
+        <v>251</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -9961,7 +9981,7 @@
         <v>2021</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>268</v>
@@ -9978,7 +9998,7 @@
         <v>684</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -9987,7 +10007,7 @@
         <v>2021</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>13</v>
+        <v>253</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>268</v>
@@ -9995,18 +10015,16 @@
       <c r="I63" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J63" s="13" t="s">
-        <v>722</v>
-      </c>
+      <c r="J63" s="13"/>
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
     </row>
-    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>327</v>
+        <v>254</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -10015,7 +10033,7 @@
         <v>2021</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>268</v>
@@ -10023,18 +10041,16 @@
       <c r="I64" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J64" s="13" t="s">
-        <v>723</v>
-      </c>
+      <c r="J64" s="13"/>
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
     </row>
-    <row r="65" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -10043,7 +10059,7 @@
         <v>2021</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>724</v>
+        <v>231</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>268</v>
@@ -10055,12 +10071,12 @@
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
     </row>
-    <row r="66" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>258</v>
+        <v>718</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -10069,7 +10085,7 @@
         <v>2021</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>259</v>
+        <v>318</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>268</v>
@@ -10077,20 +10093,16 @@
       <c r="I66" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J66" s="13" t="s">
-        <v>725</v>
-      </c>
-      <c r="K66" s="13" t="s">
-        <v>726</v>
-      </c>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
       <c r="L66" s="13"/>
     </row>
-    <row r="67" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>260</v>
+        <v>719</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -10099,7 +10111,7 @@
         <v>2021</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>268</v>
@@ -10111,12 +10123,12 @@
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
     </row>
-    <row r="68" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>262</v>
+        <v>721</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -10125,7 +10137,7 @@
         <v>2021</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>727</v>
+        <v>13</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>268</v>
@@ -10133,7 +10145,9 @@
       <c r="I68" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J68" s="13"/>
+      <c r="J68" s="13" t="s">
+        <v>722</v>
+      </c>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
     </row>
@@ -10142,7 +10156,7 @@
         <v>684</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -10151,7 +10165,7 @@
         <v>2021</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>268</v>
@@ -10159,7 +10173,9 @@
       <c r="I69" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J69" s="13"/>
+      <c r="J69" s="13" t="s">
+        <v>723</v>
+      </c>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
     </row>
@@ -10168,7 +10184,7 @@
         <v>684</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -10177,7 +10193,7 @@
         <v>2021</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>268</v>
@@ -10191,141 +10207,135 @@
     </row>
     <row r="71" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>728</v>
-      </c>
-      <c r="B71" s="39" t="s">
-        <v>202</v>
+        <v>684</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>258</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="70">
+      <c r="E71" s="13"/>
+      <c r="F71" s="23">
         <v>2021</v>
       </c>
-      <c r="G71" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="H71" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="I71" s="39" t="s">
+      <c r="G71" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J71" s="41" t="s">
-        <v>729</v>
-      </c>
-      <c r="K71" s="41"/>
+      <c r="J71" s="13" t="s">
+        <v>725</v>
+      </c>
+      <c r="K71" s="13" t="s">
+        <v>726</v>
+      </c>
       <c r="L71" s="13"/>
     </row>
     <row r="72" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>728</v>
+        <v>684</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>197</v>
+        <v>260</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
-      <c r="E72" s="71"/>
+      <c r="E72" s="13"/>
       <c r="F72" s="23">
         <v>2021</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>42</v>
+        <v>727</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>88</v>
+        <v>268</v>
       </c>
       <c r="I72" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J72" s="13" t="s">
-        <v>730</v>
-      </c>
+      <c r="J72" s="13"/>
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
     </row>
     <row r="73" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>728</v>
+        <v>684</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
-      <c r="E73" s="71"/>
+      <c r="E73" s="13"/>
       <c r="F73" s="23">
         <v>2021</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>42</v>
+        <v>727</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>574</v>
+        <v>268</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J73" s="13" t="s">
-        <v>731</v>
-      </c>
+      <c r="J73" s="13"/>
       <c r="K73" s="13"/>
       <c r="L73" s="13"/>
     </row>
     <row r="74" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>728</v>
+        <v>684</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>203</v>
+        <v>263</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
-      <c r="E74" s="71"/>
+      <c r="E74" s="13"/>
       <c r="F74" s="23">
         <v>2021</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>42</v>
+        <v>727</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>506</v>
+        <v>268</v>
       </c>
       <c r="I74" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J74" s="13" t="s">
-        <v>732</v>
-      </c>
+      <c r="J74" s="13"/>
       <c r="K74" s="13"/>
       <c r="L74" s="13"/>
     </row>
     <row r="75" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>728</v>
+        <v>684</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>733</v>
+        <v>264</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
-      <c r="E75" s="71"/>
+      <c r="E75" s="13"/>
       <c r="F75" s="23">
         <v>2021</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>211</v>
+        <v>727</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J75" s="13" t="s">
-        <v>734</v>
-      </c>
+      <c r="J75" s="13"/>
       <c r="K75" s="13"/>
       <c r="L75" s="13"/>
     </row>
@@ -10333,28 +10343,28 @@
       <c r="A76" s="13" t="s">
         <v>728</v>
       </c>
-      <c r="B76" s="8" t="s">
-        <v>49</v>
+      <c r="B76" s="39" t="s">
+        <v>202</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
-      <c r="E76" s="71"/>
-      <c r="F76" s="23">
+      <c r="E76" s="69"/>
+      <c r="F76" s="70">
         <v>2021</v>
       </c>
-      <c r="G76" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="I76" s="8" t="s">
+      <c r="G76" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H76" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I76" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J76" s="13" t="s">
-        <v>735</v>
-      </c>
-      <c r="K76" s="13"/>
+      <c r="J76" s="41" t="s">
+        <v>729</v>
+      </c>
+      <c r="K76" s="41"/>
       <c r="L76" s="13"/>
     </row>
     <row r="77" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10362,7 +10372,7 @@
         <v>728</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
@@ -10374,13 +10384,13 @@
         <v>42</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>594</v>
+        <v>88</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="K77" s="13"/>
       <c r="L77" s="13"/>
@@ -10390,7 +10400,7 @@
         <v>728</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>737</v>
+        <v>200</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
@@ -10402,13 +10412,13 @@
         <v>42</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>95</v>
+        <v>574</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="K78" s="13"/>
       <c r="L78" s="13"/>
@@ -10418,7 +10428,7 @@
         <v>728</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>31</v>
+        <v>203</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -10427,16 +10437,16 @@
         <v>2021</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>31</v>
+        <v>506</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>31</v>
+        <v>732</v>
       </c>
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
@@ -10446,7 +10456,7 @@
         <v>728</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>180</v>
+        <v>733</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -10455,16 +10465,16 @@
         <v>2021</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>739</v>
+        <v>211</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="I80" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
@@ -10474,7 +10484,7 @@
         <v>728</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>196</v>
+        <v>49</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
@@ -10486,13 +10496,13 @@
         <v>211</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>72</v>
+        <v>269</v>
       </c>
       <c r="I81" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
@@ -10502,7 +10512,7 @@
         <v>728</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
@@ -10511,16 +10521,16 @@
         <v>2021</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>77</v>
+        <v>594</v>
       </c>
       <c r="I82" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
@@ -10530,13 +10540,11 @@
         <v>728</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>205</v>
+        <v>737</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
-      <c r="E83" s="13" t="s">
-        <v>742</v>
-      </c>
+      <c r="E83" s="71"/>
       <c r="F83" s="23">
         <v>2021</v>
       </c>
@@ -10544,17 +10552,15 @@
         <v>42</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>268</v>
+        <v>95</v>
       </c>
       <c r="I83" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>743</v>
-      </c>
-      <c r="K83" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>738</v>
+      </c>
+      <c r="K83" s="13"/>
       <c r="L83" s="13"/>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10562,31 +10568,27 @@
         <v>728</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>206</v>
+        <v>31</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
-      <c r="E84" s="13" t="s">
-        <v>742</v>
-      </c>
+      <c r="E84" s="71"/>
       <c r="F84" s="23">
         <v>2021</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>268</v>
+        <v>31</v>
       </c>
       <c r="I84" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>743</v>
-      </c>
-      <c r="K84" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K84" s="13"/>
       <c r="L84" s="13"/>
     </row>
     <row r="85" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10594,7 +10596,7 @@
         <v>728</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
@@ -10603,150 +10605,158 @@
         <v>2021</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H85" s="9" t="s">
-        <v>23</v>
+        <v>739</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>356</v>
       </c>
       <c r="I85" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J85" s="13"/>
+      <c r="J85" s="13" t="s">
+        <v>740</v>
+      </c>
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
     </row>
     <row r="86" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B86" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="C86" s="72" t="s">
-        <v>452</v>
-      </c>
-      <c r="D86" s="72"/>
-      <c r="E86" s="73"/>
-      <c r="F86" s="74">
-        <v>2010</v>
-      </c>
-      <c r="G86" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="H86" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="I86" s="39" t="s">
+        <v>728</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I86" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J86" s="41"/>
+      <c r="J86" s="13" t="s">
+        <v>741</v>
+      </c>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
     </row>
     <row r="87" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B87" s="75" t="s">
-        <v>202</v>
-      </c>
-      <c r="C87" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D87" s="75"/>
-      <c r="E87" s="76"/>
-      <c r="F87" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G87" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H87" s="39" t="s">
-        <v>469</v>
+        <v>728</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J87" s="13"/>
+      <c r="J87" s="13" t="s">
+        <v>741</v>
+      </c>
       <c r="K87" s="13"/>
       <c r="L87" s="13"/>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B88" s="75" t="s">
-        <v>197</v>
-      </c>
-      <c r="C88" s="75" t="s">
-        <v>452</v>
-      </c>
-      <c r="D88" s="75"/>
-      <c r="E88" s="76"/>
-      <c r="F88" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G88" s="75" t="s">
-        <v>198</v>
+        <v>728</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="F88" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G88" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>88</v>
+        <v>268</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
+      <c r="J88" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="K88" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L88" s="13"/>
     </row>
     <row r="89" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B89" s="75" t="s">
-        <v>204</v>
-      </c>
-      <c r="C89" s="75" t="s">
-        <v>452</v>
-      </c>
-      <c r="D89" s="75"/>
-      <c r="E89" s="76"/>
-      <c r="F89" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G89" s="75" t="s">
-        <v>198</v>
+        <v>728</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="F89" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>204</v>
+        <v>268</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
+      <c r="J89" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="K89" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L89" s="13"/>
     </row>
     <row r="90" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="75" t="s">
-        <v>204</v>
-      </c>
-      <c r="C90" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D90" s="75"/>
-      <c r="E90" s="76"/>
-      <c r="F90" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G90" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>204</v>
+        <v>728</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="71"/>
+      <c r="F90" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>280</v>
@@ -10759,27 +10769,27 @@
       <c r="A91" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B91" s="75" t="s">
-        <v>200</v>
-      </c>
-      <c r="C91" s="75" t="s">
+      <c r="B91" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" s="72" t="s">
         <v>452</v>
       </c>
-      <c r="D91" s="75"/>
-      <c r="E91" s="76"/>
-      <c r="F91" s="77">
+      <c r="D91" s="72"/>
+      <c r="E91" s="73"/>
+      <c r="F91" s="74">
         <v>2010</v>
       </c>
-      <c r="G91" s="75" t="s">
+      <c r="G91" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="H91" s="7" t="s">
-        <v>574</v>
-      </c>
-      <c r="I91" s="8" t="s">
+      <c r="H91" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I91" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J91" s="13"/>
+      <c r="J91" s="41"/>
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
     </row>
@@ -10788,7 +10798,7 @@
         <v>119</v>
       </c>
       <c r="B92" s="75" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C92" s="75" t="s">
         <v>13</v>
@@ -10801,8 +10811,8 @@
       <c r="G92" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="H92" s="7" t="s">
-        <v>574</v>
+      <c r="H92" s="39" t="s">
+        <v>469</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>280</v>
@@ -10816,7 +10826,7 @@
         <v>119</v>
       </c>
       <c r="B93" s="75" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C93" s="75" t="s">
         <v>452</v>
@@ -10830,7 +10840,7 @@
         <v>198</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>506</v>
+        <v>88</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>280</v>
@@ -10844,10 +10854,10 @@
         <v>119</v>
       </c>
       <c r="B94" s="75" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C94" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D94" s="75"/>
       <c r="E94" s="76"/>
@@ -10858,7 +10868,7 @@
         <v>198</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>506</v>
+        <v>204</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>280</v>
@@ -10872,10 +10882,10 @@
         <v>119</v>
       </c>
       <c r="B95" s="75" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C95" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D95" s="75"/>
       <c r="E95" s="76"/>
@@ -10883,10 +10893,10 @@
         <v>2010</v>
       </c>
       <c r="G95" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>347</v>
+        <v>204</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>280</v>
@@ -10900,10 +10910,10 @@
         <v>119</v>
       </c>
       <c r="B96" s="75" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C96" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D96" s="75"/>
       <c r="E96" s="76"/>
@@ -10911,10 +10921,10 @@
         <v>2010</v>
       </c>
       <c r="G96" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>347</v>
+        <v>574</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>280</v>
@@ -10928,10 +10938,10 @@
         <v>119</v>
       </c>
       <c r="B97" s="75" t="s">
-        <v>49</v>
+        <v>200</v>
       </c>
       <c r="C97" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D97" s="75"/>
       <c r="E97" s="76"/>
@@ -10939,10 +10949,10 @@
         <v>2010</v>
       </c>
       <c r="G97" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>269</v>
+        <v>574</v>
       </c>
       <c r="I97" s="8" t="s">
         <v>280</v>
@@ -10956,10 +10966,10 @@
         <v>119</v>
       </c>
       <c r="B98" s="75" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="C98" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D98" s="75"/>
       <c r="E98" s="76"/>
@@ -10967,10 +10977,10 @@
         <v>2010</v>
       </c>
       <c r="G98" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>269</v>
+        <v>506</v>
       </c>
       <c r="I98" s="8" t="s">
         <v>280</v>
@@ -10984,10 +10994,10 @@
         <v>119</v>
       </c>
       <c r="B99" s="75" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C99" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D99" s="75"/>
       <c r="E99" s="76"/>
@@ -10998,7 +11008,7 @@
         <v>198</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>594</v>
+        <v>506</v>
       </c>
       <c r="I99" s="8" t="s">
         <v>280</v>
@@ -11012,10 +11022,10 @@
         <v>119</v>
       </c>
       <c r="B100" s="75" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C100" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D100" s="75"/>
       <c r="E100" s="76"/>
@@ -11023,10 +11033,10 @@
         <v>2010</v>
       </c>
       <c r="G100" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>594</v>
+        <v>347</v>
       </c>
       <c r="I100" s="8" t="s">
         <v>280</v>
@@ -11040,10 +11050,10 @@
         <v>119</v>
       </c>
       <c r="B101" s="75" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="C101" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D101" s="75"/>
       <c r="E101" s="76"/>
@@ -11053,31 +11063,25 @@
       <c r="G101" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H101" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="I101" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J101" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="K101" s="13" t="s">
-        <v>746</v>
-      </c>
-      <c r="L101" s="13" t="s">
-        <v>397</v>
-      </c>
+      <c r="H101" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J101" s="13"/>
+      <c r="K101" s="13"/>
+      <c r="L101" s="13"/>
     </row>
     <row r="102" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B102" s="75" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="C102" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D102" s="75"/>
       <c r="E102" s="76"/>
@@ -11087,31 +11091,25 @@
       <c r="G102" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H102" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="I102" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J102" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="K102" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="L102" s="13" t="s">
-        <v>397</v>
-      </c>
+      <c r="H102" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I102" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J102" s="13"/>
+      <c r="K102" s="13"/>
+      <c r="L102" s="13"/>
     </row>
     <row r="103" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B103" s="75" t="s">
-        <v>208</v>
+        <v>49</v>
       </c>
       <c r="C103" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D103" s="75"/>
       <c r="E103" s="76"/>
@@ -11121,31 +11119,25 @@
       <c r="G103" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H103" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I103" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J103" s="13" t="s">
-        <v>748</v>
-      </c>
-      <c r="K103" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="L103" s="13" t="s">
-        <v>397</v>
-      </c>
+      <c r="H103" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
     </row>
     <row r="104" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B104" s="75" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C104" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D104" s="75"/>
       <c r="E104" s="76"/>
@@ -11153,33 +11145,27 @@
         <v>2010</v>
       </c>
       <c r="G104" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H104" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I104" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J104" s="13" t="s">
-        <v>748</v>
-      </c>
-      <c r="K104" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="L104" s="13" t="s">
-        <v>397</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H104" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="I104" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J104" s="13"/>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
     </row>
     <row r="105" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B105" s="75" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C105" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D105" s="75"/>
       <c r="E105" s="76"/>
@@ -11187,33 +11173,27 @@
         <v>2010</v>
       </c>
       <c r="G105" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H105" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I105" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J105" s="13" t="s">
-        <v>749</v>
-      </c>
-      <c r="K105" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="L105" s="13" t="s">
-        <v>397</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J105" s="13"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
     </row>
     <row r="106" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B106" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C106" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D106" s="75"/>
       <c r="E106" s="76"/>
@@ -11224,16 +11204,16 @@
         <v>194</v>
       </c>
       <c r="H106" s="15" t="s">
-        <v>59</v>
+        <v>620</v>
       </c>
       <c r="I106" s="15" t="s">
         <v>744</v>
       </c>
       <c r="J106" s="13" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="K106" s="13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L106" s="13" t="s">
         <v>397</v>
@@ -11244,10 +11224,10 @@
         <v>119</v>
       </c>
       <c r="B107" s="75" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D107" s="75"/>
       <c r="E107" s="76"/>
@@ -11255,27 +11235,33 @@
         <v>2010</v>
       </c>
       <c r="G107" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H107" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I107" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="H107" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="I107" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="J107" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="K107" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="L107" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="108" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B108" s="75" t="s">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>452</v>
+        <v>485</v>
       </c>
       <c r="D108" s="75"/>
       <c r="E108" s="76"/>
@@ -11285,22 +11271,28 @@
       <c r="G108" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H108" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I108" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
+      <c r="H108" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I108" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="J108" s="13" t="s">
+        <v>748</v>
+      </c>
+      <c r="K108" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="L108" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="109" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B109" s="75" t="s">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="C109" s="75" t="s">
         <v>13</v>
@@ -11313,22 +11305,28 @@
       <c r="G109" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H109" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I109" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
+      <c r="H109" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I109" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="J109" s="13" t="s">
+        <v>748</v>
+      </c>
+      <c r="K109" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="L109" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="110" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B110" s="75" t="s">
-        <v>319</v>
+        <v>210</v>
       </c>
       <c r="C110" s="75" t="s">
         <v>485</v>
@@ -11339,24 +11337,30 @@
         <v>2010</v>
       </c>
       <c r="G110" s="75" t="s">
-        <v>750</v>
-      </c>
-      <c r="H110" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="I110" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J110" s="13"/>
-      <c r="K110" s="13"/>
-      <c r="L110" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="H110" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I110" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="J110" s="13" t="s">
+        <v>749</v>
+      </c>
+      <c r="K110" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="L110" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="111" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B111" s="75" t="s">
-        <v>319</v>
+        <v>210</v>
       </c>
       <c r="C111" s="75" t="s">
         <v>13</v>
@@ -11367,24 +11371,30 @@
         <v>2010</v>
       </c>
       <c r="G111" s="75" t="s">
-        <v>750</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="I111" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="H111" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I111" s="15" t="s">
+        <v>744</v>
+      </c>
+      <c r="J111" s="13" t="s">
+        <v>749</v>
+      </c>
+      <c r="K111" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="L111" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="112" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B112" s="75" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="C112" s="75" t="s">
         <v>452</v>
@@ -11398,14 +11408,12 @@
         <v>198</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>356</v>
+        <v>95</v>
       </c>
       <c r="I112" s="8" t="s">
-        <v>751</v>
-      </c>
-      <c r="J112" s="13" t="s">
-        <v>752</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="J112" s="13"/>
       <c r="K112" s="13"/>
       <c r="L112" s="13"/>
     </row>
@@ -11414,10 +11422,10 @@
         <v>119</v>
       </c>
       <c r="B113" s="75" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="C113" s="75" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D113" s="75"/>
       <c r="E113" s="76"/>
@@ -11428,7 +11436,7 @@
         <v>194</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="I113" s="8" t="s">
         <v>280</v>
@@ -11442,10 +11450,10 @@
         <v>119</v>
       </c>
       <c r="B114" s="75" t="s">
-        <v>195</v>
+        <v>31</v>
       </c>
       <c r="C114" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D114" s="75"/>
       <c r="E114" s="76"/>
@@ -11456,7 +11464,7 @@
         <v>194</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="I114" s="8" t="s">
         <v>280</v>
@@ -11470,10 +11478,10 @@
         <v>119</v>
       </c>
       <c r="B115" s="75" t="s">
-        <v>205</v>
+        <v>319</v>
       </c>
       <c r="C115" s="75" t="s">
-        <v>438</v>
+        <v>485</v>
       </c>
       <c r="D115" s="75"/>
       <c r="E115" s="76"/>
@@ -11481,20 +11489,16 @@
         <v>2010</v>
       </c>
       <c r="G115" s="75" t="s">
-        <v>198</v>
+        <v>750</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="I115" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="J115" s="13" t="s">
-        <v>754</v>
-      </c>
-      <c r="K115" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="J115" s="13"/>
+      <c r="K115" s="13"/>
       <c r="L115" s="13"/>
     </row>
     <row r="116" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11502,7 +11506,7 @@
         <v>119</v>
       </c>
       <c r="B116" s="75" t="s">
-        <v>205</v>
+        <v>319</v>
       </c>
       <c r="C116" s="75" t="s">
         <v>13</v>
@@ -11513,18 +11517,16 @@
         <v>2010</v>
       </c>
       <c r="G116" s="75" t="s">
-        <v>198</v>
+        <v>750</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>753</v>
+        <v>280</v>
       </c>
       <c r="J116" s="13"/>
-      <c r="K116" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="K116" s="13"/>
       <c r="L116" s="13"/>
     </row>
     <row r="117" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11532,10 +11534,10 @@
         <v>119</v>
       </c>
       <c r="B117" s="75" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="C117" s="75" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D117" s="75"/>
       <c r="E117" s="76"/>
@@ -11546,15 +11548,15 @@
         <v>198</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="J117" s="13"/>
-      <c r="K117" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>751</v>
+      </c>
+      <c r="J117" s="13" t="s">
+        <v>752</v>
+      </c>
+      <c r="K117" s="13"/>
       <c r="L117" s="13"/>
     </row>
     <row r="118" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11562,10 +11564,10 @@
         <v>119</v>
       </c>
       <c r="B118" s="75" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C118" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D118" s="75"/>
       <c r="E118" s="76"/>
@@ -11573,18 +11575,16 @@
         <v>2010</v>
       </c>
       <c r="G118" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>268</v>
+        <v>72</v>
       </c>
       <c r="I118" s="8" t="s">
-        <v>753</v>
+        <v>280</v>
       </c>
       <c r="J118" s="13"/>
-      <c r="K118" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="K118" s="13"/>
       <c r="L118" s="13"/>
     </row>
     <row r="119" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11592,7 +11592,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="75" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C119" s="75" t="s">
         <v>438</v>
@@ -11606,7 +11606,7 @@
         <v>194</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="I119" s="8" t="s">
         <v>280</v>
@@ -11620,10 +11620,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="75" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C120" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D120" s="75"/>
       <c r="E120" s="76"/>
@@ -11631,17 +11631,167 @@
         <v>2010</v>
       </c>
       <c r="G120" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H120" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I120" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="J120" s="13" t="s">
+        <v>754</v>
+      </c>
+      <c r="K120" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L120" s="13"/>
+    </row>
+    <row r="121" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B121" s="75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C121" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" s="75"/>
+      <c r="E121" s="76"/>
+      <c r="F121" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G121" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I121" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="J121" s="13"/>
+      <c r="K121" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L121" s="13"/>
+    </row>
+    <row r="122" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B122" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="C122" s="75" t="s">
+        <v>438</v>
+      </c>
+      <c r="D122" s="75"/>
+      <c r="E122" s="76"/>
+      <c r="F122" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G122" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H122" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I122" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="J122" s="13"/>
+      <c r="K122" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L122" s="13"/>
+    </row>
+    <row r="123" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B123" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="C123" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="75"/>
+      <c r="E123" s="76"/>
+      <c r="F123" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G123" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I123" s="8" t="s">
+        <v>753</v>
+      </c>
+      <c r="J123" s="13"/>
+      <c r="K123" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L123" s="13"/>
+    </row>
+    <row r="124" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B124" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="C124" s="75" t="s">
+        <v>438</v>
+      </c>
+      <c r="D124" s="75"/>
+      <c r="E124" s="76"/>
+      <c r="F124" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G124" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H120" s="7" t="s">
+      <c r="H124" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I120" s="15" t="s">
+      <c r="I124" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J124" s="13"/>
+      <c r="K124" s="13"/>
+      <c r="L124" s="13"/>
+    </row>
+    <row r="125" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B125" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="C125" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="75"/>
+      <c r="E125" s="76"/>
+      <c r="F125" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G125" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I125" s="15" t="s">
         <v>755</v>
       </c>
-      <c r="J120" s="13"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
+      <c r="J125" s="13"/>
+      <c r="K125" s="13"/>
+      <c r="L125" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12054,8 +12204,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="80"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12092,8 +12242,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="89"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12130,8 +12280,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="79"/>
-      <c r="L4" s="81"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="89"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12166,8 +12316,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="79"/>
-      <c r="L5" s="81"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="89"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12204,10 +12354,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="87" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="84"/>
+      <c r="L6" s="92"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12244,8 +12394,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="79"/>
-      <c r="L7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12280,8 +12430,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="83"/>
-      <c r="L8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="94"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12318,10 +12468,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="95" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="89" t="s">
+      <c r="L9" s="90" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12360,8 +12510,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="88"/>
-      <c r="L10" s="81"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="89"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12398,8 +12548,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="88"/>
-      <c r="L11" s="81"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="89"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12678,7 +12828,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="82"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12716,7 +12866,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="83"/>
+      <c r="K19" s="86"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12754,10 +12904,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="87" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="89" t="s">
+      <c r="L20" s="90" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -12796,8 +12946,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="79"/>
-      <c r="L21" s="81"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="89"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -12832,8 +12982,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="81"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="89"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -12870,8 +13020,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="81"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="89"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -12908,8 +13058,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="79"/>
-      <c r="L24" s="81"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="89"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -12946,10 +13096,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="78" t="s">
+      <c r="K25" s="84" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="80" t="s">
+      <c r="L25" s="88" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -12988,8 +13138,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="79"/>
-      <c r="L26" s="81"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="89"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13026,8 +13176,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="79"/>
-      <c r="L27" s="81"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13062,8 +13212,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="83"/>
-      <c r="L28" s="90"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="91"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13100,7 +13250,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="82" t="s">
+      <c r="K29" s="87" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13140,7 +13290,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="79"/>
+      <c r="K30" s="85"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13178,7 +13328,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="79"/>
+      <c r="K31" s="85"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13214,7 +13364,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="79"/>
+      <c r="K32" s="85"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13252,7 +13402,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="78" t="s">
+      <c r="K33" s="84" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13294,7 +13444,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="83"/>
+      <c r="K34" s="86"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13332,7 +13482,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="82" t="s">
+      <c r="K35" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13374,7 +13524,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="79"/>
+      <c r="K36" s="85"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13491,7 +13641,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="80"/>
+      <c r="L39" s="88"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13529,7 +13679,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="81"/>
+      <c r="L40" s="89"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13608,10 +13758,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="82" t="s">
+      <c r="K42" s="87" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="89" t="s">
+      <c r="L42" s="90" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13650,8 +13800,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="79"/>
-      <c r="L43" s="81"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="89"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13688,8 +13838,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="81"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="89"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13724,8 +13874,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="81"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13762,8 +13912,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="81"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="89"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -13800,8 +13950,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="79"/>
-      <c r="L47" s="81"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="89"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -13918,7 +14068,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="91" t="s">
+      <c r="K50" s="78" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -13958,7 +14108,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="88"/>
+      <c r="K51" s="79"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -13996,7 +14146,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="88"/>
+      <c r="K52" s="79"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14034,7 +14184,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="88"/>
+      <c r="K53" s="79"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14070,7 +14220,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="92"/>
+      <c r="K54" s="80"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14190,7 +14340,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="82" t="s">
+      <c r="K57" s="87" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14230,7 +14380,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="79"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14266,7 +14416,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="79"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14304,7 +14454,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="80" t="s">
+      <c r="K60" s="88" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14344,7 +14494,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="81"/>
+      <c r="K61" s="89"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14384,7 +14534,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="81"/>
+      <c r="K62" s="89"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14424,7 +14574,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="82"/>
+      <c r="K63" s="87"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14462,7 +14612,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="79"/>
+      <c r="K64" s="85"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14500,7 +14650,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="79"/>
+      <c r="K65" s="85"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14538,7 +14688,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="79"/>
+      <c r="K66" s="85"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14652,7 +14802,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="82" t="s">
+      <c r="K69" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14694,7 +14844,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="79"/>
+      <c r="K70" s="85"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14772,7 +14922,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="82"/>
+      <c r="K72" s="87"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -14808,7 +14958,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="79"/>
+      <c r="K73" s="85"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -14844,7 +14994,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="79"/>
+      <c r="K74" s="85"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -14878,7 +15028,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="83"/>
+      <c r="K75" s="86"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -14956,10 +15106,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="91" t="s">
+      <c r="K77" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="78" t="s">
+      <c r="L77" s="84" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15000,8 +15150,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="92"/>
-      <c r="L78" s="93"/>
+      <c r="K78" s="80"/>
+      <c r="L78" s="82"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15041,7 +15191,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="93"/>
+      <c r="L79" s="82"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15081,7 +15231,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="83"/>
+      <c r="L80" s="86"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15118,7 +15268,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="82" t="s">
+      <c r="K81" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15160,7 +15310,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="79"/>
+      <c r="K82" s="85"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15282,7 +15432,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="82" t="s">
+      <c r="K85" s="87" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15322,7 +15472,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="79"/>
+      <c r="K86" s="85"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15360,7 +15510,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="79"/>
+      <c r="K87" s="85"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15396,7 +15546,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="79"/>
+      <c r="K88" s="85"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15434,7 +15584,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="79"/>
+      <c r="K89" s="85"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15472,7 +15622,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="79"/>
+      <c r="K90" s="85"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15510,10 +15660,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="91" t="s">
+      <c r="K91" s="78" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="94" t="s">
+      <c r="L91" s="81" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15552,8 +15702,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="88"/>
-      <c r="L92" s="93"/>
+      <c r="K92" s="79"/>
+      <c r="L92" s="82"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15590,8 +15740,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="88"/>
-      <c r="L93" s="93"/>
+      <c r="K93" s="79"/>
+      <c r="L93" s="82"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15626,8 +15776,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="92"/>
-      <c r="L94" s="95"/>
+      <c r="K94" s="80"/>
+      <c r="L94" s="83"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15664,7 +15814,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="78"/>
+      <c r="K95" s="84"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15702,7 +15852,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="79"/>
+      <c r="K96" s="85"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15740,7 +15890,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="79"/>
+      <c r="K97" s="85"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15778,7 +15928,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="79"/>
+      <c r="K98" s="85"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -15814,7 +15964,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="83"/>
+      <c r="K99" s="86"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -15843,6 +15993,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15851,28 +16023,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed SpecificConductance because simplified with different string preprocessing
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FFC9DD3-F616-49AE-BD3E-BCF744600BD1}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C01F9768-6DA0-4585-8537-B6A7DEEC3F0F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Annie_Comments" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$74</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">GLENDA_Map!$B$1:$M$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Key!$A$1:$A$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">NCCA_Map!$A$1:$A$57</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3707" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="804">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2136,9 +2136,6 @@
   </si>
   <si>
     <t>Uncorrected conductivity</t>
-  </si>
-  <si>
-    <t>Specific.Conductance</t>
   </si>
   <si>
     <t>Probably just want specific conductance?</t>
@@ -3027,35 +3024,11 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3063,10 +3036,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3080,6 +3053,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3406,16 +3403,16 @@
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>756</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>757</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3429,7 +3426,7 @@
         <v>281</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>42</v>
@@ -3440,13 +3437,13 @@
         <v>347</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>22</v>
@@ -3457,13 +3454,13 @@
         <v>465</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>22</v>
@@ -3474,13 +3471,13 @@
         <v>469</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>42</v>
@@ -3491,13 +3488,13 @@
         <v>473</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>42</v>
@@ -3508,13 +3505,13 @@
         <v>620</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
@@ -3525,13 +3522,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>42</v>
@@ -3548,7 +3545,7 @@
         <v>282</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -3559,13 +3556,13 @@
         <v>93</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>227</v>
@@ -3582,7 +3579,7 @@
         <v>281</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>42</v>
@@ -3593,13 +3590,13 @@
         <v>506</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>42</v>
@@ -3610,13 +3607,13 @@
         <v>507</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>42</v>
@@ -3627,13 +3624,13 @@
         <v>509</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>22</v>
@@ -3644,13 +3641,13 @@
         <v>511</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>22</v>
@@ -3661,13 +3658,13 @@
         <v>515</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>233</v>
@@ -3678,13 +3675,13 @@
         <v>517</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>22</v>
@@ -3695,13 +3692,13 @@
         <v>63</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>22</v>
@@ -3712,13 +3709,13 @@
         <v>55</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>22</v>
@@ -3729,13 +3726,13 @@
         <v>538</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>539</v>
@@ -3746,13 +3743,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>22</v>
@@ -3763,13 +3760,13 @@
         <v>204</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>42</v>
@@ -3780,13 +3777,13 @@
         <v>486</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>42</v>
@@ -3797,13 +3794,13 @@
         <v>478</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>539</v>
@@ -3814,13 +3811,13 @@
         <v>269</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>22</v>
@@ -3831,13 +3828,13 @@
         <v>223</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>42</v>
@@ -3851,13 +3848,13 @@
         <v>83</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3865,13 +3862,13 @@
         <v>66</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>22</v>
@@ -3882,13 +3879,13 @@
         <v>59</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>22</v>
@@ -3899,13 +3896,13 @@
         <v>572</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>539</v>
@@ -3916,13 +3913,13 @@
         <v>77</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>22</v>
@@ -3933,13 +3930,13 @@
         <v>232</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>233</v>
@@ -3950,13 +3947,13 @@
         <v>574</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>42</v>
@@ -3967,13 +3964,13 @@
         <v>575</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>42</v>
@@ -3990,7 +3987,7 @@
         <v>318</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>318</v>
@@ -4001,13 +3998,13 @@
         <v>588</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>22</v>
@@ -4018,13 +4015,13 @@
         <v>356</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>42</v>
@@ -4035,13 +4032,13 @@
         <v>594</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>42</v>
@@ -4052,13 +4049,13 @@
         <v>595</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>42</v>
@@ -4069,13 +4066,13 @@
         <v>95</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>42</v>
@@ -4086,13 +4083,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>22</v>
@@ -4109,7 +4106,7 @@
         <v>326</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>326</v>
@@ -4120,13 +4117,13 @@
         <v>612</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>276</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>276</v>
@@ -4137,13 +4134,13 @@
         <v>609</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>277</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>277</v>
@@ -8177,10 +8174,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L125"/>
+  <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9212,7 +9209,7 @@
         <v>684</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -9298,7 +9295,7 @@
         <v>684</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -9316,10 +9313,10 @@
         <v>280</v>
       </c>
       <c r="J38" s="13" t="s">
+        <v>691</v>
+      </c>
+      <c r="K38" s="13" t="s">
         <v>692</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>693</v>
       </c>
       <c r="L38" s="13"/>
     </row>
@@ -9328,7 +9325,7 @@
         <v>684</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>691</v>
+        <v>242</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -9337,28 +9334,28 @@
         <v>2021</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>93</v>
+        <v>268</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="L39" s="13"/>
     </row>
-    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -9367,7 +9364,7 @@
         <v>2021</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>268</v>
@@ -9376,94 +9373,94 @@
         <v>280</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K40" s="13" t="s">
         <v>695</v>
       </c>
       <c r="L40" s="13"/>
     </row>
-    <row r="41" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="B41" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="23">
-        <v>2021</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H41" s="7" t="s">
+      <c r="F41" s="71"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I41" s="13" t="s">
         <v>280</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="L41" s="13"/>
     </row>
-    <row r="42" spans="1:12" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>697</v>
-      </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13" t="s">
+      <c r="B42" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="13" t="s">
+        <v>643</v>
+      </c>
+      <c r="F42" s="23">
+        <v>2015</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="I42" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>698</v>
-      </c>
+      <c r="I42" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="J42" s="13"/>
       <c r="K42" s="13" t="s">
-        <v>696</v>
+        <v>644</v>
       </c>
       <c r="L42" s="13"/>
     </row>
-    <row r="43" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>224</v>
+        <v>802</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="13" t="s">
-        <v>643</v>
-      </c>
+      <c r="E43" s="13"/>
       <c r="F43" s="23">
-        <v>2015</v>
-      </c>
-      <c r="G43" s="8"/>
+        <v>2021</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>698</v>
+      </c>
       <c r="H43" s="20" t="s">
         <v>268</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="J43" s="13"/>
+        <v>280</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>699</v>
+      </c>
       <c r="K43" s="13" t="s">
-        <v>644</v>
+        <v>700</v>
       </c>
       <c r="L43" s="13"/>
     </row>
@@ -9481,7 +9478,7 @@
         <v>2021</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H44" s="20" t="s">
         <v>268</v>
@@ -9490,10 +9487,10 @@
         <v>280</v>
       </c>
       <c r="J44" s="13" t="s">
+        <v>699</v>
+      </c>
+      <c r="K44" s="13" t="s">
         <v>700</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>701</v>
       </c>
       <c r="L44" s="13"/>
     </row>
@@ -9502,7 +9499,7 @@
         <v>684</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>804</v>
+        <v>244</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -9511,19 +9508,19 @@
         <v>2021</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>699</v>
-      </c>
-      <c r="H45" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>268</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J45" s="13" t="s">
+        <v>699</v>
+      </c>
+      <c r="K45" s="13" t="s">
         <v>700</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>701</v>
       </c>
       <c r="L45" s="13"/>
     </row>
@@ -9532,7 +9529,7 @@
         <v>684</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -9541,7 +9538,7 @@
         <v>2021</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>268</v>
@@ -9550,19 +9547,19 @@
         <v>280</v>
       </c>
       <c r="J46" s="13" t="s">
+        <v>699</v>
+      </c>
+      <c r="K46" s="13" t="s">
         <v>700</v>
       </c>
-      <c r="K46" s="13" t="s">
-        <v>701</v>
-      </c>
       <c r="L46" s="13"/>
     </row>
-    <row r="47" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>245</v>
+        <v>369</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -9571,20 +9568,16 @@
         <v>2021</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>699</v>
-      </c>
-      <c r="H47" s="7" t="s">
-        <v>268</v>
+        <v>231</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J47" s="13" t="s">
-        <v>700</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>701</v>
-      </c>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
       <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9592,7 +9585,7 @@
         <v>684</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>369</v>
+        <v>701</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -9603,7 +9596,7 @@
       <c r="G48" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H48" s="20" t="s">
+      <c r="H48" s="7" t="s">
         <v>232</v>
       </c>
       <c r="I48" s="8" t="s">
@@ -9627,15 +9620,17 @@
         <v>2021</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>231</v>
+        <v>703</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J49" s="13"/>
+      <c r="J49" s="13" t="s">
+        <v>704</v>
+      </c>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
     </row>
@@ -9644,7 +9639,7 @@
         <v>684</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -9653,7 +9648,7 @@
         <v>2021</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>268</v>
@@ -9662,7 +9657,7 @@
         <v>280</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
@@ -9672,7 +9667,7 @@
         <v>684</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -9681,7 +9676,7 @@
         <v>2021</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>268</v>
@@ -9690,7 +9685,7 @@
         <v>280</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
@@ -9700,7 +9695,7 @@
         <v>684</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -9709,7 +9704,7 @@
         <v>2021</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>709</v>
+        <v>13</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>268</v>
@@ -9718,7 +9713,7 @@
         <v>280</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
@@ -9737,7 +9732,7 @@
         <v>2021</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>13</v>
+        <v>708</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>268</v>
@@ -9746,7 +9741,7 @@
         <v>280</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
@@ -9756,7 +9751,7 @@
         <v>684</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>711</v>
+        <v>328</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -9765,16 +9760,16 @@
         <v>2021</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>709</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>268</v>
+        <v>277</v>
+      </c>
+      <c r="H54" s="20" t="s">
+        <v>609</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
@@ -9784,7 +9779,7 @@
         <v>684</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>328</v>
+        <v>711</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -9793,16 +9788,16 @@
         <v>2021</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="H55" s="20" t="s">
-        <v>609</v>
+        <v>712</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
@@ -9812,7 +9807,7 @@
         <v>684</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>712</v>
+        <v>83</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -9821,26 +9816,24 @@
         <v>2021</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>713</v>
+        <v>13</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J56" s="13" t="s">
-        <v>705</v>
-      </c>
+      <c r="J56" s="13"/>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
     </row>
-    <row r="57" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>83</v>
+        <v>713</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -9849,24 +9842,26 @@
         <v>2021</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>13</v>
+        <v>714</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>83</v>
+        <v>268</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J57" s="13"/>
-      <c r="K57" s="13"/>
+      <c r="K57" s="13" t="s">
+        <v>715</v>
+      </c>
       <c r="L57" s="13"/>
     </row>
-    <row r="58" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>714</v>
+        <v>247</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -9875,7 +9870,7 @@
         <v>2021</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>268</v>
@@ -9884,9 +9879,7 @@
         <v>280</v>
       </c>
       <c r="J58" s="13"/>
-      <c r="K58" s="13" t="s">
-        <v>716</v>
-      </c>
+      <c r="K58" s="13"/>
       <c r="L58" s="13"/>
     </row>
     <row r="59" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9894,7 +9887,7 @@
         <v>684</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -9903,7 +9896,7 @@
         <v>2021</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>268</v>
@@ -9920,7 +9913,7 @@
         <v>684</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -9929,7 +9922,7 @@
         <v>2021</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>268</v>
@@ -9946,7 +9939,7 @@
         <v>684</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -9955,7 +9948,7 @@
         <v>2021</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>268</v>
@@ -9972,7 +9965,7 @@
         <v>684</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -9981,7 +9974,7 @@
         <v>2021</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>717</v>
+        <v>253</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>268</v>
@@ -9998,7 +9991,7 @@
         <v>684</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -10007,7 +10000,7 @@
         <v>2021</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>253</v>
+        <v>716</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>268</v>
@@ -10024,7 +10017,7 @@
         <v>684</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -10033,7 +10026,7 @@
         <v>2021</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>717</v>
+        <v>231</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>268</v>
@@ -10050,7 +10043,7 @@
         <v>684</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>255</v>
+        <v>717</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -10059,7 +10052,7 @@
         <v>2021</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>231</v>
+        <v>318</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>268</v>
@@ -10085,7 +10078,7 @@
         <v>2021</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>318</v>
+        <v>719</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>268</v>
@@ -10102,7 +10095,7 @@
         <v>684</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -10111,7 +10104,7 @@
         <v>2021</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>720</v>
+        <v>13</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>268</v>
@@ -10119,16 +10112,18 @@
       <c r="I67" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J67" s="13"/>
+      <c r="J67" s="13" t="s">
+        <v>721</v>
+      </c>
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
     </row>
-    <row r="68" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>721</v>
+        <v>327</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -10137,7 +10132,7 @@
         <v>2021</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>13</v>
+        <v>719</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>268</v>
@@ -10156,7 +10151,7 @@
         <v>684</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>327</v>
+        <v>256</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -10165,7 +10160,7 @@
         <v>2021</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>268</v>
@@ -10173,9 +10168,7 @@
       <c r="I69" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J69" s="13" t="s">
-        <v>723</v>
-      </c>
+      <c r="J69" s="13"/>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
     </row>
@@ -10184,7 +10177,7 @@
         <v>684</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -10193,7 +10186,7 @@
         <v>2021</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>724</v>
+        <v>259</v>
       </c>
       <c r="H70" s="7" t="s">
         <v>268</v>
@@ -10201,8 +10194,12 @@
       <c r="I70" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
+      <c r="J70" s="13" t="s">
+        <v>724</v>
+      </c>
+      <c r="K70" s="13" t="s">
+        <v>725</v>
+      </c>
       <c r="L70" s="13"/>
     </row>
     <row r="71" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10210,7 +10207,7 @@
         <v>684</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
@@ -10219,7 +10216,7 @@
         <v>2021</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>259</v>
+        <v>726</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>268</v>
@@ -10227,12 +10224,8 @@
       <c r="I71" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J71" s="13" t="s">
-        <v>725</v>
-      </c>
-      <c r="K71" s="13" t="s">
-        <v>726</v>
-      </c>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
       <c r="L71" s="13"/>
     </row>
     <row r="72" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10240,7 +10233,7 @@
         <v>684</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
@@ -10249,7 +10242,7 @@
         <v>2021</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>268</v>
@@ -10266,7 +10259,7 @@
         <v>684</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -10275,7 +10268,7 @@
         <v>2021</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H73" s="7" t="s">
         <v>268</v>
@@ -10292,7 +10285,7 @@
         <v>684</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -10301,7 +10294,7 @@
         <v>2021</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H74" s="7" t="s">
         <v>268</v>
@@ -10315,64 +10308,66 @@
     </row>
     <row r="75" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>684</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>264</v>
+        <v>727</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>202</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="23">
+      <c r="E75" s="69"/>
+      <c r="F75" s="70">
         <v>2021</v>
       </c>
-      <c r="G75" s="8" t="s">
-        <v>727</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I75" s="8" t="s">
+      <c r="G75" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="H75" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I75" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
+      <c r="J75" s="41" t="s">
+        <v>728</v>
+      </c>
+      <c r="K75" s="41"/>
       <c r="L75" s="13"/>
     </row>
     <row r="76" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>728</v>
-      </c>
-      <c r="B76" s="39" t="s">
-        <v>202</v>
+        <v>727</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="70">
+      <c r="E76" s="71"/>
+      <c r="F76" s="23">
         <v>2021</v>
       </c>
-      <c r="G76" s="39" t="s">
+      <c r="G76" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H76" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="I76" s="39" t="s">
+      <c r="H76" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I76" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J76" s="41" t="s">
+      <c r="J76" s="13" t="s">
         <v>729</v>
       </c>
-      <c r="K76" s="41"/>
+      <c r="K76" s="13"/>
       <c r="L76" s="13"/>
     </row>
     <row r="77" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
@@ -10384,7 +10379,7 @@
         <v>42</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>88</v>
+        <v>574</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>280</v>
@@ -10397,10 +10392,10 @@
     </row>
     <row r="78" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
@@ -10412,7 +10407,7 @@
         <v>42</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>574</v>
+        <v>506</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>280</v>
@@ -10425,10 +10420,10 @@
     </row>
     <row r="79" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>203</v>
+        <v>732</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -10437,26 +10432,26 @@
         <v>2021</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>506</v>
+        <v>347</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>733</v>
+        <v>49</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -10468,7 +10463,7 @@
         <v>211</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>347</v>
+        <v>269</v>
       </c>
       <c r="I80" s="8" t="s">
         <v>280</v>
@@ -10481,10 +10476,10 @@
     </row>
     <row r="81" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>49</v>
+        <v>201</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
@@ -10493,10 +10488,10 @@
         <v>2021</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>269</v>
+        <v>594</v>
       </c>
       <c r="I81" s="8" t="s">
         <v>280</v>
@@ -10509,10 +10504,10 @@
     </row>
     <row r="82" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>201</v>
+        <v>736</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
@@ -10524,23 +10519,23 @@
         <v>42</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>594</v>
+        <v>95</v>
       </c>
       <c r="I82" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
     </row>
     <row r="83" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>737</v>
+        <v>31</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
@@ -10549,26 +10544,26 @@
         <v>2021</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>42</v>
+        <v>212</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="I83" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>738</v>
+        <v>31</v>
       </c>
       <c r="K83" s="13"/>
       <c r="L83" s="13"/>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>31</v>
+        <v>180</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -10577,26 +10572,26 @@
         <v>2021</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>212</v>
+        <v>738</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>31</v>
+        <v>356</v>
       </c>
       <c r="I84" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>31</v>
+        <v>739</v>
       </c>
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
     </row>
     <row r="85" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
@@ -10605,10 +10600,10 @@
         <v>2021</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>739</v>
+        <v>211</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>356</v>
+        <v>72</v>
       </c>
       <c r="I85" s="8" t="s">
         <v>280</v>
@@ -10621,10 +10616,10 @@
     </row>
     <row r="86" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
@@ -10633,59 +10628,63 @@
         <v>2021</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
     </row>
     <row r="87" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
-      <c r="E87" s="71"/>
+      <c r="E87" s="13" t="s">
+        <v>741</v>
+      </c>
       <c r="F87" s="23">
         <v>2021</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>212</v>
+        <v>42</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>77</v>
+        <v>268</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>741</v>
-      </c>
-      <c r="K87" s="13"/>
+        <v>742</v>
+      </c>
+      <c r="K87" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L87" s="13"/>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="13" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F88" s="23">
         <v>2021</v>
@@ -10700,7 +10699,7 @@
         <v>280</v>
       </c>
       <c r="J88" s="13" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="K88" s="13" t="s">
         <v>599</v>
@@ -10709,59 +10708,55 @@
     </row>
     <row r="89" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
-      <c r="E89" s="13" t="s">
-        <v>742</v>
-      </c>
+      <c r="E89" s="71"/>
       <c r="F89" s="23">
         <v>2021</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H89" s="7" t="s">
-        <v>268</v>
+        <v>22</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J89" s="13" t="s">
-        <v>743</v>
-      </c>
-      <c r="K89" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
       <c r="L89" s="13"/>
     </row>
     <row r="90" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>728</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="71"/>
-      <c r="F90" s="23">
-        <v>2021</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H90" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I90" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" s="72" t="s">
+        <v>452</v>
+      </c>
+      <c r="D90" s="72"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="74">
+        <v>2010</v>
+      </c>
+      <c r="G90" s="72" t="s">
+        <v>198</v>
+      </c>
+      <c r="H90" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I90" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J90" s="13"/>
+      <c r="J90" s="41"/>
       <c r="K90" s="13"/>
       <c r="L90" s="13"/>
     </row>
@@ -10769,27 +10764,27 @@
       <c r="A91" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B91" s="72" t="s">
+      <c r="B91" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="C91" s="72" t="s">
-        <v>452</v>
-      </c>
-      <c r="D91" s="72"/>
-      <c r="E91" s="73"/>
-      <c r="F91" s="74">
+      <c r="C91" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="75"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="77">
         <v>2010</v>
       </c>
-      <c r="G91" s="72" t="s">
+      <c r="G91" s="75" t="s">
         <v>198</v>
       </c>
       <c r="H91" s="39" t="s">
         <v>469</v>
       </c>
-      <c r="I91" s="39" t="s">
+      <c r="I91" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J91" s="41"/>
+      <c r="J91" s="13"/>
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
     </row>
@@ -10798,10 +10793,10 @@
         <v>119</v>
       </c>
       <c r="B92" s="75" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C92" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D92" s="75"/>
       <c r="E92" s="76"/>
@@ -10811,8 +10806,8 @@
       <c r="G92" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="H92" s="39" t="s">
-        <v>469</v>
+      <c r="H92" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>280</v>
@@ -10826,7 +10821,7 @@
         <v>119</v>
       </c>
       <c r="B93" s="75" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C93" s="75" t="s">
         <v>452</v>
@@ -10840,7 +10835,7 @@
         <v>198</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>88</v>
+        <v>204</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>280</v>
@@ -10857,7 +10852,7 @@
         <v>204</v>
       </c>
       <c r="C94" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D94" s="75"/>
       <c r="E94" s="76"/>
@@ -10882,10 +10877,10 @@
         <v>119</v>
       </c>
       <c r="B95" s="75" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C95" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D95" s="75"/>
       <c r="E95" s="76"/>
@@ -10896,7 +10891,7 @@
         <v>198</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>204</v>
+        <v>574</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>280</v>
@@ -10913,7 +10908,7 @@
         <v>200</v>
       </c>
       <c r="C96" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D96" s="75"/>
       <c r="E96" s="76"/>
@@ -10938,10 +10933,10 @@
         <v>119</v>
       </c>
       <c r="B97" s="75" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C97" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D97" s="75"/>
       <c r="E97" s="76"/>
@@ -10952,7 +10947,7 @@
         <v>198</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>574</v>
+        <v>506</v>
       </c>
       <c r="I97" s="8" t="s">
         <v>280</v>
@@ -10969,7 +10964,7 @@
         <v>203</v>
       </c>
       <c r="C98" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D98" s="75"/>
       <c r="E98" s="76"/>
@@ -10994,10 +10989,10 @@
         <v>119</v>
       </c>
       <c r="B99" s="75" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C99" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D99" s="75"/>
       <c r="E99" s="76"/>
@@ -11005,10 +11000,10 @@
         <v>2010</v>
       </c>
       <c r="G99" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>506</v>
+        <v>347</v>
       </c>
       <c r="I99" s="8" t="s">
         <v>280</v>
@@ -11025,7 +11020,7 @@
         <v>193</v>
       </c>
       <c r="C100" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D100" s="75"/>
       <c r="E100" s="76"/>
@@ -11050,10 +11045,10 @@
         <v>119</v>
       </c>
       <c r="B101" s="75" t="s">
-        <v>193</v>
+        <v>49</v>
       </c>
       <c r="C101" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D101" s="75"/>
       <c r="E101" s="76"/>
@@ -11064,7 +11059,7 @@
         <v>194</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>347</v>
+        <v>269</v>
       </c>
       <c r="I101" s="8" t="s">
         <v>280</v>
@@ -11081,7 +11076,7 @@
         <v>49</v>
       </c>
       <c r="C102" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D102" s="75"/>
       <c r="E102" s="76"/>
@@ -11106,10 +11101,10 @@
         <v>119</v>
       </c>
       <c r="B103" s="75" t="s">
-        <v>49</v>
+        <v>201</v>
       </c>
       <c r="C103" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D103" s="75"/>
       <c r="E103" s="76"/>
@@ -11117,10 +11112,10 @@
         <v>2010</v>
       </c>
       <c r="G103" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>269</v>
+        <v>594</v>
       </c>
       <c r="I103" s="8" t="s">
         <v>280</v>
@@ -11137,7 +11132,7 @@
         <v>201</v>
       </c>
       <c r="C104" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D104" s="75"/>
       <c r="E104" s="76"/>
@@ -11162,10 +11157,10 @@
         <v>119</v>
       </c>
       <c r="B105" s="75" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C105" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D105" s="75"/>
       <c r="E105" s="76"/>
@@ -11173,17 +11168,23 @@
         <v>2010</v>
       </c>
       <c r="G105" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>594</v>
-      </c>
-      <c r="I105" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="H105" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="I105" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="J105" s="13" t="s">
+        <v>744</v>
+      </c>
+      <c r="K105" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="L105" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="106" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
@@ -11193,7 +11194,7 @@
         <v>209</v>
       </c>
       <c r="C106" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D106" s="75"/>
       <c r="E106" s="76"/>
@@ -11207,10 +11208,10 @@
         <v>620</v>
       </c>
       <c r="I106" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="J106" s="13" t="s">
         <v>744</v>
-      </c>
-      <c r="J106" s="13" t="s">
-        <v>745</v>
       </c>
       <c r="K106" s="13" t="s">
         <v>746</v>
@@ -11224,10 +11225,10 @@
         <v>119</v>
       </c>
       <c r="B107" s="75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D107" s="75"/>
       <c r="E107" s="76"/>
@@ -11238,16 +11239,16 @@
         <v>194</v>
       </c>
       <c r="H107" s="15" t="s">
-        <v>620</v>
+        <v>55</v>
       </c>
       <c r="I107" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J107" s="13" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="K107" s="13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L107" s="13" t="s">
         <v>397</v>
@@ -11261,7 +11262,7 @@
         <v>208</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D108" s="75"/>
       <c r="E108" s="76"/>
@@ -11275,13 +11276,13 @@
         <v>55</v>
       </c>
       <c r="I108" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="K108" s="13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L108" s="13" t="s">
         <v>397</v>
@@ -11292,10 +11293,10 @@
         <v>119</v>
       </c>
       <c r="B109" s="75" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C109" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D109" s="75"/>
       <c r="E109" s="76"/>
@@ -11306,16 +11307,16 @@
         <v>194</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I109" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J109" s="13" t="s">
         <v>748</v>
       </c>
       <c r="K109" s="13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L109" s="13" t="s">
         <v>397</v>
@@ -11329,7 +11330,7 @@
         <v>210</v>
       </c>
       <c r="C110" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D110" s="75"/>
       <c r="E110" s="76"/>
@@ -11343,13 +11344,13 @@
         <v>59</v>
       </c>
       <c r="I110" s="15" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J110" s="13" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="K110" s="13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="L110" s="13" t="s">
         <v>397</v>
@@ -11360,10 +11361,10 @@
         <v>119</v>
       </c>
       <c r="B111" s="75" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C111" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D111" s="75"/>
       <c r="E111" s="76"/>
@@ -11371,30 +11372,24 @@
         <v>2010</v>
       </c>
       <c r="G111" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H111" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I111" s="15" t="s">
-        <v>744</v>
-      </c>
-      <c r="J111" s="13" t="s">
-        <v>749</v>
-      </c>
-      <c r="K111" s="13" t="s">
-        <v>747</v>
-      </c>
-      <c r="L111" s="13" t="s">
-        <v>397</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I111" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
     </row>
     <row r="112" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B112" s="75" t="s">
-        <v>199</v>
+        <v>31</v>
       </c>
       <c r="C112" s="75" t="s">
         <v>452</v>
@@ -11405,10 +11400,10 @@
         <v>2010</v>
       </c>
       <c r="G112" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="I112" s="8" t="s">
         <v>280</v>
@@ -11425,7 +11420,7 @@
         <v>31</v>
       </c>
       <c r="C113" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D113" s="75"/>
       <c r="E113" s="76"/>
@@ -11450,10 +11445,10 @@
         <v>119</v>
       </c>
       <c r="B114" s="75" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="C114" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D114" s="75"/>
       <c r="E114" s="76"/>
@@ -11461,10 +11456,10 @@
         <v>2010</v>
       </c>
       <c r="G114" s="75" t="s">
-        <v>194</v>
+        <v>749</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="I114" s="8" t="s">
         <v>280</v>
@@ -11481,7 +11476,7 @@
         <v>319</v>
       </c>
       <c r="C115" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D115" s="75"/>
       <c r="E115" s="76"/>
@@ -11489,7 +11484,7 @@
         <v>2010</v>
       </c>
       <c r="G115" s="75" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>319</v>
@@ -11506,10 +11501,10 @@
         <v>119</v>
       </c>
       <c r="B116" s="75" t="s">
-        <v>319</v>
+        <v>180</v>
       </c>
       <c r="C116" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D116" s="75"/>
       <c r="E116" s="76"/>
@@ -11517,15 +11512,17 @@
         <v>2010</v>
       </c>
       <c r="G116" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="I116" s="8" t="s">
         <v>750</v>
       </c>
-      <c r="H116" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="I116" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J116" s="13"/>
+      <c r="J116" s="13" t="s">
+        <v>751</v>
+      </c>
       <c r="K116" s="13"/>
       <c r="L116" s="13"/>
     </row>
@@ -11534,10 +11531,10 @@
         <v>119</v>
       </c>
       <c r="B117" s="75" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C117" s="75" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="D117" s="75"/>
       <c r="E117" s="76"/>
@@ -11545,17 +11542,15 @@
         <v>2010</v>
       </c>
       <c r="G117" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>356</v>
+        <v>72</v>
       </c>
       <c r="I117" s="8" t="s">
-        <v>751</v>
-      </c>
-      <c r="J117" s="13" t="s">
-        <v>752</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="J117" s="13"/>
       <c r="K117" s="13"/>
       <c r="L117" s="13"/>
     </row>
@@ -11564,7 +11559,7 @@
         <v>119</v>
       </c>
       <c r="B118" s="75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C118" s="75" t="s">
         <v>438</v>
@@ -11578,7 +11573,7 @@
         <v>194</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I118" s="8" t="s">
         <v>280</v>
@@ -11592,7 +11587,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="75" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C119" s="75" t="s">
         <v>438</v>
@@ -11603,16 +11598,20 @@
         <v>2010</v>
       </c>
       <c r="G119" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>77</v>
+        <v>268</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
+        <v>752</v>
+      </c>
+      <c r="J119" s="13" t="s">
+        <v>753</v>
+      </c>
+      <c r="K119" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L119" s="13"/>
     </row>
     <row r="120" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11623,7 +11622,7 @@
         <v>205</v>
       </c>
       <c r="C120" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D120" s="75"/>
       <c r="E120" s="76"/>
@@ -11637,11 +11636,9 @@
         <v>268</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>753</v>
-      </c>
-      <c r="J120" s="13" t="s">
-        <v>754</v>
-      </c>
+        <v>752</v>
+      </c>
+      <c r="J120" s="13"/>
       <c r="K120" s="13" t="s">
         <v>599</v>
       </c>
@@ -11652,10 +11649,10 @@
         <v>119</v>
       </c>
       <c r="B121" s="75" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C121" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D121" s="75"/>
       <c r="E121" s="76"/>
@@ -11669,7 +11666,7 @@
         <v>268</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J121" s="13"/>
       <c r="K121" s="13" t="s">
@@ -11685,7 +11682,7 @@
         <v>206</v>
       </c>
       <c r="C122" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D122" s="75"/>
       <c r="E122" s="76"/>
@@ -11699,7 +11696,7 @@
         <v>268</v>
       </c>
       <c r="I122" s="8" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J122" s="13"/>
       <c r="K122" s="13" t="s">
@@ -11712,10 +11709,10 @@
         <v>119</v>
       </c>
       <c r="B123" s="75" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C123" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D123" s="75"/>
       <c r="E123" s="76"/>
@@ -11723,18 +11720,16 @@
         <v>2010</v>
       </c>
       <c r="G123" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>268</v>
+        <v>23</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>753</v>
+        <v>280</v>
       </c>
       <c r="J123" s="13"/>
-      <c r="K123" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="K123" s="13"/>
       <c r="L123" s="13"/>
     </row>
     <row r="124" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11745,7 +11740,7 @@
         <v>207</v>
       </c>
       <c r="C124" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D124" s="75"/>
       <c r="E124" s="76"/>
@@ -11758,40 +11753,12 @@
       <c r="H124" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I124" s="8" t="s">
-        <v>280</v>
+      <c r="I124" s="15" t="s">
+        <v>754</v>
       </c>
       <c r="J124" s="13"/>
       <c r="K124" s="13"/>
       <c r="L124" s="13"/>
-    </row>
-    <row r="125" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B125" s="75" t="s">
-        <v>207</v>
-      </c>
-      <c r="C125" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D125" s="75"/>
-      <c r="E125" s="76"/>
-      <c r="F125" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G125" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H125" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I125" s="15" t="s">
-        <v>755</v>
-      </c>
-      <c r="J125" s="13"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12204,8 +12171,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="88"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="80"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12242,8 +12209,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="89"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="81"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12280,8 +12247,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="89"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="81"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12316,8 +12283,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="89"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="81"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12354,10 +12321,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="82" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="92"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12394,8 +12361,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="85"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="85"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12430,8 +12397,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="86"/>
-      <c r="L8" s="94"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12468,10 +12435,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="95" t="s">
+      <c r="K9" s="87" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="90" t="s">
+      <c r="L9" s="89" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12510,8 +12477,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="79"/>
-      <c r="L10" s="89"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12548,8 +12515,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="79"/>
-      <c r="L11" s="89"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12828,7 +12795,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="87"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12866,7 +12833,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="86"/>
+      <c r="K19" s="83"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12904,10 +12871,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="87" t="s">
+      <c r="K20" s="82" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="90" t="s">
+      <c r="L20" s="89" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -12946,8 +12913,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="85"/>
-      <c r="L21" s="89"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -12982,8 +12949,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="85"/>
-      <c r="L22" s="89"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -13020,8 +12987,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="85"/>
-      <c r="L23" s="89"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -13058,8 +13025,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="85"/>
-      <c r="L24" s="89"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -13096,10 +13063,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="84" t="s">
+      <c r="K25" s="78" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="88" t="s">
+      <c r="L25" s="80" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -13138,8 +13105,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="85"/>
-      <c r="L26" s="89"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13176,8 +13143,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="85"/>
-      <c r="L27" s="89"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13212,8 +13179,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="86"/>
-      <c r="L28" s="91"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="90"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13250,7 +13217,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="87" t="s">
+      <c r="K29" s="82" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13290,7 +13257,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="85"/>
+      <c r="K30" s="79"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13328,7 +13295,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="85"/>
+      <c r="K31" s="79"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13364,7 +13331,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="85"/>
+      <c r="K32" s="79"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13402,7 +13369,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="84" t="s">
+      <c r="K33" s="78" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13444,7 +13411,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="86"/>
+      <c r="K34" s="83"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13482,7 +13449,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="87" t="s">
+      <c r="K35" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13524,7 +13491,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="85"/>
+      <c r="K36" s="79"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13641,7 +13608,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="88"/>
+      <c r="L39" s="80"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13679,7 +13646,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="89"/>
+      <c r="L40" s="81"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13758,10 +13725,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="87" t="s">
+      <c r="K42" s="82" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="L42" s="89" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13800,8 +13767,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="85"/>
-      <c r="L43" s="89"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="81"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13838,8 +13805,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="85"/>
-      <c r="L44" s="89"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="81"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13874,8 +13841,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="85"/>
-      <c r="L45" s="89"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="81"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13912,8 +13879,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="85"/>
-      <c r="L46" s="89"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="81"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -13950,8 +13917,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="85"/>
-      <c r="L47" s="89"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -14068,7 +14035,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="78" t="s">
+      <c r="K50" s="91" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -14108,7 +14075,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="79"/>
+      <c r="K51" s="88"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -14146,7 +14113,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="79"/>
+      <c r="K52" s="88"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14184,7 +14151,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="79"/>
+      <c r="K53" s="88"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14220,7 +14187,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="80"/>
+      <c r="K54" s="92"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14340,7 +14307,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="87" t="s">
+      <c r="K57" s="82" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14380,7 +14347,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="85"/>
+      <c r="K58" s="79"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14416,7 +14383,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="85"/>
+      <c r="K59" s="79"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14454,7 +14421,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="88" t="s">
+      <c r="K60" s="80" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14494,7 +14461,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="89"/>
+      <c r="K61" s="81"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14534,7 +14501,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="89"/>
+      <c r="K62" s="81"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14574,7 +14541,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="87"/>
+      <c r="K63" s="82"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14612,7 +14579,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="85"/>
+      <c r="K64" s="79"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14650,7 +14617,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="85"/>
+      <c r="K65" s="79"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14688,7 +14655,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="85"/>
+      <c r="K66" s="79"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14802,7 +14769,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="87" t="s">
+      <c r="K69" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14844,7 +14811,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="85"/>
+      <c r="K70" s="79"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14922,7 +14889,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="87"/>
+      <c r="K72" s="82"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -14958,7 +14925,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="85"/>
+      <c r="K73" s="79"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -14994,7 +14961,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="85"/>
+      <c r="K74" s="79"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -15028,7 +14995,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="86"/>
+      <c r="K75" s="83"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -15106,10 +15073,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="78" t="s">
+      <c r="K77" s="91" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="84" t="s">
+      <c r="L77" s="78" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15150,8 +15117,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="80"/>
-      <c r="L78" s="82"/>
+      <c r="K78" s="92"/>
+      <c r="L78" s="94"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15191,7 +15158,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="82"/>
+      <c r="L79" s="94"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15231,7 +15198,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="86"/>
+      <c r="L80" s="83"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15268,7 +15235,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="87" t="s">
+      <c r="K81" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15310,7 +15277,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="85"/>
+      <c r="K82" s="79"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15432,7 +15399,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="87" t="s">
+      <c r="K85" s="82" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15472,7 +15439,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="85"/>
+      <c r="K86" s="79"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15510,7 +15477,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="85"/>
+      <c r="K87" s="79"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15546,7 +15513,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="85"/>
+      <c r="K88" s="79"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15584,7 +15551,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="85"/>
+      <c r="K89" s="79"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15622,7 +15589,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="85"/>
+      <c r="K90" s="79"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15660,10 +15627,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="78" t="s">
+      <c r="K91" s="91" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="81" t="s">
+      <c r="L91" s="93" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15702,8 +15669,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="79"/>
-      <c r="L92" s="82"/>
+      <c r="K92" s="88"/>
+      <c r="L92" s="94"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15740,8 +15707,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="79"/>
-      <c r="L93" s="82"/>
+      <c r="K93" s="88"/>
+      <c r="L93" s="94"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15776,8 +15743,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="80"/>
-      <c r="L94" s="83"/>
+      <c r="K94" s="92"/>
+      <c r="L94" s="95"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15814,7 +15781,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="84"/>
+      <c r="K95" s="78"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15852,7 +15819,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="85"/>
+      <c r="K96" s="79"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15890,7 +15857,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="85"/>
+      <c r="K97" s="79"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15928,7 +15895,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="85"/>
+      <c r="K98" s="79"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -15964,7 +15931,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="86"/>
+      <c r="K99" s="83"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -15993,28 +15960,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -16023,6 +15968,28 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Re-added line for % to percent in UnitConversions
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C01F9768-6DA0-4585-8537-B6A7DEEC3F0F}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DDA6596-DEE3-4BA8-AD39-615D0F9B15AA}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="804">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -3024,11 +3024,35 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3036,10 +3060,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3053,30 +3077,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8176,7 +8176,7 @@
   </sheetPr>
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
@@ -12171,8 +12171,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="80"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12209,8 +12209,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="89"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12247,8 +12247,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="79"/>
-      <c r="L4" s="81"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="89"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12283,8 +12283,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="79"/>
-      <c r="L5" s="81"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="89"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12321,10 +12321,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="87" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="84"/>
+      <c r="L6" s="92"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12361,8 +12361,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="79"/>
-      <c r="L7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12397,8 +12397,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="83"/>
-      <c r="L8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="94"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12435,10 +12435,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="95" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="89" t="s">
+      <c r="L9" s="90" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12477,8 +12477,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="88"/>
-      <c r="L10" s="81"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="89"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12515,8 +12515,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="88"/>
-      <c r="L11" s="81"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="89"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12795,7 +12795,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="82"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12833,7 +12833,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="83"/>
+      <c r="K19" s="86"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12871,10 +12871,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="87" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="89" t="s">
+      <c r="L20" s="90" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -12913,8 +12913,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="79"/>
-      <c r="L21" s="81"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="89"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -12949,8 +12949,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="81"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="89"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -12987,8 +12987,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="81"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="89"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -13025,8 +13025,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="79"/>
-      <c r="L24" s="81"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="89"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -13063,10 +13063,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="78" t="s">
+      <c r="K25" s="84" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="80" t="s">
+      <c r="L25" s="88" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -13105,8 +13105,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="79"/>
-      <c r="L26" s="81"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="89"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13143,8 +13143,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="79"/>
-      <c r="L27" s="81"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13179,8 +13179,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="83"/>
-      <c r="L28" s="90"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="91"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13217,7 +13217,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="82" t="s">
+      <c r="K29" s="87" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13257,7 +13257,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="79"/>
+      <c r="K30" s="85"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13295,7 +13295,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="79"/>
+      <c r="K31" s="85"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13331,7 +13331,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="79"/>
+      <c r="K32" s="85"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13369,7 +13369,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="78" t="s">
+      <c r="K33" s="84" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13411,7 +13411,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="83"/>
+      <c r="K34" s="86"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13449,7 +13449,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="82" t="s">
+      <c r="K35" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13491,7 +13491,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="79"/>
+      <c r="K36" s="85"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13608,7 +13608,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="80"/>
+      <c r="L39" s="88"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="81"/>
+      <c r="L40" s="89"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13725,10 +13725,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="82" t="s">
+      <c r="K42" s="87" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="89" t="s">
+      <c r="L42" s="90" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13767,8 +13767,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="79"/>
-      <c r="L43" s="81"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="89"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13805,8 +13805,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="81"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="89"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13841,8 +13841,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="81"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13879,8 +13879,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="81"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="89"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -13917,8 +13917,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="79"/>
-      <c r="L47" s="81"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="89"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -14035,7 +14035,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="91" t="s">
+      <c r="K50" s="78" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -14075,7 +14075,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="88"/>
+      <c r="K51" s="79"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -14113,7 +14113,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="88"/>
+      <c r="K52" s="79"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14151,7 +14151,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="88"/>
+      <c r="K53" s="79"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14187,7 +14187,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="92"/>
+      <c r="K54" s="80"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14307,7 +14307,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="82" t="s">
+      <c r="K57" s="87" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14347,7 +14347,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="79"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14383,7 +14383,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="79"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14421,7 +14421,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="80" t="s">
+      <c r="K60" s="88" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14461,7 +14461,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="81"/>
+      <c r="K61" s="89"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14501,7 +14501,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="81"/>
+      <c r="K62" s="89"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14541,7 +14541,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="82"/>
+      <c r="K63" s="87"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14579,7 +14579,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="79"/>
+      <c r="K64" s="85"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14617,7 +14617,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="79"/>
+      <c r="K65" s="85"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14655,7 +14655,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="79"/>
+      <c r="K66" s="85"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14769,7 +14769,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="82" t="s">
+      <c r="K69" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14811,7 +14811,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="79"/>
+      <c r="K70" s="85"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14889,7 +14889,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="82"/>
+      <c r="K72" s="87"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -14925,7 +14925,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="79"/>
+      <c r="K73" s="85"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -14961,7 +14961,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="79"/>
+      <c r="K74" s="85"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -14995,7 +14995,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="83"/>
+      <c r="K75" s="86"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -15073,10 +15073,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="91" t="s">
+      <c r="K77" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="78" t="s">
+      <c r="L77" s="84" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15117,8 +15117,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="92"/>
-      <c r="L78" s="94"/>
+      <c r="K78" s="80"/>
+      <c r="L78" s="82"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15158,7 +15158,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="94"/>
+      <c r="L79" s="82"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15198,7 +15198,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="83"/>
+      <c r="L80" s="86"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15235,7 +15235,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="82" t="s">
+      <c r="K81" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15277,7 +15277,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="79"/>
+      <c r="K82" s="85"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15399,7 +15399,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="82" t="s">
+      <c r="K85" s="87" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15439,7 +15439,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="79"/>
+      <c r="K86" s="85"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15477,7 +15477,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="79"/>
+      <c r="K87" s="85"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15513,7 +15513,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="79"/>
+      <c r="K88" s="85"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15551,7 +15551,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="79"/>
+      <c r="K89" s="85"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15589,7 +15589,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="79"/>
+      <c r="K90" s="85"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15627,10 +15627,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="91" t="s">
+      <c r="K91" s="78" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="93" t="s">
+      <c r="L91" s="81" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15669,8 +15669,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="88"/>
-      <c r="L92" s="94"/>
+      <c r="K92" s="79"/>
+      <c r="L92" s="82"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15707,8 +15707,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="88"/>
-      <c r="L93" s="94"/>
+      <c r="K93" s="79"/>
+      <c r="L93" s="82"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15743,8 +15743,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="92"/>
-      <c r="L94" s="95"/>
+      <c r="K94" s="80"/>
+      <c r="L94" s="83"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15781,7 +15781,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="78"/>
+      <c r="K95" s="84"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15819,7 +15819,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="79"/>
+      <c r="K96" s="85"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15857,7 +15857,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="79"/>
+      <c r="K97" s="85"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15895,7 +15895,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="79"/>
+      <c r="K98" s="85"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -15931,7 +15931,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="83"/>
+      <c r="K99" s="86"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -15960,6 +15960,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15968,28 +15990,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20398,9 +20398,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20455,86 +20457,87 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" s="27">
-        <v>1E-3</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="A4" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="23">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>13</v>
+        <v>282</v>
+      </c>
+      <c r="C5" s="27">
+        <v>1E-3</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="C6" s="23">
-        <v>1000</v>
+        <v>276</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>283</v>
+        <v>194</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C7" s="23">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>286</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>194</v>
+        <v>283</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C8" s="23">
         <v>1</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>288</v>
+        <v>194</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" s="23">
         <v>1</v>
@@ -20547,7 +20550,7 @@
         <v>288</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C10" s="23">
         <v>1</v>
@@ -20557,10 +20560,10 @@
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>198</v>
+        <v>288</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C11" s="23">
         <v>1</v>
@@ -20570,10 +20573,10 @@
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C12" s="23">
         <v>1</v>
@@ -20583,39 +20586,39 @@
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C13" s="27">
-        <v>1E-3</v>
+        <v>291</v>
+      </c>
+      <c r="C13" s="23">
+        <v>1</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>284</v>
+        <v>198</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="C14" s="23">
-        <v>1</v>
+        <v>194</v>
+      </c>
+      <c r="C14" s="27">
+        <v>1E-3</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C15" s="23">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -20625,7 +20628,7 @@
         <v>194</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>198</v>
+        <v>293</v>
       </c>
       <c r="C16" s="23">
         <v>1000</v>
@@ -20635,23 +20638,23 @@
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>294</v>
+        <v>194</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>295</v>
+        <v>198</v>
       </c>
       <c r="C17" s="23">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="23">
         <v>1</v>
@@ -20664,10 +20667,10 @@
         <v>284</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C19" s="23">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -20677,7 +20680,7 @@
         <v>284</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C20" s="23">
         <v>1000</v>
@@ -20687,10 +20690,10 @@
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C21" s="23">
         <v>1000</v>
@@ -20700,23 +20703,23 @@
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>300</v>
+        <v>194</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C22" s="23">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>194</v>
+        <v>300</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="C23" s="23">
         <v>1</v>
@@ -20729,7 +20732,7 @@
         <v>194</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C24" s="23">
         <v>1</v>
@@ -20739,18 +20742,31 @@
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C25" s="23">
         <v>1</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" s="23">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed analyte names for csmi 2021 water chem
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DDA6596-DEE3-4BA8-AD39-615D0F9B15AA}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC01310B-AD51-451A-8A3D-A62B81AA7DBD}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="802">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2261,9 +2261,6 @@
     <t>Dissolved magnesium</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>dissolved ammonium</t>
   </si>
   <si>
@@ -2271,9 +2268,6 @@
   </si>
   <si>
     <t>Dissolved sodium</t>
-  </si>
-  <si>
-    <t>SO</t>
   </si>
   <si>
     <t>Dissolved sulfate</t>
@@ -3024,35 +3018,11 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3060,10 +3030,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3077,6 +3047,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3385,7 +3379,7 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -3403,16 +3397,16 @@
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3426,7 +3420,7 @@
         <v>281</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>42</v>
@@ -3437,13 +3431,13 @@
         <v>347</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>22</v>
@@ -3454,13 +3448,13 @@
         <v>465</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>22</v>
@@ -3471,13 +3465,13 @@
         <v>469</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>42</v>
@@ -3488,13 +3482,13 @@
         <v>473</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>42</v>
@@ -3505,13 +3499,13 @@
         <v>620</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
@@ -3522,13 +3516,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>42</v>
@@ -3545,7 +3539,7 @@
         <v>282</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -3556,13 +3550,13 @@
         <v>93</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>227</v>
@@ -3579,7 +3573,7 @@
         <v>281</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>42</v>
@@ -3590,13 +3584,13 @@
         <v>506</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>42</v>
@@ -3607,13 +3601,13 @@
         <v>507</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>42</v>
@@ -3624,13 +3618,13 @@
         <v>509</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>22</v>
@@ -3641,13 +3635,13 @@
         <v>511</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>22</v>
@@ -3658,13 +3652,13 @@
         <v>515</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>233</v>
@@ -3675,13 +3669,13 @@
         <v>517</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>22</v>
@@ -3692,13 +3686,13 @@
         <v>63</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>22</v>
@@ -3709,13 +3703,13 @@
         <v>55</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>22</v>
@@ -3726,13 +3720,13 @@
         <v>538</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>539</v>
@@ -3743,13 +3737,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>22</v>
@@ -3760,13 +3754,13 @@
         <v>204</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>42</v>
@@ -3777,13 +3771,13 @@
         <v>486</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>42</v>
@@ -3794,13 +3788,13 @@
         <v>478</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>539</v>
@@ -3811,13 +3805,13 @@
         <v>269</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>22</v>
@@ -3828,13 +3822,13 @@
         <v>223</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>42</v>
@@ -3848,13 +3842,13 @@
         <v>83</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3862,13 +3856,13 @@
         <v>66</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>22</v>
@@ -3879,13 +3873,13 @@
         <v>59</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>22</v>
@@ -3896,13 +3890,13 @@
         <v>572</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>539</v>
@@ -3913,13 +3907,13 @@
         <v>77</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>22</v>
@@ -3930,13 +3924,13 @@
         <v>232</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>233</v>
@@ -3947,13 +3941,13 @@
         <v>574</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>42</v>
@@ -3964,13 +3958,13 @@
         <v>575</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>42</v>
@@ -3987,7 +3981,7 @@
         <v>318</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>318</v>
@@ -3998,13 +3992,13 @@
         <v>588</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>22</v>
@@ -4015,13 +4009,13 @@
         <v>356</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>42</v>
@@ -4032,13 +4026,13 @@
         <v>594</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>42</v>
@@ -4049,13 +4043,13 @@
         <v>595</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>42</v>
@@ -4066,13 +4060,13 @@
         <v>95</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>42</v>
@@ -4083,13 +4077,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>22</v>
@@ -4106,7 +4100,7 @@
         <v>326</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>326</v>
@@ -4117,13 +4111,13 @@
         <v>612</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>276</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>276</v>
@@ -4134,13 +4128,13 @@
         <v>609</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>277</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>277</v>
@@ -4544,7 +4538,7 @@
   </sheetPr>
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A32" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8176,8 +8170,8 @@
   </sheetPr>
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9209,7 +9203,7 @@
         <v>684</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -9295,7 +9289,7 @@
         <v>684</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -9439,7 +9433,7 @@
         <v>684</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -9469,7 +9463,7 @@
         <v>684</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -10423,7 +10417,7 @@
         <v>727</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>732</v>
+        <v>193</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -10441,7 +10435,7 @@
         <v>280</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
@@ -10469,7 +10463,7 @@
         <v>280</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
@@ -10497,7 +10491,7 @@
         <v>280</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
@@ -10507,7 +10501,7 @@
         <v>727</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>736</v>
+        <v>199</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
@@ -10525,7 +10519,7 @@
         <v>280</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
@@ -10572,7 +10566,7 @@
         <v>2021</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H84" s="7" t="s">
         <v>356</v>
@@ -10581,7 +10575,7 @@
         <v>280</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
@@ -10609,7 +10603,7 @@
         <v>280</v>
       </c>
       <c r="J85" s="13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
@@ -10637,7 +10631,7 @@
         <v>280</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
@@ -10652,7 +10646,7 @@
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F87" s="23">
         <v>2021</v>
@@ -10667,7 +10661,7 @@
         <v>280</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K87" s="13" t="s">
         <v>599</v>
@@ -10684,7 +10678,7 @@
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="13" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F88" s="23">
         <v>2021</v>
@@ -10699,7 +10693,7 @@
         <v>280</v>
       </c>
       <c r="J88" s="13" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="K88" s="13" t="s">
         <v>599</v>
@@ -11174,13 +11168,13 @@
         <v>620</v>
       </c>
       <c r="I105" s="15" t="s">
+        <v>741</v>
+      </c>
+      <c r="J105" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="K105" s="13" t="s">
         <v>743</v>
-      </c>
-      <c r="J105" s="13" t="s">
-        <v>744</v>
-      </c>
-      <c r="K105" s="13" t="s">
-        <v>745</v>
       </c>
       <c r="L105" s="13" t="s">
         <v>397</v>
@@ -11208,13 +11202,13 @@
         <v>620</v>
       </c>
       <c r="I106" s="15" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J106" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="K106" s="13" t="s">
         <v>744</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>746</v>
       </c>
       <c r="L106" s="13" t="s">
         <v>397</v>
@@ -11242,13 +11236,13 @@
         <v>55</v>
       </c>
       <c r="I107" s="15" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J107" s="13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="K107" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L107" s="13" t="s">
         <v>397</v>
@@ -11276,13 +11270,13 @@
         <v>55</v>
       </c>
       <c r="I108" s="15" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J108" s="13" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="K108" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L108" s="13" t="s">
         <v>397</v>
@@ -11310,13 +11304,13 @@
         <v>59</v>
       </c>
       <c r="I109" s="15" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J109" s="13" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="K109" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L109" s="13" t="s">
         <v>397</v>
@@ -11344,13 +11338,13 @@
         <v>59</v>
       </c>
       <c r="I110" s="15" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J110" s="13" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="K110" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L110" s="13" t="s">
         <v>397</v>
@@ -11456,7 +11450,7 @@
         <v>2010</v>
       </c>
       <c r="G114" s="75" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>319</v>
@@ -11484,7 +11478,7 @@
         <v>2010</v>
       </c>
       <c r="G115" s="75" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>319</v>
@@ -11518,10 +11512,10 @@
         <v>356</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J116" s="13" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="K116" s="13"/>
       <c r="L116" s="13"/>
@@ -11604,10 +11598,10 @@
         <v>268</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J119" s="13" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="K119" s="13" t="s">
         <v>599</v>
@@ -11636,7 +11630,7 @@
         <v>268</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J120" s="13"/>
       <c r="K120" s="13" t="s">
@@ -11666,7 +11660,7 @@
         <v>268</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J121" s="13"/>
       <c r="K121" s="13" t="s">
@@ -11696,7 +11690,7 @@
         <v>268</v>
       </c>
       <c r="I122" s="8" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J122" s="13"/>
       <c r="K122" s="13" t="s">
@@ -11754,7 +11748,7 @@
         <v>23</v>
       </c>
       <c r="I124" s="15" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J124" s="13"/>
       <c r="K124" s="13"/>
@@ -12171,8 +12165,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="88"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="80"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12209,8 +12203,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="89"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="81"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12247,8 +12241,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="89"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="81"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12283,8 +12277,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="89"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="81"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12321,10 +12315,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="82" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="92"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12361,8 +12355,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="85"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="85"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12397,8 +12391,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="86"/>
-      <c r="L8" s="94"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12435,10 +12429,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="95" t="s">
+      <c r="K9" s="87" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="90" t="s">
+      <c r="L9" s="89" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12477,8 +12471,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="79"/>
-      <c r="L10" s="89"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12515,8 +12509,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="79"/>
-      <c r="L11" s="89"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12795,7 +12789,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="87"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12833,7 +12827,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="86"/>
+      <c r="K19" s="83"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12871,10 +12865,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="87" t="s">
+      <c r="K20" s="82" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="90" t="s">
+      <c r="L20" s="89" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -12913,8 +12907,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="85"/>
-      <c r="L21" s="89"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -12949,8 +12943,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="85"/>
-      <c r="L22" s="89"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -12987,8 +12981,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="85"/>
-      <c r="L23" s="89"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -13025,8 +13019,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="85"/>
-      <c r="L24" s="89"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -13063,10 +13057,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="84" t="s">
+      <c r="K25" s="78" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="88" t="s">
+      <c r="L25" s="80" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -13105,8 +13099,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="85"/>
-      <c r="L26" s="89"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13143,8 +13137,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="85"/>
-      <c r="L27" s="89"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13179,8 +13173,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="86"/>
-      <c r="L28" s="91"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="90"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13217,7 +13211,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="87" t="s">
+      <c r="K29" s="82" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13257,7 +13251,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="85"/>
+      <c r="K30" s="79"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13295,7 +13289,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="85"/>
+      <c r="K31" s="79"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13331,7 +13325,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="85"/>
+      <c r="K32" s="79"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13369,7 +13363,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="84" t="s">
+      <c r="K33" s="78" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13411,7 +13405,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="86"/>
+      <c r="K34" s="83"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13449,7 +13443,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="87" t="s">
+      <c r="K35" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13491,7 +13485,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="85"/>
+      <c r="K36" s="79"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13608,7 +13602,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="88"/>
+      <c r="L39" s="80"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13646,7 +13640,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="89"/>
+      <c r="L40" s="81"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13725,10 +13719,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="87" t="s">
+      <c r="K42" s="82" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="L42" s="89" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13767,8 +13761,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="85"/>
-      <c r="L43" s="89"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="81"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13805,8 +13799,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="85"/>
-      <c r="L44" s="89"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="81"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13841,8 +13835,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="85"/>
-      <c r="L45" s="89"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="81"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13879,8 +13873,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="85"/>
-      <c r="L46" s="89"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="81"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -13917,8 +13911,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="85"/>
-      <c r="L47" s="89"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -14035,7 +14029,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="78" t="s">
+      <c r="K50" s="91" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -14075,7 +14069,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="79"/>
+      <c r="K51" s="88"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -14113,7 +14107,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="79"/>
+      <c r="K52" s="88"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14151,7 +14145,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="79"/>
+      <c r="K53" s="88"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14187,7 +14181,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="80"/>
+      <c r="K54" s="92"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14307,7 +14301,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="87" t="s">
+      <c r="K57" s="82" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14347,7 +14341,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="85"/>
+      <c r="K58" s="79"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14383,7 +14377,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="85"/>
+      <c r="K59" s="79"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14421,7 +14415,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="88" t="s">
+      <c r="K60" s="80" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14461,7 +14455,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="89"/>
+      <c r="K61" s="81"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14501,7 +14495,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="89"/>
+      <c r="K62" s="81"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14541,7 +14535,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="87"/>
+      <c r="K63" s="82"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14579,7 +14573,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="85"/>
+      <c r="K64" s="79"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14617,7 +14611,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="85"/>
+      <c r="K65" s="79"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14655,7 +14649,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="85"/>
+      <c r="K66" s="79"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14769,7 +14763,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="87" t="s">
+      <c r="K69" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14811,7 +14805,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="85"/>
+      <c r="K70" s="79"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14889,7 +14883,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="87"/>
+      <c r="K72" s="82"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -14925,7 +14919,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="85"/>
+      <c r="K73" s="79"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -14961,7 +14955,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="85"/>
+      <c r="K74" s="79"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -14995,7 +14989,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="86"/>
+      <c r="K75" s="83"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -15073,10 +15067,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="78" t="s">
+      <c r="K77" s="91" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="84" t="s">
+      <c r="L77" s="78" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15117,8 +15111,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="80"/>
-      <c r="L78" s="82"/>
+      <c r="K78" s="92"/>
+      <c r="L78" s="94"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15158,7 +15152,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="82"/>
+      <c r="L79" s="94"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15198,7 +15192,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="86"/>
+      <c r="L80" s="83"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15235,7 +15229,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="87" t="s">
+      <c r="K81" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15277,7 +15271,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="85"/>
+      <c r="K82" s="79"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15399,7 +15393,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="87" t="s">
+      <c r="K85" s="82" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15439,7 +15433,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="85"/>
+      <c r="K86" s="79"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15477,7 +15471,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="85"/>
+      <c r="K87" s="79"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15513,7 +15507,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="85"/>
+      <c r="K88" s="79"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15551,7 +15545,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="85"/>
+      <c r="K89" s="79"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15589,7 +15583,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="85"/>
+      <c r="K90" s="79"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15627,10 +15621,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="78" t="s">
+      <c r="K91" s="91" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="81" t="s">
+      <c r="L91" s="93" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15669,8 +15663,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="79"/>
-      <c r="L92" s="82"/>
+      <c r="K92" s="88"/>
+      <c r="L92" s="94"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15707,8 +15701,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="79"/>
-      <c r="L93" s="82"/>
+      <c r="K93" s="88"/>
+      <c r="L93" s="94"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15743,8 +15737,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="80"/>
-      <c r="L94" s="83"/>
+      <c r="K94" s="92"/>
+      <c r="L94" s="95"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15781,7 +15775,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="84"/>
+      <c r="K95" s="78"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15819,7 +15813,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="85"/>
+      <c r="K96" s="79"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15857,7 +15851,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="85"/>
+      <c r="K97" s="79"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15895,7 +15889,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="85"/>
+      <c r="K98" s="79"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -15931,7 +15925,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="86"/>
+      <c r="K99" s="83"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -15960,28 +15954,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15990,6 +15962,28 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20400,7 +20394,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Differentiated USGS 2021 CSMI CTD par names from EPA to avoid mapping mistakes
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC01310B-AD51-451A-8A3D-A62B81AA7DBD}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DACD712-8B8A-4774-9D3A-B8E3A322D6CD}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Annie_Comments" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">CSMI_Map!$H$1:$H$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">GLENDA_Map!$B$1:$M$99</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Key!$A$1:$A$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">NCCA_Map!$A$1:$A$57</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="815">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2231,9 +2231,6 @@
     <t>This one is for Fluoremeter, which we are not using</t>
   </si>
   <si>
-    <t>Note: there are 2 temps - probably remove this one from Sequoia</t>
-  </si>
-  <si>
     <t>μm</t>
   </si>
   <si>
@@ -2462,13 +2459,55 @@
     <t>SpecificConductance</t>
   </si>
   <si>
-    <t>Oxy</t>
-  </si>
-  <si>
-    <t>CDOM</t>
-  </si>
-  <si>
-    <t>PAR</t>
+    <t>USGS DO</t>
+  </si>
+  <si>
+    <t>USGS fluorescence</t>
+  </si>
+  <si>
+    <t>USGS PAR from CTD</t>
+  </si>
+  <si>
+    <t>USGS turbidity - NTU. EPA doesn't seem to have turbidity.</t>
+  </si>
+  <si>
+    <t>This is USGS specific conductivity. Incorrectly mapped to remove due to copy/paste from EPA. Likely should have dealt with these by giving own study ID</t>
+  </si>
+  <si>
+    <t>USGS CDOM. Removing because only present in USGS CSMI 2021 CTD</t>
+  </si>
+  <si>
+    <t>Manually added for mapping USGS and EPA cpar</t>
+  </si>
+  <si>
+    <t>EPA temp. Note: there are 2 temps -  remove this one from Sequoia. Need to differentiate from USGS Temp</t>
+  </si>
+  <si>
+    <t>Cond_USGS</t>
+  </si>
+  <si>
+    <t>CDOM_USGS</t>
+  </si>
+  <si>
+    <t>PAR_USGS</t>
+  </si>
+  <si>
+    <t>Temp_USGS</t>
+  </si>
+  <si>
+    <t>Oxy_USGS</t>
+  </si>
+  <si>
+    <t>pH_USGS</t>
+  </si>
+  <si>
+    <t>cpar_USGS</t>
+  </si>
+  <si>
+    <t>Manually added for mapping USGS cpar</t>
+  </si>
+  <si>
+    <t>Turbidity_USGS</t>
   </si>
 </sst>
 </file>
@@ -3018,11 +3057,35 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3030,10 +3093,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3047,30 +3110,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3379,7 +3418,7 @@
   </sheetPr>
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -3397,16 +3436,16 @@
         <v>5</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>753</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>754</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3420,7 +3459,7 @@
         <v>281</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>42</v>
@@ -3431,13 +3470,13 @@
         <v>347</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>22</v>
@@ -3448,13 +3487,13 @@
         <v>465</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>22</v>
@@ -3465,13 +3504,13 @@
         <v>469</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>42</v>
@@ -3482,13 +3521,13 @@
         <v>473</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>42</v>
@@ -3499,13 +3538,13 @@
         <v>620</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
@@ -3516,13 +3555,13 @@
         <v>88</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>42</v>
@@ -3539,7 +3578,7 @@
         <v>282</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -3550,13 +3589,13 @@
         <v>93</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>284</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>227</v>
@@ -3573,7 +3612,7 @@
         <v>281</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>42</v>
@@ -3584,13 +3623,13 @@
         <v>506</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>42</v>
@@ -3601,13 +3640,13 @@
         <v>507</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>42</v>
@@ -3618,13 +3657,13 @@
         <v>509</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>22</v>
@@ -3635,13 +3674,13 @@
         <v>511</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>22</v>
@@ -3652,13 +3691,13 @@
         <v>515</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>233</v>
@@ -3669,13 +3708,13 @@
         <v>517</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>22</v>
@@ -3686,13 +3725,13 @@
         <v>63</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>22</v>
@@ -3703,13 +3742,13 @@
         <v>55</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>22</v>
@@ -3720,13 +3759,13 @@
         <v>538</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>539</v>
@@ -3737,13 +3776,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>22</v>
@@ -3754,13 +3793,13 @@
         <v>204</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>42</v>
@@ -3771,13 +3810,13 @@
         <v>486</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>42</v>
@@ -3788,13 +3827,13 @@
         <v>478</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>539</v>
@@ -3805,13 +3844,13 @@
         <v>269</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>22</v>
@@ -3822,13 +3861,13 @@
         <v>223</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>42</v>
@@ -3842,13 +3881,13 @@
         <v>83</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3856,13 +3895,13 @@
         <v>66</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>22</v>
@@ -3873,13 +3912,13 @@
         <v>59</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>22</v>
@@ -3890,13 +3929,13 @@
         <v>572</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>279</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>539</v>
@@ -3907,13 +3946,13 @@
         <v>77</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>22</v>
@@ -3924,13 +3963,13 @@
         <v>232</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>233</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>233</v>
@@ -3941,13 +3980,13 @@
         <v>574</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>42</v>
@@ -3958,13 +3997,13 @@
         <v>575</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>42</v>
@@ -3981,7 +4020,7 @@
         <v>318</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>318</v>
@@ -3992,13 +4031,13 @@
         <v>588</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>22</v>
@@ -4009,13 +4048,13 @@
         <v>356</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>42</v>
@@ -4026,13 +4065,13 @@
         <v>594</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>42</v>
@@ -4043,13 +4082,13 @@
         <v>595</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>42</v>
@@ -4060,13 +4099,13 @@
         <v>95</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>281</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>42</v>
@@ -4077,13 +4116,13 @@
         <v>31</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>282</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>22</v>
@@ -4100,7 +4139,7 @@
         <v>326</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>326</v>
@@ -4111,13 +4150,13 @@
         <v>612</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>276</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>276</v>
@@ -4128,13 +4167,13 @@
         <v>609</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>277</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>277</v>
@@ -8168,10 +8207,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:XFD79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9172,7 +9211,7 @@
       </c>
       <c r="L33" s="13"/>
     </row>
-    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
         <v>684</v>
       </c>
@@ -9203,7 +9242,7 @@
         <v>684</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>799</v>
+        <v>240</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -9212,16 +9251,20 @@
         <v>2021</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
+      <c r="J35" s="13" t="s">
+        <v>689</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>690</v>
+      </c>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -9229,7 +9272,7 @@
         <v>684</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>93</v>
+        <v>797</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -9241,16 +9284,16 @@
         <v>227</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>268</v>
+        <v>93</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="L36" s="13"/>
     </row>
@@ -9259,7 +9302,7 @@
         <v>684</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -9268,7 +9311,7 @@
         <v>2021</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>268</v>
@@ -9277,19 +9320,19 @@
         <v>280</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="L37" s="13"/>
     </row>
-    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>798</v>
+        <v>243</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -9298,49 +9341,45 @@
         <v>2021</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>93</v>
+        <v>231</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="L38" s="13"/>
     </row>
-    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="B39" s="13" t="s">
+        <v>696</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
       <c r="E39" s="13"/>
-      <c r="F39" s="23">
-        <v>2021</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H39" s="7" t="s">
+      <c r="F39" s="71"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="13" t="s">
         <v>280</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="L39" s="13"/>
     </row>
@@ -9349,7 +9388,7 @@
         <v>684</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -9358,7 +9397,7 @@
         <v>2021</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>231</v>
+        <v>698</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>268</v>
@@ -9367,73 +9406,77 @@
         <v>280</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>693</v>
+        <v>699</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="L40" s="13"/>
     </row>
-    <row r="41" spans="1:12" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>684</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>696</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13" t="s">
+      <c r="F41" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="I41" s="13" t="s">
+      <c r="I41" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="L41" s="13"/>
     </row>
-    <row r="42" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>224</v>
+        <v>369</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="13" t="s">
-        <v>643</v>
-      </c>
+      <c r="E42" s="13"/>
       <c r="F42" s="23">
-        <v>2015</v>
-      </c>
-      <c r="G42" s="8"/>
+        <v>2021</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>231</v>
+      </c>
       <c r="H42" s="20" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13" t="s">
-        <v>644</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>804</v>
+      </c>
+      <c r="K42" s="13"/>
       <c r="L42" s="13"/>
     </row>
-    <row r="43" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>800</v>
+        <v>701</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -9442,28 +9485,24 @@
         <v>2021</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="H43" s="20" t="s">
-        <v>268</v>
+        <v>231</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J43" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>700</v>
-      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
       <c r="L43" s="13"/>
     </row>
-    <row r="44" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>801</v>
+        <v>702</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -9472,28 +9511,26 @@
         <v>2021</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="H44" s="20" t="s">
+        <v>703</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>268</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>700</v>
-      </c>
+        <v>704</v>
+      </c>
+      <c r="K44" s="13"/>
       <c r="L44" s="13"/>
     </row>
-    <row r="45" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>244</v>
+        <v>705</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -9502,7 +9539,7 @@
         <v>2021</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>698</v>
+        <v>706</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>268</v>
@@ -9511,19 +9548,17 @@
         <v>280</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>700</v>
-      </c>
+        <v>704</v>
+      </c>
+      <c r="K45" s="13"/>
       <c r="L45" s="13"/>
     </row>
-    <row r="46" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>245</v>
+        <v>707</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -9532,7 +9567,7 @@
         <v>2021</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>698</v>
+        <v>708</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>268</v>
@@ -9541,11 +9576,9 @@
         <v>280</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>700</v>
-      </c>
+        <v>704</v>
+      </c>
+      <c r="K46" s="13"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9553,7 +9586,7 @@
         <v>684</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>369</v>
+        <v>709</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -9562,15 +9595,17 @@
         <v>2021</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H47" s="20" t="s">
-        <v>232</v>
+        <v>13</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J47" s="13"/>
+      <c r="J47" s="13" t="s">
+        <v>704</v>
+      </c>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
     </row>
@@ -9579,7 +9614,7 @@
         <v>684</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>701</v>
+        <v>710</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -9588,15 +9623,17 @@
         <v>2021</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>231</v>
+        <v>708</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J48" s="13"/>
+      <c r="J48" s="13" t="s">
+        <v>704</v>
+      </c>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
     </row>
@@ -9605,7 +9642,7 @@
         <v>684</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -9614,7 +9651,7 @@
         <v>2021</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>268</v>
@@ -9633,7 +9670,7 @@
         <v>684</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>705</v>
+        <v>83</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -9642,26 +9679,24 @@
         <v>2021</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>706</v>
+        <v>13</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J50" s="13" t="s">
-        <v>704</v>
-      </c>
+      <c r="J50" s="13"/>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
     </row>
-    <row r="51" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>707</v>
+        <v>713</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -9670,7 +9705,7 @@
         <v>2021</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>268</v>
@@ -9678,10 +9713,10 @@
       <c r="I51" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J51" s="13" t="s">
-        <v>704</v>
-      </c>
-      <c r="K51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13" t="s">
+        <v>715</v>
+      </c>
       <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9689,7 +9724,7 @@
         <v>684</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>709</v>
+        <v>247</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -9698,7 +9733,7 @@
         <v>2021</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>13</v>
+        <v>716</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>268</v>
@@ -9706,9 +9741,7 @@
       <c r="I52" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J52" s="13" t="s">
-        <v>704</v>
-      </c>
+      <c r="J52" s="13"/>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
     </row>
@@ -9717,7 +9750,7 @@
         <v>684</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>710</v>
+        <v>249</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -9726,7 +9759,7 @@
         <v>2021</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>268</v>
@@ -9734,9 +9767,7 @@
       <c r="I53" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J53" s="13" t="s">
-        <v>704</v>
-      </c>
+      <c r="J53" s="13"/>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
     </row>
@@ -9745,7 +9776,7 @@
         <v>684</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>328</v>
+        <v>250</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -9754,17 +9785,15 @@
         <v>2021</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="H54" s="20" t="s">
-        <v>609</v>
+        <v>716</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J54" s="13" t="s">
-        <v>704</v>
-      </c>
+      <c r="J54" s="13"/>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
     </row>
@@ -9773,7 +9802,7 @@
         <v>684</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>711</v>
+        <v>251</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -9782,7 +9811,7 @@
         <v>2021</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>268</v>
@@ -9790,9 +9819,7 @@
       <c r="I55" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J55" s="13" t="s">
-        <v>704</v>
-      </c>
+      <c r="J55" s="13"/>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
     </row>
@@ -9801,7 +9828,7 @@
         <v>684</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -9810,10 +9837,10 @@
         <v>2021</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>13</v>
+        <v>253</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>83</v>
+        <v>268</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>280</v>
@@ -9822,12 +9849,12 @@
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
     </row>
-    <row r="57" spans="1:12" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>713</v>
+        <v>254</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -9836,7 +9863,7 @@
         <v>2021</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="H57" s="7" t="s">
         <v>268</v>
@@ -9845,9 +9872,7 @@
         <v>280</v>
       </c>
       <c r="J57" s="13"/>
-      <c r="K57" s="13" t="s">
-        <v>715</v>
-      </c>
+      <c r="K57" s="13"/>
       <c r="L57" s="13"/>
     </row>
     <row r="58" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9855,7 +9880,7 @@
         <v>684</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -9864,7 +9889,7 @@
         <v>2021</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>716</v>
+        <v>231</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>268</v>
@@ -9881,7 +9906,7 @@
         <v>684</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>249</v>
+        <v>717</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -9890,7 +9915,7 @@
         <v>2021</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>716</v>
+        <v>318</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>268</v>
@@ -9907,7 +9932,7 @@
         <v>684</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>250</v>
+        <v>718</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -9916,7 +9941,7 @@
         <v>2021</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>268</v>
@@ -9933,7 +9958,7 @@
         <v>684</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>251</v>
+        <v>720</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -9942,7 +9967,7 @@
         <v>2021</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>716</v>
+        <v>13</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>268</v>
@@ -9950,16 +9975,18 @@
       <c r="I61" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J61" s="13"/>
+      <c r="J61" s="13" t="s">
+        <v>721</v>
+      </c>
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
     </row>
-    <row r="62" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -9968,7 +9995,7 @@
         <v>2021</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>253</v>
+        <v>719</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>268</v>
@@ -9976,16 +10003,18 @@
       <c r="I62" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J62" s="13"/>
+      <c r="J62" s="13" t="s">
+        <v>805</v>
+      </c>
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
     </row>
-    <row r="63" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -9994,7 +10023,7 @@
         <v>2021</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>716</v>
+        <v>722</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>268</v>
@@ -10006,12 +10035,12 @@
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
     </row>
-    <row r="64" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -10020,7 +10049,7 @@
         <v>2021</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>268</v>
@@ -10028,16 +10057,20 @@
       <c r="I64" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
+      <c r="J64" s="13" t="s">
+        <v>723</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>724</v>
+      </c>
       <c r="L64" s="13"/>
     </row>
-    <row r="65" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>717</v>
+        <v>260</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -10046,7 +10079,7 @@
         <v>2021</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>318</v>
+        <v>725</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>268</v>
@@ -10058,12 +10091,12 @@
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
     </row>
-    <row r="66" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>718</v>
+        <v>262</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -10072,7 +10105,7 @@
         <v>2021</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>268</v>
@@ -10084,12 +10117,12 @@
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
     </row>
-    <row r="67" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>720</v>
+        <v>263</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -10098,7 +10131,7 @@
         <v>2021</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>13</v>
+        <v>725</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>268</v>
@@ -10106,9 +10139,7 @@
       <c r="I67" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J67" s="13" t="s">
-        <v>721</v>
-      </c>
+      <c r="J67" s="13"/>
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
     </row>
@@ -10117,7 +10148,7 @@
         <v>684</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>327</v>
+        <v>264</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -10126,7 +10157,7 @@
         <v>2021</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>268</v>
@@ -10134,18 +10165,16 @@
       <c r="I68" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J68" s="13" t="s">
-        <v>722</v>
-      </c>
+      <c r="J68" s="13"/>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
     </row>
-    <row r="69" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>256</v>
+        <v>651</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -10153,16 +10182,16 @@
       <c r="F69" s="23">
         <v>2021</v>
       </c>
-      <c r="G69" s="8" t="s">
-        <v>723</v>
-      </c>
-      <c r="H69" s="7" t="s">
+      <c r="G69" s="8"/>
+      <c r="H69" s="20" t="s">
         <v>268</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J69" s="13"/>
+        <v>437</v>
+      </c>
+      <c r="J69" s="13" t="s">
+        <v>799</v>
+      </c>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
     </row>
@@ -10171,7 +10200,7 @@
         <v>684</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>258</v>
+        <v>810</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -10180,20 +10209,18 @@
         <v>2021</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
       <c r="I70" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>724</v>
-      </c>
-      <c r="K70" s="13" t="s">
-        <v>725</v>
-      </c>
+        <v>798</v>
+      </c>
+      <c r="K70" s="13"/>
       <c r="L70" s="13"/>
     </row>
     <row r="71" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10201,7 +10228,7 @@
         <v>684</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>260</v>
+        <v>806</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
@@ -10210,15 +10237,17 @@
         <v>2021</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>726</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>268</v>
+        <v>227</v>
+      </c>
+      <c r="H71" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="I71" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J71" s="13"/>
+      <c r="J71" s="13" t="s">
+        <v>802</v>
+      </c>
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
     </row>
@@ -10227,7 +10256,7 @@
         <v>684</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>262</v>
+        <v>811</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
@@ -10235,25 +10264,21 @@
       <c r="F72" s="23">
         <v>2021</v>
       </c>
-      <c r="G72" s="8" t="s">
-        <v>726</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I72" s="8" t="s">
-        <v>280</v>
-      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I72" s="8"/>
       <c r="J72" s="13"/>
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
     </row>
-    <row r="73" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>263</v>
+        <v>814</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -10262,24 +10287,26 @@
         <v>2021</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>726</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>268</v>
+        <v>277</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>609</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J73" s="13"/>
+      <c r="J73" s="13" t="s">
+        <v>801</v>
+      </c>
       <c r="K73" s="13"/>
       <c r="L73" s="13"/>
     </row>
-    <row r="74" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
         <v>684</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>264</v>
+        <v>809</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -10287,137 +10314,129 @@
       <c r="F74" s="23">
         <v>2021</v>
       </c>
-      <c r="G74" s="8" t="s">
-        <v>726</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="I74" s="8" t="s">
-        <v>280</v>
-      </c>
+      <c r="G74" s="8"/>
+      <c r="H74" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="I74" s="8"/>
       <c r="J74" s="13"/>
       <c r="K74" s="13"/>
       <c r="L74" s="13"/>
     </row>
-    <row r="75" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>727</v>
-      </c>
-      <c r="B75" s="39" t="s">
-        <v>202</v>
+        <v>684</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>807</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="70">
+      <c r="E75" s="13"/>
+      <c r="F75" s="23">
         <v>2021</v>
       </c>
-      <c r="G75" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="H75" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="I75" s="39" t="s">
+      <c r="G75" s="8"/>
+      <c r="H75" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="I75" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J75" s="41" t="s">
-        <v>728</v>
-      </c>
-      <c r="K75" s="41"/>
+      <c r="J75" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="K75" s="13"/>
       <c r="L75" s="13"/>
     </row>
-    <row r="76" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>727</v>
+        <v>684</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>197</v>
+        <v>808</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
-      <c r="E76" s="71"/>
+      <c r="E76" s="13"/>
       <c r="F76" s="23">
         <v>2021</v>
       </c>
-      <c r="G76" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>88</v>
+      <c r="G76" s="8"/>
+      <c r="H76" s="20" t="s">
+        <v>268</v>
       </c>
       <c r="I76" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J76" s="13" t="s">
-        <v>729</v>
+        <v>800</v>
       </c>
       <c r="K76" s="13"/>
       <c r="L76" s="13"/>
     </row>
-    <row r="77" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>727</v>
+        <v>684</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>200</v>
+        <v>812</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
-      <c r="E77" s="71"/>
+      <c r="E77" s="13"/>
       <c r="F77" s="23">
         <v>2021</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>574</v>
+        <v>231</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J77" s="13" t="s">
-        <v>730</v>
+        <v>813</v>
       </c>
       <c r="K77" s="13"/>
       <c r="L77" s="13"/>
     </row>
     <row r="78" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>727</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>203</v>
+        <v>726</v>
+      </c>
+      <c r="B78" s="39" t="s">
+        <v>202</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
-      <c r="E78" s="71"/>
-      <c r="F78" s="23">
+      <c r="E78" s="69"/>
+      <c r="F78" s="70">
         <v>2021</v>
       </c>
-      <c r="G78" s="8" t="s">
+      <c r="G78" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="H78" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="I78" s="8" t="s">
+      <c r="H78" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I78" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J78" s="13" t="s">
-        <v>731</v>
-      </c>
-      <c r="K78" s="13"/>
+      <c r="J78" s="41" t="s">
+        <v>727</v>
+      </c>
+      <c r="K78" s="41"/>
       <c r="L78" s="13"/>
     </row>
     <row r="79" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
@@ -10426,26 +10445,26 @@
         <v>2021</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>347</v>
+        <v>88</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
     </row>
     <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>49</v>
+        <v>200</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
@@ -10454,26 +10473,26 @@
         <v>2021</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>269</v>
+        <v>574</v>
       </c>
       <c r="I80" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
     </row>
     <row r="81" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
@@ -10485,23 +10504,23 @@
         <v>42</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>594</v>
+        <v>506</v>
       </c>
       <c r="I81" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
     </row>
     <row r="82" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
@@ -10510,26 +10529,26 @@
         <v>2021</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>95</v>
+        <v>347</v>
       </c>
       <c r="I82" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
     </row>
     <row r="83" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
@@ -10538,26 +10557,26 @@
         <v>2021</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>31</v>
+        <v>269</v>
       </c>
       <c r="I83" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>31</v>
+        <v>732</v>
       </c>
       <c r="K83" s="13"/>
       <c r="L83" s="13"/>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
@@ -10566,26 +10585,26 @@
         <v>2021</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>736</v>
+        <v>42</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>356</v>
+        <v>594</v>
       </c>
       <c r="I84" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
     </row>
     <row r="85" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
@@ -10594,26 +10613,26 @@
         <v>2021</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="I85" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J85" s="13" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
     </row>
     <row r="86" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>195</v>
+        <v>31</v>
       </c>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
@@ -10625,87 +10644,79 @@
         <v>212</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>738</v>
+        <v>31</v>
       </c>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
     </row>
     <row r="87" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
-      <c r="E87" s="13" t="s">
-        <v>739</v>
-      </c>
+      <c r="E87" s="71"/>
       <c r="F87" s="23">
         <v>2021</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>42</v>
+        <v>735</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>740</v>
-      </c>
-      <c r="K87" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>736</v>
+      </c>
+      <c r="K87" s="13"/>
       <c r="L87" s="13"/>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
-      <c r="E88" s="13" t="s">
-        <v>739</v>
-      </c>
+      <c r="E88" s="71"/>
       <c r="F88" s="23">
         <v>2021</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>268</v>
+        <v>72</v>
       </c>
       <c r="I88" s="8" t="s">
         <v>280</v>
       </c>
       <c r="J88" s="13" t="s">
-        <v>740</v>
-      </c>
-      <c r="K88" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>737</v>
+      </c>
+      <c r="K88" s="13"/>
       <c r="L88" s="13"/>
     </row>
     <row r="89" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
@@ -10714,94 +10725,102 @@
         <v>2021</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>23</v>
+        <v>212</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="I89" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J89" s="13"/>
+      <c r="J89" s="13" t="s">
+        <v>737</v>
+      </c>
       <c r="K89" s="13"/>
       <c r="L89" s="13"/>
     </row>
     <row r="90" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="C90" s="72" t="s">
-        <v>452</v>
-      </c>
-      <c r="D90" s="72"/>
-      <c r="E90" s="73"/>
-      <c r="F90" s="74">
-        <v>2010</v>
-      </c>
-      <c r="G90" s="72" t="s">
-        <v>198</v>
-      </c>
-      <c r="H90" s="39" t="s">
-        <v>469</v>
-      </c>
-      <c r="I90" s="39" t="s">
+        <v>726</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="13" t="s">
+        <v>738</v>
+      </c>
+      <c r="F90" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H90" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I90" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J90" s="41"/>
-      <c r="K90" s="13"/>
+      <c r="J90" s="13" t="s">
+        <v>739</v>
+      </c>
+      <c r="K90" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L90" s="13"/>
     </row>
     <row r="91" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B91" s="75" t="s">
-        <v>202</v>
-      </c>
-      <c r="C91" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="D91" s="75"/>
-      <c r="E91" s="76"/>
-      <c r="F91" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G91" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H91" s="39" t="s">
-        <v>469</v>
+        <v>726</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="13" t="s">
+        <v>738</v>
+      </c>
+      <c r="F91" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>268</v>
       </c>
       <c r="I91" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
+      <c r="J91" s="13" t="s">
+        <v>739</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L91" s="13"/>
     </row>
     <row r="92" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B92" s="75" t="s">
-        <v>197</v>
-      </c>
-      <c r="C92" s="75" t="s">
-        <v>452</v>
-      </c>
-      <c r="D92" s="75"/>
-      <c r="E92" s="76"/>
-      <c r="F92" s="77">
-        <v>2010</v>
-      </c>
-      <c r="G92" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>88</v>
+        <v>726</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="71"/>
+      <c r="F92" s="23">
+        <v>2021</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H92" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I92" s="8" t="s">
         <v>280</v>
@@ -10814,27 +10833,27 @@
       <c r="A93" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B93" s="75" t="s">
-        <v>204</v>
-      </c>
-      <c r="C93" s="75" t="s">
+      <c r="B93" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="C93" s="72" t="s">
         <v>452</v>
       </c>
-      <c r="D93" s="75"/>
-      <c r="E93" s="76"/>
-      <c r="F93" s="77">
+      <c r="D93" s="72"/>
+      <c r="E93" s="73"/>
+      <c r="F93" s="74">
         <v>2010</v>
       </c>
-      <c r="G93" s="75" t="s">
+      <c r="G93" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="H93" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="I93" s="8" t="s">
+      <c r="H93" s="39" t="s">
+        <v>469</v>
+      </c>
+      <c r="I93" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="J93" s="13"/>
+      <c r="J93" s="41"/>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
     </row>
@@ -10843,7 +10862,7 @@
         <v>119</v>
       </c>
       <c r="B94" s="75" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C94" s="75" t="s">
         <v>13</v>
@@ -10856,8 +10875,8 @@
       <c r="G94" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="H94" s="7" t="s">
-        <v>204</v>
+      <c r="H94" s="39" t="s">
+        <v>469</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>280</v>
@@ -10871,7 +10890,7 @@
         <v>119</v>
       </c>
       <c r="B95" s="75" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C95" s="75" t="s">
         <v>452</v>
@@ -10885,7 +10904,7 @@
         <v>198</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>574</v>
+        <v>88</v>
       </c>
       <c r="I95" s="8" t="s">
         <v>280</v>
@@ -10899,10 +10918,10 @@
         <v>119</v>
       </c>
       <c r="B96" s="75" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C96" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D96" s="75"/>
       <c r="E96" s="76"/>
@@ -10913,7 +10932,7 @@
         <v>198</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>574</v>
+        <v>204</v>
       </c>
       <c r="I96" s="8" t="s">
         <v>280</v>
@@ -10927,10 +10946,10 @@
         <v>119</v>
       </c>
       <c r="B97" s="75" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C97" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D97" s="75"/>
       <c r="E97" s="76"/>
@@ -10941,7 +10960,7 @@
         <v>198</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>506</v>
+        <v>204</v>
       </c>
       <c r="I97" s="8" t="s">
         <v>280</v>
@@ -10955,10 +10974,10 @@
         <v>119</v>
       </c>
       <c r="B98" s="75" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C98" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D98" s="75"/>
       <c r="E98" s="76"/>
@@ -10969,7 +10988,7 @@
         <v>198</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>506</v>
+        <v>574</v>
       </c>
       <c r="I98" s="8" t="s">
         <v>280</v>
@@ -10983,10 +11002,10 @@
         <v>119</v>
       </c>
       <c r="B99" s="75" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C99" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D99" s="75"/>
       <c r="E99" s="76"/>
@@ -10994,10 +11013,10 @@
         <v>2010</v>
       </c>
       <c r="G99" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>347</v>
+        <v>574</v>
       </c>
       <c r="I99" s="8" t="s">
         <v>280</v>
@@ -11011,10 +11030,10 @@
         <v>119</v>
       </c>
       <c r="B100" s="75" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C100" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D100" s="75"/>
       <c r="E100" s="76"/>
@@ -11022,10 +11041,10 @@
         <v>2010</v>
       </c>
       <c r="G100" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>347</v>
+        <v>506</v>
       </c>
       <c r="I100" s="8" t="s">
         <v>280</v>
@@ -11039,10 +11058,10 @@
         <v>119</v>
       </c>
       <c r="B101" s="75" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="C101" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D101" s="75"/>
       <c r="E101" s="76"/>
@@ -11050,10 +11069,10 @@
         <v>2010</v>
       </c>
       <c r="G101" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>269</v>
+        <v>506</v>
       </c>
       <c r="I101" s="8" t="s">
         <v>280</v>
@@ -11067,10 +11086,10 @@
         <v>119</v>
       </c>
       <c r="B102" s="75" t="s">
-        <v>49</v>
+        <v>193</v>
       </c>
       <c r="C102" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D102" s="75"/>
       <c r="E102" s="76"/>
@@ -11081,7 +11100,7 @@
         <v>194</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>269</v>
+        <v>347</v>
       </c>
       <c r="I102" s="8" t="s">
         <v>280</v>
@@ -11095,10 +11114,10 @@
         <v>119</v>
       </c>
       <c r="B103" s="75" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C103" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D103" s="75"/>
       <c r="E103" s="76"/>
@@ -11106,10 +11125,10 @@
         <v>2010</v>
       </c>
       <c r="G103" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>594</v>
+        <v>347</v>
       </c>
       <c r="I103" s="8" t="s">
         <v>280</v>
@@ -11123,10 +11142,10 @@
         <v>119</v>
       </c>
       <c r="B104" s="75" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="C104" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D104" s="75"/>
       <c r="E104" s="76"/>
@@ -11134,10 +11153,10 @@
         <v>2010</v>
       </c>
       <c r="G104" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>594</v>
+        <v>269</v>
       </c>
       <c r="I104" s="8" t="s">
         <v>280</v>
@@ -11151,10 +11170,10 @@
         <v>119</v>
       </c>
       <c r="B105" s="75" t="s">
-        <v>209</v>
+        <v>49</v>
       </c>
       <c r="C105" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D105" s="75"/>
       <c r="E105" s="76"/>
@@ -11164,31 +11183,25 @@
       <c r="G105" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H105" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="I105" s="15" t="s">
-        <v>741</v>
-      </c>
-      <c r="J105" s="13" t="s">
-        <v>742</v>
-      </c>
-      <c r="K105" s="13" t="s">
-        <v>743</v>
-      </c>
-      <c r="L105" s="13" t="s">
-        <v>397</v>
-      </c>
+      <c r="H105" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J105" s="13"/>
+      <c r="K105" s="13"/>
+      <c r="L105" s="13"/>
     </row>
     <row r="106" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B106" s="75" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C106" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D106" s="75"/>
       <c r="E106" s="76"/>
@@ -11196,33 +11209,27 @@
         <v>2010</v>
       </c>
       <c r="G106" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H106" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="I106" s="15" t="s">
-        <v>741</v>
-      </c>
-      <c r="J106" s="13" t="s">
-        <v>742</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>744</v>
-      </c>
-      <c r="L106" s="13" t="s">
-        <v>397</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H106" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="I106" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J106" s="13"/>
+      <c r="K106" s="13"/>
+      <c r="L106" s="13"/>
     </row>
     <row r="107" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B107" s="75" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C107" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D107" s="75"/>
       <c r="E107" s="76"/>
@@ -11230,33 +11237,27 @@
         <v>2010</v>
       </c>
       <c r="G107" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I107" s="15" t="s">
-        <v>741</v>
-      </c>
-      <c r="J107" s="13" t="s">
-        <v>745</v>
-      </c>
-      <c r="K107" s="13" t="s">
-        <v>744</v>
-      </c>
-      <c r="L107" s="13" t="s">
-        <v>397</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="I107" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J107" s="13"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
     </row>
     <row r="108" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B108" s="75" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C108" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D108" s="75"/>
       <c r="E108" s="76"/>
@@ -11267,16 +11268,16 @@
         <v>194</v>
       </c>
       <c r="H108" s="15" t="s">
-        <v>55</v>
+        <v>620</v>
       </c>
       <c r="I108" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="J108" s="13" t="s">
         <v>741</v>
       </c>
-      <c r="J108" s="13" t="s">
-        <v>745</v>
-      </c>
       <c r="K108" s="13" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="L108" s="13" t="s">
         <v>397</v>
@@ -11287,10 +11288,10 @@
         <v>119</v>
       </c>
       <c r="B109" s="75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C109" s="75" t="s">
-        <v>485</v>
+        <v>13</v>
       </c>
       <c r="D109" s="75"/>
       <c r="E109" s="76"/>
@@ -11301,16 +11302,16 @@
         <v>194</v>
       </c>
       <c r="H109" s="15" t="s">
-        <v>59</v>
+        <v>620</v>
       </c>
       <c r="I109" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="J109" s="13" t="s">
         <v>741</v>
       </c>
-      <c r="J109" s="13" t="s">
-        <v>746</v>
-      </c>
       <c r="K109" s="13" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="L109" s="13" t="s">
         <v>397</v>
@@ -11321,10 +11322,10 @@
         <v>119</v>
       </c>
       <c r="B110" s="75" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C110" s="75" t="s">
-        <v>13</v>
+        <v>485</v>
       </c>
       <c r="D110" s="75"/>
       <c r="E110" s="76"/>
@@ -11335,16 +11336,16 @@
         <v>194</v>
       </c>
       <c r="H110" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I110" s="15" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J110" s="13" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="K110" s="13" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="L110" s="13" t="s">
         <v>397</v>
@@ -11355,10 +11356,10 @@
         <v>119</v>
       </c>
       <c r="B111" s="75" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C111" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D111" s="75"/>
       <c r="E111" s="76"/>
@@ -11366,27 +11367,33 @@
         <v>2010</v>
       </c>
       <c r="G111" s="75" t="s">
-        <v>198</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I111" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
+        <v>194</v>
+      </c>
+      <c r="H111" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I111" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="J111" s="13" t="s">
+        <v>744</v>
+      </c>
+      <c r="K111" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="L111" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="112" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B112" s="75" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C112" s="75" t="s">
-        <v>452</v>
+        <v>485</v>
       </c>
       <c r="D112" s="75"/>
       <c r="E112" s="76"/>
@@ -11396,22 +11403,28 @@
       <c r="G112" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H112" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I112" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J112" s="13"/>
-      <c r="K112" s="13"/>
-      <c r="L112" s="13"/>
+      <c r="H112" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I112" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="J112" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="K112" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="L112" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="113" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B113" s="75" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C113" s="75" t="s">
         <v>13</v>
@@ -11424,25 +11437,31 @@
       <c r="G113" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H113" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I113" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="J113" s="13"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="13"/>
+      <c r="H113" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I113" s="15" t="s">
+        <v>740</v>
+      </c>
+      <c r="J113" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="K113" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="L113" s="13" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="114" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B114" s="75" t="s">
-        <v>319</v>
+        <v>199</v>
       </c>
       <c r="C114" s="75" t="s">
-        <v>485</v>
+        <v>452</v>
       </c>
       <c r="D114" s="75"/>
       <c r="E114" s="76"/>
@@ -11450,10 +11469,10 @@
         <v>2010</v>
       </c>
       <c r="G114" s="75" t="s">
-        <v>747</v>
+        <v>198</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>319</v>
+        <v>95</v>
       </c>
       <c r="I114" s="8" t="s">
         <v>280</v>
@@ -11467,10 +11486,10 @@
         <v>119</v>
       </c>
       <c r="B115" s="75" t="s">
-        <v>319</v>
+        <v>31</v>
       </c>
       <c r="C115" s="75" t="s">
-        <v>13</v>
+        <v>452</v>
       </c>
       <c r="D115" s="75"/>
       <c r="E115" s="76"/>
@@ -11478,10 +11497,10 @@
         <v>2010</v>
       </c>
       <c r="G115" s="75" t="s">
-        <v>747</v>
+        <v>194</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>319</v>
+        <v>31</v>
       </c>
       <c r="I115" s="8" t="s">
         <v>280</v>
@@ -11495,10 +11514,10 @@
         <v>119</v>
       </c>
       <c r="B116" s="75" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
       <c r="C116" s="75" t="s">
-        <v>452</v>
+        <v>13</v>
       </c>
       <c r="D116" s="75"/>
       <c r="E116" s="76"/>
@@ -11506,17 +11525,15 @@
         <v>2010</v>
       </c>
       <c r="G116" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>356</v>
+        <v>31</v>
       </c>
       <c r="I116" s="8" t="s">
-        <v>748</v>
-      </c>
-      <c r="J116" s="13" t="s">
-        <v>749</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="J116" s="13"/>
       <c r="K116" s="13"/>
       <c r="L116" s="13"/>
     </row>
@@ -11525,10 +11542,10 @@
         <v>119</v>
       </c>
       <c r="B117" s="75" t="s">
-        <v>196</v>
+        <v>319</v>
       </c>
       <c r="C117" s="75" t="s">
-        <v>438</v>
+        <v>485</v>
       </c>
       <c r="D117" s="75"/>
       <c r="E117" s="76"/>
@@ -11536,10 +11553,10 @@
         <v>2010</v>
       </c>
       <c r="G117" s="75" t="s">
-        <v>194</v>
+        <v>746</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>72</v>
+        <v>319</v>
       </c>
       <c r="I117" s="8" t="s">
         <v>280</v>
@@ -11553,10 +11570,10 @@
         <v>119</v>
       </c>
       <c r="B118" s="75" t="s">
-        <v>195</v>
+        <v>319</v>
       </c>
       <c r="C118" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D118" s="75"/>
       <c r="E118" s="76"/>
@@ -11564,10 +11581,10 @@
         <v>2010</v>
       </c>
       <c r="G118" s="75" t="s">
-        <v>194</v>
+        <v>746</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>77</v>
+        <v>319</v>
       </c>
       <c r="I118" s="8" t="s">
         <v>280</v>
@@ -11581,10 +11598,10 @@
         <v>119</v>
       </c>
       <c r="B119" s="75" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C119" s="75" t="s">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="D119" s="75"/>
       <c r="E119" s="76"/>
@@ -11595,17 +11612,15 @@
         <v>198</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="I119" s="8" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="J119" s="13" t="s">
-        <v>751</v>
-      </c>
-      <c r="K119" s="13" t="s">
-        <v>599</v>
-      </c>
+        <v>748</v>
+      </c>
+      <c r="K119" s="13"/>
       <c r="L119" s="13"/>
     </row>
     <row r="120" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11613,10 +11628,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="75" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C120" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D120" s="75"/>
       <c r="E120" s="76"/>
@@ -11624,18 +11639,16 @@
         <v>2010</v>
       </c>
       <c r="G120" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>268</v>
+        <v>72</v>
       </c>
       <c r="I120" s="8" t="s">
-        <v>750</v>
+        <v>280</v>
       </c>
       <c r="J120" s="13"/>
-      <c r="K120" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="K120" s="13"/>
       <c r="L120" s="13"/>
     </row>
     <row r="121" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11643,7 +11656,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="75" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C121" s="75" t="s">
         <v>438</v>
@@ -11654,18 +11667,16 @@
         <v>2010</v>
       </c>
       <c r="G121" s="75" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>268</v>
+        <v>77</v>
       </c>
       <c r="I121" s="8" t="s">
-        <v>750</v>
+        <v>280</v>
       </c>
       <c r="J121" s="13"/>
-      <c r="K121" s="13" t="s">
-        <v>599</v>
-      </c>
+      <c r="K121" s="13"/>
       <c r="L121" s="13"/>
     </row>
     <row r="122" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11673,10 +11684,10 @@
         <v>119</v>
       </c>
       <c r="B122" s="75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C122" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D122" s="75"/>
       <c r="E122" s="76"/>
@@ -11690,9 +11701,11 @@
         <v>268</v>
       </c>
       <c r="I122" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="J122" s="13" t="s">
         <v>750</v>
       </c>
-      <c r="J122" s="13"/>
       <c r="K122" s="13" t="s">
         <v>599</v>
       </c>
@@ -11703,10 +11716,10 @@
         <v>119</v>
       </c>
       <c r="B123" s="75" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C123" s="75" t="s">
-        <v>438</v>
+        <v>13</v>
       </c>
       <c r="D123" s="75"/>
       <c r="E123" s="76"/>
@@ -11714,16 +11727,18 @@
         <v>2010</v>
       </c>
       <c r="G123" s="75" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>23</v>
+        <v>268</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>280</v>
+        <v>749</v>
       </c>
       <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
+      <c r="K123" s="13" t="s">
+        <v>599</v>
+      </c>
       <c r="L123" s="13"/>
     </row>
     <row r="124" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -11731,10 +11746,10 @@
         <v>119</v>
       </c>
       <c r="B124" s="75" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C124" s="75" t="s">
-        <v>13</v>
+        <v>438</v>
       </c>
       <c r="D124" s="75"/>
       <c r="E124" s="76"/>
@@ -11742,17 +11757,105 @@
         <v>2010</v>
       </c>
       <c r="G124" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I124" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="J124" s="13"/>
+      <c r="K124" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L124" s="13"/>
+    </row>
+    <row r="125" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B125" s="75" t="s">
+        <v>206</v>
+      </c>
+      <c r="C125" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="75"/>
+      <c r="E125" s="76"/>
+      <c r="F125" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G125" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="I125" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="J125" s="13"/>
+      <c r="K125" s="13" t="s">
+        <v>599</v>
+      </c>
+      <c r="L125" s="13"/>
+    </row>
+    <row r="126" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B126" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="C126" s="75" t="s">
+        <v>438</v>
+      </c>
+      <c r="D126" s="75"/>
+      <c r="E126" s="76"/>
+      <c r="F126" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G126" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="H124" s="7" t="s">
+      <c r="H126" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I124" s="15" t="s">
-        <v>752</v>
-      </c>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
+      <c r="I126" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="J126" s="13"/>
+      <c r="K126" s="13"/>
+      <c r="L126" s="13"/>
+    </row>
+    <row r="127" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127" s="75" t="s">
+        <v>207</v>
+      </c>
+      <c r="C127" s="75" t="s">
+        <v>13</v>
+      </c>
+      <c r="D127" s="75"/>
+      <c r="E127" s="76"/>
+      <c r="F127" s="77">
+        <v>2010</v>
+      </c>
+      <c r="G127" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I127" s="15" t="s">
+        <v>751</v>
+      </c>
+      <c r="J127" s="13"/>
+      <c r="K127" s="13"/>
+      <c r="L127" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12165,8 +12268,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="78"/>
-      <c r="L2" s="80"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12203,8 +12306,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="81"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="89"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12241,8 +12344,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="79"/>
-      <c r="L4" s="81"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="89"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12277,8 +12380,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="79"/>
-      <c r="L5" s="81"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="89"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12315,10 +12418,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="82" t="s">
+      <c r="K6" s="87" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="84"/>
+      <c r="L6" s="92"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12355,8 +12458,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="79"/>
-      <c r="L7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="93"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12391,8 +12494,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="83"/>
-      <c r="L8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="94"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12429,10 +12532,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="95" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="89" t="s">
+      <c r="L9" s="90" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12471,8 +12574,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="88"/>
-      <c r="L10" s="81"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="89"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12509,8 +12612,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="88"/>
-      <c r="L11" s="81"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="89"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12789,7 +12892,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="82"/>
+      <c r="K18" s="87"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12827,7 +12930,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="83"/>
+      <c r="K19" s="86"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12865,10 +12968,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="87" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="89" t="s">
+      <c r="L20" s="90" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -12907,8 +13010,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="79"/>
-      <c r="L21" s="81"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="89"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -12943,8 +13046,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="79"/>
-      <c r="L22" s="81"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="89"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -12981,8 +13084,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="81"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="89"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -13019,8 +13122,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="79"/>
-      <c r="L24" s="81"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="89"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -13057,10 +13160,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="78" t="s">
+      <c r="K25" s="84" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="80" t="s">
+      <c r="L25" s="88" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -13099,8 +13202,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="79"/>
-      <c r="L26" s="81"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="89"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13137,8 +13240,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="79"/>
-      <c r="L27" s="81"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="89"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13173,8 +13276,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="83"/>
-      <c r="L28" s="90"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="91"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13211,7 +13314,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="82" t="s">
+      <c r="K29" s="87" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13251,7 +13354,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="79"/>
+      <c r="K30" s="85"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13289,7 +13392,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="79"/>
+      <c r="K31" s="85"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13325,7 +13428,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="79"/>
+      <c r="K32" s="85"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13363,7 +13466,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="78" t="s">
+      <c r="K33" s="84" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13405,7 +13508,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="83"/>
+      <c r="K34" s="86"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13443,7 +13546,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="82" t="s">
+      <c r="K35" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13485,7 +13588,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="79"/>
+      <c r="K36" s="85"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13602,7 +13705,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="80"/>
+      <c r="L39" s="88"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13640,7 +13743,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="81"/>
+      <c r="L40" s="89"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13719,10 +13822,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="82" t="s">
+      <c r="K42" s="87" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="89" t="s">
+      <c r="L42" s="90" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13761,8 +13864,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="79"/>
-      <c r="L43" s="81"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="89"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13799,8 +13902,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="81"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="89"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13835,8 +13938,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="81"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="89"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13873,8 +13976,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="81"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="89"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -13911,8 +14014,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="79"/>
-      <c r="L47" s="81"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="89"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -14029,7 +14132,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="91" t="s">
+      <c r="K50" s="78" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -14069,7 +14172,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="88"/>
+      <c r="K51" s="79"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -14107,7 +14210,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="88"/>
+      <c r="K52" s="79"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14145,7 +14248,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="88"/>
+      <c r="K53" s="79"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14181,7 +14284,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="92"/>
+      <c r="K54" s="80"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14301,7 +14404,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="82" t="s">
+      <c r="K57" s="87" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14341,7 +14444,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="79"/>
+      <c r="K58" s="85"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14377,7 +14480,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="79"/>
+      <c r="K59" s="85"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14415,7 +14518,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="80" t="s">
+      <c r="K60" s="88" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14455,7 +14558,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="81"/>
+      <c r="K61" s="89"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14495,7 +14598,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="81"/>
+      <c r="K62" s="89"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14535,7 +14638,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="82"/>
+      <c r="K63" s="87"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14573,7 +14676,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="79"/>
+      <c r="K64" s="85"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14611,7 +14714,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="79"/>
+      <c r="K65" s="85"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14649,7 +14752,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="79"/>
+      <c r="K66" s="85"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14763,7 +14866,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="82" t="s">
+      <c r="K69" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14805,7 +14908,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="79"/>
+      <c r="K70" s="85"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14883,7 +14986,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="82"/>
+      <c r="K72" s="87"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -14919,7 +15022,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="79"/>
+      <c r="K73" s="85"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -14955,7 +15058,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="79"/>
+      <c r="K74" s="85"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -14989,7 +15092,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="83"/>
+      <c r="K75" s="86"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -15067,10 +15170,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="91" t="s">
+      <c r="K77" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="78" t="s">
+      <c r="L77" s="84" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15111,8 +15214,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="92"/>
-      <c r="L78" s="94"/>
+      <c r="K78" s="80"/>
+      <c r="L78" s="82"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15152,7 +15255,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="94"/>
+      <c r="L79" s="82"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15192,7 +15295,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="83"/>
+      <c r="L80" s="86"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15229,7 +15332,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="82" t="s">
+      <c r="K81" s="87" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15271,7 +15374,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="79"/>
+      <c r="K82" s="85"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15393,7 +15496,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="82" t="s">
+      <c r="K85" s="87" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15433,7 +15536,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="79"/>
+      <c r="K86" s="85"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15471,7 +15574,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="79"/>
+      <c r="K87" s="85"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15507,7 +15610,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="79"/>
+      <c r="K88" s="85"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15545,7 +15648,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="79"/>
+      <c r="K89" s="85"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15583,7 +15686,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="79"/>
+      <c r="K90" s="85"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15621,10 +15724,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="91" t="s">
+      <c r="K91" s="78" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="93" t="s">
+      <c r="L91" s="81" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15663,8 +15766,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="88"/>
-      <c r="L92" s="94"/>
+      <c r="K92" s="79"/>
+      <c r="L92" s="82"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15701,8 +15804,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="88"/>
-      <c r="L93" s="94"/>
+      <c r="K93" s="79"/>
+      <c r="L93" s="82"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15737,8 +15840,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="92"/>
-      <c r="L94" s="95"/>
+      <c r="K94" s="80"/>
+      <c r="L94" s="83"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15775,7 +15878,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="78"/>
+      <c r="K95" s="84"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15813,7 +15916,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="79"/>
+      <c r="K96" s="85"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15851,7 +15954,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="79"/>
+      <c r="K97" s="85"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15889,7 +15992,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="79"/>
+      <c r="K98" s="85"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -15925,7 +16028,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="83"/>
+      <c r="K99" s="86"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -15954,6 +16057,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -15962,28 +16087,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added par to NOAA_Map
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DACD712-8B8A-4774-9D3A-B8E3A322D6CD}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60E1EFB6-ACEC-45DE-9A93-8D246996F446}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3715" uniqueCount="817">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2508,6 +2508,12 @@
   </si>
   <si>
     <t>Turbidity_USGS</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>Remove because no surface PAR to compute CPAR</t>
   </si>
 </sst>
 </file>
@@ -3057,35 +3063,11 @@
     <xf numFmtId="3" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3093,10 +3075,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3110,6 +3092,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8209,7 +8215,7 @@
   </sheetPr>
   <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
@@ -11867,10 +11873,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12165,6 +12171,20 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>815</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>816</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12268,8 +12288,8 @@
       <c r="J2" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K2" s="84"/>
-      <c r="L2" s="88"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="80"/>
       <c r="M2" s="40" t="s">
         <v>437</v>
       </c>
@@ -12306,8 +12326,8 @@
       <c r="J3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="89"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="81"/>
       <c r="M3" s="9" t="s">
         <v>437</v>
       </c>
@@ -12344,8 +12364,8 @@
       <c r="J4" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="89"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="81"/>
       <c r="M4" s="9" t="s">
         <v>437</v>
       </c>
@@ -12380,8 +12400,8 @@
       <c r="J5" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="89"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="81"/>
       <c r="M5" s="9" t="s">
         <v>437</v>
       </c>
@@ -12418,10 +12438,10 @@
       <c r="J6" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K6" s="82" t="s">
         <v>447</v>
       </c>
-      <c r="L6" s="92"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="9" t="s">
         <v>437</v>
       </c>
@@ -12458,8 +12478,8 @@
       <c r="J7" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K7" s="85"/>
-      <c r="L7" s="93"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="85"/>
       <c r="M7" s="9" t="s">
         <v>437</v>
       </c>
@@ -12494,8 +12514,8 @@
       <c r="J8" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K8" s="86"/>
-      <c r="L8" s="94"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="86"/>
       <c r="M8" s="9" t="s">
         <v>437</v>
       </c>
@@ -12532,10 +12552,10 @@
       <c r="J9" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K9" s="95" t="s">
+      <c r="K9" s="87" t="s">
         <v>455</v>
       </c>
-      <c r="L9" s="90" t="s">
+      <c r="L9" s="89" t="s">
         <v>456</v>
       </c>
       <c r="M9" s="40" t="s">
@@ -12574,8 +12594,8 @@
       <c r="J10" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K10" s="79"/>
-      <c r="L10" s="89"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="9" t="s">
         <v>437</v>
       </c>
@@ -12612,8 +12632,8 @@
       <c r="J11" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K11" s="79"/>
-      <c r="L11" s="89"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="81"/>
       <c r="M11" s="9" t="s">
         <v>437</v>
       </c>
@@ -12892,7 +12912,7 @@
       <c r="J18" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K18" s="87"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="38"/>
       <c r="M18" s="9" t="s">
         <v>437</v>
@@ -12930,7 +12950,7 @@
       <c r="J19" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K19" s="86"/>
+      <c r="K19" s="83"/>
       <c r="L19" s="60"/>
       <c r="M19" s="43" t="s">
         <v>437</v>
@@ -12968,10 +12988,10 @@
       <c r="J20" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K20" s="87" t="s">
+      <c r="K20" s="82" t="s">
         <v>490</v>
       </c>
-      <c r="L20" s="90" t="s">
+      <c r="L20" s="89" t="s">
         <v>491</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -13010,8 +13030,8 @@
       <c r="J21" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K21" s="85"/>
-      <c r="L21" s="89"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="9" t="s">
         <v>437</v>
       </c>
@@ -13046,8 +13066,8 @@
       <c r="J22" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K22" s="85"/>
-      <c r="L22" s="89"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="81"/>
       <c r="M22" s="9" t="s">
         <v>437</v>
       </c>
@@ -13084,8 +13104,8 @@
       <c r="J23" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K23" s="85"/>
-      <c r="L23" s="89"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="9" t="s">
         <v>437</v>
       </c>
@@ -13122,8 +13142,8 @@
       <c r="J24" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K24" s="85"/>
-      <c r="L24" s="89"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="9" t="s">
         <v>437</v>
       </c>
@@ -13160,10 +13180,10 @@
       <c r="J25" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K25" s="84" t="s">
+      <c r="K25" s="78" t="s">
         <v>497</v>
       </c>
-      <c r="L25" s="88" t="s">
+      <c r="L25" s="80" t="s">
         <v>498</v>
       </c>
       <c r="M25" s="40" t="s">
@@ -13202,8 +13222,8 @@
       <c r="J26" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K26" s="85"/>
-      <c r="L26" s="89"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="9" t="s">
         <v>437</v>
       </c>
@@ -13240,8 +13260,8 @@
       <c r="J27" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K27" s="85"/>
-      <c r="L27" s="89"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="9" t="s">
         <v>437</v>
       </c>
@@ -13276,8 +13296,8 @@
       <c r="J28" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K28" s="86"/>
-      <c r="L28" s="91"/>
+      <c r="K28" s="83"/>
+      <c r="L28" s="90"/>
       <c r="M28" s="43" t="s">
         <v>437</v>
       </c>
@@ -13314,7 +13334,7 @@
       <c r="J29" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K29" s="87" t="s">
+      <c r="K29" s="82" t="s">
         <v>503</v>
       </c>
       <c r="L29" s="38"/>
@@ -13354,7 +13374,7 @@
       <c r="J30" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K30" s="85"/>
+      <c r="K30" s="79"/>
       <c r="L30" s="38"/>
       <c r="M30" s="9" t="s">
         <v>437</v>
@@ -13392,7 +13412,7 @@
       <c r="J31" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K31" s="85"/>
+      <c r="K31" s="79"/>
       <c r="L31" s="38"/>
       <c r="M31" s="9" t="s">
         <v>437</v>
@@ -13428,7 +13448,7 @@
       <c r="J32" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K32" s="85"/>
+      <c r="K32" s="79"/>
       <c r="L32" s="38"/>
       <c r="M32" s="9" t="s">
         <v>437</v>
@@ -13466,7 +13486,7 @@
       <c r="J33" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K33" s="84" t="s">
+      <c r="K33" s="78" t="s">
         <v>470</v>
       </c>
       <c r="L33" s="59" t="s">
@@ -13508,7 +13528,7 @@
       <c r="J34" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K34" s="86"/>
+      <c r="K34" s="83"/>
       <c r="L34" s="60"/>
       <c r="M34" s="43" t="s">
         <v>437</v>
@@ -13546,7 +13566,7 @@
       <c r="J35" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K35" s="87" t="s">
+      <c r="K35" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L35" s="38" t="s">
@@ -13588,7 +13608,7 @@
       <c r="J36" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K36" s="85"/>
+      <c r="K36" s="79"/>
       <c r="L36" s="38"/>
       <c r="M36" s="9" t="s">
         <v>437</v>
@@ -13705,7 +13725,7 @@
       <c r="K39" s="62" t="s">
         <v>520</v>
       </c>
-      <c r="L39" s="88"/>
+      <c r="L39" s="80"/>
       <c r="M39" s="40" t="s">
         <v>437</v>
       </c>
@@ -13743,7 +13763,7 @@
         <v>437</v>
       </c>
       <c r="K40" s="51"/>
-      <c r="L40" s="89"/>
+      <c r="L40" s="81"/>
       <c r="M40" s="9" t="s">
         <v>437</v>
       </c>
@@ -13822,10 +13842,10 @@
       <c r="J42" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K42" s="87" t="s">
+      <c r="K42" s="82" t="s">
         <v>527</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="L42" s="89" t="s">
         <v>528</v>
       </c>
       <c r="M42" s="40" t="s">
@@ -13864,8 +13884,8 @@
       <c r="J43" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K43" s="85"/>
-      <c r="L43" s="89"/>
+      <c r="K43" s="79"/>
+      <c r="L43" s="81"/>
       <c r="M43" s="9" t="s">
         <v>437</v>
       </c>
@@ -13902,8 +13922,8 @@
       <c r="J44" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K44" s="85"/>
-      <c r="L44" s="89"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="81"/>
       <c r="M44" s="9" t="s">
         <v>437</v>
       </c>
@@ -13938,8 +13958,8 @@
       <c r="J45" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K45" s="85"/>
-      <c r="L45" s="89"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="81"/>
       <c r="M45" s="9" t="s">
         <v>437</v>
       </c>
@@ -13976,8 +13996,8 @@
       <c r="J46" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K46" s="85"/>
-      <c r="L46" s="89"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="81"/>
       <c r="M46" s="9" t="s">
         <v>437</v>
       </c>
@@ -14014,8 +14034,8 @@
       <c r="J47" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K47" s="85"/>
-      <c r="L47" s="89"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="9" t="s">
         <v>437</v>
       </c>
@@ -14132,7 +14152,7 @@
       <c r="J50" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K50" s="78" t="s">
+      <c r="K50" s="91" t="s">
         <v>541</v>
       </c>
       <c r="L50" s="59"/>
@@ -14172,7 +14192,7 @@
       <c r="J51" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K51" s="79"/>
+      <c r="K51" s="88"/>
       <c r="L51" s="38"/>
       <c r="M51" s="40" t="s">
         <v>437</v>
@@ -14210,7 +14230,7 @@
       <c r="J52" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K52" s="79"/>
+      <c r="K52" s="88"/>
       <c r="L52" s="38"/>
       <c r="M52" s="40" t="s">
         <v>437</v>
@@ -14248,7 +14268,7 @@
       <c r="J53" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K53" s="79"/>
+      <c r="K53" s="88"/>
       <c r="L53" s="38"/>
       <c r="M53" s="40" t="s">
         <v>437</v>
@@ -14284,7 +14304,7 @@
       <c r="J54" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K54" s="80"/>
+      <c r="K54" s="92"/>
       <c r="L54" s="60"/>
       <c r="M54" s="40" t="s">
         <v>437</v>
@@ -14404,7 +14424,7 @@
       <c r="J57" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K57" s="87" t="s">
+      <c r="K57" s="82" t="s">
         <v>558</v>
       </c>
       <c r="L57" s="38"/>
@@ -14444,7 +14464,7 @@
       <c r="J58" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K58" s="85"/>
+      <c r="K58" s="79"/>
       <c r="L58" s="38"/>
       <c r="M58" s="9" t="s">
         <v>437</v>
@@ -14480,7 +14500,7 @@
       <c r="J59" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K59" s="85"/>
+      <c r="K59" s="79"/>
       <c r="L59" s="38"/>
       <c r="M59" s="9" t="s">
         <v>437</v>
@@ -14518,7 +14538,7 @@
       <c r="J60" s="40" t="s">
         <v>437</v>
       </c>
-      <c r="K60" s="88" t="s">
+      <c r="K60" s="80" t="s">
         <v>563</v>
       </c>
       <c r="L60" s="59"/>
@@ -14558,7 +14578,7 @@
       <c r="J61" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K61" s="89"/>
+      <c r="K61" s="81"/>
       <c r="L61" s="38" t="s">
         <v>565</v>
       </c>
@@ -14598,7 +14618,7 @@
       <c r="J62" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K62" s="89"/>
+      <c r="K62" s="81"/>
       <c r="L62" s="38" t="s">
         <v>567</v>
       </c>
@@ -14638,7 +14658,7 @@
       <c r="J63" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K63" s="87"/>
+      <c r="K63" s="82"/>
       <c r="L63" s="38"/>
       <c r="M63" s="9" t="s">
         <v>437</v>
@@ -14676,7 +14696,7 @@
       <c r="J64" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K64" s="85"/>
+      <c r="K64" s="79"/>
       <c r="L64" s="38"/>
       <c r="M64" s="9" t="s">
         <v>437</v>
@@ -14714,7 +14734,7 @@
       <c r="J65" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K65" s="85"/>
+      <c r="K65" s="79"/>
       <c r="L65" s="38" t="s">
         <v>567</v>
       </c>
@@ -14752,7 +14772,7 @@
       <c r="J66" s="63" t="s">
         <v>437</v>
       </c>
-      <c r="K66" s="85"/>
+      <c r="K66" s="79"/>
       <c r="L66" s="13"/>
       <c r="M66" s="50" t="s">
         <v>437</v>
@@ -14866,7 +14886,7 @@
       <c r="J69" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K69" s="87" t="s">
+      <c r="K69" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L69" s="38" t="s">
@@ -14908,7 +14928,7 @@
       <c r="J70" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K70" s="85"/>
+      <c r="K70" s="79"/>
       <c r="L70" s="38"/>
       <c r="M70" s="9" t="s">
         <v>437</v>
@@ -14986,7 +15006,7 @@
       <c r="J72" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K72" s="87"/>
+      <c r="K72" s="82"/>
       <c r="L72" s="38"/>
       <c r="M72" s="9" t="s">
         <v>437</v>
@@ -15022,7 +15042,7 @@
       <c r="J73" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K73" s="85"/>
+      <c r="K73" s="79"/>
       <c r="L73" s="38"/>
       <c r="M73" s="9" t="s">
         <v>437</v>
@@ -15058,7 +15078,7 @@
       <c r="J74" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K74" s="85"/>
+      <c r="K74" s="79"/>
       <c r="L74" s="38"/>
       <c r="M74" s="9" t="s">
         <v>437</v>
@@ -15092,7 +15112,7 @@
       <c r="J75" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K75" s="86"/>
+      <c r="K75" s="83"/>
       <c r="L75" s="60"/>
       <c r="M75" s="9" t="s">
         <v>437</v>
@@ -15170,10 +15190,10 @@
       <c r="J77" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="K77" s="78" t="s">
+      <c r="K77" s="91" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="84" t="s">
+      <c r="L77" s="78" t="s">
         <v>591</v>
       </c>
       <c r="M77" s="40" t="s">
@@ -15214,8 +15234,8 @@
       <c r="J78" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K78" s="80"/>
-      <c r="L78" s="82"/>
+      <c r="K78" s="92"/>
+      <c r="L78" s="94"/>
       <c r="M78" s="50" t="s">
         <v>437</v>
       </c>
@@ -15255,7 +15275,7 @@
       <c r="K79" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L79" s="82"/>
+      <c r="L79" s="94"/>
       <c r="M79" s="50" t="s">
         <v>437</v>
       </c>
@@ -15295,7 +15315,7 @@
       <c r="K80" s="38" t="s">
         <v>592</v>
       </c>
-      <c r="L80" s="86"/>
+      <c r="L80" s="83"/>
       <c r="M80" s="9" t="s">
         <v>437</v>
       </c>
@@ -15332,7 +15352,7 @@
       <c r="J81" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K81" s="87" t="s">
+      <c r="K81" s="82" t="s">
         <v>470</v>
       </c>
       <c r="L81" s="38" t="s">
@@ -15374,7 +15394,7 @@
       <c r="J82" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K82" s="85"/>
+      <c r="K82" s="79"/>
       <c r="L82" s="38"/>
       <c r="M82" s="9" t="s">
         <v>437</v>
@@ -15496,7 +15516,7 @@
       <c r="J85" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K85" s="87" t="s">
+      <c r="K85" s="82" t="s">
         <v>604</v>
       </c>
       <c r="L85" s="38"/>
@@ -15536,7 +15556,7 @@
       <c r="J86" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K86" s="85"/>
+      <c r="K86" s="79"/>
       <c r="L86" s="38"/>
       <c r="M86" s="9" t="s">
         <v>437</v>
@@ -15574,7 +15594,7 @@
       <c r="J87" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K87" s="85"/>
+      <c r="K87" s="79"/>
       <c r="L87" s="38"/>
       <c r="M87" s="9" t="s">
         <v>437</v>
@@ -15610,7 +15630,7 @@
       <c r="J88" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K88" s="85"/>
+      <c r="K88" s="79"/>
       <c r="L88" s="38"/>
       <c r="M88" s="9" t="s">
         <v>437</v>
@@ -15648,7 +15668,7 @@
       <c r="J89" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K89" s="85"/>
+      <c r="K89" s="79"/>
       <c r="L89" s="38"/>
       <c r="M89" s="9" t="s">
         <v>437</v>
@@ -15686,7 +15706,7 @@
       <c r="J90" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K90" s="85"/>
+      <c r="K90" s="79"/>
       <c r="L90" s="38"/>
       <c r="M90" s="9" t="s">
         <v>437</v>
@@ -15724,10 +15744,10 @@
       <c r="J91" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K91" s="78" t="s">
+      <c r="K91" s="91" t="s">
         <v>610</v>
       </c>
-      <c r="L91" s="81" t="s">
+      <c r="L91" s="93" t="s">
         <v>611</v>
       </c>
       <c r="M91" s="40" t="s">
@@ -15766,8 +15786,8 @@
       <c r="J92" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K92" s="79"/>
-      <c r="L92" s="82"/>
+      <c r="K92" s="88"/>
+      <c r="L92" s="94"/>
       <c r="M92" s="9" t="s">
         <v>437</v>
       </c>
@@ -15804,8 +15824,8 @@
       <c r="J93" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="K93" s="79"/>
-      <c r="L93" s="82"/>
+      <c r="K93" s="88"/>
+      <c r="L93" s="94"/>
       <c r="M93" s="9" t="s">
         <v>437</v>
       </c>
@@ -15840,8 +15860,8 @@
       <c r="J94" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K94" s="80"/>
-      <c r="L94" s="83"/>
+      <c r="K94" s="92"/>
+      <c r="L94" s="95"/>
       <c r="M94" s="9" t="s">
         <v>437</v>
       </c>
@@ -15878,7 +15898,7 @@
       <c r="J95" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K95" s="84"/>
+      <c r="K95" s="78"/>
       <c r="L95" s="38"/>
       <c r="M95" s="40" t="s">
         <v>437</v>
@@ -15916,7 +15936,7 @@
       <c r="J96" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K96" s="85"/>
+      <c r="K96" s="79"/>
       <c r="L96" s="38"/>
       <c r="M96" s="40" t="s">
         <v>437</v>
@@ -15954,7 +15974,7 @@
       <c r="J97" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K97" s="85"/>
+      <c r="K97" s="79"/>
       <c r="L97" s="38"/>
       <c r="M97" s="40" t="s">
         <v>437</v>
@@ -15992,7 +16012,7 @@
       <c r="J98" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="K98" s="85"/>
+      <c r="K98" s="79"/>
       <c r="L98" s="38"/>
       <c r="M98" s="40" t="s">
         <v>437</v>
@@ -16028,7 +16048,7 @@
       <c r="J99" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="K99" s="86"/>
+      <c r="K99" s="83"/>
       <c r="L99" s="53"/>
       <c r="M99" s="55" t="s">
         <v>437</v>
@@ -16057,28 +16077,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -16087,6 +16085,28 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed surface temp from NOAA
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF82A00-9F4E-4DF2-9E26-9AEB735E2279}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F85E95FD-3AA8-40C7-8385-571CFBC23C84}"/>
   <bookViews>
-    <workbookView xWindow="-61548" yWindow="-1872" windowWidth="30936" windowHeight="16776" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-61548" yWindow="-1872" windowWidth="30936" windowHeight="16776" tabRatio="772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">NCCA_Map!$A$1:$A$57</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">Key!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="694">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2137,6 +2137,9 @@
   </si>
   <si>
     <t>Verbose description of decision made off of qa flags - PROBABLY DELETE THIS IN FINAL VESION</t>
+  </si>
+  <si>
+    <t>This is at the very surface with a hand held thermometer.  It's pretty sensitive to air temp/solar heating, but is a back up for when the CTD does not work or is not dropped.</t>
   </si>
 </sst>
 </file>
@@ -2624,35 +2627,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2660,10 +2639,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2677,6 +2656,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2982,7 +2985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944E5B29-DA5B-4213-9FBD-6DB720F31476}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -7695,8 +7698,8 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7753,11 +7756,13 @@
         <v>204</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>205</v>
+        <v>148</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>693</v>
+      </c>
       <c r="I2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8108,8 +8113,8 @@
       <c r="J2" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="77"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="26" t="s">
         <v>261</v>
       </c>
@@ -8146,8 +8151,8 @@
       <c r="J3" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="78"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="70"/>
       <c r="M3" s="9" t="s">
         <v>261</v>
       </c>
@@ -8184,8 +8189,8 @@
       <c r="J4" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="78"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="70"/>
       <c r="M4" s="9" t="s">
         <v>261</v>
       </c>
@@ -8220,8 +8225,8 @@
       <c r="J5" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="74"/>
-      <c r="L5" s="78"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="70"/>
       <c r="M5" s="9" t="s">
         <v>261</v>
       </c>
@@ -8258,10 +8263,10 @@
       <c r="J6" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K6" s="76" t="s">
+      <c r="K6" s="71" t="s">
         <v>271</v>
       </c>
-      <c r="L6" s="81"/>
+      <c r="L6" s="73"/>
       <c r="M6" s="9" t="s">
         <v>261</v>
       </c>
@@ -8298,8 +8303,8 @@
       <c r="J7" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K7" s="74"/>
-      <c r="L7" s="82"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="74"/>
       <c r="M7" s="9" t="s">
         <v>261</v>
       </c>
@@ -8334,8 +8339,8 @@
       <c r="J8" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K8" s="75"/>
-      <c r="L8" s="83"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="75"/>
       <c r="M8" s="9" t="s">
         <v>261</v>
       </c>
@@ -8372,10 +8377,10 @@
       <c r="J9" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K9" s="84" t="s">
+      <c r="K9" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="L9" s="79" t="s">
+      <c r="L9" s="78" t="s">
         <v>280</v>
       </c>
       <c r="M9" s="26" t="s">
@@ -8414,8 +8419,8 @@
       <c r="J10" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K10" s="68"/>
-      <c r="L10" s="78"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="70"/>
       <c r="M10" s="9" t="s">
         <v>261</v>
       </c>
@@ -8452,8 +8457,8 @@
       <c r="J11" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K11" s="68"/>
-      <c r="L11" s="78"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="70"/>
       <c r="M11" s="9" t="s">
         <v>261</v>
       </c>
@@ -8732,7 +8737,7 @@
       <c r="J18" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K18" s="76"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="24"/>
       <c r="M18" s="9" t="s">
         <v>261</v>
@@ -8770,7 +8775,7 @@
       <c r="J19" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K19" s="75"/>
+      <c r="K19" s="72"/>
       <c r="L19" s="46"/>
       <c r="M19" s="29" t="s">
         <v>261</v>
@@ -8808,10 +8813,10 @@
       <c r="J20" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K20" s="76" t="s">
+      <c r="K20" s="71" t="s">
         <v>314</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="L20" s="78" t="s">
         <v>315</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -8850,8 +8855,8 @@
       <c r="J21" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K21" s="74"/>
-      <c r="L21" s="78"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="70"/>
       <c r="M21" s="9" t="s">
         <v>261</v>
       </c>
@@ -8886,8 +8891,8 @@
       <c r="J22" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K22" s="74"/>
-      <c r="L22" s="78"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="70"/>
       <c r="M22" s="9" t="s">
         <v>261</v>
       </c>
@@ -8924,8 +8929,8 @@
       <c r="J23" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K23" s="74"/>
-      <c r="L23" s="78"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="70"/>
       <c r="M23" s="9" t="s">
         <v>261</v>
       </c>
@@ -8962,8 +8967,8 @@
       <c r="J24" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K24" s="74"/>
-      <c r="L24" s="78"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="70"/>
       <c r="M24" s="9" t="s">
         <v>261</v>
       </c>
@@ -9000,10 +9005,10 @@
       <c r="J25" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="K25" s="73" t="s">
+      <c r="K25" s="67" t="s">
         <v>321</v>
       </c>
-      <c r="L25" s="77" t="s">
+      <c r="L25" s="69" t="s">
         <v>322</v>
       </c>
       <c r="M25" s="26" t="s">
@@ -9042,8 +9047,8 @@
       <c r="J26" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K26" s="74"/>
-      <c r="L26" s="78"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="70"/>
       <c r="M26" s="9" t="s">
         <v>261</v>
       </c>
@@ -9080,8 +9085,8 @@
       <c r="J27" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K27" s="74"/>
-      <c r="L27" s="78"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="70"/>
       <c r="M27" s="9" t="s">
         <v>261</v>
       </c>
@@ -9116,8 +9121,8 @@
       <c r="J28" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K28" s="75"/>
-      <c r="L28" s="80"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="79"/>
       <c r="M28" s="29" t="s">
         <v>261</v>
       </c>
@@ -9154,7 +9159,7 @@
       <c r="J29" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K29" s="76" t="s">
+      <c r="K29" s="71" t="s">
         <v>327</v>
       </c>
       <c r="L29" s="24"/>
@@ -9194,7 +9199,7 @@
       <c r="J30" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K30" s="74"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="24"/>
       <c r="M30" s="9" t="s">
         <v>261</v>
@@ -9232,7 +9237,7 @@
       <c r="J31" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K31" s="74"/>
+      <c r="K31" s="68"/>
       <c r="L31" s="24"/>
       <c r="M31" s="9" t="s">
         <v>261</v>
@@ -9268,7 +9273,7 @@
       <c r="J32" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K32" s="74"/>
+      <c r="K32" s="68"/>
       <c r="L32" s="24"/>
       <c r="M32" s="9" t="s">
         <v>261</v>
@@ -9306,7 +9311,7 @@
       <c r="J33" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="K33" s="73" t="s">
+      <c r="K33" s="67" t="s">
         <v>294</v>
       </c>
       <c r="L33" s="45" t="s">
@@ -9348,7 +9353,7 @@
       <c r="J34" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K34" s="75"/>
+      <c r="K34" s="72"/>
       <c r="L34" s="46"/>
       <c r="M34" s="29" t="s">
         <v>261</v>
@@ -9386,7 +9391,7 @@
       <c r="J35" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K35" s="76" t="s">
+      <c r="K35" s="71" t="s">
         <v>294</v>
       </c>
       <c r="L35" s="24" t="s">
@@ -9428,7 +9433,7 @@
       <c r="J36" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K36" s="74"/>
+      <c r="K36" s="68"/>
       <c r="L36" s="24"/>
       <c r="M36" s="9" t="s">
         <v>261</v>
@@ -9545,7 +9550,7 @@
       <c r="K39" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="L39" s="77"/>
+      <c r="L39" s="69"/>
       <c r="M39" s="26" t="s">
         <v>261</v>
       </c>
@@ -9583,7 +9588,7 @@
         <v>261</v>
       </c>
       <c r="K40" s="37"/>
-      <c r="L40" s="78"/>
+      <c r="L40" s="70"/>
       <c r="M40" s="9" t="s">
         <v>261</v>
       </c>
@@ -9662,10 +9667,10 @@
       <c r="J42" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K42" s="76" t="s">
+      <c r="K42" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="L42" s="79" t="s">
+      <c r="L42" s="78" t="s">
         <v>352</v>
       </c>
       <c r="M42" s="26" t="s">
@@ -9704,8 +9709,8 @@
       <c r="J43" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K43" s="74"/>
-      <c r="L43" s="78"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="70"/>
       <c r="M43" s="9" t="s">
         <v>261</v>
       </c>
@@ -9742,8 +9747,8 @@
       <c r="J44" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K44" s="74"/>
-      <c r="L44" s="78"/>
+      <c r="K44" s="68"/>
+      <c r="L44" s="70"/>
       <c r="M44" s="9" t="s">
         <v>261</v>
       </c>
@@ -9778,8 +9783,8 @@
       <c r="J45" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K45" s="74"/>
-      <c r="L45" s="78"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="70"/>
       <c r="M45" s="9" t="s">
         <v>261</v>
       </c>
@@ -9816,8 +9821,8 @@
       <c r="J46" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K46" s="74"/>
-      <c r="L46" s="78"/>
+      <c r="K46" s="68"/>
+      <c r="L46" s="70"/>
       <c r="M46" s="9" t="s">
         <v>261</v>
       </c>
@@ -9854,8 +9859,8 @@
       <c r="J47" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K47" s="74"/>
-      <c r="L47" s="78"/>
+      <c r="K47" s="68"/>
+      <c r="L47" s="70"/>
       <c r="M47" s="9" t="s">
         <v>261</v>
       </c>
@@ -9972,7 +9977,7 @@
       <c r="J50" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="K50" s="67" t="s">
+      <c r="K50" s="80" t="s">
         <v>365</v>
       </c>
       <c r="L50" s="45"/>
@@ -10012,7 +10017,7 @@
       <c r="J51" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K51" s="68"/>
+      <c r="K51" s="77"/>
       <c r="L51" s="24"/>
       <c r="M51" s="26" t="s">
         <v>261</v>
@@ -10050,7 +10055,7 @@
       <c r="J52" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K52" s="68"/>
+      <c r="K52" s="77"/>
       <c r="L52" s="24"/>
       <c r="M52" s="26" t="s">
         <v>261</v>
@@ -10088,7 +10093,7 @@
       <c r="J53" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K53" s="68"/>
+      <c r="K53" s="77"/>
       <c r="L53" s="24"/>
       <c r="M53" s="26" t="s">
         <v>261</v>
@@ -10124,7 +10129,7 @@
       <c r="J54" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K54" s="69"/>
+      <c r="K54" s="81"/>
       <c r="L54" s="46"/>
       <c r="M54" s="26" t="s">
         <v>261</v>
@@ -10244,7 +10249,7 @@
       <c r="J57" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K57" s="76" t="s">
+      <c r="K57" s="71" t="s">
         <v>382</v>
       </c>
       <c r="L57" s="24"/>
@@ -10284,7 +10289,7 @@
       <c r="J58" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K58" s="74"/>
+      <c r="K58" s="68"/>
       <c r="L58" s="24"/>
       <c r="M58" s="9" t="s">
         <v>261</v>
@@ -10320,7 +10325,7 @@
       <c r="J59" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K59" s="74"/>
+      <c r="K59" s="68"/>
       <c r="L59" s="24"/>
       <c r="M59" s="9" t="s">
         <v>261</v>
@@ -10358,7 +10363,7 @@
       <c r="J60" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="K60" s="77" t="s">
+      <c r="K60" s="69" t="s">
         <v>387</v>
       </c>
       <c r="L60" s="45"/>
@@ -10398,7 +10403,7 @@
       <c r="J61" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="K61" s="78"/>
+      <c r="K61" s="70"/>
       <c r="L61" s="24" t="s">
         <v>389</v>
       </c>
@@ -10438,7 +10443,7 @@
       <c r="J62" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K62" s="78"/>
+      <c r="K62" s="70"/>
       <c r="L62" s="24" t="s">
         <v>391</v>
       </c>
@@ -10478,7 +10483,7 @@
       <c r="J63" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="K63" s="76"/>
+      <c r="K63" s="71"/>
       <c r="L63" s="24"/>
       <c r="M63" s="9" t="s">
         <v>261</v>
@@ -10516,7 +10521,7 @@
       <c r="J64" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="K64" s="74"/>
+      <c r="K64" s="68"/>
       <c r="L64" s="24"/>
       <c r="M64" s="9" t="s">
         <v>261</v>
@@ -10554,7 +10559,7 @@
       <c r="J65" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="K65" s="74"/>
+      <c r="K65" s="68"/>
       <c r="L65" s="24" t="s">
         <v>391</v>
       </c>
@@ -10592,7 +10597,7 @@
       <c r="J66" s="49" t="s">
         <v>261</v>
       </c>
-      <c r="K66" s="74"/>
+      <c r="K66" s="68"/>
       <c r="L66" s="13"/>
       <c r="M66" s="36" t="s">
         <v>261</v>
@@ -10706,7 +10711,7 @@
       <c r="J69" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K69" s="76" t="s">
+      <c r="K69" s="71" t="s">
         <v>294</v>
       </c>
       <c r="L69" s="24" t="s">
@@ -10748,7 +10753,7 @@
       <c r="J70" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K70" s="74"/>
+      <c r="K70" s="68"/>
       <c r="L70" s="24"/>
       <c r="M70" s="9" t="s">
         <v>261</v>
@@ -10826,7 +10831,7 @@
       <c r="J72" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K72" s="76"/>
+      <c r="K72" s="71"/>
       <c r="L72" s="24"/>
       <c r="M72" s="9" t="s">
         <v>261</v>
@@ -10862,7 +10867,7 @@
       <c r="J73" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K73" s="74"/>
+      <c r="K73" s="68"/>
       <c r="L73" s="24"/>
       <c r="M73" s="9" t="s">
         <v>261</v>
@@ -10898,7 +10903,7 @@
       <c r="J74" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K74" s="74"/>
+      <c r="K74" s="68"/>
       <c r="L74" s="24"/>
       <c r="M74" s="9" t="s">
         <v>261</v>
@@ -10932,7 +10937,7 @@
       <c r="J75" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K75" s="75"/>
+      <c r="K75" s="72"/>
       <c r="L75" s="46"/>
       <c r="M75" s="9" t="s">
         <v>261</v>
@@ -11010,10 +11015,10 @@
       <c r="J77" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="K77" s="67" t="s">
+      <c r="K77" s="80" t="s">
         <v>414</v>
       </c>
-      <c r="L77" s="73" t="s">
+      <c r="L77" s="67" t="s">
         <v>415</v>
       </c>
       <c r="M77" s="26" t="s">
@@ -11054,8 +11059,8 @@
       <c r="J78" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K78" s="69"/>
-      <c r="L78" s="71"/>
+      <c r="K78" s="81"/>
+      <c r="L78" s="83"/>
       <c r="M78" s="36" t="s">
         <v>261</v>
       </c>
@@ -11095,7 +11100,7 @@
       <c r="K79" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="L79" s="71"/>
+      <c r="L79" s="83"/>
       <c r="M79" s="36" t="s">
         <v>261</v>
       </c>
@@ -11135,7 +11140,7 @@
       <c r="K80" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="L80" s="75"/>
+      <c r="L80" s="72"/>
       <c r="M80" s="9" t="s">
         <v>261</v>
       </c>
@@ -11172,7 +11177,7 @@
       <c r="J81" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K81" s="76" t="s">
+      <c r="K81" s="71" t="s">
         <v>294</v>
       </c>
       <c r="L81" s="24" t="s">
@@ -11214,7 +11219,7 @@
       <c r="J82" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K82" s="74"/>
+      <c r="K82" s="68"/>
       <c r="L82" s="24"/>
       <c r="M82" s="9" t="s">
         <v>261</v>
@@ -11336,7 +11341,7 @@
       <c r="J85" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K85" s="76" t="s">
+      <c r="K85" s="71" t="s">
         <v>428</v>
       </c>
       <c r="L85" s="24"/>
@@ -11376,7 +11381,7 @@
       <c r="J86" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K86" s="74"/>
+      <c r="K86" s="68"/>
       <c r="L86" s="24"/>
       <c r="M86" s="9" t="s">
         <v>261</v>
@@ -11414,7 +11419,7 @@
       <c r="J87" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K87" s="74"/>
+      <c r="K87" s="68"/>
       <c r="L87" s="24"/>
       <c r="M87" s="9" t="s">
         <v>261</v>
@@ -11450,7 +11455,7 @@
       <c r="J88" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K88" s="74"/>
+      <c r="K88" s="68"/>
       <c r="L88" s="24"/>
       <c r="M88" s="9" t="s">
         <v>261</v>
@@ -11488,7 +11493,7 @@
       <c r="J89" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K89" s="74"/>
+      <c r="K89" s="68"/>
       <c r="L89" s="24"/>
       <c r="M89" s="9" t="s">
         <v>261</v>
@@ -11526,7 +11531,7 @@
       <c r="J90" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K90" s="74"/>
+      <c r="K90" s="68"/>
       <c r="L90" s="24"/>
       <c r="M90" s="9" t="s">
         <v>261</v>
@@ -11564,10 +11569,10 @@
       <c r="J91" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K91" s="67" t="s">
+      <c r="K91" s="80" t="s">
         <v>434</v>
       </c>
-      <c r="L91" s="70" t="s">
+      <c r="L91" s="82" t="s">
         <v>435</v>
       </c>
       <c r="M91" s="26" t="s">
@@ -11606,8 +11611,8 @@
       <c r="J92" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="K92" s="68"/>
-      <c r="L92" s="71"/>
+      <c r="K92" s="77"/>
+      <c r="L92" s="83"/>
       <c r="M92" s="9" t="s">
         <v>261</v>
       </c>
@@ -11644,8 +11649,8 @@
       <c r="J93" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="K93" s="68"/>
-      <c r="L93" s="71"/>
+      <c r="K93" s="77"/>
+      <c r="L93" s="83"/>
       <c r="M93" s="9" t="s">
         <v>261</v>
       </c>
@@ -11680,8 +11685,8 @@
       <c r="J94" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K94" s="69"/>
-      <c r="L94" s="72"/>
+      <c r="K94" s="81"/>
+      <c r="L94" s="84"/>
       <c r="M94" s="9" t="s">
         <v>261</v>
       </c>
@@ -11718,7 +11723,7 @@
       <c r="J95" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K95" s="73"/>
+      <c r="K95" s="67"/>
       <c r="L95" s="24"/>
       <c r="M95" s="26" t="s">
         <v>261</v>
@@ -11756,7 +11761,7 @@
       <c r="J96" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K96" s="74"/>
+      <c r="K96" s="68"/>
       <c r="L96" s="24"/>
       <c r="M96" s="26" t="s">
         <v>261</v>
@@ -11794,7 +11799,7 @@
       <c r="J97" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K97" s="74"/>
+      <c r="K97" s="68"/>
       <c r="L97" s="24"/>
       <c r="M97" s="26" t="s">
         <v>261</v>
@@ -11832,7 +11837,7 @@
       <c r="J98" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K98" s="74"/>
+      <c r="K98" s="68"/>
       <c r="L98" s="24"/>
       <c r="M98" s="26" t="s">
         <v>261</v>
@@ -11868,7 +11873,7 @@
       <c r="J99" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="K99" s="75"/>
+      <c r="K99" s="72"/>
       <c r="L99" s="39"/>
       <c r="M99" s="41" t="s">
         <v>261</v>
@@ -11897,28 +11902,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -11927,6 +11910,28 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added flags for imputed station depth.
</commit_message>
<xml_diff>
--- a/Meta/Analytes3.xlsx
+++ b/Meta/Analytes3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0590F522-D08C-4A00-9657-FC9AD45A1A26}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="11_CFA7FA0AC8BEC675FF6906A82B7A2EC91D13FE60" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8361E64-7C45-4EF3-BCFD-77BAB08BCB01}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="772" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="802" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="693">
   <si>
     <t>ANALYTE</t>
   </si>
@@ -2125,6 +2125,18 @@
   </si>
   <si>
     <t>Units of associated measurement. SHOULD PROBABLY BE REMOVED - FROM ANALYTES3, NOT THE DATA</t>
+  </si>
+  <si>
+    <t>sampleDate</t>
+  </si>
+  <si>
+    <t>sampleTime</t>
+  </si>
+  <si>
+    <t>Date of sampling event (1983/04/19--2023/08/05)</t>
+  </si>
+  <si>
+    <t>Hour of sampling event. Missing if time was not recorded</t>
   </si>
 </sst>
 </file>
@@ -2602,11 +2614,35 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2614,10 +2650,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2631,30 +2667,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2958,10 +2970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944E5B29-DA5B-4213-9FBD-6DB720F31476}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3048,185 +3060,201 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="65" t="s">
-        <v>647</v>
+        <v>689</v>
       </c>
       <c r="B14" t="s">
-        <v>648</v>
+        <v>691</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="65" t="s">
-        <v>649</v>
+        <v>690</v>
       </c>
       <c r="B15" t="s">
-        <v>650</v>
+        <v>692</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="65" t="s">
-        <v>5</v>
+        <v>647</v>
       </c>
       <c r="B16" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="65" t="s">
-        <v>568</v>
+        <v>649</v>
       </c>
       <c r="B17" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="65" t="s">
-        <v>653</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="65" t="s">
-        <v>4</v>
+        <v>568</v>
       </c>
       <c r="B19" t="s">
-        <v>688</v>
+        <v>652</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="65" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B20" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="65" t="s">
-        <v>657</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>658</v>
+        <v>688</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="65" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B22" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="65" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B23" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="65" t="s">
-        <v>569</v>
+        <v>659</v>
       </c>
       <c r="B24" t="s">
-        <v>679</v>
+        <v>660</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="65" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B25" t="s">
-        <v>680</v>
+        <v>662</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="65" t="s">
-        <v>664</v>
+        <v>569</v>
       </c>
       <c r="B26" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="65" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B27" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B28" t="s">
-        <v>668</v>
+        <v>681</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="65" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B29" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="65" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="B30" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="65" t="s">
-        <v>151</v>
+        <v>669</v>
       </c>
       <c r="B31" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="65" t="s">
-        <v>150</v>
+        <v>671</v>
       </c>
       <c r="B32" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="65" t="s">
-        <v>676</v>
+        <v>150</v>
       </c>
       <c r="B34" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="65" t="s">
+        <v>676</v>
+      </c>
+      <c r="B36" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="65" t="s">
         <v>677</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="63"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="64"/>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="63"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8084,8 +8112,8 @@
       <c r="J2" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="68"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="76"/>
       <c r="M2" s="25" t="s">
         <v>259</v>
       </c>
@@ -8122,8 +8150,8 @@
       <c r="J3" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K3" s="67"/>
-      <c r="L3" s="69"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="77"/>
       <c r="M3" s="9" t="s">
         <v>259</v>
       </c>
@@ -8160,8 +8188,8 @@
       <c r="J4" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K4" s="67"/>
-      <c r="L4" s="69"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="77"/>
       <c r="M4" s="9" t="s">
         <v>259</v>
       </c>
@@ -8196,8 +8224,8 @@
       <c r="J5" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="69"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="77"/>
       <c r="M5" s="9" t="s">
         <v>259</v>
       </c>
@@ -8234,10 +8262,10 @@
       <c r="J6" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K6" s="70" t="s">
+      <c r="K6" s="75" t="s">
         <v>269</v>
       </c>
-      <c r="L6" s="72"/>
+      <c r="L6" s="80"/>
       <c r="M6" s="9" t="s">
         <v>259</v>
       </c>
@@ -8274,8 +8302,8 @@
       <c r="J7" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K7" s="67"/>
-      <c r="L7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="81"/>
       <c r="M7" s="9" t="s">
         <v>259</v>
       </c>
@@ -8310,8 +8338,8 @@
       <c r="J8" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K8" s="71"/>
-      <c r="L8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="82"/>
       <c r="M8" s="9" t="s">
         <v>259</v>
       </c>
@@ -8348,10 +8376,10 @@
       <c r="J9" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K9" s="75" t="s">
+      <c r="K9" s="83" t="s">
         <v>277</v>
       </c>
-      <c r="L9" s="77" t="s">
+      <c r="L9" s="78" t="s">
         <v>278</v>
       </c>
       <c r="M9" s="25" t="s">
@@ -8390,8 +8418,8 @@
       <c r="J10" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K10" s="76"/>
-      <c r="L10" s="69"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="77"/>
       <c r="M10" s="9" t="s">
         <v>259</v>
       </c>
@@ -8428,8 +8456,8 @@
       <c r="J11" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K11" s="76"/>
-      <c r="L11" s="69"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="77"/>
       <c r="M11" s="9" t="s">
         <v>259</v>
       </c>
@@ -8708,7 +8736,7 @@
       <c r="J18" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K18" s="70"/>
+      <c r="K18" s="75"/>
       <c r="L18" s="23"/>
       <c r="M18" s="9" t="s">
         <v>259</v>
@@ -8746,7 +8774,7 @@
       <c r="J19" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K19" s="71"/>
+      <c r="K19" s="74"/>
       <c r="L19" s="45"/>
       <c r="M19" s="28" t="s">
         <v>259</v>
@@ -8784,10 +8812,10 @@
       <c r="J20" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="K20" s="75" t="s">
         <v>312</v>
       </c>
-      <c r="L20" s="77" t="s">
+      <c r="L20" s="78" t="s">
         <v>313</v>
       </c>
       <c r="M20" s="9" t="s">
@@ -8826,8 +8854,8 @@
       <c r="J21" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K21" s="67"/>
-      <c r="L21" s="69"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="77"/>
       <c r="M21" s="9" t="s">
         <v>259</v>
       </c>
@@ -8862,8 +8890,8 @@
       <c r="J22" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K22" s="67"/>
-      <c r="L22" s="69"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="77"/>
       <c r="M22" s="9" t="s">
         <v>259</v>
       </c>
@@ -8900,8 +8928,8 @@
       <c r="J23" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K23" s="67"/>
-      <c r="L23" s="69"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="77"/>
       <c r="M23" s="9" t="s">
         <v>259</v>
       </c>
@@ -8938,8 +8966,8 @@
       <c r="J24" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K24" s="67"/>
-      <c r="L24" s="69"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="77"/>
       <c r="M24" s="9" t="s">
         <v>259</v>
       </c>
@@ -8976,10 +9004,10 @@
       <c r="J25" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="K25" s="66" t="s">
+      <c r="K25" s="72" t="s">
         <v>319</v>
       </c>
-      <c r="L25" s="68" t="s">
+      <c r="L25" s="76" t="s">
         <v>320</v>
       </c>
       <c r="M25" s="25" t="s">
@@ -9018,8 +9046,8 @@
       <c r="J26" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K26" s="67"/>
-      <c r="L26" s="69"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="77"/>
       <c r="M26" s="9" t="s">
         <v>259</v>
       </c>
@@ -9056,8 +9084,8 @@
       <c r="J27" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K27" s="67"/>
-      <c r="L27" s="69"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="77"/>
       <c r="M27" s="9" t="s">
         <v>259</v>
       </c>
@@ -9092,8 +9120,8 @@
       <c r="J28" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K28" s="71"/>
-      <c r="L28" s="78"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="79"/>
       <c r="M28" s="28" t="s">
         <v>259</v>
       </c>
@@ -9130,7 +9158,7 @@
       <c r="J29" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K29" s="70" t="s">
+      <c r="K29" s="75" t="s">
         <v>325</v>
       </c>
       <c r="L29" s="23"/>
@@ -9170,7 +9198,7 @@
       <c r="J30" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K30" s="67"/>
+      <c r="K30" s="73"/>
       <c r="L30" s="23"/>
       <c r="M30" s="9" t="s">
         <v>259</v>
@@ -9208,7 +9236,7 @@
       <c r="J31" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K31" s="67"/>
+      <c r="K31" s="73"/>
       <c r="L31" s="23"/>
       <c r="M31" s="9" t="s">
         <v>259</v>
@@ -9244,7 +9272,7 @@
       <c r="J32" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K32" s="67"/>
+      <c r="K32" s="73"/>
       <c r="L32" s="23"/>
       <c r="M32" s="9" t="s">
         <v>259</v>
@@ -9282,7 +9310,7 @@
       <c r="J33" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="K33" s="66" t="s">
+      <c r="K33" s="72" t="s">
         <v>292</v>
       </c>
       <c r="L33" s="44" t="s">
@@ -9324,7 +9352,7 @@
       <c r="J34" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K34" s="71"/>
+      <c r="K34" s="74"/>
       <c r="L34" s="45"/>
       <c r="M34" s="28" t="s">
         <v>259</v>
@@ -9362,7 +9390,7 @@
       <c r="J35" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K35" s="70" t="s">
+      <c r="K35" s="75" t="s">
         <v>292</v>
       </c>
       <c r="L35" s="23" t="s">
@@ -9404,7 +9432,7 @@
       <c r="J36" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K36" s="67"/>
+      <c r="K36" s="73"/>
       <c r="L36" s="23"/>
       <c r="M36" s="9" t="s">
         <v>259</v>
@@ -9521,7 +9549,7 @@
       <c r="K39" s="47" t="s">
         <v>342</v>
       </c>
-      <c r="L39" s="68"/>
+      <c r="L39" s="76"/>
       <c r="M39" s="25" t="s">
         <v>259</v>
       </c>
@@ -9559,7 +9587,7 @@
         <v>259</v>
       </c>
       <c r="K40" s="36"/>
-      <c r="L40" s="69"/>
+      <c r="L40" s="77"/>
       <c r="M40" s="9" t="s">
         <v>259</v>
       </c>
@@ -9638,10 +9666,10 @@
       <c r="J42" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K42" s="70" t="s">
+      <c r="K42" s="75" t="s">
         <v>349</v>
       </c>
-      <c r="L42" s="77" t="s">
+      <c r="L42" s="78" t="s">
         <v>350</v>
       </c>
       <c r="M42" s="25" t="s">
@@ -9680,8 +9708,8 @@
       <c r="J43" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K43" s="67"/>
-      <c r="L43" s="69"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="77"/>
       <c r="M43" s="9" t="s">
         <v>259</v>
       </c>
@@ -9718,8 +9746,8 @@
       <c r="J44" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K44" s="67"/>
-      <c r="L44" s="69"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="77"/>
       <c r="M44" s="9" t="s">
         <v>259</v>
       </c>
@@ -9754,8 +9782,8 @@
       <c r="J45" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K45" s="67"/>
-      <c r="L45" s="69"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="77"/>
       <c r="M45" s="9" t="s">
         <v>259</v>
       </c>
@@ -9792,8 +9820,8 @@
       <c r="J46" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K46" s="67"/>
-      <c r="L46" s="69"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="77"/>
       <c r="M46" s="9" t="s">
         <v>259</v>
       </c>
@@ -9830,8 +9858,8 @@
       <c r="J47" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K47" s="67"/>
-      <c r="L47" s="69"/>
+      <c r="K47" s="73"/>
+      <c r="L47" s="77"/>
       <c r="M47" s="9" t="s">
         <v>259</v>
       </c>
@@ -9948,7 +9976,7 @@
       <c r="J50" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="K50" s="79" t="s">
+      <c r="K50" s="66" t="s">
         <v>363</v>
       </c>
       <c r="L50" s="44"/>
@@ -9988,7 +10016,7 @@
       <c r="J51" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K51" s="76"/>
+      <c r="K51" s="67"/>
       <c r="L51" s="23"/>
       <c r="M51" s="25" t="s">
         <v>259</v>
@@ -10026,7 +10054,7 @@
       <c r="J52" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K52" s="76"/>
+      <c r="K52" s="67"/>
       <c r="L52" s="23"/>
       <c r="M52" s="25" t="s">
         <v>259</v>
@@ -10064,7 +10092,7 @@
       <c r="J53" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K53" s="76"/>
+      <c r="K53" s="67"/>
       <c r="L53" s="23"/>
       <c r="M53" s="25" t="s">
         <v>259</v>
@@ -10100,7 +10128,7 @@
       <c r="J54" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K54" s="80"/>
+      <c r="K54" s="68"/>
       <c r="L54" s="45"/>
       <c r="M54" s="25" t="s">
         <v>259</v>
@@ -10220,7 +10248,7 @@
       <c r="J57" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K57" s="70" t="s">
+      <c r="K57" s="75" t="s">
         <v>380</v>
       </c>
       <c r="L57" s="23"/>
@@ -10260,7 +10288,7 @@
       <c r="J58" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K58" s="67"/>
+      <c r="K58" s="73"/>
       <c r="L58" s="23"/>
       <c r="M58" s="9" t="s">
         <v>259</v>
@@ -10296,7 +10324,7 @@
       <c r="J59" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K59" s="67"/>
+      <c r="K59" s="73"/>
       <c r="L59" s="23"/>
       <c r="M59" s="9" t="s">
         <v>259</v>
@@ -10334,7 +10362,7 @@
       <c r="J60" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="K60" s="68" t="s">
+      <c r="K60" s="76" t="s">
         <v>385</v>
       </c>
       <c r="L60" s="44"/>
@@ -10374,7 +10402,7 @@
       <c r="J61" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="K61" s="69"/>
+      <c r="K61" s="77"/>
       <c r="L61" s="23" t="s">
         <v>387</v>
       </c>
@@ -10414,7 +10442,7 @@
       <c r="J62" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K62" s="69"/>
+      <c r="K62" s="77"/>
       <c r="L62" s="23" t="s">
         <v>389</v>
       </c>
@@ -10454,7 +10482,7 @@
       <c r="J63" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="K63" s="70"/>
+      <c r="K63" s="75"/>
       <c r="L63" s="23"/>
       <c r="M63" s="9" t="s">
         <v>259</v>
@@ -10492,7 +10520,7 @@
       <c r="J64" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="K64" s="67"/>
+      <c r="K64" s="73"/>
       <c r="L64" s="23"/>
       <c r="M64" s="9" t="s">
         <v>259</v>
@@ -10530,7 +10558,7 @@
       <c r="J65" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="K65" s="67"/>
+      <c r="K65" s="73"/>
       <c r="L65" s="23" t="s">
         <v>389</v>
       </c>
@@ -10568,7 +10596,7 @@
       <c r="J66" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="K66" s="67"/>
+      <c r="K66" s="73"/>
       <c r="L66" s="13"/>
       <c r="M66" s="35" t="s">
         <v>259</v>
@@ -10682,7 +10710,7 @@
       <c r="J69" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K69" s="70" t="s">
+      <c r="K69" s="75" t="s">
         <v>292</v>
       </c>
       <c r="L69" s="23" t="s">
@@ -10724,7 +10752,7 @@
       <c r="J70" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K70" s="67"/>
+      <c r="K70" s="73"/>
       <c r="L70" s="23"/>
       <c r="M70" s="9" t="s">
         <v>259</v>
@@ -10802,7 +10830,7 @@
       <c r="J72" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K72" s="70"/>
+      <c r="K72" s="75"/>
       <c r="L72" s="23"/>
       <c r="M72" s="9" t="s">
         <v>259</v>
@@ -10838,7 +10866,7 @@
       <c r="J73" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K73" s="67"/>
+      <c r="K73" s="73"/>
       <c r="L73" s="23"/>
       <c r="M73" s="9" t="s">
         <v>259</v>
@@ -10874,7 +10902,7 @@
       <c r="J74" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K74" s="67"/>
+      <c r="K74" s="73"/>
       <c r="L74" s="23"/>
       <c r="M74" s="9" t="s">
         <v>259</v>
@@ -10908,7 +10936,7 @@
       <c r="J75" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K75" s="71"/>
+      <c r="K75" s="74"/>
       <c r="L75" s="45"/>
       <c r="M75" s="9" t="s">
         <v>259</v>
@@ -10986,10 +11014,10 @@
       <c r="J77" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="K77" s="79" t="s">
+      <c r="K77" s="66" t="s">
         <v>412</v>
       </c>
-      <c r="L77" s="66" t="s">
+      <c r="L77" s="72" t="s">
         <v>413</v>
       </c>
       <c r="M77" s="25" t="s">
@@ -11030,8 +11058,8 @@
       <c r="J78" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K78" s="80"/>
-      <c r="L78" s="82"/>
+      <c r="K78" s="68"/>
+      <c r="L78" s="70"/>
       <c r="M78" s="35" t="s">
         <v>259</v>
       </c>
@@ -11071,7 +11099,7 @@
       <c r="K79" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="L79" s="82"/>
+      <c r="L79" s="70"/>
       <c r="M79" s="35" t="s">
         <v>259</v>
       </c>
@@ -11111,7 +11139,7 @@
       <c r="K80" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="L80" s="71"/>
+      <c r="L80" s="74"/>
       <c r="M80" s="9" t="s">
         <v>259</v>
       </c>
@@ -11148,7 +11176,7 @@
       <c r="J81" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K81" s="70" t="s">
+      <c r="K81" s="75" t="s">
         <v>292</v>
       </c>
       <c r="L81" s="23" t="s">
@@ -11190,7 +11218,7 @@
       <c r="J82" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K82" s="67"/>
+      <c r="K82" s="73"/>
       <c r="L82" s="23"/>
       <c r="M82" s="9" t="s">
         <v>259</v>
@@ -11312,7 +11340,7 @@
       <c r="J85" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K85" s="70" t="s">
+      <c r="K85" s="75" t="s">
         <v>426</v>
       </c>
       <c r="L85" s="23"/>
@@ -11352,7 +11380,7 @@
       <c r="J86" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K86" s="67"/>
+      <c r="K86" s="73"/>
       <c r="L86" s="23"/>
       <c r="M86" s="9" t="s">
         <v>259</v>
@@ -11390,7 +11418,7 @@
       <c r="J87" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K87" s="67"/>
+      <c r="K87" s="73"/>
       <c r="L87" s="23"/>
       <c r="M87" s="9" t="s">
         <v>259</v>
@@ -11426,7 +11454,7 @@
       <c r="J88" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K88" s="67"/>
+      <c r="K88" s="73"/>
       <c r="L88" s="23"/>
       <c r="M88" s="9" t="s">
         <v>259</v>
@@ -11464,7 +11492,7 @@
       <c r="J89" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K89" s="67"/>
+      <c r="K89" s="73"/>
       <c r="L89" s="23"/>
       <c r="M89" s="9" t="s">
         <v>259</v>
@@ -11502,7 +11530,7 @@
       <c r="J90" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K90" s="67"/>
+      <c r="K90" s="73"/>
       <c r="L90" s="23"/>
       <c r="M90" s="9" t="s">
         <v>259</v>
@@ -11540,10 +11568,10 @@
       <c r="J91" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K91" s="79" t="s">
+      <c r="K91" s="66" t="s">
         <v>432</v>
       </c>
-      <c r="L91" s="81" t="s">
+      <c r="L91" s="69" t="s">
         <v>433</v>
       </c>
       <c r="M91" s="25" t="s">
@@ -11582,8 +11610,8 @@
       <c r="J92" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="K92" s="76"/>
-      <c r="L92" s="82"/>
+      <c r="K92" s="67"/>
+      <c r="L92" s="70"/>
       <c r="M92" s="9" t="s">
         <v>259</v>
       </c>
@@ -11620,8 +11648,8 @@
       <c r="J93" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="K93" s="76"/>
-      <c r="L93" s="82"/>
+      <c r="K93" s="67"/>
+      <c r="L93" s="70"/>
       <c r="M93" s="9" t="s">
         <v>259</v>
       </c>
@@ -11656,8 +11684,8 @@
       <c r="J94" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K94" s="80"/>
-      <c r="L94" s="83"/>
+      <c r="K94" s="68"/>
+      <c r="L94" s="71"/>
       <c r="M94" s="9" t="s">
         <v>259</v>
       </c>
@@ -11694,7 +11722,7 @@
       <c r="J95" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K95" s="66"/>
+      <c r="K95" s="72"/>
       <c r="L95" s="23"/>
       <c r="M95" s="25" t="s">
         <v>259</v>
@@ -11732,7 +11760,7 @@
       <c r="J96" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K96" s="67"/>
+      <c r="K96" s="73"/>
       <c r="L96" s="23"/>
       <c r="M96" s="25" t="s">
         <v>259</v>
@@ -11770,7 +11798,7 @@
       <c r="J97" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K97" s="67"/>
+      <c r="K97" s="73"/>
       <c r="L97" s="23"/>
       <c r="M97" s="25" t="s">
         <v>259</v>
@@ -11808,7 +11836,7 @@
       <c r="J98" s="35" t="s">
         <v>259</v>
       </c>
-      <c r="K98" s="67"/>
+      <c r="K98" s="73"/>
       <c r="L98" s="23"/>
       <c r="M98" s="25" t="s">
         <v>259</v>
@@ -11844,7 +11872,7 @@
       <c r="J99" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K99" s="71"/>
+      <c r="K99" s="74"/>
       <c r="L99" s="38"/>
       <c r="M99" s="40" t="s">
         <v>259</v>
@@ -11873,6 +11901,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K2:K5"/>
+    <mergeCell ref="L2:L5"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K25:K28"/>
+    <mergeCell ref="L25:L28"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="K42:K47"/>
+    <mergeCell ref="L42:L47"/>
+    <mergeCell ref="K50:K54"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="K63:K66"/>
+    <mergeCell ref="K69:K70"/>
     <mergeCell ref="K91:K94"/>
     <mergeCell ref="L91:L94"/>
     <mergeCell ref="K95:K99"/>
@@ -11881,28 +11931,6 @@
     <mergeCell ref="L77:L80"/>
     <mergeCell ref="K81:K82"/>
     <mergeCell ref="K85:K90"/>
-    <mergeCell ref="K50:K54"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="K60:K62"/>
-    <mergeCell ref="K63:K66"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="K42:K47"/>
-    <mergeCell ref="L42:L47"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K25:K28"/>
-    <mergeCell ref="L25:L28"/>
-    <mergeCell ref="K2:K5"/>
-    <mergeCell ref="L2:L5"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="L9:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11975,7 +12003,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>